<commit_message>
HoangNH - Update Manager Test Case
</commit_message>
<xml_diff>
--- a/3. Users/HoangNHHE130395/Testing/TestCase - Hoang.xlsx
+++ b/3. Users/HoangNHHE130395/Testing/TestCase - Hoang.xlsx
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="466">
   <si>
     <t>SYSTEM TEST CASE</t>
   </si>
@@ -1813,6 +1813,162 @@
     <t>1. Display text 'aa' on the search box 
 2. Border of the search box change to blue
 3. Display list of user have email contain character 'a'</t>
+  </si>
+  <si>
+    <t>[Manager-16]</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'User' tab in the menu bar
+3. Choose 'Fullname' from the drop down list
+4. Click on the search box 'Search user'
+5. Input text 'a' on the search box</t>
+  </si>
+  <si>
+    <t>1. Display text 'a' on the search box 
+2. Border of the search box change to blue
+3. Display list of user have fullname contain character 'a'</t>
+  </si>
+  <si>
+    <t>[Manager-17]</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'User' tab in the menu bar
+3. Choose 'Fullname' from the drop down list
+4. Click on the search box 'Search user'
+5. Input text 'a' on the search box
+6. Input text 'a' on the search box</t>
+  </si>
+  <si>
+    <t>1. Display text 'aa' on the search box 
+2. Border of the search box change to blue
+3. Display list of user have fullname contain character 'aa'</t>
+  </si>
+  <si>
+    <t>[Manager-18]</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'User' tab in the menu bar
+3. Choose 'Fullname' from the drop down list
+4. Click on the search box 'Search user'
+5. Input text 'a' on the search box
+6. Input text 'a' on the search box
+7. Press delete button on keyboard</t>
+  </si>
+  <si>
+    <t>1. Display text 'aa' on the search box 
+2. Border of the search box change to blue
+3. Display list of user have fullname contain character 'a'</t>
+  </si>
+  <si>
+    <t>[Manager-19]</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'User' tab in the menu bar
+3. Choose 'Phone' from the drop down list
+4. Click on the search box 'Search user'
+5. Input text 'a' on the search box</t>
+  </si>
+  <si>
+    <t>1. Display text 'a' on the search box 
+2. Border of the search box change to blue
+3. Display list of user have phone contain character 'a'</t>
+  </si>
+  <si>
+    <t>[Manager-20]</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'User' tab in the menu bar
+3. Choose 'Phone' from the drop down list
+4. Click on the search box 'Search user'
+5. Input text 'a' on the search box
+6. Input text 'a' on the search box</t>
+  </si>
+  <si>
+    <t>1. Display text 'aa' on the search box 
+2. Border of the search box change to blue
+3. Display list of user have phone contain character 'aa'</t>
+  </si>
+  <si>
+    <t>[Manager-21]</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'User' tab in the menu bar
+3. Choose 'Phone' from the drop down list
+4. Click on the search box 'Search user'
+5. Input text 'a' on the search box
+6. Input text 'a' on the search box
+7. Press delete button on keyboard</t>
+  </si>
+  <si>
+    <t>1. Display text 'aa' on the search box 
+2. Border of the search box change to blue
+3. Display list of user have phone contain character 'a'</t>
+  </si>
+  <si>
+    <t>[Manager-22]</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'User' tab in the menu bar
+3. Choose 'Phone' from the drop down list
+4. Click on the search box 'Search user'
+5. Input text 'a' on the search box
+6. Choose 'Username' from the drop down list</t>
+  </si>
+  <si>
+    <t>[Manager-23]</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'User' tab in the menu bar
+3. Choose 'Phone' from the drop down list
+4. Click on the search box 'Search user'
+5. Input text 'a' on the search box
+6. Choose 'Email' from the drop down list</t>
+  </si>
+  <si>
+    <t>[Manager-24]</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'User' tab in the menu bar
+3. Choose 'Phone' from the drop down list
+4. Click on the search box 'Search user'
+5. Input text 'a' on the search box
+6. Choose 'Fullname' from the drop down list</t>
+  </si>
+  <si>
+    <t>[Manager-25]</t>
+  </si>
+  <si>
+    <t>Check GUI list users</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Login into the web server
+2. Click on 'User' tab in the menu bar
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Display list users with following column: "ID, Username, Email, Fullname, Phone, Date created, Avatar, Status, Option" </t>
+  </si>
+  <si>
+    <t>[Manager-26]</t>
+  </si>
+  <si>
+    <t>Check data in column of list users</t>
+  </si>
+  <si>
+    <t>1. Display list users with following column: "ID, Username, Email, Fullname, Phone, Date created, Avatar, Status, Option" 
+2. The data of user is mapping wit the column name</t>
+  </si>
+  <si>
+    <t>[Manager-27]</t>
   </si>
   <si>
     <t>TEST REPORT</t>
@@ -2675,7 +2831,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="204">
+  <cellXfs count="203">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -3105,9 +3261,6 @@
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -28516,7 +28669,9 @@
       <c r="E22" s="160" t="s">
         <v>372</v>
       </c>
-      <c r="F22" s="117"/>
+      <c r="F22" s="161" t="s">
+        <v>408</v>
+      </c>
       <c r="G22" s="162" t="s">
         <v>83</v>
       </c>
@@ -28561,7 +28716,9 @@
       <c r="E23" s="160" t="s">
         <v>372</v>
       </c>
-      <c r="F23" s="117"/>
+      <c r="F23" s="161" t="s">
+        <v>412</v>
+      </c>
       <c r="G23" s="162" t="s">
         <v>83</v>
       </c>
@@ -28606,7 +28763,9 @@
       <c r="E24" s="160" t="s">
         <v>372</v>
       </c>
-      <c r="F24" s="161"/>
+      <c r="F24" s="161" t="s">
+        <v>412</v>
+      </c>
       <c r="G24" s="162" t="s">
         <v>83</v>
       </c>
@@ -28637,21 +28796,23 @@
     </row>
     <row r="25" ht="82.5" customHeight="1">
       <c r="A25" s="160" t="s">
-        <v>416</v>
+        <v>425</v>
       </c>
       <c r="B25" s="160" t="s">
         <v>405</v>
       </c>
       <c r="C25" s="166" t="s">
-        <v>417</v>
+        <v>426</v>
       </c>
       <c r="D25" s="166" t="s">
-        <v>418</v>
+        <v>427</v>
       </c>
       <c r="E25" s="160" t="s">
         <v>372</v>
       </c>
-      <c r="F25" s="117"/>
+      <c r="F25" s="161" t="s">
+        <v>408</v>
+      </c>
       <c r="G25" s="162" t="s">
         <v>83</v>
       </c>
@@ -28682,21 +28843,23 @@
     </row>
     <row r="26" ht="91.5" customHeight="1">
       <c r="A26" s="160" t="s">
-        <v>419</v>
+        <v>428</v>
       </c>
       <c r="B26" s="160" t="s">
         <v>405</v>
       </c>
       <c r="C26" s="166" t="s">
-        <v>420</v>
+        <v>429</v>
       </c>
       <c r="D26" s="166" t="s">
-        <v>421</v>
+        <v>430</v>
       </c>
       <c r="E26" s="160" t="s">
         <v>372</v>
       </c>
-      <c r="F26" s="117"/>
+      <c r="F26" s="161" t="s">
+        <v>412</v>
+      </c>
       <c r="G26" s="162" t="s">
         <v>83</v>
       </c>
@@ -28727,21 +28890,23 @@
     </row>
     <row r="27" ht="104.25" customHeight="1">
       <c r="A27" s="160" t="s">
-        <v>422</v>
+        <v>431</v>
       </c>
       <c r="B27" s="160" t="s">
         <v>405</v>
       </c>
       <c r="C27" s="166" t="s">
-        <v>423</v>
+        <v>432</v>
       </c>
       <c r="D27" s="166" t="s">
-        <v>424</v>
+        <v>433</v>
       </c>
       <c r="E27" s="160" t="s">
         <v>372</v>
       </c>
-      <c r="F27" s="161"/>
+      <c r="F27" s="161" t="s">
+        <v>412</v>
+      </c>
       <c r="G27" s="162" t="s">
         <v>83</v>
       </c>
@@ -28772,21 +28937,23 @@
     </row>
     <row r="28" ht="80.25" customHeight="1">
       <c r="A28" s="160" t="s">
-        <v>416</v>
+        <v>434</v>
       </c>
       <c r="B28" s="160" t="s">
         <v>405</v>
       </c>
       <c r="C28" s="166" t="s">
-        <v>417</v>
+        <v>435</v>
       </c>
       <c r="D28" s="166" t="s">
-        <v>418</v>
+        <v>436</v>
       </c>
       <c r="E28" s="160" t="s">
         <v>372</v>
       </c>
-      <c r="F28" s="117"/>
+      <c r="F28" s="161" t="s">
+        <v>408</v>
+      </c>
       <c r="G28" s="162" t="s">
         <v>83</v>
       </c>
@@ -28817,21 +28984,23 @@
     </row>
     <row r="29" ht="90.75" customHeight="1">
       <c r="A29" s="160" t="s">
-        <v>419</v>
+        <v>437</v>
       </c>
       <c r="B29" s="160" t="s">
         <v>405</v>
       </c>
       <c r="C29" s="166" t="s">
-        <v>420</v>
+        <v>438</v>
       </c>
       <c r="D29" s="166" t="s">
-        <v>421</v>
+        <v>439</v>
       </c>
       <c r="E29" s="160" t="s">
         <v>372</v>
       </c>
-      <c r="F29" s="117"/>
+      <c r="F29" s="161" t="s">
+        <v>412</v>
+      </c>
       <c r="G29" s="162" t="s">
         <v>83</v>
       </c>
@@ -28862,28 +29031,30 @@
     </row>
     <row r="30" ht="110.25" customHeight="1">
       <c r="A30" s="160" t="s">
-        <v>422</v>
+        <v>440</v>
       </c>
       <c r="B30" s="160" t="s">
         <v>405</v>
       </c>
-      <c r="C30" s="167" t="s">
-        <v>423</v>
-      </c>
-      <c r="D30" s="167" t="s">
-        <v>424</v>
+      <c r="C30" s="166" t="s">
+        <v>441</v>
+      </c>
+      <c r="D30" s="166" t="s">
+        <v>442</v>
       </c>
       <c r="E30" s="160" t="s">
         <v>372</v>
       </c>
-      <c r="F30" s="161"/>
+      <c r="F30" s="161" t="s">
+        <v>412</v>
+      </c>
       <c r="G30" s="162" t="s">
         <v>83</v>
       </c>
       <c r="H30" s="163">
         <v>44302.0</v>
       </c>
-      <c r="I30" s="168" t="s">
+      <c r="I30" s="167" t="s">
         <v>376</v>
       </c>
       <c r="J30" s="116"/>
@@ -28905,17 +29076,35 @@
       <c r="Z30" s="11"/>
       <c r="AA30" s="11"/>
     </row>
-    <row r="31" ht="12.75" customHeight="1">
-      <c r="A31" s="125"/>
-      <c r="B31" s="125"/>
-      <c r="C31" s="125"/>
-      <c r="D31" s="125"/>
-      <c r="E31" s="125"/>
-      <c r="F31" s="125"/>
-      <c r="G31" s="169"/>
-      <c r="H31" s="169"/>
-      <c r="I31" s="169"/>
-      <c r="J31" s="125"/>
+    <row r="31" ht="93.0" customHeight="1">
+      <c r="A31" s="160" t="s">
+        <v>443</v>
+      </c>
+      <c r="B31" s="160" t="s">
+        <v>405</v>
+      </c>
+      <c r="C31" s="166" t="s">
+        <v>444</v>
+      </c>
+      <c r="D31" s="166" t="s">
+        <v>407</v>
+      </c>
+      <c r="E31" s="160" t="s">
+        <v>372</v>
+      </c>
+      <c r="F31" s="161" t="s">
+        <v>408</v>
+      </c>
+      <c r="G31" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H31" s="163">
+        <v>44302.0</v>
+      </c>
+      <c r="I31" s="165" t="s">
+        <v>376</v>
+      </c>
+      <c r="J31" s="116"/>
       <c r="K31" s="155"/>
       <c r="L31" s="156"/>
       <c r="M31" s="155"/>
@@ -28934,17 +29123,35 @@
       <c r="Z31" s="155"/>
       <c r="AA31" s="155"/>
     </row>
-    <row r="32" ht="12.75" customHeight="1">
-      <c r="A32" s="125"/>
-      <c r="B32" s="125"/>
-      <c r="C32" s="125"/>
-      <c r="D32" s="125"/>
-      <c r="E32" s="125"/>
-      <c r="F32" s="125"/>
-      <c r="G32" s="169"/>
-      <c r="H32" s="169"/>
-      <c r="I32" s="169"/>
-      <c r="J32" s="125"/>
+    <row r="32" ht="85.5" customHeight="1">
+      <c r="A32" s="160" t="s">
+        <v>445</v>
+      </c>
+      <c r="B32" s="160" t="s">
+        <v>405</v>
+      </c>
+      <c r="C32" s="166" t="s">
+        <v>446</v>
+      </c>
+      <c r="D32" s="166" t="s">
+        <v>418</v>
+      </c>
+      <c r="E32" s="160" t="s">
+        <v>372</v>
+      </c>
+      <c r="F32" s="161" t="s">
+        <v>408</v>
+      </c>
+      <c r="G32" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H32" s="163">
+        <v>44302.0</v>
+      </c>
+      <c r="I32" s="165" t="s">
+        <v>376</v>
+      </c>
+      <c r="J32" s="116"/>
       <c r="K32" s="155"/>
       <c r="L32" s="156"/>
       <c r="M32" s="155"/>
@@ -28963,17 +29170,35 @@
       <c r="Z32" s="155"/>
       <c r="AA32" s="155"/>
     </row>
-    <row r="33" ht="12.75" customHeight="1">
-      <c r="A33" s="125"/>
-      <c r="B33" s="125"/>
-      <c r="C33" s="125"/>
-      <c r="D33" s="125"/>
-      <c r="E33" s="125"/>
-      <c r="F33" s="125"/>
-      <c r="G33" s="169"/>
-      <c r="H33" s="169"/>
-      <c r="I33" s="169"/>
-      <c r="J33" s="125"/>
+    <row r="33" ht="94.5" customHeight="1">
+      <c r="A33" s="160" t="s">
+        <v>447</v>
+      </c>
+      <c r="B33" s="160" t="s">
+        <v>405</v>
+      </c>
+      <c r="C33" s="166" t="s">
+        <v>448</v>
+      </c>
+      <c r="D33" s="166" t="s">
+        <v>427</v>
+      </c>
+      <c r="E33" s="160" t="s">
+        <v>372</v>
+      </c>
+      <c r="F33" s="161" t="s">
+        <v>408</v>
+      </c>
+      <c r="G33" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H33" s="163">
+        <v>44302.0</v>
+      </c>
+      <c r="I33" s="165" t="s">
+        <v>376</v>
+      </c>
+      <c r="J33" s="116"/>
       <c r="K33" s="155"/>
       <c r="L33" s="156"/>
       <c r="M33" s="155"/>
@@ -28992,17 +29217,33 @@
       <c r="Z33" s="155"/>
       <c r="AA33" s="155"/>
     </row>
-    <row r="34" ht="12.75" customHeight="1">
-      <c r="A34" s="125"/>
-      <c r="B34" s="125"/>
-      <c r="C34" s="125"/>
-      <c r="D34" s="125"/>
-      <c r="E34" s="125"/>
-      <c r="F34" s="125"/>
-      <c r="G34" s="169"/>
-      <c r="H34" s="169"/>
-      <c r="I34" s="169"/>
-      <c r="J34" s="125"/>
+    <row r="34" ht="61.5" customHeight="1">
+      <c r="A34" s="160" t="s">
+        <v>449</v>
+      </c>
+      <c r="B34" s="160" t="s">
+        <v>450</v>
+      </c>
+      <c r="C34" s="166" t="s">
+        <v>451</v>
+      </c>
+      <c r="D34" s="166" t="s">
+        <v>452</v>
+      </c>
+      <c r="E34" s="160" t="s">
+        <v>372</v>
+      </c>
+      <c r="F34" s="161"/>
+      <c r="G34" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H34" s="163">
+        <v>44302.0</v>
+      </c>
+      <c r="I34" s="165" t="s">
+        <v>376</v>
+      </c>
+      <c r="J34" s="116"/>
       <c r="K34" s="155"/>
       <c r="L34" s="156"/>
       <c r="M34" s="155"/>
@@ -29021,17 +29262,33 @@
       <c r="Z34" s="155"/>
       <c r="AA34" s="155"/>
     </row>
-    <row r="35" ht="12.75" customHeight="1">
-      <c r="A35" s="125"/>
-      <c r="B35" s="125"/>
-      <c r="C35" s="125"/>
-      <c r="D35" s="125"/>
-      <c r="E35" s="125"/>
-      <c r="F35" s="125"/>
-      <c r="G35" s="169"/>
-      <c r="H35" s="169"/>
-      <c r="I35" s="169"/>
-      <c r="J35" s="125"/>
+    <row r="35" ht="93.75" customHeight="1">
+      <c r="A35" s="160" t="s">
+        <v>453</v>
+      </c>
+      <c r="B35" s="160" t="s">
+        <v>454</v>
+      </c>
+      <c r="C35" s="166" t="s">
+        <v>451</v>
+      </c>
+      <c r="D35" s="166" t="s">
+        <v>455</v>
+      </c>
+      <c r="E35" s="160" t="s">
+        <v>372</v>
+      </c>
+      <c r="F35" s="161"/>
+      <c r="G35" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H35" s="163">
+        <v>44302.0</v>
+      </c>
+      <c r="I35" s="165" t="s">
+        <v>376</v>
+      </c>
+      <c r="J35" s="116"/>
       <c r="K35" s="155"/>
       <c r="L35" s="156"/>
       <c r="M35" s="155"/>
@@ -29050,17 +29307,33 @@
       <c r="Z35" s="155"/>
       <c r="AA35" s="155"/>
     </row>
-    <row r="36" ht="12.75" customHeight="1">
-      <c r="A36" s="125"/>
-      <c r="B36" s="125"/>
-      <c r="C36" s="125"/>
-      <c r="D36" s="125"/>
-      <c r="E36" s="125"/>
-      <c r="F36" s="125"/>
-      <c r="G36" s="169"/>
-      <c r="H36" s="169"/>
-      <c r="I36" s="169"/>
-      <c r="J36" s="125"/>
+    <row r="36" ht="90.75" customHeight="1">
+      <c r="A36" s="160" t="s">
+        <v>456</v>
+      </c>
+      <c r="B36" s="160" t="s">
+        <v>405</v>
+      </c>
+      <c r="C36" s="166" t="s">
+        <v>448</v>
+      </c>
+      <c r="D36" s="166" t="s">
+        <v>427</v>
+      </c>
+      <c r="E36" s="160" t="s">
+        <v>372</v>
+      </c>
+      <c r="F36" s="161"/>
+      <c r="G36" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H36" s="163">
+        <v>44302.0</v>
+      </c>
+      <c r="I36" s="165" t="s">
+        <v>376</v>
+      </c>
+      <c r="J36" s="116"/>
       <c r="K36" s="155"/>
       <c r="L36" s="156"/>
       <c r="M36" s="155"/>
@@ -29086,9 +29359,9 @@
       <c r="D37" s="125"/>
       <c r="E37" s="125"/>
       <c r="F37" s="125"/>
-      <c r="G37" s="169"/>
-      <c r="H37" s="169"/>
-      <c r="I37" s="169"/>
+      <c r="G37" s="168"/>
+      <c r="H37" s="168"/>
+      <c r="I37" s="168"/>
       <c r="J37" s="125"/>
       <c r="K37" s="155"/>
       <c r="L37" s="156"/>
@@ -29115,9 +29388,9 @@
       <c r="D38" s="125"/>
       <c r="E38" s="125"/>
       <c r="F38" s="125"/>
-      <c r="G38" s="169"/>
-      <c r="H38" s="169"/>
-      <c r="I38" s="169"/>
+      <c r="G38" s="168"/>
+      <c r="H38" s="168"/>
+      <c r="I38" s="168"/>
       <c r="J38" s="125"/>
       <c r="K38" s="155"/>
       <c r="L38" s="156"/>
@@ -29144,9 +29417,9 @@
       <c r="D39" s="125"/>
       <c r="E39" s="125"/>
       <c r="F39" s="125"/>
-      <c r="G39" s="169"/>
-      <c r="H39" s="169"/>
-      <c r="I39" s="169"/>
+      <c r="G39" s="168"/>
+      <c r="H39" s="168"/>
+      <c r="I39" s="168"/>
       <c r="J39" s="125"/>
       <c r="K39" s="155"/>
       <c r="L39" s="156"/>
@@ -29173,9 +29446,9 @@
       <c r="D40" s="125"/>
       <c r="E40" s="125"/>
       <c r="F40" s="125"/>
-      <c r="G40" s="169"/>
-      <c r="H40" s="169"/>
-      <c r="I40" s="169"/>
+      <c r="G40" s="168"/>
+      <c r="H40" s="168"/>
+      <c r="I40" s="168"/>
       <c r="J40" s="125"/>
       <c r="K40" s="155"/>
       <c r="L40" s="156"/>
@@ -29202,9 +29475,9 @@
       <c r="D41" s="125"/>
       <c r="E41" s="125"/>
       <c r="F41" s="125"/>
-      <c r="G41" s="169"/>
-      <c r="H41" s="169"/>
-      <c r="I41" s="169"/>
+      <c r="G41" s="168"/>
+      <c r="H41" s="168"/>
+      <c r="I41" s="168"/>
       <c r="J41" s="125"/>
       <c r="K41" s="155"/>
       <c r="L41" s="156"/>
@@ -29231,9 +29504,9 @@
       <c r="D42" s="125"/>
       <c r="E42" s="125"/>
       <c r="F42" s="125"/>
-      <c r="G42" s="169"/>
-      <c r="H42" s="169"/>
-      <c r="I42" s="169"/>
+      <c r="G42" s="168"/>
+      <c r="H42" s="168"/>
+      <c r="I42" s="168"/>
       <c r="J42" s="125"/>
       <c r="K42" s="155"/>
       <c r="L42" s="156"/>
@@ -29260,9 +29533,9 @@
       <c r="D43" s="125"/>
       <c r="E43" s="125"/>
       <c r="F43" s="125"/>
-      <c r="G43" s="169"/>
-      <c r="H43" s="169"/>
-      <c r="I43" s="169"/>
+      <c r="G43" s="168"/>
+      <c r="H43" s="168"/>
+      <c r="I43" s="168"/>
       <c r="J43" s="125"/>
       <c r="K43" s="155"/>
       <c r="L43" s="156"/>
@@ -29289,9 +29562,9 @@
       <c r="D44" s="125"/>
       <c r="E44" s="125"/>
       <c r="F44" s="125"/>
-      <c r="G44" s="169"/>
-      <c r="H44" s="169"/>
-      <c r="I44" s="169"/>
+      <c r="G44" s="168"/>
+      <c r="H44" s="168"/>
+      <c r="I44" s="168"/>
       <c r="J44" s="125"/>
       <c r="K44" s="155"/>
       <c r="L44" s="156"/>
@@ -29318,9 +29591,9 @@
       <c r="D45" s="125"/>
       <c r="E45" s="125"/>
       <c r="F45" s="125"/>
-      <c r="G45" s="169"/>
-      <c r="H45" s="169"/>
-      <c r="I45" s="169"/>
+      <c r="G45" s="168"/>
+      <c r="H45" s="168"/>
+      <c r="I45" s="168"/>
       <c r="J45" s="125"/>
       <c r="K45" s="155"/>
       <c r="L45" s="156"/>
@@ -29347,9 +29620,9 @@
       <c r="D46" s="125"/>
       <c r="E46" s="125"/>
       <c r="F46" s="125"/>
-      <c r="G46" s="169"/>
-      <c r="H46" s="169"/>
-      <c r="I46" s="169"/>
+      <c r="G46" s="168"/>
+      <c r="H46" s="168"/>
+      <c r="I46" s="168"/>
       <c r="J46" s="125"/>
       <c r="K46" s="155"/>
       <c r="L46" s="156"/>
@@ -29376,9 +29649,9 @@
       <c r="D47" s="125"/>
       <c r="E47" s="125"/>
       <c r="F47" s="125"/>
-      <c r="G47" s="169"/>
-      <c r="H47" s="169"/>
-      <c r="I47" s="169"/>
+      <c r="G47" s="168"/>
+      <c r="H47" s="168"/>
+      <c r="I47" s="168"/>
       <c r="J47" s="125"/>
       <c r="K47" s="155"/>
       <c r="L47" s="156"/>
@@ -29405,9 +29678,9 @@
       <c r="D48" s="125"/>
       <c r="E48" s="125"/>
       <c r="F48" s="125"/>
-      <c r="G48" s="169"/>
-      <c r="H48" s="169"/>
-      <c r="I48" s="169"/>
+      <c r="G48" s="168"/>
+      <c r="H48" s="168"/>
+      <c r="I48" s="168"/>
       <c r="J48" s="125"/>
       <c r="K48" s="155"/>
       <c r="L48" s="156"/>
@@ -29434,9 +29707,9 @@
       <c r="D49" s="125"/>
       <c r="E49" s="125"/>
       <c r="F49" s="125"/>
-      <c r="G49" s="169"/>
-      <c r="H49" s="169"/>
-      <c r="I49" s="169"/>
+      <c r="G49" s="168"/>
+      <c r="H49" s="168"/>
+      <c r="I49" s="168"/>
       <c r="J49" s="125"/>
       <c r="K49" s="155"/>
       <c r="L49" s="156"/>
@@ -29463,9 +29736,9 @@
       <c r="D50" s="125"/>
       <c r="E50" s="125"/>
       <c r="F50" s="125"/>
-      <c r="G50" s="169"/>
-      <c r="H50" s="169"/>
-      <c r="I50" s="169"/>
+      <c r="G50" s="168"/>
+      <c r="H50" s="168"/>
+      <c r="I50" s="168"/>
       <c r="J50" s="125"/>
       <c r="K50" s="155"/>
       <c r="L50" s="156"/>
@@ -29488,13 +29761,13 @@
     <row r="51" ht="12.75" customHeight="1">
       <c r="A51" s="50"/>
       <c r="B51" s="50"/>
-      <c r="C51" s="170"/>
-      <c r="D51" s="170"/>
+      <c r="C51" s="169"/>
+      <c r="D51" s="169"/>
       <c r="E51" s="50"/>
       <c r="F51" s="50"/>
-      <c r="G51" s="171"/>
-      <c r="H51" s="171"/>
-      <c r="I51" s="171"/>
+      <c r="G51" s="170"/>
+      <c r="H51" s="170"/>
+      <c r="I51" s="170"/>
       <c r="J51" s="50"/>
       <c r="K51" s="86"/>
       <c r="L51" s="11"/>
@@ -29517,13 +29790,13 @@
     <row r="52" ht="12.75" customHeight="1">
       <c r="A52" s="50"/>
       <c r="B52" s="50"/>
-      <c r="C52" s="170"/>
-      <c r="D52" s="170"/>
+      <c r="C52" s="169"/>
+      <c r="D52" s="169"/>
       <c r="E52" s="50"/>
       <c r="F52" s="50"/>
-      <c r="G52" s="171"/>
-      <c r="H52" s="171"/>
-      <c r="I52" s="171"/>
+      <c r="G52" s="170"/>
+      <c r="H52" s="170"/>
+      <c r="I52" s="170"/>
       <c r="J52" s="50"/>
       <c r="K52" s="86"/>
       <c r="L52" s="11"/>
@@ -29546,13 +29819,13 @@
     <row r="53" ht="12.75" customHeight="1">
       <c r="A53" s="50"/>
       <c r="B53" s="50"/>
-      <c r="C53" s="170"/>
-      <c r="D53" s="170"/>
+      <c r="C53" s="169"/>
+      <c r="D53" s="169"/>
       <c r="E53" s="50"/>
       <c r="F53" s="50"/>
-      <c r="G53" s="171"/>
-      <c r="H53" s="171"/>
-      <c r="I53" s="171"/>
+      <c r="G53" s="170"/>
+      <c r="H53" s="170"/>
+      <c r="I53" s="170"/>
       <c r="J53" s="50"/>
       <c r="K53" s="86"/>
       <c r="L53" s="11"/>
@@ -29575,13 +29848,13 @@
     <row r="54" ht="12.75" customHeight="1">
       <c r="A54" s="50"/>
       <c r="B54" s="50"/>
-      <c r="C54" s="170"/>
-      <c r="D54" s="170"/>
+      <c r="C54" s="169"/>
+      <c r="D54" s="169"/>
       <c r="E54" s="50"/>
       <c r="F54" s="50"/>
-      <c r="G54" s="171"/>
-      <c r="H54" s="171"/>
-      <c r="I54" s="171"/>
+      <c r="G54" s="170"/>
+      <c r="H54" s="170"/>
+      <c r="I54" s="170"/>
       <c r="J54" s="50"/>
       <c r="K54" s="86"/>
       <c r="L54" s="11"/>
@@ -29605,12 +29878,12 @@
       <c r="A55" s="50"/>
       <c r="B55" s="50"/>
       <c r="C55" s="50"/>
-      <c r="D55" s="170"/>
+      <c r="D55" s="169"/>
       <c r="E55" s="50"/>
       <c r="F55" s="50"/>
-      <c r="G55" s="171"/>
-      <c r="H55" s="171"/>
-      <c r="I55" s="171"/>
+      <c r="G55" s="170"/>
+      <c r="H55" s="170"/>
+      <c r="I55" s="170"/>
       <c r="J55" s="50"/>
       <c r="K55" s="86"/>
       <c r="L55" s="11"/>
@@ -29634,12 +29907,12 @@
       <c r="A56" s="50"/>
       <c r="B56" s="50"/>
       <c r="C56" s="50"/>
-      <c r="D56" s="170"/>
+      <c r="D56" s="169"/>
       <c r="E56" s="50"/>
       <c r="F56" s="50"/>
-      <c r="G56" s="171"/>
-      <c r="H56" s="171"/>
-      <c r="I56" s="171"/>
+      <c r="G56" s="170"/>
+      <c r="H56" s="170"/>
+      <c r="I56" s="170"/>
       <c r="J56" s="50"/>
       <c r="K56" s="86"/>
       <c r="L56" s="11"/>
@@ -29663,12 +29936,12 @@
       <c r="A57" s="50"/>
       <c r="B57" s="50"/>
       <c r="C57" s="50"/>
-      <c r="D57" s="170"/>
+      <c r="D57" s="169"/>
       <c r="E57" s="50"/>
       <c r="F57" s="50"/>
-      <c r="G57" s="171"/>
-      <c r="H57" s="171"/>
-      <c r="I57" s="171"/>
+      <c r="G57" s="170"/>
+      <c r="H57" s="170"/>
+      <c r="I57" s="170"/>
       <c r="J57" s="50"/>
       <c r="K57" s="86"/>
       <c r="L57" s="11"/>
@@ -29692,12 +29965,12 @@
       <c r="A58" s="50"/>
       <c r="B58" s="50"/>
       <c r="C58" s="50"/>
-      <c r="D58" s="170"/>
+      <c r="D58" s="169"/>
       <c r="E58" s="50"/>
       <c r="F58" s="50"/>
-      <c r="G58" s="171"/>
-      <c r="H58" s="171"/>
-      <c r="I58" s="171"/>
+      <c r="G58" s="170"/>
+      <c r="H58" s="170"/>
+      <c r="I58" s="170"/>
       <c r="J58" s="50"/>
       <c r="K58" s="86"/>
       <c r="L58" s="11"/>
@@ -29721,12 +29994,12 @@
       <c r="A59" s="50"/>
       <c r="B59" s="50"/>
       <c r="C59" s="50"/>
-      <c r="D59" s="170"/>
+      <c r="D59" s="169"/>
       <c r="E59" s="50"/>
       <c r="F59" s="50"/>
-      <c r="G59" s="171"/>
-      <c r="H59" s="171"/>
-      <c r="I59" s="171"/>
+      <c r="G59" s="170"/>
+      <c r="H59" s="170"/>
+      <c r="I59" s="170"/>
       <c r="J59" s="50"/>
       <c r="K59" s="86"/>
       <c r="L59" s="11"/>
@@ -29750,12 +30023,12 @@
       <c r="A60" s="50"/>
       <c r="B60" s="50"/>
       <c r="C60" s="50"/>
-      <c r="D60" s="170"/>
+      <c r="D60" s="169"/>
       <c r="E60" s="50"/>
       <c r="F60" s="50"/>
-      <c r="G60" s="171"/>
-      <c r="H60" s="171"/>
-      <c r="I60" s="171"/>
+      <c r="G60" s="170"/>
+      <c r="H60" s="170"/>
+      <c r="I60" s="170"/>
       <c r="J60" s="50"/>
       <c r="K60" s="86"/>
       <c r="L60" s="11"/>
@@ -29779,12 +30052,12 @@
       <c r="A61" s="50"/>
       <c r="B61" s="50"/>
       <c r="C61" s="50"/>
-      <c r="D61" s="170"/>
+      <c r="D61" s="169"/>
       <c r="E61" s="50"/>
       <c r="F61" s="50"/>
-      <c r="G61" s="171"/>
-      <c r="H61" s="171"/>
-      <c r="I61" s="171"/>
+      <c r="G61" s="170"/>
+      <c r="H61" s="170"/>
+      <c r="I61" s="170"/>
       <c r="J61" s="50"/>
       <c r="K61" s="86"/>
       <c r="L61" s="11"/>
@@ -29808,12 +30081,12 @@
       <c r="A62" s="50"/>
       <c r="B62" s="50"/>
       <c r="C62" s="50"/>
-      <c r="D62" s="170"/>
+      <c r="D62" s="169"/>
       <c r="E62" s="50"/>
       <c r="F62" s="50"/>
-      <c r="G62" s="171"/>
-      <c r="H62" s="171"/>
-      <c r="I62" s="171"/>
+      <c r="G62" s="170"/>
+      <c r="H62" s="170"/>
+      <c r="I62" s="170"/>
       <c r="J62" s="50"/>
       <c r="K62" s="86"/>
       <c r="L62" s="11"/>
@@ -29837,12 +30110,12 @@
       <c r="A63" s="50"/>
       <c r="B63" s="50"/>
       <c r="C63" s="50"/>
-      <c r="D63" s="170"/>
+      <c r="D63" s="169"/>
       <c r="E63" s="50"/>
       <c r="F63" s="50"/>
-      <c r="G63" s="171"/>
-      <c r="H63" s="171"/>
-      <c r="I63" s="171"/>
+      <c r="G63" s="170"/>
+      <c r="H63" s="170"/>
+      <c r="I63" s="170"/>
       <c r="J63" s="50"/>
       <c r="K63" s="86"/>
       <c r="L63" s="11"/>
@@ -29866,12 +30139,12 @@
       <c r="A64" s="50"/>
       <c r="B64" s="50"/>
       <c r="C64" s="50"/>
-      <c r="D64" s="170"/>
+      <c r="D64" s="169"/>
       <c r="E64" s="50"/>
       <c r="F64" s="50"/>
-      <c r="G64" s="171"/>
-      <c r="H64" s="171"/>
-      <c r="I64" s="171"/>
+      <c r="G64" s="170"/>
+      <c r="H64" s="170"/>
+      <c r="I64" s="170"/>
       <c r="J64" s="50"/>
       <c r="K64" s="86"/>
       <c r="L64" s="11"/>
@@ -29895,12 +30168,12 @@
       <c r="A65" s="50"/>
       <c r="B65" s="50"/>
       <c r="C65" s="50"/>
-      <c r="D65" s="170"/>
+      <c r="D65" s="169"/>
       <c r="E65" s="50"/>
       <c r="F65" s="50"/>
-      <c r="G65" s="171"/>
-      <c r="H65" s="171"/>
-      <c r="I65" s="171"/>
+      <c r="G65" s="170"/>
+      <c r="H65" s="170"/>
+      <c r="I65" s="170"/>
       <c r="J65" s="50"/>
       <c r="K65" s="86"/>
       <c r="L65" s="11"/>
@@ -29924,12 +30197,12 @@
       <c r="A66" s="50"/>
       <c r="B66" s="50"/>
       <c r="C66" s="50"/>
-      <c r="D66" s="170"/>
+      <c r="D66" s="169"/>
       <c r="E66" s="50"/>
       <c r="F66" s="50"/>
-      <c r="G66" s="171"/>
-      <c r="H66" s="171"/>
-      <c r="I66" s="171"/>
+      <c r="G66" s="170"/>
+      <c r="H66" s="170"/>
+      <c r="I66" s="170"/>
       <c r="J66" s="50"/>
       <c r="K66" s="86"/>
       <c r="L66" s="11"/>
@@ -29953,12 +30226,12 @@
       <c r="A67" s="50"/>
       <c r="B67" s="50"/>
       <c r="C67" s="50"/>
-      <c r="D67" s="170"/>
+      <c r="D67" s="169"/>
       <c r="E67" s="50"/>
       <c r="F67" s="50"/>
-      <c r="G67" s="171"/>
-      <c r="H67" s="171"/>
-      <c r="I67" s="171"/>
+      <c r="G67" s="170"/>
+      <c r="H67" s="170"/>
+      <c r="I67" s="170"/>
       <c r="J67" s="50"/>
       <c r="K67" s="86"/>
       <c r="L67" s="11"/>
@@ -29982,12 +30255,12 @@
       <c r="A68" s="50"/>
       <c r="B68" s="50"/>
       <c r="C68" s="50"/>
-      <c r="D68" s="170"/>
+      <c r="D68" s="169"/>
       <c r="E68" s="50"/>
       <c r="F68" s="50"/>
-      <c r="G68" s="171"/>
-      <c r="H68" s="171"/>
-      <c r="I68" s="171"/>
+      <c r="G68" s="170"/>
+      <c r="H68" s="170"/>
+      <c r="I68" s="170"/>
       <c r="J68" s="50"/>
       <c r="K68" s="86"/>
       <c r="L68" s="11"/>
@@ -30011,12 +30284,12 @@
       <c r="A69" s="50"/>
       <c r="B69" s="50"/>
       <c r="C69" s="50"/>
-      <c r="D69" s="170"/>
+      <c r="D69" s="169"/>
       <c r="E69" s="50"/>
       <c r="F69" s="50"/>
-      <c r="G69" s="171"/>
-      <c r="H69" s="171"/>
-      <c r="I69" s="171"/>
+      <c r="G69" s="170"/>
+      <c r="H69" s="170"/>
+      <c r="I69" s="170"/>
       <c r="J69" s="50"/>
       <c r="K69" s="86"/>
       <c r="L69" s="11"/>
@@ -30040,12 +30313,12 @@
       <c r="A70" s="50"/>
       <c r="B70" s="50"/>
       <c r="C70" s="50"/>
-      <c r="D70" s="170"/>
+      <c r="D70" s="169"/>
       <c r="E70" s="50"/>
       <c r="F70" s="50"/>
-      <c r="G70" s="171"/>
-      <c r="H70" s="171"/>
-      <c r="I70" s="171"/>
+      <c r="G70" s="170"/>
+      <c r="H70" s="170"/>
+      <c r="I70" s="170"/>
       <c r="J70" s="50"/>
       <c r="K70" s="86"/>
       <c r="L70" s="11"/>
@@ -30069,12 +30342,12 @@
       <c r="A71" s="50"/>
       <c r="B71" s="50"/>
       <c r="C71" s="50"/>
-      <c r="D71" s="170"/>
+      <c r="D71" s="169"/>
       <c r="E71" s="50"/>
       <c r="F71" s="50"/>
-      <c r="G71" s="171"/>
-      <c r="H71" s="171"/>
-      <c r="I71" s="171"/>
+      <c r="G71" s="170"/>
+      <c r="H71" s="170"/>
+      <c r="I71" s="170"/>
       <c r="J71" s="50"/>
       <c r="K71" s="86"/>
       <c r="L71" s="11"/>
@@ -30098,12 +30371,12 @@
       <c r="A72" s="50"/>
       <c r="B72" s="50"/>
       <c r="C72" s="50"/>
-      <c r="D72" s="170"/>
+      <c r="D72" s="169"/>
       <c r="E72" s="50"/>
       <c r="F72" s="50"/>
-      <c r="G72" s="171"/>
-      <c r="H72" s="171"/>
-      <c r="I72" s="171"/>
+      <c r="G72" s="170"/>
+      <c r="H72" s="170"/>
+      <c r="I72" s="170"/>
       <c r="J72" s="50"/>
       <c r="K72" s="86"/>
       <c r="L72" s="11"/>
@@ -30127,12 +30400,12 @@
       <c r="A73" s="50"/>
       <c r="B73" s="50"/>
       <c r="C73" s="50"/>
-      <c r="D73" s="170"/>
+      <c r="D73" s="169"/>
       <c r="E73" s="50"/>
       <c r="F73" s="50"/>
-      <c r="G73" s="171"/>
-      <c r="H73" s="171"/>
-      <c r="I73" s="171"/>
+      <c r="G73" s="170"/>
+      <c r="H73" s="170"/>
+      <c r="I73" s="170"/>
       <c r="J73" s="50"/>
       <c r="K73" s="86"/>
       <c r="L73" s="11"/>
@@ -30156,12 +30429,12 @@
       <c r="A74" s="50"/>
       <c r="B74" s="50"/>
       <c r="C74" s="50"/>
-      <c r="D74" s="170"/>
+      <c r="D74" s="169"/>
       <c r="E74" s="50"/>
       <c r="F74" s="50"/>
-      <c r="G74" s="171"/>
-      <c r="H74" s="171"/>
-      <c r="I74" s="171"/>
+      <c r="G74" s="170"/>
+      <c r="H74" s="170"/>
+      <c r="I74" s="170"/>
       <c r="J74" s="50"/>
       <c r="K74" s="86"/>
       <c r="L74" s="11"/>
@@ -30185,12 +30458,12 @@
       <c r="A75" s="50"/>
       <c r="B75" s="50"/>
       <c r="C75" s="50"/>
-      <c r="D75" s="170"/>
+      <c r="D75" s="169"/>
       <c r="E75" s="50"/>
       <c r="F75" s="50"/>
-      <c r="G75" s="171"/>
-      <c r="H75" s="171"/>
-      <c r="I75" s="171"/>
+      <c r="G75" s="170"/>
+      <c r="H75" s="170"/>
+      <c r="I75" s="170"/>
       <c r="J75" s="50"/>
       <c r="K75" s="86"/>
       <c r="L75" s="11"/>
@@ -30214,12 +30487,12 @@
       <c r="A76" s="50"/>
       <c r="B76" s="50"/>
       <c r="C76" s="50"/>
-      <c r="D76" s="170"/>
+      <c r="D76" s="169"/>
       <c r="E76" s="50"/>
       <c r="F76" s="50"/>
-      <c r="G76" s="171"/>
-      <c r="H76" s="171"/>
-      <c r="I76" s="171"/>
+      <c r="G76" s="170"/>
+      <c r="H76" s="170"/>
+      <c r="I76" s="170"/>
       <c r="J76" s="50"/>
       <c r="K76" s="86"/>
       <c r="L76" s="11"/>
@@ -30246,9 +30519,9 @@
       <c r="D77" s="50"/>
       <c r="E77" s="50"/>
       <c r="F77" s="50"/>
-      <c r="G77" s="171"/>
-      <c r="H77" s="171"/>
-      <c r="I77" s="171"/>
+      <c r="G77" s="170"/>
+      <c r="H77" s="170"/>
+      <c r="I77" s="170"/>
       <c r="J77" s="50"/>
       <c r="K77" s="86"/>
       <c r="L77" s="11"/>
@@ -30275,9 +30548,9 @@
       <c r="D78" s="50"/>
       <c r="E78" s="50"/>
       <c r="F78" s="50"/>
-      <c r="G78" s="171"/>
-      <c r="H78" s="171"/>
-      <c r="I78" s="171"/>
+      <c r="G78" s="170"/>
+      <c r="H78" s="170"/>
+      <c r="I78" s="170"/>
       <c r="J78" s="50"/>
       <c r="K78" s="86"/>
       <c r="L78" s="11"/>
@@ -30304,9 +30577,9 @@
       <c r="D79" s="50"/>
       <c r="E79" s="50"/>
       <c r="F79" s="50"/>
-      <c r="G79" s="171"/>
-      <c r="H79" s="171"/>
-      <c r="I79" s="171"/>
+      <c r="G79" s="170"/>
+      <c r="H79" s="170"/>
+      <c r="I79" s="170"/>
       <c r="J79" s="50"/>
       <c r="K79" s="86"/>
       <c r="L79" s="11"/>
@@ -30333,9 +30606,9 @@
       <c r="D80" s="50"/>
       <c r="E80" s="50"/>
       <c r="F80" s="50"/>
-      <c r="G80" s="171"/>
-      <c r="H80" s="171"/>
-      <c r="I80" s="171"/>
+      <c r="G80" s="170"/>
+      <c r="H80" s="170"/>
+      <c r="I80" s="170"/>
       <c r="J80" s="50"/>
       <c r="K80" s="86"/>
       <c r="L80" s="11"/>
@@ -30362,9 +30635,9 @@
       <c r="D81" s="50"/>
       <c r="E81" s="50"/>
       <c r="F81" s="50"/>
-      <c r="G81" s="171"/>
-      <c r="H81" s="171"/>
-      <c r="I81" s="171"/>
+      <c r="G81" s="170"/>
+      <c r="H81" s="170"/>
+      <c r="I81" s="170"/>
       <c r="J81" s="50"/>
       <c r="K81" s="86"/>
       <c r="L81" s="11"/>
@@ -30391,9 +30664,9 @@
       <c r="D82" s="50"/>
       <c r="E82" s="50"/>
       <c r="F82" s="50"/>
-      <c r="G82" s="171"/>
-      <c r="H82" s="171"/>
-      <c r="I82" s="171"/>
+      <c r="G82" s="170"/>
+      <c r="H82" s="170"/>
+      <c r="I82" s="170"/>
       <c r="J82" s="50"/>
       <c r="K82" s="86"/>
       <c r="L82" s="11"/>
@@ -30420,9 +30693,9 @@
       <c r="D83" s="50"/>
       <c r="E83" s="50"/>
       <c r="F83" s="50"/>
-      <c r="G83" s="171"/>
-      <c r="H83" s="171"/>
-      <c r="I83" s="171"/>
+      <c r="G83" s="170"/>
+      <c r="H83" s="170"/>
+      <c r="I83" s="170"/>
       <c r="J83" s="50"/>
       <c r="K83" s="86"/>
       <c r="L83" s="11"/>
@@ -30449,9 +30722,9 @@
       <c r="D84" s="50"/>
       <c r="E84" s="50"/>
       <c r="F84" s="50"/>
-      <c r="G84" s="171"/>
-      <c r="H84" s="171"/>
-      <c r="I84" s="171"/>
+      <c r="G84" s="170"/>
+      <c r="H84" s="170"/>
+      <c r="I84" s="170"/>
       <c r="J84" s="50"/>
       <c r="K84" s="86"/>
       <c r="L84" s="11"/>
@@ -30478,9 +30751,9 @@
       <c r="D85" s="50"/>
       <c r="E85" s="50"/>
       <c r="F85" s="50"/>
-      <c r="G85" s="171"/>
-      <c r="H85" s="171"/>
-      <c r="I85" s="171"/>
+      <c r="G85" s="170"/>
+      <c r="H85" s="170"/>
+      <c r="I85" s="170"/>
       <c r="J85" s="50"/>
       <c r="K85" s="86"/>
       <c r="L85" s="11"/>
@@ -30507,9 +30780,9 @@
       <c r="D86" s="50"/>
       <c r="E86" s="50"/>
       <c r="F86" s="50"/>
-      <c r="G86" s="171"/>
-      <c r="H86" s="171"/>
-      <c r="I86" s="171"/>
+      <c r="G86" s="170"/>
+      <c r="H86" s="170"/>
+      <c r="I86" s="170"/>
       <c r="J86" s="50"/>
       <c r="K86" s="86"/>
       <c r="L86" s="11"/>
@@ -30536,7 +30809,7 @@
       <c r="D87" s="50"/>
       <c r="E87" s="50"/>
       <c r="F87" s="50"/>
-      <c r="G87" s="171"/>
+      <c r="G87" s="170"/>
       <c r="H87" s="103"/>
       <c r="I87" s="103"/>
       <c r="J87" s="50"/>
@@ -30565,7 +30838,7 @@
       <c r="D88" s="50"/>
       <c r="E88" s="50"/>
       <c r="F88" s="50"/>
-      <c r="G88" s="171"/>
+      <c r="G88" s="170"/>
       <c r="H88" s="103"/>
       <c r="I88" s="103"/>
       <c r="J88" s="50"/>
@@ -30594,7 +30867,7 @@
       <c r="D89" s="50"/>
       <c r="E89" s="50"/>
       <c r="F89" s="50"/>
-      <c r="G89" s="171"/>
+      <c r="G89" s="170"/>
       <c r="H89" s="103"/>
       <c r="I89" s="103"/>
       <c r="J89" s="50"/>
@@ -30623,7 +30896,7 @@
       <c r="D90" s="50"/>
       <c r="E90" s="50"/>
       <c r="F90" s="50"/>
-      <c r="G90" s="171"/>
+      <c r="G90" s="170"/>
       <c r="H90" s="103"/>
       <c r="I90" s="103"/>
       <c r="J90" s="50"/>
@@ -30652,7 +30925,7 @@
       <c r="D91" s="50"/>
       <c r="E91" s="50"/>
       <c r="F91" s="50"/>
-      <c r="G91" s="171"/>
+      <c r="G91" s="170"/>
       <c r="H91" s="103"/>
       <c r="I91" s="103"/>
       <c r="J91" s="50"/>
@@ -30681,7 +30954,7 @@
       <c r="D92" s="50"/>
       <c r="E92" s="50"/>
       <c r="F92" s="50"/>
-      <c r="G92" s="171"/>
+      <c r="G92" s="170"/>
       <c r="H92" s="103"/>
       <c r="I92" s="103"/>
       <c r="J92" s="50"/>
@@ -30710,7 +30983,7 @@
       <c r="D93" s="50"/>
       <c r="E93" s="50"/>
       <c r="F93" s="50"/>
-      <c r="G93" s="171"/>
+      <c r="G93" s="170"/>
       <c r="H93" s="103"/>
       <c r="I93" s="103"/>
       <c r="J93" s="50"/>
@@ -30739,7 +31012,7 @@
       <c r="D94" s="50"/>
       <c r="E94" s="50"/>
       <c r="F94" s="50"/>
-      <c r="G94" s="171"/>
+      <c r="G94" s="170"/>
       <c r="H94" s="103"/>
       <c r="I94" s="103"/>
       <c r="J94" s="50"/>
@@ -30768,7 +31041,7 @@
       <c r="D95" s="50"/>
       <c r="E95" s="50"/>
       <c r="F95" s="50"/>
-      <c r="G95" s="171"/>
+      <c r="G95" s="170"/>
       <c r="H95" s="103"/>
       <c r="I95" s="103"/>
       <c r="J95" s="50"/>
@@ -30797,7 +31070,7 @@
       <c r="D96" s="50"/>
       <c r="E96" s="50"/>
       <c r="F96" s="50"/>
-      <c r="G96" s="171"/>
+      <c r="G96" s="170"/>
       <c r="H96" s="103"/>
       <c r="I96" s="103"/>
       <c r="J96" s="50"/>
@@ -30826,7 +31099,7 @@
       <c r="D97" s="50"/>
       <c r="E97" s="50"/>
       <c r="F97" s="50"/>
-      <c r="G97" s="171"/>
+      <c r="G97" s="170"/>
       <c r="H97" s="103"/>
       <c r="I97" s="103"/>
       <c r="J97" s="50"/>
@@ -30855,7 +31128,7 @@
       <c r="D98" s="50"/>
       <c r="E98" s="50"/>
       <c r="F98" s="50"/>
-      <c r="G98" s="171"/>
+      <c r="G98" s="170"/>
       <c r="H98" s="103"/>
       <c r="I98" s="103"/>
       <c r="J98" s="50"/>
@@ -30884,7 +31157,7 @@
       <c r="D99" s="50"/>
       <c r="E99" s="50"/>
       <c r="F99" s="50"/>
-      <c r="G99" s="171"/>
+      <c r="G99" s="170"/>
       <c r="H99" s="103"/>
       <c r="I99" s="103"/>
       <c r="J99" s="50"/>
@@ -30913,7 +31186,7 @@
       <c r="D100" s="50"/>
       <c r="E100" s="50"/>
       <c r="F100" s="50"/>
-      <c r="G100" s="172"/>
+      <c r="G100" s="171"/>
       <c r="H100" s="50"/>
       <c r="I100" s="50"/>
       <c r="J100" s="50"/>
@@ -30942,7 +31215,7 @@
       <c r="D101" s="50"/>
       <c r="E101" s="50"/>
       <c r="F101" s="50"/>
-      <c r="G101" s="172"/>
+      <c r="G101" s="171"/>
       <c r="H101" s="50"/>
       <c r="I101" s="50"/>
       <c r="J101" s="50"/>
@@ -30971,7 +31244,7 @@
       <c r="D102" s="50"/>
       <c r="E102" s="50"/>
       <c r="F102" s="50"/>
-      <c r="G102" s="172"/>
+      <c r="G102" s="171"/>
       <c r="H102" s="50"/>
       <c r="I102" s="50"/>
       <c r="J102" s="50"/>
@@ -31000,7 +31273,7 @@
       <c r="D103" s="50"/>
       <c r="E103" s="50"/>
       <c r="F103" s="50"/>
-      <c r="G103" s="172"/>
+      <c r="G103" s="171"/>
       <c r="H103" s="50"/>
       <c r="I103" s="50"/>
       <c r="J103" s="50"/>
@@ -31029,7 +31302,7 @@
       <c r="D104" s="50"/>
       <c r="E104" s="50"/>
       <c r="F104" s="50"/>
-      <c r="G104" s="172"/>
+      <c r="G104" s="171"/>
       <c r="H104" s="50"/>
       <c r="I104" s="50"/>
       <c r="J104" s="50"/>
@@ -31058,7 +31331,7 @@
       <c r="D105" s="50"/>
       <c r="E105" s="50"/>
       <c r="F105" s="50"/>
-      <c r="G105" s="172"/>
+      <c r="G105" s="171"/>
       <c r="H105" s="50"/>
       <c r="I105" s="50"/>
       <c r="J105" s="50"/>
@@ -31087,7 +31360,7 @@
       <c r="D106" s="50"/>
       <c r="E106" s="50"/>
       <c r="F106" s="50"/>
-      <c r="G106" s="172"/>
+      <c r="G106" s="171"/>
       <c r="H106" s="50"/>
       <c r="I106" s="50"/>
       <c r="J106" s="50"/>
@@ -31116,7 +31389,7 @@
       <c r="D107" s="50"/>
       <c r="E107" s="50"/>
       <c r="F107" s="50"/>
-      <c r="G107" s="172"/>
+      <c r="G107" s="171"/>
       <c r="H107" s="50"/>
       <c r="I107" s="50"/>
       <c r="J107" s="50"/>
@@ -31145,7 +31418,7 @@
       <c r="D108" s="50"/>
       <c r="E108" s="50"/>
       <c r="F108" s="50"/>
-      <c r="G108" s="172"/>
+      <c r="G108" s="171"/>
       <c r="H108" s="50"/>
       <c r="I108" s="50"/>
       <c r="J108" s="50"/>
@@ -33432,15 +33705,15 @@
   <sheetData>
     <row r="1" ht="25.5" customHeight="1">
       <c r="A1" s="11"/>
-      <c r="B1" s="173" t="s">
-        <v>425</v>
-      </c>
-      <c r="C1" s="174"/>
-      <c r="D1" s="174"/>
-      <c r="E1" s="174"/>
-      <c r="F1" s="174"/>
-      <c r="G1" s="174"/>
-      <c r="H1" s="174"/>
+      <c r="B1" s="172" t="s">
+        <v>457</v>
+      </c>
+      <c r="C1" s="173"/>
+      <c r="D1" s="173"/>
+      <c r="E1" s="173"/>
+      <c r="F1" s="173"/>
+      <c r="G1" s="173"/>
+      <c r="H1" s="173"/>
       <c r="I1" s="11"/>
       <c r="J1" s="11"/>
       <c r="K1" s="11"/>
@@ -33461,14 +33734,14 @@
       <c r="Z1" s="11"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="175"/>
-      <c r="B2" s="175"/>
+      <c r="A2" s="174"/>
+      <c r="B2" s="174"/>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
       <c r="F2" s="11"/>
       <c r="G2" s="11"/>
-      <c r="H2" s="176"/>
+      <c r="H2" s="175"/>
       <c r="I2" s="11"/>
       <c r="J2" s="11"/>
       <c r="K2" s="11"/>
@@ -33490,19 +33763,19 @@
     </row>
     <row r="3" ht="12.0" customHeight="1">
       <c r="A3" s="11"/>
-      <c r="B3" s="177" t="s">
+      <c r="B3" s="176" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="49" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="6"/>
-      <c r="E3" s="178" t="s">
+      <c r="E3" s="177" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="6"/>
-      <c r="G3" s="179"/>
-      <c r="H3" s="180" t="s">
+      <c r="G3" s="178"/>
+      <c r="H3" s="179" t="s">
         <v>4</v>
       </c>
       <c r="I3" s="11"/>
@@ -33526,19 +33799,19 @@
     </row>
     <row r="4" ht="12.0" customHeight="1">
       <c r="A4" s="11"/>
-      <c r="B4" s="177" t="s">
+      <c r="B4" s="176" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="49" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="6"/>
-      <c r="E4" s="178" t="s">
+      <c r="E4" s="177" t="s">
         <v>6</v>
       </c>
       <c r="F4" s="6"/>
-      <c r="G4" s="179"/>
-      <c r="H4" s="180" t="s">
+      <c r="G4" s="178"/>
+      <c r="H4" s="179" t="s">
         <v>7</v>
       </c>
       <c r="I4" s="11"/>
@@ -33562,7 +33835,7 @@
     </row>
     <row r="5" ht="12.0" customHeight="1">
       <c r="A5" s="11"/>
-      <c r="B5" s="181" t="s">
+      <c r="B5" s="180" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="49" t="str">
@@ -33570,12 +33843,12 @@
         <v>SoFa_Test Report_vx.x</v>
       </c>
       <c r="D5" s="6"/>
-      <c r="E5" s="178" t="s">
+      <c r="E5" s="177" t="s">
         <v>9</v>
       </c>
       <c r="F5" s="6"/>
-      <c r="G5" s="179"/>
-      <c r="H5" s="182">
+      <c r="G5" s="178"/>
+      <c r="H5" s="181">
         <v>44534.0</v>
       </c>
       <c r="I5" s="11"/>
@@ -33598,12 +33871,12 @@
       <c r="Z5" s="11"/>
     </row>
     <row r="6" ht="21.75" customHeight="1">
-      <c r="A6" s="175"/>
-      <c r="B6" s="181" t="s">
-        <v>426</v>
-      </c>
-      <c r="C6" s="183" t="s">
-        <v>427</v>
+      <c r="A6" s="174"/>
+      <c r="B6" s="180" t="s">
+        <v>458</v>
+      </c>
+      <c r="C6" s="182" t="s">
+        <v>459</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -33630,14 +33903,14 @@
       <c r="Z6" s="11"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="175"/>
+      <c r="A7" s="174"/>
       <c r="B7" s="25"/>
-      <c r="C7" s="184"/>
+      <c r="C7" s="183"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
-      <c r="H7" s="176"/>
+      <c r="H7" s="175"/>
       <c r="I7" s="11"/>
       <c r="J7" s="11"/>
       <c r="K7" s="11"/>
@@ -33660,12 +33933,12 @@
     <row r="8" ht="12.75" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="25"/>
-      <c r="C8" s="184"/>
+      <c r="C8" s="183"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
-      <c r="H8" s="176"/>
+      <c r="H8" s="175"/>
       <c r="I8" s="11"/>
       <c r="J8" s="11"/>
       <c r="K8" s="11"/>
@@ -33714,27 +33987,27 @@
       <c r="Z9" s="11"/>
     </row>
     <row r="10" ht="12.75" customHeight="1">
-      <c r="A10" s="185"/>
-      <c r="B10" s="186" t="s">
+      <c r="A10" s="184"/>
+      <c r="B10" s="185" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="187" t="s">
-        <v>428</v>
-      </c>
-      <c r="D10" s="188" t="s">
+      <c r="C10" s="186" t="s">
+        <v>460</v>
+      </c>
+      <c r="D10" s="187" t="s">
         <v>83</v>
       </c>
-      <c r="E10" s="187" t="s">
+      <c r="E10" s="186" t="s">
         <v>86</v>
       </c>
-      <c r="F10" s="187" t="s">
+      <c r="F10" s="186" t="s">
         <v>89</v>
       </c>
-      <c r="G10" s="189" t="s">
+      <c r="G10" s="188" t="s">
         <v>90</v>
       </c>
-      <c r="H10" s="190" t="s">
-        <v>429</v>
+      <c r="H10" s="189" t="s">
+        <v>461</v>
       </c>
       <c r="I10" s="11"/>
       <c r="J10" s="11"/>
@@ -33756,31 +34029,31 @@
       <c r="Z10" s="11"/>
     </row>
     <row r="11" ht="12.75" customHeight="1">
-      <c r="A11" s="185"/>
-      <c r="B11" s="191">
+      <c r="A11" s="184"/>
+      <c r="B11" s="190">
         <v>1.0</v>
       </c>
-      <c r="C11" s="192" t="str">
+      <c r="C11" s="191" t="str">
         <f>Guest!B2</f>
         <v>Guest</v>
       </c>
-      <c r="D11" s="193">
+      <c r="D11" s="192">
         <f>Guest!A6</f>
         <v>43</v>
       </c>
-      <c r="E11" s="193">
+      <c r="E11" s="192">
         <f>Guest!B6</f>
         <v>4</v>
       </c>
-      <c r="F11" s="193">
+      <c r="F11" s="192">
         <f>Guest!C6</f>
         <v>3</v>
       </c>
-      <c r="G11" s="194">
+      <c r="G11" s="193">
         <f>Guest!D6</f>
         <v>0</v>
       </c>
-      <c r="H11" s="195">
+      <c r="H11" s="194">
         <f>Guest!E6</f>
         <v>50</v>
       </c>
@@ -33804,31 +34077,31 @@
       <c r="Z11" s="11"/>
     </row>
     <row r="12" ht="12.75" customHeight="1">
-      <c r="A12" s="185"/>
-      <c r="B12" s="191">
+      <c r="A12" s="184"/>
+      <c r="B12" s="190">
         <v>2.0</v>
       </c>
-      <c r="C12" s="192" t="str">
+      <c r="C12" s="191" t="str">
         <f>User!B2</f>
         <v>User</v>
       </c>
-      <c r="D12" s="193">
+      <c r="D12" s="192">
         <f>User!A6</f>
         <v>0</v>
       </c>
-      <c r="E12" s="193">
+      <c r="E12" s="192">
         <f>User!B6</f>
         <v>0</v>
       </c>
-      <c r="F12" s="193">
+      <c r="F12" s="192">
         <f>User!C6</f>
         <v>51</v>
       </c>
-      <c r="G12" s="193">
+      <c r="G12" s="192">
         <f>User!D6</f>
         <v>0</v>
       </c>
-      <c r="H12" s="193">
+      <c r="H12" s="192">
         <f>User!E6</f>
         <v>51</v>
       </c>
@@ -33852,31 +34125,31 @@
       <c r="Z12" s="11"/>
     </row>
     <row r="13" ht="12.75" customHeight="1">
-      <c r="A13" s="185"/>
-      <c r="B13" s="191">
+      <c r="A13" s="184"/>
+      <c r="B13" s="190">
         <v>1.0</v>
       </c>
-      <c r="C13" s="192" t="str">
+      <c r="C13" s="191" t="str">
         <f>Manager!B2</f>
         <v>Manager</v>
       </c>
-      <c r="D13" s="193">
+      <c r="D13" s="192">
         <f>Manager!A6</f>
         <v>0</v>
       </c>
-      <c r="E13" s="193">
+      <c r="E13" s="192">
         <f>Manager!B6</f>
         <v>0</v>
       </c>
-      <c r="F13" s="193">
+      <c r="F13" s="192">
         <f>Manager!C6</f>
         <v>0</v>
       </c>
-      <c r="G13" s="194">
+      <c r="G13" s="193">
         <f>Manager!D6</f>
         <v>0</v>
       </c>
-      <c r="H13" s="195">
+      <c r="H13" s="194">
         <f>Manager!E6</f>
         <v>0</v>
       </c>
@@ -33900,28 +34173,28 @@
       <c r="Z13" s="11"/>
     </row>
     <row r="14" ht="12.75" customHeight="1">
-      <c r="A14" s="185"/>
-      <c r="B14" s="196"/>
-      <c r="C14" s="197" t="s">
-        <v>430</v>
-      </c>
-      <c r="D14" s="198">
+      <c r="A14" s="184"/>
+      <c r="B14" s="195"/>
+      <c r="C14" s="196" t="s">
+        <v>462</v>
+      </c>
+      <c r="D14" s="197">
         <f t="shared" ref="D14:H14" si="1">SUM(D9:D13)</f>
         <v>43</v>
       </c>
-      <c r="E14" s="198">
+      <c r="E14" s="197">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="F14" s="198">
+      <c r="F14" s="197">
         <f t="shared" si="1"/>
         <v>54</v>
       </c>
-      <c r="G14" s="198">
+      <c r="G14" s="197">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H14" s="199">
+      <c r="H14" s="198">
         <f t="shared" si="1"/>
         <v>101</v>
       </c>
@@ -33946,13 +34219,13 @@
     </row>
     <row r="15" ht="12.75" customHeight="1">
       <c r="A15" s="11"/>
-      <c r="B15" s="200"/>
+      <c r="B15" s="199"/>
       <c r="C15" s="11"/>
-      <c r="D15" s="201"/>
-      <c r="E15" s="202"/>
-      <c r="F15" s="202"/>
-      <c r="G15" s="202"/>
-      <c r="H15" s="202"/>
+      <c r="D15" s="200"/>
+      <c r="E15" s="201"/>
+      <c r="F15" s="201"/>
+      <c r="G15" s="201"/>
+      <c r="H15" s="201"/>
       <c r="I15" s="11"/>
       <c r="J15" s="11"/>
       <c r="K15" s="11"/>
@@ -33976,15 +34249,15 @@
       <c r="A16" s="11"/>
       <c r="B16" s="11"/>
       <c r="C16" s="9" t="s">
-        <v>431</v>
+        <v>463</v>
       </c>
       <c r="D16" s="11"/>
-      <c r="E16" s="203">
+      <c r="E16" s="202">
         <f>(D14+E14)*100/(H14-G14)</f>
         <v>46.53465347</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>432</v>
+        <v>464</v>
       </c>
       <c r="G16" s="11"/>
       <c r="H16" s="132"/>
@@ -34011,15 +34284,15 @@
       <c r="A17" s="11"/>
       <c r="B17" s="11"/>
       <c r="C17" s="9" t="s">
-        <v>433</v>
+        <v>465</v>
       </c>
       <c r="D17" s="11"/>
-      <c r="E17" s="203">
+      <c r="E17" s="202">
         <f>D14*100/(H14-G14)</f>
         <v>42.57425743</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>432</v>
+        <v>464</v>
       </c>
       <c r="G17" s="11"/>
       <c r="H17" s="132"/>

</xml_diff>

<commit_message>
HoangNH - Update test case 28 - 38
</commit_message>
<xml_diff>
--- a/3. Users/HoangNHHE130395/Testing/TestCase - Hoang.xlsx
+++ b/3. Users/HoangNHHE130395/Testing/TestCase - Hoang.xlsx
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="458">
   <si>
     <t>SYSTEM TEST CASE</t>
   </si>
@@ -1587,9 +1587,6 @@
     <t>Function Manage User</t>
   </si>
   <si>
-    <t>[Manager-1]</t>
-  </si>
-  <si>
     <t>Check GUI 'User' screen</t>
   </si>
   <si>
@@ -1606,9 +1603,6 @@
     <t>HoangNH</t>
   </si>
   <si>
-    <t>[Manager-2]</t>
-  </si>
-  <si>
     <t>Check paging user list</t>
   </si>
   <si>
@@ -1622,9 +1616,6 @@
 3. Item 'Next &gt;&gt;' is disabled</t>
   </si>
   <si>
-    <t>[Manager-3]</t>
-  </si>
-  <si>
     <t>1. Login into the web server
 2. Click on 'User' tab in the menu bar
 3. Click on 'Next &gt;&gt;' on the paging</t>
@@ -1633,9 +1624,6 @@
     <t>1. List of user in page 2 is displayed
 2. Item '&lt;&lt; Previous'  is enabled
 3. Item 'Next &gt;&gt;' is disabled</t>
-  </si>
-  <si>
-    <t>[Manager-4]</t>
   </si>
   <si>
     <t>1. Login into the web server
@@ -1648,18 +1636,12 @@
 2. "Previous" item is disabled</t>
   </si>
   <si>
-    <t>[Manager-5]</t>
-  </si>
-  <si>
     <t>1. Login into the web server
 2. Click on 'User' tab in the menu bar
 3. Click on '2' on the paging
 3. Click on '&lt;&lt; Previous' on the paging</t>
   </si>
   <si>
-    <t>[Manager-6]</t>
-  </si>
-  <si>
     <t>1. Login into the web server
 2. Click on 'User' tab in the menu bar
 3. Click on '2' on the paging
@@ -1669,9 +1651,6 @@
     <t>1. List of user in page 2 is displayed</t>
   </si>
   <si>
-    <t>[Manager-7]</t>
-  </si>
-  <si>
     <t>Check GUI search box 'Search User'</t>
   </si>
   <si>
@@ -1680,9 +1659,6 @@
   </si>
   <si>
     <t xml:space="preserve">1. Display text 'Search user' on the search box </t>
-  </si>
-  <si>
-    <t>[Manager-8]</t>
   </si>
   <si>
     <t>Check focus on search box 'Search User'</t>
@@ -1695,9 +1671,6 @@
   <si>
     <t>1. Display text 'Search user' on the search box 
 2. Border of the search box change to blue</t>
-  </si>
-  <si>
-    <t>[Manager-9]</t>
   </si>
   <si>
     <t>Check focus out search box 'Search User'</t>
@@ -1713,9 +1686,6 @@
 2. Border of the search box change from blue to white</t>
   </si>
   <si>
-    <t>[Manager-10]</t>
-  </si>
-  <si>
     <t>Check function seach box 'Search User'</t>
   </si>
   <si>
@@ -1731,9 +1701,6 @@
   </si>
   <si>
     <t>Text 'a'</t>
-  </si>
-  <si>
-    <t>[Manager-11]</t>
   </si>
   <si>
     <t>1. Login into the web server
@@ -1749,9 +1716,6 @@
   </si>
   <si>
     <t>Text 'aa'</t>
-  </si>
-  <si>
-    <t>[Manager-12]</t>
   </si>
   <si>
     <t>1. Login into the web server
@@ -1767,9 +1731,6 @@
 3. Display list of user have username contain character 'a'</t>
   </si>
   <si>
-    <t>[Manager-13]</t>
-  </si>
-  <si>
     <t>1. Login into the web server
 2. Click on 'User' tab in the menu bar
 3. Choose 'Email' from the drop down list
@@ -1780,9 +1741,6 @@
     <t>1. Display text 'a' on the search box 
 2. Border of the search box change to blue
 3. Display list of user have email contain character 'a'</t>
-  </si>
-  <si>
-    <t>[Manager-14]</t>
   </si>
   <si>
     <t>1. Login into the web server
@@ -1796,9 +1754,6 @@
     <t>1. Display text 'aa' on the search box 
 2. Border of the search box change to blue
 3. Display list of user have email contain character 'aa'</t>
-  </si>
-  <si>
-    <t>[Manager-15]</t>
   </si>
   <si>
     <t>1. Login into the web server
@@ -1815,9 +1770,6 @@
 3. Display list of user have email contain character 'a'</t>
   </si>
   <si>
-    <t>[Manager-16]</t>
-  </si>
-  <si>
     <t>1. Login into the web server
 2. Click on 'User' tab in the menu bar
 3. Choose 'Fullname' from the drop down list
@@ -1828,9 +1780,6 @@
     <t>1. Display text 'a' on the search box 
 2. Border of the search box change to blue
 3. Display list of user have fullname contain character 'a'</t>
-  </si>
-  <si>
-    <t>[Manager-17]</t>
   </si>
   <si>
     <t>1. Login into the web server
@@ -1844,9 +1793,6 @@
     <t>1. Display text 'aa' on the search box 
 2. Border of the search box change to blue
 3. Display list of user have fullname contain character 'aa'</t>
-  </si>
-  <si>
-    <t>[Manager-18]</t>
   </si>
   <si>
     <t>1. Login into the web server
@@ -1863,9 +1809,6 @@
 3. Display list of user have fullname contain character 'a'</t>
   </si>
   <si>
-    <t>[Manager-19]</t>
-  </si>
-  <si>
     <t>1. Login into the web server
 2. Click on 'User' tab in the menu bar
 3. Choose 'Phone' from the drop down list
@@ -1876,9 +1819,6 @@
     <t>1. Display text 'a' on the search box 
 2. Border of the search box change to blue
 3. Display list of user have phone contain character 'a'</t>
-  </si>
-  <si>
-    <t>[Manager-20]</t>
   </si>
   <si>
     <t>1. Login into the web server
@@ -1892,9 +1832,6 @@
     <t>1. Display text 'aa' on the search box 
 2. Border of the search box change to blue
 3. Display list of user have phone contain character 'aa'</t>
-  </si>
-  <si>
-    <t>[Manager-21]</t>
   </si>
   <si>
     <t>1. Login into the web server
@@ -1911,9 +1848,6 @@
 3. Display list of user have phone contain character 'a'</t>
   </si>
   <si>
-    <t>[Manager-22]</t>
-  </si>
-  <si>
     <t>1. Login into the web server
 2. Click on 'User' tab in the menu bar
 3. Choose 'Phone' from the drop down list
@@ -1922,9 +1856,6 @@
 6. Choose 'Username' from the drop down list</t>
   </si>
   <si>
-    <t>[Manager-23]</t>
-  </si>
-  <si>
     <t>1. Login into the web server
 2. Click on 'User' tab in the menu bar
 3. Choose 'Phone' from the drop down list
@@ -1933,9 +1864,6 @@
 6. Choose 'Email' from the drop down list</t>
   </si>
   <si>
-    <t>[Manager-24]</t>
-  </si>
-  <si>
     <t>1. Login into the web server
 2. Click on 'User' tab in the menu bar
 3. Choose 'Phone' from the drop down list
@@ -1944,9 +1872,6 @@
 6. Choose 'Fullname' from the drop down list</t>
   </si>
   <si>
-    <t>[Manager-25]</t>
-  </si>
-  <si>
     <t>Check GUI list users</t>
   </si>
   <si>
@@ -1958,9 +1883,6 @@
     <t xml:space="preserve">1. Display list users with following column: "ID, Username, Email, Fullname, Phone, Date created, Avatar, Status, Option" </t>
   </si>
   <si>
-    <t>[Manager-26]</t>
-  </si>
-  <si>
     <t>Check data in column of list users</t>
   </si>
   <si>
@@ -1968,7 +1890,81 @@
 2. The data of user is mapping wit the column name</t>
   </si>
   <si>
-    <t>[Manager-27]</t>
+    <t>Check function of  item 'edit' in 'Option' column</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'User' tab in the menu bar
+3. Click on the 'edit' in column 'Option' of user have id = '22'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Display detail information of user have id = '22' </t>
+  </si>
+  <si>
+    <t>User have id = '22'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check GUI user detail </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Display User's avatar, name, join date, email, phone, gender, address, date of birth, height, weight, bust, waist, hip, user's balance, user's post </t>
+  </si>
+  <si>
+    <t>Check GUI user status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Login into the web server
+2. Click on 'User' tab in the menu bar
+3. Click on the 'edit' in column 'Option' of user have id = '7'
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Display 'Active' if user is unbaned
+2. Display 'Inactive' if user is baned </t>
+  </si>
+  <si>
+    <t>User have id = '7'</t>
+  </si>
+  <si>
+    <t>Check GUI button Ban/Unban</t>
+  </si>
+  <si>
+    <t>1. Display 'Ban' if user is active
+2. Display 'Unban' if user is inactive</t>
+  </si>
+  <si>
+    <t>Check function button 'Ban'</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'User' tab in the menu bar
+3. Click on the 'edit' in column 'Option' of user have id = '7'
+4. Click Button 'Ban'</t>
+  </si>
+  <si>
+    <t>1. Display popup confirm 'Bạn có muốn ban đồ dùng này'</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'User' tab in the menu bar
+3. Click on the 'edit' in column 'Option' of user have id = '7'
+4. Click Button 'Ban'
+5. Click option 'Hủy' on the popup</t>
+  </si>
+  <si>
+    <t>1. Popup is disappear and user status is 'Active'</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'User' tab in the menu bar
+3. Click on the 'edit' in column 'Option' of user have id = '7'
+4. Click Button 'Ban'
+5. Click option 'Ok' on the popup</t>
+  </si>
+  <si>
+    <t>1. Toast notification 'Ban nguời dùng thành công' 
+2. Status of user change to 'Inactive'
+3. Button 'Ban' change to 'Unban'</t>
   </si>
   <si>
     <t>TEST REPORT</t>
@@ -2831,7 +2827,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="203">
+  <cellXfs count="204">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -3254,16 +3250,19 @@
     <xf borderId="5" fillId="2" fontId="1" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="0" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="0" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -28110,17 +28109,18 @@
       <c r="AA9" s="93"/>
     </row>
     <row r="10" ht="52.5" customHeight="1">
-      <c r="A10" s="160" t="s">
+      <c r="A10" s="160" t="str">
+        <f t="shared" ref="A10:A50" si="1">IF(OR(B10&lt;&gt;"",D10&lt;&gt;""),"["&amp;TEXT($B$2,"##")&amp;"-"&amp;TEXT(ROW()-9,"##")&amp;"]","")</f>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="B10" s="160" t="s">
         <v>372</v>
       </c>
-      <c r="B10" s="160" t="s">
+      <c r="C10" s="160" t="s">
         <v>373</v>
       </c>
-      <c r="C10" s="160" t="s">
+      <c r="D10" s="161" t="s">
         <v>374</v>
-      </c>
-      <c r="D10" s="161" t="s">
-        <v>375</v>
       </c>
       <c r="E10" s="117"/>
       <c r="F10" s="117"/>
@@ -28131,7 +28131,7 @@
         <v>44302.0</v>
       </c>
       <c r="I10" s="164" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J10" s="116"/>
       <c r="K10" s="11"/>
@@ -28153,20 +28153,22 @@
       <c r="AA10" s="11"/>
     </row>
     <row r="11" ht="49.5" customHeight="1">
-      <c r="A11" s="160" t="s">
+      <c r="A11" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v>[Manager-2]</v>
+      </c>
+      <c r="B11" s="160" t="s">
+        <v>376</v>
+      </c>
+      <c r="C11" s="160" t="s">
         <v>377</v>
       </c>
-      <c r="B11" s="160" t="s">
+      <c r="D11" s="161" t="s">
         <v>378</v>
       </c>
-      <c r="C11" s="160" t="s">
-        <v>379</v>
-      </c>
-      <c r="D11" s="161" t="s">
-        <v>380</v>
-      </c>
-      <c r="E11" s="160" t="s">
-        <v>372</v>
+      <c r="E11" s="160" t="str">
+        <f t="shared" ref="E11:E42" si="2">$A$10</f>
+        <v>[Manager-1]</v>
       </c>
       <c r="F11" s="117"/>
       <c r="G11" s="162" t="s">
@@ -28176,7 +28178,7 @@
         <v>44302.0</v>
       </c>
       <c r="I11" s="164" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J11" s="116"/>
       <c r="K11" s="11"/>
@@ -28198,20 +28200,22 @@
       <c r="AA11" s="11"/>
     </row>
     <row r="12" ht="65.25" customHeight="1">
-      <c r="A12" s="160" t="s">
-        <v>381</v>
+      <c r="A12" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v>[Manager-3]</v>
       </c>
       <c r="B12" s="160" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C12" s="160" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="D12" s="161" t="s">
-        <v>383</v>
-      </c>
-      <c r="E12" s="160" t="s">
-        <v>372</v>
+        <v>380</v>
+      </c>
+      <c r="E12" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
       </c>
       <c r="F12" s="117"/>
       <c r="G12" s="162" t="s">
@@ -28221,7 +28225,7 @@
         <v>44302.0</v>
       </c>
       <c r="I12" s="164" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J12" s="116"/>
       <c r="K12" s="11"/>
@@ -28243,20 +28247,22 @@
       <c r="AA12" s="11"/>
     </row>
     <row r="13" ht="66.0" customHeight="1">
-      <c r="A13" s="160" t="s">
-        <v>384</v>
+      <c r="A13" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v>[Manager-4]</v>
       </c>
       <c r="B13" s="160" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C13" s="160" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="D13" s="161" t="s">
-        <v>386</v>
-      </c>
-      <c r="E13" s="160" t="s">
-        <v>372</v>
+        <v>382</v>
+      </c>
+      <c r="E13" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
       </c>
       <c r="F13" s="117"/>
       <c r="G13" s="162" t="s">
@@ -28266,7 +28272,7 @@
         <v>44302.0</v>
       </c>
       <c r="I13" s="165" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J13" s="116"/>
       <c r="K13" s="11"/>
@@ -28288,20 +28294,22 @@
       <c r="AA13" s="11"/>
     </row>
     <row r="14" ht="65.25" customHeight="1">
-      <c r="A14" s="160" t="s">
-        <v>387</v>
+      <c r="A14" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v>[Manager-5]</v>
       </c>
       <c r="B14" s="160" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C14" s="160" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="D14" s="161" t="s">
-        <v>386</v>
-      </c>
-      <c r="E14" s="160" t="s">
-        <v>372</v>
+        <v>382</v>
+      </c>
+      <c r="E14" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
       </c>
       <c r="F14" s="117"/>
       <c r="G14" s="162" t="s">
@@ -28311,7 +28319,7 @@
         <v>44302.0</v>
       </c>
       <c r="I14" s="165" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J14" s="116"/>
       <c r="K14" s="11"/>
@@ -28333,20 +28341,22 @@
       <c r="AA14" s="11"/>
     </row>
     <row r="15" ht="61.5" customHeight="1">
-      <c r="A15" s="160" t="s">
-        <v>389</v>
+      <c r="A15" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v>[Manager-6]</v>
       </c>
       <c r="B15" s="160" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C15" s="160" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="D15" s="161" t="s">
-        <v>391</v>
-      </c>
-      <c r="E15" s="160" t="s">
-        <v>372</v>
+        <v>385</v>
+      </c>
+      <c r="E15" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
       </c>
       <c r="F15" s="117"/>
       <c r="G15" s="162" t="s">
@@ -28356,7 +28366,7 @@
         <v>44302.0</v>
       </c>
       <c r="I15" s="165" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J15" s="116"/>
       <c r="K15" s="11"/>
@@ -28378,20 +28388,22 @@
       <c r="AA15" s="11"/>
     </row>
     <row r="16" ht="49.5" customHeight="1">
-      <c r="A16" s="160" t="s">
-        <v>392</v>
+      <c r="A16" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v>[Manager-7]</v>
       </c>
       <c r="B16" s="160" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="C16" s="166" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
       <c r="D16" s="166" t="s">
-        <v>395</v>
-      </c>
-      <c r="E16" s="160" t="s">
-        <v>372</v>
+        <v>388</v>
+      </c>
+      <c r="E16" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
       </c>
       <c r="F16" s="117"/>
       <c r="G16" s="162" t="s">
@@ -28401,7 +28413,7 @@
         <v>44302.0</v>
       </c>
       <c r="I16" s="165" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J16" s="116"/>
       <c r="K16" s="11"/>
@@ -28423,20 +28435,22 @@
       <c r="AA16" s="11"/>
     </row>
     <row r="17" ht="49.5" customHeight="1">
-      <c r="A17" s="160" t="s">
-        <v>396</v>
+      <c r="A17" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v>[Manager-8]</v>
       </c>
       <c r="B17" s="160" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="C17" s="166" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="D17" s="166" t="s">
-        <v>399</v>
-      </c>
-      <c r="E17" s="160" t="s">
-        <v>372</v>
+        <v>391</v>
+      </c>
+      <c r="E17" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
       </c>
       <c r="F17" s="117"/>
       <c r="G17" s="162" t="s">
@@ -28446,7 +28460,7 @@
         <v>44302.0</v>
       </c>
       <c r="I17" s="165" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J17" s="116"/>
       <c r="K17" s="11"/>
@@ -28468,20 +28482,22 @@
       <c r="AA17" s="11"/>
     </row>
     <row r="18" ht="63.0" customHeight="1">
-      <c r="A18" s="160" t="s">
-        <v>400</v>
+      <c r="A18" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v>[Manager-9]</v>
       </c>
       <c r="B18" s="160" t="s">
-        <v>401</v>
+        <v>392</v>
       </c>
       <c r="C18" s="166" t="s">
-        <v>402</v>
+        <v>393</v>
       </c>
       <c r="D18" s="166" t="s">
-        <v>403</v>
-      </c>
-      <c r="E18" s="160" t="s">
-        <v>372</v>
+        <v>394</v>
+      </c>
+      <c r="E18" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
       </c>
       <c r="F18" s="117"/>
       <c r="G18" s="162" t="s">
@@ -28491,7 +28507,7 @@
         <v>44302.0</v>
       </c>
       <c r="I18" s="165" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J18" s="116"/>
       <c r="K18" s="11"/>
@@ -28513,23 +28529,25 @@
       <c r="AA18" s="11"/>
     </row>
     <row r="19" ht="61.5" customHeight="1">
-      <c r="A19" s="160" t="s">
-        <v>404</v>
+      <c r="A19" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v>[Manager-10]</v>
       </c>
       <c r="B19" s="160" t="s">
-        <v>405</v>
+        <v>395</v>
       </c>
       <c r="C19" s="166" t="s">
-        <v>406</v>
+        <v>396</v>
       </c>
       <c r="D19" s="166" t="s">
-        <v>407</v>
-      </c>
-      <c r="E19" s="160" t="s">
-        <v>372</v>
+        <v>397</v>
+      </c>
+      <c r="E19" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
       </c>
       <c r="F19" s="161" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
       <c r="G19" s="162" t="s">
         <v>83</v>
@@ -28538,7 +28556,7 @@
         <v>44302.0</v>
       </c>
       <c r="I19" s="165" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J19" s="116"/>
       <c r="K19" s="11"/>
@@ -28560,23 +28578,25 @@
       <c r="AA19" s="11"/>
     </row>
     <row r="20" ht="79.5" customHeight="1">
-      <c r="A20" s="160" t="s">
-        <v>409</v>
+      <c r="A20" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v>[Manager-11]</v>
       </c>
       <c r="B20" s="160" t="s">
-        <v>405</v>
+        <v>395</v>
       </c>
       <c r="C20" s="166" t="s">
-        <v>410</v>
+        <v>399</v>
       </c>
       <c r="D20" s="166" t="s">
-        <v>411</v>
-      </c>
-      <c r="E20" s="160" t="s">
-        <v>372</v>
+        <v>400</v>
+      </c>
+      <c r="E20" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
       </c>
       <c r="F20" s="161" t="s">
-        <v>412</v>
+        <v>401</v>
       </c>
       <c r="G20" s="162" t="s">
         <v>83</v>
@@ -28585,7 +28605,7 @@
         <v>44302.0</v>
       </c>
       <c r="I20" s="165" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J20" s="116"/>
       <c r="K20" s="11"/>
@@ -28607,23 +28627,25 @@
       <c r="AA20" s="11"/>
     </row>
     <row r="21" ht="89.25" customHeight="1">
-      <c r="A21" s="160" t="s">
-        <v>413</v>
+      <c r="A21" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v>[Manager-12]</v>
       </c>
       <c r="B21" s="160" t="s">
-        <v>405</v>
+        <v>395</v>
       </c>
       <c r="C21" s="166" t="s">
-        <v>414</v>
+        <v>402</v>
       </c>
       <c r="D21" s="166" t="s">
-        <v>415</v>
-      </c>
-      <c r="E21" s="160" t="s">
-        <v>372</v>
+        <v>403</v>
+      </c>
+      <c r="E21" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
       </c>
       <c r="F21" s="161" t="s">
-        <v>412</v>
+        <v>401</v>
       </c>
       <c r="G21" s="162" t="s">
         <v>83</v>
@@ -28632,7 +28654,7 @@
         <v>44302.0</v>
       </c>
       <c r="I21" s="165" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J21" s="116"/>
       <c r="K21" s="11"/>
@@ -28654,23 +28676,25 @@
       <c r="AA21" s="11"/>
     </row>
     <row r="22" ht="77.25" customHeight="1">
-      <c r="A22" s="160" t="s">
-        <v>416</v>
+      <c r="A22" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v>[Manager-13]</v>
       </c>
       <c r="B22" s="160" t="s">
+        <v>395</v>
+      </c>
+      <c r="C22" s="166" t="s">
+        <v>404</v>
+      </c>
+      <c r="D22" s="166" t="s">
         <v>405</v>
       </c>
-      <c r="C22" s="166" t="s">
-        <v>417</v>
-      </c>
-      <c r="D22" s="166" t="s">
-        <v>418</v>
-      </c>
-      <c r="E22" s="160" t="s">
-        <v>372</v>
+      <c r="E22" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
       </c>
       <c r="F22" s="161" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
       <c r="G22" s="162" t="s">
         <v>83</v>
@@ -28679,7 +28703,7 @@
         <v>44302.0</v>
       </c>
       <c r="I22" s="165" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J22" s="116"/>
       <c r="K22" s="11"/>
@@ -28701,23 +28725,25 @@
       <c r="AA22" s="11"/>
     </row>
     <row r="23" ht="90.0" customHeight="1">
-      <c r="A23" s="160" t="s">
-        <v>419</v>
+      <c r="A23" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v>[Manager-14]</v>
       </c>
       <c r="B23" s="160" t="s">
-        <v>405</v>
+        <v>395</v>
       </c>
       <c r="C23" s="166" t="s">
-        <v>420</v>
+        <v>406</v>
       </c>
       <c r="D23" s="166" t="s">
-        <v>421</v>
-      </c>
-      <c r="E23" s="160" t="s">
-        <v>372</v>
+        <v>407</v>
+      </c>
+      <c r="E23" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
       </c>
       <c r="F23" s="161" t="s">
-        <v>412</v>
+        <v>401</v>
       </c>
       <c r="G23" s="162" t="s">
         <v>83</v>
@@ -28726,7 +28752,7 @@
         <v>44302.0</v>
       </c>
       <c r="I23" s="165" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J23" s="116"/>
       <c r="K23" s="11"/>
@@ -28748,23 +28774,25 @@
       <c r="AA23" s="11"/>
     </row>
     <row r="24" ht="108.0" customHeight="1">
-      <c r="A24" s="160" t="s">
-        <v>422</v>
+      <c r="A24" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v>[Manager-15]</v>
       </c>
       <c r="B24" s="160" t="s">
-        <v>405</v>
+        <v>395</v>
       </c>
       <c r="C24" s="166" t="s">
-        <v>423</v>
+        <v>408</v>
       </c>
       <c r="D24" s="166" t="s">
-        <v>424</v>
-      </c>
-      <c r="E24" s="160" t="s">
-        <v>372</v>
+        <v>409</v>
+      </c>
+      <c r="E24" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
       </c>
       <c r="F24" s="161" t="s">
-        <v>412</v>
+        <v>401</v>
       </c>
       <c r="G24" s="162" t="s">
         <v>83</v>
@@ -28773,7 +28801,7 @@
         <v>44302.0</v>
       </c>
       <c r="I24" s="165" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J24" s="116"/>
       <c r="K24" s="11"/>
@@ -28795,23 +28823,25 @@
       <c r="AA24" s="11"/>
     </row>
     <row r="25" ht="82.5" customHeight="1">
-      <c r="A25" s="160" t="s">
-        <v>425</v>
+      <c r="A25" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v>[Manager-16]</v>
       </c>
       <c r="B25" s="160" t="s">
-        <v>405</v>
+        <v>395</v>
       </c>
       <c r="C25" s="166" t="s">
-        <v>426</v>
+        <v>410</v>
       </c>
       <c r="D25" s="166" t="s">
-        <v>427</v>
-      </c>
-      <c r="E25" s="160" t="s">
-        <v>372</v>
+        <v>411</v>
+      </c>
+      <c r="E25" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
       </c>
       <c r="F25" s="161" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
       <c r="G25" s="162" t="s">
         <v>83</v>
@@ -28820,7 +28850,7 @@
         <v>44302.0</v>
       </c>
       <c r="I25" s="165" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J25" s="116"/>
       <c r="K25" s="70"/>
@@ -28842,23 +28872,25 @@
       <c r="AA25" s="11"/>
     </row>
     <row r="26" ht="91.5" customHeight="1">
-      <c r="A26" s="160" t="s">
-        <v>428</v>
+      <c r="A26" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v>[Manager-17]</v>
       </c>
       <c r="B26" s="160" t="s">
-        <v>405</v>
+        <v>395</v>
       </c>
       <c r="C26" s="166" t="s">
-        <v>429</v>
+        <v>412</v>
       </c>
       <c r="D26" s="166" t="s">
-        <v>430</v>
-      </c>
-      <c r="E26" s="160" t="s">
-        <v>372</v>
+        <v>413</v>
+      </c>
+      <c r="E26" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
       </c>
       <c r="F26" s="161" t="s">
-        <v>412</v>
+        <v>401</v>
       </c>
       <c r="G26" s="162" t="s">
         <v>83</v>
@@ -28867,7 +28899,7 @@
         <v>44302.0</v>
       </c>
       <c r="I26" s="165" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J26" s="116"/>
       <c r="K26" s="93"/>
@@ -28889,23 +28921,25 @@
       <c r="AA26" s="93"/>
     </row>
     <row r="27" ht="104.25" customHeight="1">
-      <c r="A27" s="160" t="s">
-        <v>431</v>
+      <c r="A27" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v>[Manager-18]</v>
       </c>
       <c r="B27" s="160" t="s">
-        <v>405</v>
+        <v>395</v>
       </c>
       <c r="C27" s="166" t="s">
-        <v>432</v>
+        <v>414</v>
       </c>
       <c r="D27" s="166" t="s">
-        <v>433</v>
-      </c>
-      <c r="E27" s="160" t="s">
-        <v>372</v>
+        <v>415</v>
+      </c>
+      <c r="E27" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
       </c>
       <c r="F27" s="161" t="s">
-        <v>412</v>
+        <v>401</v>
       </c>
       <c r="G27" s="162" t="s">
         <v>83</v>
@@ -28914,7 +28948,7 @@
         <v>44302.0</v>
       </c>
       <c r="I27" s="165" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J27" s="116"/>
       <c r="K27" s="11"/>
@@ -28936,23 +28970,25 @@
       <c r="AA27" s="11"/>
     </row>
     <row r="28" ht="80.25" customHeight="1">
-      <c r="A28" s="160" t="s">
-        <v>434</v>
+      <c r="A28" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v>[Manager-19]</v>
       </c>
       <c r="B28" s="160" t="s">
-        <v>405</v>
+        <v>395</v>
       </c>
       <c r="C28" s="166" t="s">
-        <v>435</v>
+        <v>416</v>
       </c>
       <c r="D28" s="166" t="s">
-        <v>436</v>
-      </c>
-      <c r="E28" s="160" t="s">
-        <v>372</v>
+        <v>417</v>
+      </c>
+      <c r="E28" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
       </c>
       <c r="F28" s="161" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
       <c r="G28" s="162" t="s">
         <v>83</v>
@@ -28961,7 +28997,7 @@
         <v>44302.0</v>
       </c>
       <c r="I28" s="165" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J28" s="116"/>
       <c r="K28" s="11"/>
@@ -28983,23 +29019,25 @@
       <c r="AA28" s="11"/>
     </row>
     <row r="29" ht="90.75" customHeight="1">
-      <c r="A29" s="160" t="s">
-        <v>437</v>
+      <c r="A29" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v>[Manager-20]</v>
       </c>
       <c r="B29" s="160" t="s">
-        <v>405</v>
+        <v>395</v>
       </c>
       <c r="C29" s="166" t="s">
-        <v>438</v>
+        <v>418</v>
       </c>
       <c r="D29" s="166" t="s">
-        <v>439</v>
-      </c>
-      <c r="E29" s="160" t="s">
-        <v>372</v>
+        <v>419</v>
+      </c>
+      <c r="E29" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
       </c>
       <c r="F29" s="161" t="s">
-        <v>412</v>
+        <v>401</v>
       </c>
       <c r="G29" s="162" t="s">
         <v>83</v>
@@ -29008,7 +29046,7 @@
         <v>44302.0</v>
       </c>
       <c r="I29" s="165" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J29" s="116"/>
       <c r="K29" s="93"/>
@@ -29030,23 +29068,25 @@
       <c r="AA29" s="93"/>
     </row>
     <row r="30" ht="110.25" customHeight="1">
-      <c r="A30" s="160" t="s">
-        <v>440</v>
+      <c r="A30" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v>[Manager-21]</v>
       </c>
       <c r="B30" s="160" t="s">
-        <v>405</v>
+        <v>395</v>
       </c>
       <c r="C30" s="166" t="s">
-        <v>441</v>
+        <v>420</v>
       </c>
       <c r="D30" s="166" t="s">
-        <v>442</v>
-      </c>
-      <c r="E30" s="160" t="s">
-        <v>372</v>
+        <v>421</v>
+      </c>
+      <c r="E30" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
       </c>
       <c r="F30" s="161" t="s">
-        <v>412</v>
+        <v>401</v>
       </c>
       <c r="G30" s="162" t="s">
         <v>83</v>
@@ -29054,8 +29094,8 @@
       <c r="H30" s="163">
         <v>44302.0</v>
       </c>
-      <c r="I30" s="167" t="s">
-        <v>376</v>
+      <c r="I30" s="165" t="s">
+        <v>375</v>
       </c>
       <c r="J30" s="116"/>
       <c r="K30" s="11"/>
@@ -29077,23 +29117,25 @@
       <c r="AA30" s="11"/>
     </row>
     <row r="31" ht="93.0" customHeight="1">
-      <c r="A31" s="160" t="s">
-        <v>443</v>
+      <c r="A31" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v>[Manager-22]</v>
       </c>
       <c r="B31" s="160" t="s">
-        <v>405</v>
+        <v>395</v>
       </c>
       <c r="C31" s="166" t="s">
-        <v>444</v>
+        <v>422</v>
       </c>
       <c r="D31" s="166" t="s">
-        <v>407</v>
-      </c>
-      <c r="E31" s="160" t="s">
-        <v>372</v>
+        <v>397</v>
+      </c>
+      <c r="E31" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
       </c>
       <c r="F31" s="161" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
       <c r="G31" s="162" t="s">
         <v>83</v>
@@ -29102,7 +29144,7 @@
         <v>44302.0</v>
       </c>
       <c r="I31" s="165" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J31" s="116"/>
       <c r="K31" s="155"/>
@@ -29124,23 +29166,25 @@
       <c r="AA31" s="155"/>
     </row>
     <row r="32" ht="85.5" customHeight="1">
-      <c r="A32" s="160" t="s">
-        <v>445</v>
+      <c r="A32" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v>[Manager-23]</v>
       </c>
       <c r="B32" s="160" t="s">
+        <v>395</v>
+      </c>
+      <c r="C32" s="166" t="s">
+        <v>423</v>
+      </c>
+      <c r="D32" s="166" t="s">
         <v>405</v>
       </c>
-      <c r="C32" s="166" t="s">
-        <v>446</v>
-      </c>
-      <c r="D32" s="166" t="s">
-        <v>418</v>
-      </c>
-      <c r="E32" s="160" t="s">
-        <v>372</v>
+      <c r="E32" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
       </c>
       <c r="F32" s="161" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
       <c r="G32" s="162" t="s">
         <v>83</v>
@@ -29149,7 +29193,7 @@
         <v>44302.0</v>
       </c>
       <c r="I32" s="165" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J32" s="116"/>
       <c r="K32" s="155"/>
@@ -29171,23 +29215,25 @@
       <c r="AA32" s="155"/>
     </row>
     <row r="33" ht="94.5" customHeight="1">
-      <c r="A33" s="160" t="s">
-        <v>447</v>
+      <c r="A33" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v>[Manager-24]</v>
       </c>
       <c r="B33" s="160" t="s">
-        <v>405</v>
+        <v>395</v>
       </c>
       <c r="C33" s="166" t="s">
-        <v>448</v>
+        <v>424</v>
       </c>
       <c r="D33" s="166" t="s">
-        <v>427</v>
-      </c>
-      <c r="E33" s="160" t="s">
-        <v>372</v>
+        <v>411</v>
+      </c>
+      <c r="E33" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
       </c>
       <c r="F33" s="161" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
       <c r="G33" s="162" t="s">
         <v>83</v>
@@ -29196,7 +29242,7 @@
         <v>44302.0</v>
       </c>
       <c r="I33" s="165" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J33" s="116"/>
       <c r="K33" s="155"/>
@@ -29218,20 +29264,22 @@
       <c r="AA33" s="155"/>
     </row>
     <row r="34" ht="61.5" customHeight="1">
-      <c r="A34" s="160" t="s">
-        <v>449</v>
+      <c r="A34" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v>[Manager-25]</v>
       </c>
       <c r="B34" s="160" t="s">
-        <v>450</v>
+        <v>425</v>
       </c>
       <c r="C34" s="166" t="s">
-        <v>451</v>
+        <v>426</v>
       </c>
       <c r="D34" s="166" t="s">
-        <v>452</v>
-      </c>
-      <c r="E34" s="160" t="s">
-        <v>372</v>
+        <v>427</v>
+      </c>
+      <c r="E34" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
       </c>
       <c r="F34" s="161"/>
       <c r="G34" s="162" t="s">
@@ -29241,7 +29289,7 @@
         <v>44302.0</v>
       </c>
       <c r="I34" s="165" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J34" s="116"/>
       <c r="K34" s="155"/>
@@ -29263,20 +29311,22 @@
       <c r="AA34" s="155"/>
     </row>
     <row r="35" ht="93.75" customHeight="1">
-      <c r="A35" s="160" t="s">
-        <v>453</v>
+      <c r="A35" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v>[Manager-26]</v>
       </c>
       <c r="B35" s="160" t="s">
-        <v>454</v>
+        <v>428</v>
       </c>
       <c r="C35" s="166" t="s">
-        <v>451</v>
+        <v>426</v>
       </c>
       <c r="D35" s="166" t="s">
-        <v>455</v>
-      </c>
-      <c r="E35" s="160" t="s">
-        <v>372</v>
+        <v>429</v>
+      </c>
+      <c r="E35" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
       </c>
       <c r="F35" s="161"/>
       <c r="G35" s="162" t="s">
@@ -29286,7 +29336,7 @@
         <v>44302.0</v>
       </c>
       <c r="I35" s="165" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J35" s="116"/>
       <c r="K35" s="155"/>
@@ -29308,22 +29358,26 @@
       <c r="AA35" s="155"/>
     </row>
     <row r="36" ht="90.75" customHeight="1">
-      <c r="A36" s="160" t="s">
-        <v>456</v>
+      <c r="A36" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v>[Manager-27]</v>
       </c>
       <c r="B36" s="160" t="s">
-        <v>405</v>
+        <v>430</v>
       </c>
       <c r="C36" s="166" t="s">
-        <v>448</v>
+        <v>431</v>
       </c>
       <c r="D36" s="166" t="s">
-        <v>427</v>
-      </c>
-      <c r="E36" s="160" t="s">
-        <v>372</v>
-      </c>
-      <c r="F36" s="161"/>
+        <v>432</v>
+      </c>
+      <c r="E36" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F36" s="161" t="s">
+        <v>433</v>
+      </c>
       <c r="G36" s="162" t="s">
         <v>83</v>
       </c>
@@ -29331,7 +29385,7 @@
         <v>44302.0</v>
       </c>
       <c r="I36" s="165" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J36" s="116"/>
       <c r="K36" s="155"/>
@@ -29352,17 +29406,37 @@
       <c r="Z36" s="155"/>
       <c r="AA36" s="155"/>
     </row>
-    <row r="37" ht="12.75" customHeight="1">
-      <c r="A37" s="125"/>
-      <c r="B37" s="125"/>
-      <c r="C37" s="125"/>
-      <c r="D37" s="125"/>
-      <c r="E37" s="125"/>
-      <c r="F37" s="125"/>
-      <c r="G37" s="168"/>
-      <c r="H37" s="168"/>
-      <c r="I37" s="168"/>
-      <c r="J37" s="125"/>
+    <row r="37" ht="69.0" customHeight="1">
+      <c r="A37" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v>[Manager-28]</v>
+      </c>
+      <c r="B37" s="160" t="s">
+        <v>434</v>
+      </c>
+      <c r="C37" s="166" t="s">
+        <v>431</v>
+      </c>
+      <c r="D37" s="167" t="s">
+        <v>435</v>
+      </c>
+      <c r="E37" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F37" s="161" t="s">
+        <v>433</v>
+      </c>
+      <c r="G37" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H37" s="163">
+        <v>44302.0</v>
+      </c>
+      <c r="I37" s="165" t="s">
+        <v>375</v>
+      </c>
+      <c r="J37" s="116"/>
       <c r="K37" s="155"/>
       <c r="L37" s="156"/>
       <c r="M37" s="155"/>
@@ -29381,17 +29455,37 @@
       <c r="Z37" s="155"/>
       <c r="AA37" s="155"/>
     </row>
-    <row r="38" ht="12.75" customHeight="1">
-      <c r="A38" s="125"/>
-      <c r="B38" s="125"/>
-      <c r="C38" s="125"/>
-      <c r="D38" s="125"/>
-      <c r="E38" s="125"/>
-      <c r="F38" s="125"/>
-      <c r="G38" s="168"/>
-      <c r="H38" s="168"/>
-      <c r="I38" s="168"/>
-      <c r="J38" s="125"/>
+    <row r="38" ht="69.75" customHeight="1">
+      <c r="A38" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v>[Manager-29]</v>
+      </c>
+      <c r="B38" s="160" t="s">
+        <v>436</v>
+      </c>
+      <c r="C38" s="167" t="s">
+        <v>437</v>
+      </c>
+      <c r="D38" s="167" t="s">
+        <v>438</v>
+      </c>
+      <c r="E38" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F38" s="161" t="s">
+        <v>439</v>
+      </c>
+      <c r="G38" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H38" s="163">
+        <v>44302.0</v>
+      </c>
+      <c r="I38" s="165" t="s">
+        <v>375</v>
+      </c>
+      <c r="J38" s="116"/>
       <c r="K38" s="155"/>
       <c r="L38" s="156"/>
       <c r="M38" s="155"/>
@@ -29410,17 +29504,37 @@
       <c r="Z38" s="155"/>
       <c r="AA38" s="155"/>
     </row>
-    <row r="39" ht="12.75" customHeight="1">
-      <c r="A39" s="125"/>
-      <c r="B39" s="125"/>
-      <c r="C39" s="125"/>
-      <c r="D39" s="125"/>
-      <c r="E39" s="125"/>
-      <c r="F39" s="125"/>
-      <c r="G39" s="168"/>
-      <c r="H39" s="168"/>
-      <c r="I39" s="168"/>
-      <c r="J39" s="125"/>
+    <row r="39" ht="63.75" customHeight="1">
+      <c r="A39" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v>[Manager-30]</v>
+      </c>
+      <c r="B39" s="160" t="s">
+        <v>440</v>
+      </c>
+      <c r="C39" s="167" t="s">
+        <v>437</v>
+      </c>
+      <c r="D39" s="167" t="s">
+        <v>441</v>
+      </c>
+      <c r="E39" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F39" s="161" t="s">
+        <v>439</v>
+      </c>
+      <c r="G39" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H39" s="163">
+        <v>44302.0</v>
+      </c>
+      <c r="I39" s="165" t="s">
+        <v>375</v>
+      </c>
+      <c r="J39" s="116"/>
       <c r="K39" s="155"/>
       <c r="L39" s="156"/>
       <c r="M39" s="155"/>
@@ -29439,17 +29553,37 @@
       <c r="Z39" s="155"/>
       <c r="AA39" s="155"/>
     </row>
-    <row r="40" ht="12.75" customHeight="1">
-      <c r="A40" s="125"/>
-      <c r="B40" s="125"/>
-      <c r="C40" s="125"/>
-      <c r="D40" s="125"/>
-      <c r="E40" s="125"/>
-      <c r="F40" s="125"/>
-      <c r="G40" s="168"/>
-      <c r="H40" s="168"/>
-      <c r="I40" s="168"/>
-      <c r="J40" s="125"/>
+    <row r="40" ht="66.75" customHeight="1">
+      <c r="A40" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v>[Manager-31]</v>
+      </c>
+      <c r="B40" s="160" t="s">
+        <v>442</v>
+      </c>
+      <c r="C40" s="167" t="s">
+        <v>443</v>
+      </c>
+      <c r="D40" s="167" t="s">
+        <v>444</v>
+      </c>
+      <c r="E40" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F40" s="161" t="s">
+        <v>439</v>
+      </c>
+      <c r="G40" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H40" s="163">
+        <v>44302.0</v>
+      </c>
+      <c r="I40" s="168" t="s">
+        <v>375</v>
+      </c>
+      <c r="J40" s="116"/>
       <c r="K40" s="155"/>
       <c r="L40" s="156"/>
       <c r="M40" s="155"/>
@@ -29468,17 +29602,37 @@
       <c r="Z40" s="155"/>
       <c r="AA40" s="155"/>
     </row>
-    <row r="41" ht="12.75" customHeight="1">
-      <c r="A41" s="125"/>
-      <c r="B41" s="125"/>
-      <c r="C41" s="125"/>
-      <c r="D41" s="125"/>
-      <c r="E41" s="125"/>
-      <c r="F41" s="125"/>
-      <c r="G41" s="168"/>
-      <c r="H41" s="168"/>
-      <c r="I41" s="168"/>
-      <c r="J41" s="125"/>
+    <row r="41" ht="85.5" customHeight="1">
+      <c r="A41" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v>[Manager-32]</v>
+      </c>
+      <c r="B41" s="160" t="s">
+        <v>442</v>
+      </c>
+      <c r="C41" s="167" t="s">
+        <v>445</v>
+      </c>
+      <c r="D41" s="167" t="s">
+        <v>446</v>
+      </c>
+      <c r="E41" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F41" s="161" t="s">
+        <v>439</v>
+      </c>
+      <c r="G41" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H41" s="163">
+        <v>44302.0</v>
+      </c>
+      <c r="I41" s="168" t="s">
+        <v>375</v>
+      </c>
+      <c r="J41" s="116"/>
       <c r="K41" s="155"/>
       <c r="L41" s="156"/>
       <c r="M41" s="155"/>
@@ -29497,17 +29651,37 @@
       <c r="Z41" s="155"/>
       <c r="AA41" s="155"/>
     </row>
-    <row r="42" ht="12.75" customHeight="1">
-      <c r="A42" s="125"/>
-      <c r="B42" s="125"/>
-      <c r="C42" s="125"/>
-      <c r="D42" s="125"/>
-      <c r="E42" s="125"/>
-      <c r="F42" s="125"/>
-      <c r="G42" s="168"/>
-      <c r="H42" s="168"/>
-      <c r="I42" s="168"/>
-      <c r="J42" s="125"/>
+    <row r="42" ht="92.25" customHeight="1">
+      <c r="A42" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v>[Manager-33]</v>
+      </c>
+      <c r="B42" s="160" t="s">
+        <v>442</v>
+      </c>
+      <c r="C42" s="167" t="s">
+        <v>447</v>
+      </c>
+      <c r="D42" s="167" t="s">
+        <v>448</v>
+      </c>
+      <c r="E42" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F42" s="161" t="s">
+        <v>439</v>
+      </c>
+      <c r="G42" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H42" s="163">
+        <v>44302.0</v>
+      </c>
+      <c r="I42" s="168" t="s">
+        <v>375</v>
+      </c>
+      <c r="J42" s="116"/>
       <c r="K42" s="155"/>
       <c r="L42" s="156"/>
       <c r="M42" s="155"/>
@@ -29527,15 +29701,18 @@
       <c r="AA42" s="155"/>
     </row>
     <row r="43" ht="12.75" customHeight="1">
-      <c r="A43" s="125"/>
+      <c r="A43" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="B43" s="125"/>
       <c r="C43" s="125"/>
       <c r="D43" s="125"/>
       <c r="E43" s="125"/>
       <c r="F43" s="125"/>
-      <c r="G43" s="168"/>
-      <c r="H43" s="168"/>
-      <c r="I43" s="168"/>
+      <c r="G43" s="169"/>
+      <c r="H43" s="169"/>
+      <c r="I43" s="169"/>
       <c r="J43" s="125"/>
       <c r="K43" s="155"/>
       <c r="L43" s="156"/>
@@ -29556,15 +29733,18 @@
       <c r="AA43" s="155"/>
     </row>
     <row r="44" ht="12.75" customHeight="1">
-      <c r="A44" s="125"/>
+      <c r="A44" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="B44" s="125"/>
       <c r="C44" s="125"/>
       <c r="D44" s="125"/>
       <c r="E44" s="125"/>
       <c r="F44" s="125"/>
-      <c r="G44" s="168"/>
-      <c r="H44" s="168"/>
-      <c r="I44" s="168"/>
+      <c r="G44" s="169"/>
+      <c r="H44" s="169"/>
+      <c r="I44" s="169"/>
       <c r="J44" s="125"/>
       <c r="K44" s="155"/>
       <c r="L44" s="156"/>
@@ -29585,15 +29765,18 @@
       <c r="AA44" s="155"/>
     </row>
     <row r="45" ht="12.75" customHeight="1">
-      <c r="A45" s="125"/>
+      <c r="A45" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="B45" s="125"/>
       <c r="C45" s="125"/>
       <c r="D45" s="125"/>
       <c r="E45" s="125"/>
       <c r="F45" s="125"/>
-      <c r="G45" s="168"/>
-      <c r="H45" s="168"/>
-      <c r="I45" s="168"/>
+      <c r="G45" s="169"/>
+      <c r="H45" s="169"/>
+      <c r="I45" s="169"/>
       <c r="J45" s="125"/>
       <c r="K45" s="155"/>
       <c r="L45" s="156"/>
@@ -29614,15 +29797,18 @@
       <c r="AA45" s="155"/>
     </row>
     <row r="46" ht="12.75" customHeight="1">
-      <c r="A46" s="125"/>
+      <c r="A46" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="B46" s="125"/>
       <c r="C46" s="125"/>
       <c r="D46" s="125"/>
       <c r="E46" s="125"/>
       <c r="F46" s="125"/>
-      <c r="G46" s="168"/>
-      <c r="H46" s="168"/>
-      <c r="I46" s="168"/>
+      <c r="G46" s="169"/>
+      <c r="H46" s="169"/>
+      <c r="I46" s="169"/>
       <c r="J46" s="125"/>
       <c r="K46" s="155"/>
       <c r="L46" s="156"/>
@@ -29643,15 +29829,18 @@
       <c r="AA46" s="155"/>
     </row>
     <row r="47" ht="12.75" customHeight="1">
-      <c r="A47" s="125"/>
+      <c r="A47" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="B47" s="125"/>
       <c r="C47" s="125"/>
       <c r="D47" s="125"/>
       <c r="E47" s="125"/>
       <c r="F47" s="125"/>
-      <c r="G47" s="168"/>
-      <c r="H47" s="168"/>
-      <c r="I47" s="168"/>
+      <c r="G47" s="169"/>
+      <c r="H47" s="169"/>
+      <c r="I47" s="169"/>
       <c r="J47" s="125"/>
       <c r="K47" s="155"/>
       <c r="L47" s="156"/>
@@ -29672,15 +29861,18 @@
       <c r="AA47" s="155"/>
     </row>
     <row r="48" ht="12.75" customHeight="1">
-      <c r="A48" s="125"/>
+      <c r="A48" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="B48" s="125"/>
       <c r="C48" s="125"/>
       <c r="D48" s="125"/>
       <c r="E48" s="125"/>
       <c r="F48" s="125"/>
-      <c r="G48" s="168"/>
-      <c r="H48" s="168"/>
-      <c r="I48" s="168"/>
+      <c r="G48" s="169"/>
+      <c r="H48" s="169"/>
+      <c r="I48" s="169"/>
       <c r="J48" s="125"/>
       <c r="K48" s="155"/>
       <c r="L48" s="156"/>
@@ -29701,15 +29893,18 @@
       <c r="AA48" s="155"/>
     </row>
     <row r="49" ht="12.75" customHeight="1">
-      <c r="A49" s="125"/>
+      <c r="A49" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="B49" s="125"/>
       <c r="C49" s="125"/>
       <c r="D49" s="125"/>
       <c r="E49" s="125"/>
       <c r="F49" s="125"/>
-      <c r="G49" s="168"/>
-      <c r="H49" s="168"/>
-      <c r="I49" s="168"/>
+      <c r="G49" s="169"/>
+      <c r="H49" s="169"/>
+      <c r="I49" s="169"/>
       <c r="J49" s="125"/>
       <c r="K49" s="155"/>
       <c r="L49" s="156"/>
@@ -29730,15 +29925,18 @@
       <c r="AA49" s="155"/>
     </row>
     <row r="50" ht="12.75" customHeight="1">
-      <c r="A50" s="125"/>
+      <c r="A50" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="B50" s="125"/>
       <c r="C50" s="125"/>
       <c r="D50" s="125"/>
       <c r="E50" s="125"/>
       <c r="F50" s="125"/>
-      <c r="G50" s="168"/>
-      <c r="H50" s="168"/>
-      <c r="I50" s="168"/>
+      <c r="G50" s="169"/>
+      <c r="H50" s="169"/>
+      <c r="I50" s="169"/>
       <c r="J50" s="125"/>
       <c r="K50" s="155"/>
       <c r="L50" s="156"/>
@@ -29761,13 +29959,13 @@
     <row r="51" ht="12.75" customHeight="1">
       <c r="A51" s="50"/>
       <c r="B51" s="50"/>
-      <c r="C51" s="169"/>
-      <c r="D51" s="169"/>
+      <c r="C51" s="170"/>
+      <c r="D51" s="170"/>
       <c r="E51" s="50"/>
       <c r="F51" s="50"/>
-      <c r="G51" s="170"/>
-      <c r="H51" s="170"/>
-      <c r="I51" s="170"/>
+      <c r="G51" s="171"/>
+      <c r="H51" s="171"/>
+      <c r="I51" s="171"/>
       <c r="J51" s="50"/>
       <c r="K51" s="86"/>
       <c r="L51" s="11"/>
@@ -29790,13 +29988,13 @@
     <row r="52" ht="12.75" customHeight="1">
       <c r="A52" s="50"/>
       <c r="B52" s="50"/>
-      <c r="C52" s="169"/>
-      <c r="D52" s="169"/>
+      <c r="C52" s="170"/>
+      <c r="D52" s="170"/>
       <c r="E52" s="50"/>
       <c r="F52" s="50"/>
-      <c r="G52" s="170"/>
-      <c r="H52" s="170"/>
-      <c r="I52" s="170"/>
+      <c r="G52" s="171"/>
+      <c r="H52" s="171"/>
+      <c r="I52" s="171"/>
       <c r="J52" s="50"/>
       <c r="K52" s="86"/>
       <c r="L52" s="11"/>
@@ -29819,13 +30017,13 @@
     <row r="53" ht="12.75" customHeight="1">
       <c r="A53" s="50"/>
       <c r="B53" s="50"/>
-      <c r="C53" s="169"/>
-      <c r="D53" s="169"/>
+      <c r="C53" s="170"/>
+      <c r="D53" s="170"/>
       <c r="E53" s="50"/>
       <c r="F53" s="50"/>
-      <c r="G53" s="170"/>
-      <c r="H53" s="170"/>
-      <c r="I53" s="170"/>
+      <c r="G53" s="171"/>
+      <c r="H53" s="171"/>
+      <c r="I53" s="171"/>
       <c r="J53" s="50"/>
       <c r="K53" s="86"/>
       <c r="L53" s="11"/>
@@ -29848,13 +30046,13 @@
     <row r="54" ht="12.75" customHeight="1">
       <c r="A54" s="50"/>
       <c r="B54" s="50"/>
-      <c r="C54" s="169"/>
-      <c r="D54" s="169"/>
+      <c r="C54" s="170"/>
+      <c r="D54" s="170"/>
       <c r="E54" s="50"/>
       <c r="F54" s="50"/>
-      <c r="G54" s="170"/>
-      <c r="H54" s="170"/>
-      <c r="I54" s="170"/>
+      <c r="G54" s="171"/>
+      <c r="H54" s="171"/>
+      <c r="I54" s="171"/>
       <c r="J54" s="50"/>
       <c r="K54" s="86"/>
       <c r="L54" s="11"/>
@@ -29878,12 +30076,12 @@
       <c r="A55" s="50"/>
       <c r="B55" s="50"/>
       <c r="C55" s="50"/>
-      <c r="D55" s="169"/>
+      <c r="D55" s="170"/>
       <c r="E55" s="50"/>
       <c r="F55" s="50"/>
-      <c r="G55" s="170"/>
-      <c r="H55" s="170"/>
-      <c r="I55" s="170"/>
+      <c r="G55" s="171"/>
+      <c r="H55" s="171"/>
+      <c r="I55" s="171"/>
       <c r="J55" s="50"/>
       <c r="K55" s="86"/>
       <c r="L55" s="11"/>
@@ -29907,12 +30105,12 @@
       <c r="A56" s="50"/>
       <c r="B56" s="50"/>
       <c r="C56" s="50"/>
-      <c r="D56" s="169"/>
+      <c r="D56" s="170"/>
       <c r="E56" s="50"/>
       <c r="F56" s="50"/>
-      <c r="G56" s="170"/>
-      <c r="H56" s="170"/>
-      <c r="I56" s="170"/>
+      <c r="G56" s="171"/>
+      <c r="H56" s="171"/>
+      <c r="I56" s="171"/>
       <c r="J56" s="50"/>
       <c r="K56" s="86"/>
       <c r="L56" s="11"/>
@@ -29936,12 +30134,12 @@
       <c r="A57" s="50"/>
       <c r="B57" s="50"/>
       <c r="C57" s="50"/>
-      <c r="D57" s="169"/>
+      <c r="D57" s="170"/>
       <c r="E57" s="50"/>
       <c r="F57" s="50"/>
-      <c r="G57" s="170"/>
-      <c r="H57" s="170"/>
-      <c r="I57" s="170"/>
+      <c r="G57" s="171"/>
+      <c r="H57" s="171"/>
+      <c r="I57" s="171"/>
       <c r="J57" s="50"/>
       <c r="K57" s="86"/>
       <c r="L57" s="11"/>
@@ -29965,12 +30163,12 @@
       <c r="A58" s="50"/>
       <c r="B58" s="50"/>
       <c r="C58" s="50"/>
-      <c r="D58" s="169"/>
+      <c r="D58" s="170"/>
       <c r="E58" s="50"/>
       <c r="F58" s="50"/>
-      <c r="G58" s="170"/>
-      <c r="H58" s="170"/>
-      <c r="I58" s="170"/>
+      <c r="G58" s="171"/>
+      <c r="H58" s="171"/>
+      <c r="I58" s="171"/>
       <c r="J58" s="50"/>
       <c r="K58" s="86"/>
       <c r="L58" s="11"/>
@@ -29994,12 +30192,12 @@
       <c r="A59" s="50"/>
       <c r="B59" s="50"/>
       <c r="C59" s="50"/>
-      <c r="D59" s="169"/>
+      <c r="D59" s="170"/>
       <c r="E59" s="50"/>
       <c r="F59" s="50"/>
-      <c r="G59" s="170"/>
-      <c r="H59" s="170"/>
-      <c r="I59" s="170"/>
+      <c r="G59" s="171"/>
+      <c r="H59" s="171"/>
+      <c r="I59" s="171"/>
       <c r="J59" s="50"/>
       <c r="K59" s="86"/>
       <c r="L59" s="11"/>
@@ -30023,12 +30221,12 @@
       <c r="A60" s="50"/>
       <c r="B60" s="50"/>
       <c r="C60" s="50"/>
-      <c r="D60" s="169"/>
+      <c r="D60" s="170"/>
       <c r="E60" s="50"/>
       <c r="F60" s="50"/>
-      <c r="G60" s="170"/>
-      <c r="H60" s="170"/>
-      <c r="I60" s="170"/>
+      <c r="G60" s="171"/>
+      <c r="H60" s="171"/>
+      <c r="I60" s="171"/>
       <c r="J60" s="50"/>
       <c r="K60" s="86"/>
       <c r="L60" s="11"/>
@@ -30052,12 +30250,12 @@
       <c r="A61" s="50"/>
       <c r="B61" s="50"/>
       <c r="C61" s="50"/>
-      <c r="D61" s="169"/>
+      <c r="D61" s="170"/>
       <c r="E61" s="50"/>
       <c r="F61" s="50"/>
-      <c r="G61" s="170"/>
-      <c r="H61" s="170"/>
-      <c r="I61" s="170"/>
+      <c r="G61" s="171"/>
+      <c r="H61" s="171"/>
+      <c r="I61" s="171"/>
       <c r="J61" s="50"/>
       <c r="K61" s="86"/>
       <c r="L61" s="11"/>
@@ -30081,12 +30279,12 @@
       <c r="A62" s="50"/>
       <c r="B62" s="50"/>
       <c r="C62" s="50"/>
-      <c r="D62" s="169"/>
+      <c r="D62" s="170"/>
       <c r="E62" s="50"/>
       <c r="F62" s="50"/>
-      <c r="G62" s="170"/>
-      <c r="H62" s="170"/>
-      <c r="I62" s="170"/>
+      <c r="G62" s="171"/>
+      <c r="H62" s="171"/>
+      <c r="I62" s="171"/>
       <c r="J62" s="50"/>
       <c r="K62" s="86"/>
       <c r="L62" s="11"/>
@@ -30110,12 +30308,12 @@
       <c r="A63" s="50"/>
       <c r="B63" s="50"/>
       <c r="C63" s="50"/>
-      <c r="D63" s="169"/>
+      <c r="D63" s="170"/>
       <c r="E63" s="50"/>
       <c r="F63" s="50"/>
-      <c r="G63" s="170"/>
-      <c r="H63" s="170"/>
-      <c r="I63" s="170"/>
+      <c r="G63" s="171"/>
+      <c r="H63" s="171"/>
+      <c r="I63" s="171"/>
       <c r="J63" s="50"/>
       <c r="K63" s="86"/>
       <c r="L63" s="11"/>
@@ -30139,12 +30337,12 @@
       <c r="A64" s="50"/>
       <c r="B64" s="50"/>
       <c r="C64" s="50"/>
-      <c r="D64" s="169"/>
+      <c r="D64" s="170"/>
       <c r="E64" s="50"/>
       <c r="F64" s="50"/>
-      <c r="G64" s="170"/>
-      <c r="H64" s="170"/>
-      <c r="I64" s="170"/>
+      <c r="G64" s="171"/>
+      <c r="H64" s="171"/>
+      <c r="I64" s="171"/>
       <c r="J64" s="50"/>
       <c r="K64" s="86"/>
       <c r="L64" s="11"/>
@@ -30168,12 +30366,12 @@
       <c r="A65" s="50"/>
       <c r="B65" s="50"/>
       <c r="C65" s="50"/>
-      <c r="D65" s="169"/>
+      <c r="D65" s="170"/>
       <c r="E65" s="50"/>
       <c r="F65" s="50"/>
-      <c r="G65" s="170"/>
-      <c r="H65" s="170"/>
-      <c r="I65" s="170"/>
+      <c r="G65" s="171"/>
+      <c r="H65" s="171"/>
+      <c r="I65" s="171"/>
       <c r="J65" s="50"/>
       <c r="K65" s="86"/>
       <c r="L65" s="11"/>
@@ -30197,12 +30395,12 @@
       <c r="A66" s="50"/>
       <c r="B66" s="50"/>
       <c r="C66" s="50"/>
-      <c r="D66" s="169"/>
+      <c r="D66" s="170"/>
       <c r="E66" s="50"/>
       <c r="F66" s="50"/>
-      <c r="G66" s="170"/>
-      <c r="H66" s="170"/>
-      <c r="I66" s="170"/>
+      <c r="G66" s="171"/>
+      <c r="H66" s="171"/>
+      <c r="I66" s="171"/>
       <c r="J66" s="50"/>
       <c r="K66" s="86"/>
       <c r="L66" s="11"/>
@@ -30226,12 +30424,12 @@
       <c r="A67" s="50"/>
       <c r="B67" s="50"/>
       <c r="C67" s="50"/>
-      <c r="D67" s="169"/>
+      <c r="D67" s="170"/>
       <c r="E67" s="50"/>
       <c r="F67" s="50"/>
-      <c r="G67" s="170"/>
-      <c r="H67" s="170"/>
-      <c r="I67" s="170"/>
+      <c r="G67" s="171"/>
+      <c r="H67" s="171"/>
+      <c r="I67" s="171"/>
       <c r="J67" s="50"/>
       <c r="K67" s="86"/>
       <c r="L67" s="11"/>
@@ -30255,12 +30453,12 @@
       <c r="A68" s="50"/>
       <c r="B68" s="50"/>
       <c r="C68" s="50"/>
-      <c r="D68" s="169"/>
+      <c r="D68" s="170"/>
       <c r="E68" s="50"/>
       <c r="F68" s="50"/>
-      <c r="G68" s="170"/>
-      <c r="H68" s="170"/>
-      <c r="I68" s="170"/>
+      <c r="G68" s="171"/>
+      <c r="H68" s="171"/>
+      <c r="I68" s="171"/>
       <c r="J68" s="50"/>
       <c r="K68" s="86"/>
       <c r="L68" s="11"/>
@@ -30284,12 +30482,12 @@
       <c r="A69" s="50"/>
       <c r="B69" s="50"/>
       <c r="C69" s="50"/>
-      <c r="D69" s="169"/>
+      <c r="D69" s="170"/>
       <c r="E69" s="50"/>
       <c r="F69" s="50"/>
-      <c r="G69" s="170"/>
-      <c r="H69" s="170"/>
-      <c r="I69" s="170"/>
+      <c r="G69" s="171"/>
+      <c r="H69" s="171"/>
+      <c r="I69" s="171"/>
       <c r="J69" s="50"/>
       <c r="K69" s="86"/>
       <c r="L69" s="11"/>
@@ -30313,12 +30511,12 @@
       <c r="A70" s="50"/>
       <c r="B70" s="50"/>
       <c r="C70" s="50"/>
-      <c r="D70" s="169"/>
+      <c r="D70" s="170"/>
       <c r="E70" s="50"/>
       <c r="F70" s="50"/>
-      <c r="G70" s="170"/>
-      <c r="H70" s="170"/>
-      <c r="I70" s="170"/>
+      <c r="G70" s="171"/>
+      <c r="H70" s="171"/>
+      <c r="I70" s="171"/>
       <c r="J70" s="50"/>
       <c r="K70" s="86"/>
       <c r="L70" s="11"/>
@@ -30342,12 +30540,12 @@
       <c r="A71" s="50"/>
       <c r="B71" s="50"/>
       <c r="C71" s="50"/>
-      <c r="D71" s="169"/>
+      <c r="D71" s="170"/>
       <c r="E71" s="50"/>
       <c r="F71" s="50"/>
-      <c r="G71" s="170"/>
-      <c r="H71" s="170"/>
-      <c r="I71" s="170"/>
+      <c r="G71" s="171"/>
+      <c r="H71" s="171"/>
+      <c r="I71" s="171"/>
       <c r="J71" s="50"/>
       <c r="K71" s="86"/>
       <c r="L71" s="11"/>
@@ -30371,12 +30569,12 @@
       <c r="A72" s="50"/>
       <c r="B72" s="50"/>
       <c r="C72" s="50"/>
-      <c r="D72" s="169"/>
+      <c r="D72" s="170"/>
       <c r="E72" s="50"/>
       <c r="F72" s="50"/>
-      <c r="G72" s="170"/>
-      <c r="H72" s="170"/>
-      <c r="I72" s="170"/>
+      <c r="G72" s="171"/>
+      <c r="H72" s="171"/>
+      <c r="I72" s="171"/>
       <c r="J72" s="50"/>
       <c r="K72" s="86"/>
       <c r="L72" s="11"/>
@@ -30400,12 +30598,12 @@
       <c r="A73" s="50"/>
       <c r="B73" s="50"/>
       <c r="C73" s="50"/>
-      <c r="D73" s="169"/>
+      <c r="D73" s="170"/>
       <c r="E73" s="50"/>
       <c r="F73" s="50"/>
-      <c r="G73" s="170"/>
-      <c r="H73" s="170"/>
-      <c r="I73" s="170"/>
+      <c r="G73" s="171"/>
+      <c r="H73" s="171"/>
+      <c r="I73" s="171"/>
       <c r="J73" s="50"/>
       <c r="K73" s="86"/>
       <c r="L73" s="11"/>
@@ -30429,12 +30627,12 @@
       <c r="A74" s="50"/>
       <c r="B74" s="50"/>
       <c r="C74" s="50"/>
-      <c r="D74" s="169"/>
+      <c r="D74" s="170"/>
       <c r="E74" s="50"/>
       <c r="F74" s="50"/>
-      <c r="G74" s="170"/>
-      <c r="H74" s="170"/>
-      <c r="I74" s="170"/>
+      <c r="G74" s="171"/>
+      <c r="H74" s="171"/>
+      <c r="I74" s="171"/>
       <c r="J74" s="50"/>
       <c r="K74" s="86"/>
       <c r="L74" s="11"/>
@@ -30458,12 +30656,12 @@
       <c r="A75" s="50"/>
       <c r="B75" s="50"/>
       <c r="C75" s="50"/>
-      <c r="D75" s="169"/>
+      <c r="D75" s="170"/>
       <c r="E75" s="50"/>
       <c r="F75" s="50"/>
-      <c r="G75" s="170"/>
-      <c r="H75" s="170"/>
-      <c r="I75" s="170"/>
+      <c r="G75" s="171"/>
+      <c r="H75" s="171"/>
+      <c r="I75" s="171"/>
       <c r="J75" s="50"/>
       <c r="K75" s="86"/>
       <c r="L75" s="11"/>
@@ -30487,12 +30685,12 @@
       <c r="A76" s="50"/>
       <c r="B76" s="50"/>
       <c r="C76" s="50"/>
-      <c r="D76" s="169"/>
+      <c r="D76" s="170"/>
       <c r="E76" s="50"/>
       <c r="F76" s="50"/>
-      <c r="G76" s="170"/>
-      <c r="H76" s="170"/>
-      <c r="I76" s="170"/>
+      <c r="G76" s="171"/>
+      <c r="H76" s="171"/>
+      <c r="I76" s="171"/>
       <c r="J76" s="50"/>
       <c r="K76" s="86"/>
       <c r="L76" s="11"/>
@@ -30519,9 +30717,9 @@
       <c r="D77" s="50"/>
       <c r="E77" s="50"/>
       <c r="F77" s="50"/>
-      <c r="G77" s="170"/>
-      <c r="H77" s="170"/>
-      <c r="I77" s="170"/>
+      <c r="G77" s="171"/>
+      <c r="H77" s="171"/>
+      <c r="I77" s="171"/>
       <c r="J77" s="50"/>
       <c r="K77" s="86"/>
       <c r="L77" s="11"/>
@@ -30548,9 +30746,9 @@
       <c r="D78" s="50"/>
       <c r="E78" s="50"/>
       <c r="F78" s="50"/>
-      <c r="G78" s="170"/>
-      <c r="H78" s="170"/>
-      <c r="I78" s="170"/>
+      <c r="G78" s="171"/>
+      <c r="H78" s="171"/>
+      <c r="I78" s="171"/>
       <c r="J78" s="50"/>
       <c r="K78" s="86"/>
       <c r="L78" s="11"/>
@@ -30577,9 +30775,9 @@
       <c r="D79" s="50"/>
       <c r="E79" s="50"/>
       <c r="F79" s="50"/>
-      <c r="G79" s="170"/>
-      <c r="H79" s="170"/>
-      <c r="I79" s="170"/>
+      <c r="G79" s="171"/>
+      <c r="H79" s="171"/>
+      <c r="I79" s="171"/>
       <c r="J79" s="50"/>
       <c r="K79" s="86"/>
       <c r="L79" s="11"/>
@@ -30606,9 +30804,9 @@
       <c r="D80" s="50"/>
       <c r="E80" s="50"/>
       <c r="F80" s="50"/>
-      <c r="G80" s="170"/>
-      <c r="H80" s="170"/>
-      <c r="I80" s="170"/>
+      <c r="G80" s="171"/>
+      <c r="H80" s="171"/>
+      <c r="I80" s="171"/>
       <c r="J80" s="50"/>
       <c r="K80" s="86"/>
       <c r="L80" s="11"/>
@@ -30635,9 +30833,9 @@
       <c r="D81" s="50"/>
       <c r="E81" s="50"/>
       <c r="F81" s="50"/>
-      <c r="G81" s="170"/>
-      <c r="H81" s="170"/>
-      <c r="I81" s="170"/>
+      <c r="G81" s="171"/>
+      <c r="H81" s="171"/>
+      <c r="I81" s="171"/>
       <c r="J81" s="50"/>
       <c r="K81" s="86"/>
       <c r="L81" s="11"/>
@@ -30664,9 +30862,9 @@
       <c r="D82" s="50"/>
       <c r="E82" s="50"/>
       <c r="F82" s="50"/>
-      <c r="G82" s="170"/>
-      <c r="H82" s="170"/>
-      <c r="I82" s="170"/>
+      <c r="G82" s="171"/>
+      <c r="H82" s="171"/>
+      <c r="I82" s="171"/>
       <c r="J82" s="50"/>
       <c r="K82" s="86"/>
       <c r="L82" s="11"/>
@@ -30693,9 +30891,9 @@
       <c r="D83" s="50"/>
       <c r="E83" s="50"/>
       <c r="F83" s="50"/>
-      <c r="G83" s="170"/>
-      <c r="H83" s="170"/>
-      <c r="I83" s="170"/>
+      <c r="G83" s="171"/>
+      <c r="H83" s="171"/>
+      <c r="I83" s="171"/>
       <c r="J83" s="50"/>
       <c r="K83" s="86"/>
       <c r="L83" s="11"/>
@@ -30722,9 +30920,9 @@
       <c r="D84" s="50"/>
       <c r="E84" s="50"/>
       <c r="F84" s="50"/>
-      <c r="G84" s="170"/>
-      <c r="H84" s="170"/>
-      <c r="I84" s="170"/>
+      <c r="G84" s="171"/>
+      <c r="H84" s="171"/>
+      <c r="I84" s="171"/>
       <c r="J84" s="50"/>
       <c r="K84" s="86"/>
       <c r="L84" s="11"/>
@@ -30751,9 +30949,9 @@
       <c r="D85" s="50"/>
       <c r="E85" s="50"/>
       <c r="F85" s="50"/>
-      <c r="G85" s="170"/>
-      <c r="H85" s="170"/>
-      <c r="I85" s="170"/>
+      <c r="G85" s="171"/>
+      <c r="H85" s="171"/>
+      <c r="I85" s="171"/>
       <c r="J85" s="50"/>
       <c r="K85" s="86"/>
       <c r="L85" s="11"/>
@@ -30780,9 +30978,9 @@
       <c r="D86" s="50"/>
       <c r="E86" s="50"/>
       <c r="F86" s="50"/>
-      <c r="G86" s="170"/>
-      <c r="H86" s="170"/>
-      <c r="I86" s="170"/>
+      <c r="G86" s="171"/>
+      <c r="H86" s="171"/>
+      <c r="I86" s="171"/>
       <c r="J86" s="50"/>
       <c r="K86" s="86"/>
       <c r="L86" s="11"/>
@@ -30809,7 +31007,7 @@
       <c r="D87" s="50"/>
       <c r="E87" s="50"/>
       <c r="F87" s="50"/>
-      <c r="G87" s="170"/>
+      <c r="G87" s="171"/>
       <c r="H87" s="103"/>
       <c r="I87" s="103"/>
       <c r="J87" s="50"/>
@@ -30838,7 +31036,7 @@
       <c r="D88" s="50"/>
       <c r="E88" s="50"/>
       <c r="F88" s="50"/>
-      <c r="G88" s="170"/>
+      <c r="G88" s="171"/>
       <c r="H88" s="103"/>
       <c r="I88" s="103"/>
       <c r="J88" s="50"/>
@@ -30867,7 +31065,7 @@
       <c r="D89" s="50"/>
       <c r="E89" s="50"/>
       <c r="F89" s="50"/>
-      <c r="G89" s="170"/>
+      <c r="G89" s="171"/>
       <c r="H89" s="103"/>
       <c r="I89" s="103"/>
       <c r="J89" s="50"/>
@@ -30896,7 +31094,7 @@
       <c r="D90" s="50"/>
       <c r="E90" s="50"/>
       <c r="F90" s="50"/>
-      <c r="G90" s="170"/>
+      <c r="G90" s="171"/>
       <c r="H90" s="103"/>
       <c r="I90" s="103"/>
       <c r="J90" s="50"/>
@@ -30925,7 +31123,7 @@
       <c r="D91" s="50"/>
       <c r="E91" s="50"/>
       <c r="F91" s="50"/>
-      <c r="G91" s="170"/>
+      <c r="G91" s="171"/>
       <c r="H91" s="103"/>
       <c r="I91" s="103"/>
       <c r="J91" s="50"/>
@@ -30954,7 +31152,7 @@
       <c r="D92" s="50"/>
       <c r="E92" s="50"/>
       <c r="F92" s="50"/>
-      <c r="G92" s="170"/>
+      <c r="G92" s="171"/>
       <c r="H92" s="103"/>
       <c r="I92" s="103"/>
       <c r="J92" s="50"/>
@@ -30983,7 +31181,7 @@
       <c r="D93" s="50"/>
       <c r="E93" s="50"/>
       <c r="F93" s="50"/>
-      <c r="G93" s="170"/>
+      <c r="G93" s="171"/>
       <c r="H93" s="103"/>
       <c r="I93" s="103"/>
       <c r="J93" s="50"/>
@@ -31012,7 +31210,7 @@
       <c r="D94" s="50"/>
       <c r="E94" s="50"/>
       <c r="F94" s="50"/>
-      <c r="G94" s="170"/>
+      <c r="G94" s="171"/>
       <c r="H94" s="103"/>
       <c r="I94" s="103"/>
       <c r="J94" s="50"/>
@@ -31041,7 +31239,7 @@
       <c r="D95" s="50"/>
       <c r="E95" s="50"/>
       <c r="F95" s="50"/>
-      <c r="G95" s="170"/>
+      <c r="G95" s="171"/>
       <c r="H95" s="103"/>
       <c r="I95" s="103"/>
       <c r="J95" s="50"/>
@@ -31070,7 +31268,7 @@
       <c r="D96" s="50"/>
       <c r="E96" s="50"/>
       <c r="F96" s="50"/>
-      <c r="G96" s="170"/>
+      <c r="G96" s="171"/>
       <c r="H96" s="103"/>
       <c r="I96" s="103"/>
       <c r="J96" s="50"/>
@@ -31099,7 +31297,7 @@
       <c r="D97" s="50"/>
       <c r="E97" s="50"/>
       <c r="F97" s="50"/>
-      <c r="G97" s="170"/>
+      <c r="G97" s="171"/>
       <c r="H97" s="103"/>
       <c r="I97" s="103"/>
       <c r="J97" s="50"/>
@@ -31128,7 +31326,7 @@
       <c r="D98" s="50"/>
       <c r="E98" s="50"/>
       <c r="F98" s="50"/>
-      <c r="G98" s="170"/>
+      <c r="G98" s="171"/>
       <c r="H98" s="103"/>
       <c r="I98" s="103"/>
       <c r="J98" s="50"/>
@@ -31157,7 +31355,7 @@
       <c r="D99" s="50"/>
       <c r="E99" s="50"/>
       <c r="F99" s="50"/>
-      <c r="G99" s="170"/>
+      <c r="G99" s="171"/>
       <c r="H99" s="103"/>
       <c r="I99" s="103"/>
       <c r="J99" s="50"/>
@@ -31186,7 +31384,7 @@
       <c r="D100" s="50"/>
       <c r="E100" s="50"/>
       <c r="F100" s="50"/>
-      <c r="G100" s="171"/>
+      <c r="G100" s="172"/>
       <c r="H100" s="50"/>
       <c r="I100" s="50"/>
       <c r="J100" s="50"/>
@@ -31215,7 +31413,7 @@
       <c r="D101" s="50"/>
       <c r="E101" s="50"/>
       <c r="F101" s="50"/>
-      <c r="G101" s="171"/>
+      <c r="G101" s="172"/>
       <c r="H101" s="50"/>
       <c r="I101" s="50"/>
       <c r="J101" s="50"/>
@@ -31244,7 +31442,7 @@
       <c r="D102" s="50"/>
       <c r="E102" s="50"/>
       <c r="F102" s="50"/>
-      <c r="G102" s="171"/>
+      <c r="G102" s="172"/>
       <c r="H102" s="50"/>
       <c r="I102" s="50"/>
       <c r="J102" s="50"/>
@@ -31273,7 +31471,7 @@
       <c r="D103" s="50"/>
       <c r="E103" s="50"/>
       <c r="F103" s="50"/>
-      <c r="G103" s="171"/>
+      <c r="G103" s="172"/>
       <c r="H103" s="50"/>
       <c r="I103" s="50"/>
       <c r="J103" s="50"/>
@@ -31302,7 +31500,7 @@
       <c r="D104" s="50"/>
       <c r="E104" s="50"/>
       <c r="F104" s="50"/>
-      <c r="G104" s="171"/>
+      <c r="G104" s="172"/>
       <c r="H104" s="50"/>
       <c r="I104" s="50"/>
       <c r="J104" s="50"/>
@@ -31331,7 +31529,7 @@
       <c r="D105" s="50"/>
       <c r="E105" s="50"/>
       <c r="F105" s="50"/>
-      <c r="G105" s="171"/>
+      <c r="G105" s="172"/>
       <c r="H105" s="50"/>
       <c r="I105" s="50"/>
       <c r="J105" s="50"/>
@@ -31360,7 +31558,7 @@
       <c r="D106" s="50"/>
       <c r="E106" s="50"/>
       <c r="F106" s="50"/>
-      <c r="G106" s="171"/>
+      <c r="G106" s="172"/>
       <c r="H106" s="50"/>
       <c r="I106" s="50"/>
       <c r="J106" s="50"/>
@@ -31389,7 +31587,7 @@
       <c r="D107" s="50"/>
       <c r="E107" s="50"/>
       <c r="F107" s="50"/>
-      <c r="G107" s="171"/>
+      <c r="G107" s="172"/>
       <c r="H107" s="50"/>
       <c r="I107" s="50"/>
       <c r="J107" s="50"/>
@@ -31418,7 +31616,7 @@
       <c r="D108" s="50"/>
       <c r="E108" s="50"/>
       <c r="F108" s="50"/>
-      <c r="G108" s="171"/>
+      <c r="G108" s="172"/>
       <c r="H108" s="50"/>
       <c r="I108" s="50"/>
       <c r="J108" s="50"/>
@@ -33705,15 +33903,15 @@
   <sheetData>
     <row r="1" ht="25.5" customHeight="1">
       <c r="A1" s="11"/>
-      <c r="B1" s="172" t="s">
-        <v>457</v>
-      </c>
-      <c r="C1" s="173"/>
-      <c r="D1" s="173"/>
-      <c r="E1" s="173"/>
-      <c r="F1" s="173"/>
-      <c r="G1" s="173"/>
-      <c r="H1" s="173"/>
+      <c r="B1" s="173" t="s">
+        <v>449</v>
+      </c>
+      <c r="C1" s="174"/>
+      <c r="D1" s="174"/>
+      <c r="E1" s="174"/>
+      <c r="F1" s="174"/>
+      <c r="G1" s="174"/>
+      <c r="H1" s="174"/>
       <c r="I1" s="11"/>
       <c r="J1" s="11"/>
       <c r="K1" s="11"/>
@@ -33734,14 +33932,14 @@
       <c r="Z1" s="11"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="174"/>
-      <c r="B2" s="174"/>
+      <c r="A2" s="175"/>
+      <c r="B2" s="175"/>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
       <c r="F2" s="11"/>
       <c r="G2" s="11"/>
-      <c r="H2" s="175"/>
+      <c r="H2" s="176"/>
       <c r="I2" s="11"/>
       <c r="J2" s="11"/>
       <c r="K2" s="11"/>
@@ -33763,19 +33961,19 @@
     </row>
     <row r="3" ht="12.0" customHeight="1">
       <c r="A3" s="11"/>
-      <c r="B3" s="176" t="s">
+      <c r="B3" s="177" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="49" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="6"/>
-      <c r="E3" s="177" t="s">
+      <c r="E3" s="178" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="6"/>
-      <c r="G3" s="178"/>
-      <c r="H3" s="179" t="s">
+      <c r="G3" s="179"/>
+      <c r="H3" s="180" t="s">
         <v>4</v>
       </c>
       <c r="I3" s="11"/>
@@ -33799,19 +33997,19 @@
     </row>
     <row r="4" ht="12.0" customHeight="1">
       <c r="A4" s="11"/>
-      <c r="B4" s="176" t="s">
+      <c r="B4" s="177" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="49" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="6"/>
-      <c r="E4" s="177" t="s">
+      <c r="E4" s="178" t="s">
         <v>6</v>
       </c>
       <c r="F4" s="6"/>
-      <c r="G4" s="178"/>
-      <c r="H4" s="179" t="s">
+      <c r="G4" s="179"/>
+      <c r="H4" s="180" t="s">
         <v>7</v>
       </c>
       <c r="I4" s="11"/>
@@ -33835,7 +34033,7 @@
     </row>
     <row r="5" ht="12.0" customHeight="1">
       <c r="A5" s="11"/>
-      <c r="B5" s="180" t="s">
+      <c r="B5" s="181" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="49" t="str">
@@ -33843,12 +34041,12 @@
         <v>SoFa_Test Report_vx.x</v>
       </c>
       <c r="D5" s="6"/>
-      <c r="E5" s="177" t="s">
+      <c r="E5" s="178" t="s">
         <v>9</v>
       </c>
       <c r="F5" s="6"/>
-      <c r="G5" s="178"/>
-      <c r="H5" s="181">
+      <c r="G5" s="179"/>
+      <c r="H5" s="182">
         <v>44534.0</v>
       </c>
       <c r="I5" s="11"/>
@@ -33871,12 +34069,12 @@
       <c r="Z5" s="11"/>
     </row>
     <row r="6" ht="21.75" customHeight="1">
-      <c r="A6" s="174"/>
-      <c r="B6" s="180" t="s">
-        <v>458</v>
-      </c>
-      <c r="C6" s="182" t="s">
-        <v>459</v>
+      <c r="A6" s="175"/>
+      <c r="B6" s="181" t="s">
+        <v>450</v>
+      </c>
+      <c r="C6" s="183" t="s">
+        <v>451</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -33903,14 +34101,14 @@
       <c r="Z6" s="11"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="174"/>
+      <c r="A7" s="175"/>
       <c r="B7" s="25"/>
-      <c r="C7" s="183"/>
+      <c r="C7" s="184"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
-      <c r="H7" s="175"/>
+      <c r="H7" s="176"/>
       <c r="I7" s="11"/>
       <c r="J7" s="11"/>
       <c r="K7" s="11"/>
@@ -33933,12 +34131,12 @@
     <row r="8" ht="12.75" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="25"/>
-      <c r="C8" s="183"/>
+      <c r="C8" s="184"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
-      <c r="H8" s="175"/>
+      <c r="H8" s="176"/>
       <c r="I8" s="11"/>
       <c r="J8" s="11"/>
       <c r="K8" s="11"/>
@@ -33987,27 +34185,27 @@
       <c r="Z9" s="11"/>
     </row>
     <row r="10" ht="12.75" customHeight="1">
-      <c r="A10" s="184"/>
-      <c r="B10" s="185" t="s">
+      <c r="A10" s="185"/>
+      <c r="B10" s="186" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="186" t="s">
-        <v>460</v>
-      </c>
-      <c r="D10" s="187" t="s">
+      <c r="C10" s="187" t="s">
+        <v>452</v>
+      </c>
+      <c r="D10" s="188" t="s">
         <v>83</v>
       </c>
-      <c r="E10" s="186" t="s">
+      <c r="E10" s="187" t="s">
         <v>86</v>
       </c>
-      <c r="F10" s="186" t="s">
+      <c r="F10" s="187" t="s">
         <v>89</v>
       </c>
-      <c r="G10" s="188" t="s">
+      <c r="G10" s="189" t="s">
         <v>90</v>
       </c>
-      <c r="H10" s="189" t="s">
-        <v>461</v>
+      <c r="H10" s="190" t="s">
+        <v>453</v>
       </c>
       <c r="I10" s="11"/>
       <c r="J10" s="11"/>
@@ -34029,31 +34227,31 @@
       <c r="Z10" s="11"/>
     </row>
     <row r="11" ht="12.75" customHeight="1">
-      <c r="A11" s="184"/>
-      <c r="B11" s="190">
+      <c r="A11" s="185"/>
+      <c r="B11" s="191">
         <v>1.0</v>
       </c>
-      <c r="C11" s="191" t="str">
+      <c r="C11" s="192" t="str">
         <f>Guest!B2</f>
         <v>Guest</v>
       </c>
-      <c r="D11" s="192">
+      <c r="D11" s="193">
         <f>Guest!A6</f>
         <v>43</v>
       </c>
-      <c r="E11" s="192">
+      <c r="E11" s="193">
         <f>Guest!B6</f>
         <v>4</v>
       </c>
-      <c r="F11" s="192">
+      <c r="F11" s="193">
         <f>Guest!C6</f>
         <v>3</v>
       </c>
-      <c r="G11" s="193">
+      <c r="G11" s="194">
         <f>Guest!D6</f>
         <v>0</v>
       </c>
-      <c r="H11" s="194">
+      <c r="H11" s="195">
         <f>Guest!E6</f>
         <v>50</v>
       </c>
@@ -34077,31 +34275,31 @@
       <c r="Z11" s="11"/>
     </row>
     <row r="12" ht="12.75" customHeight="1">
-      <c r="A12" s="184"/>
-      <c r="B12" s="190">
+      <c r="A12" s="185"/>
+      <c r="B12" s="191">
         <v>2.0</v>
       </c>
-      <c r="C12" s="191" t="str">
+      <c r="C12" s="192" t="str">
         <f>User!B2</f>
         <v>User</v>
       </c>
-      <c r="D12" s="192">
+      <c r="D12" s="193">
         <f>User!A6</f>
         <v>0</v>
       </c>
-      <c r="E12" s="192">
+      <c r="E12" s="193">
         <f>User!B6</f>
         <v>0</v>
       </c>
-      <c r="F12" s="192">
+      <c r="F12" s="193">
         <f>User!C6</f>
         <v>51</v>
       </c>
-      <c r="G12" s="192">
+      <c r="G12" s="193">
         <f>User!D6</f>
         <v>0</v>
       </c>
-      <c r="H12" s="192">
+      <c r="H12" s="193">
         <f>User!E6</f>
         <v>51</v>
       </c>
@@ -34125,31 +34323,31 @@
       <c r="Z12" s="11"/>
     </row>
     <row r="13" ht="12.75" customHeight="1">
-      <c r="A13" s="184"/>
-      <c r="B13" s="190">
+      <c r="A13" s="185"/>
+      <c r="B13" s="191">
         <v>1.0</v>
       </c>
-      <c r="C13" s="191" t="str">
+      <c r="C13" s="192" t="str">
         <f>Manager!B2</f>
         <v>Manager</v>
       </c>
-      <c r="D13" s="192">
+      <c r="D13" s="193">
         <f>Manager!A6</f>
         <v>0</v>
       </c>
-      <c r="E13" s="192">
+      <c r="E13" s="193">
         <f>Manager!B6</f>
         <v>0</v>
       </c>
-      <c r="F13" s="192">
+      <c r="F13" s="193">
         <f>Manager!C6</f>
         <v>0</v>
       </c>
-      <c r="G13" s="193">
+      <c r="G13" s="194">
         <f>Manager!D6</f>
         <v>0</v>
       </c>
-      <c r="H13" s="194">
+      <c r="H13" s="195">
         <f>Manager!E6</f>
         <v>0</v>
       </c>
@@ -34173,28 +34371,28 @@
       <c r="Z13" s="11"/>
     </row>
     <row r="14" ht="12.75" customHeight="1">
-      <c r="A14" s="184"/>
-      <c r="B14" s="195"/>
-      <c r="C14" s="196" t="s">
-        <v>462</v>
-      </c>
-      <c r="D14" s="197">
+      <c r="A14" s="185"/>
+      <c r="B14" s="196"/>
+      <c r="C14" s="197" t="s">
+        <v>454</v>
+      </c>
+      <c r="D14" s="198">
         <f t="shared" ref="D14:H14" si="1">SUM(D9:D13)</f>
         <v>43</v>
       </c>
-      <c r="E14" s="197">
+      <c r="E14" s="198">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="F14" s="197">
+      <c r="F14" s="198">
         <f t="shared" si="1"/>
         <v>54</v>
       </c>
-      <c r="G14" s="197">
+      <c r="G14" s="198">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H14" s="198">
+      <c r="H14" s="199">
         <f t="shared" si="1"/>
         <v>101</v>
       </c>
@@ -34219,13 +34417,13 @@
     </row>
     <row r="15" ht="12.75" customHeight="1">
       <c r="A15" s="11"/>
-      <c r="B15" s="199"/>
+      <c r="B15" s="200"/>
       <c r="C15" s="11"/>
-      <c r="D15" s="200"/>
-      <c r="E15" s="201"/>
-      <c r="F15" s="201"/>
-      <c r="G15" s="201"/>
-      <c r="H15" s="201"/>
+      <c r="D15" s="201"/>
+      <c r="E15" s="202"/>
+      <c r="F15" s="202"/>
+      <c r="G15" s="202"/>
+      <c r="H15" s="202"/>
       <c r="I15" s="11"/>
       <c r="J15" s="11"/>
       <c r="K15" s="11"/>
@@ -34249,15 +34447,15 @@
       <c r="A16" s="11"/>
       <c r="B16" s="11"/>
       <c r="C16" s="9" t="s">
-        <v>463</v>
+        <v>455</v>
       </c>
       <c r="D16" s="11"/>
-      <c r="E16" s="202">
+      <c r="E16" s="203">
         <f>(D14+E14)*100/(H14-G14)</f>
         <v>46.53465347</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>464</v>
+        <v>456</v>
       </c>
       <c r="G16" s="11"/>
       <c r="H16" s="132"/>
@@ -34284,15 +34482,15 @@
       <c r="A17" s="11"/>
       <c r="B17" s="11"/>
       <c r="C17" s="9" t="s">
-        <v>465</v>
+        <v>457</v>
       </c>
       <c r="D17" s="11"/>
-      <c r="E17" s="202">
+      <c r="E17" s="203">
         <f>D14*100/(H14-G14)</f>
         <v>42.57425743</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>464</v>
+        <v>456</v>
       </c>
       <c r="G17" s="11"/>
       <c r="H17" s="132"/>

</xml_diff>

<commit_message>
HoangNH - Update test case 39 -> 60
</commit_message>
<xml_diff>
--- a/3. Users/HoangNHHE130395/Testing/TestCase - Hoang.xlsx
+++ b/3. Users/HoangNHHE130395/Testing/TestCase - Hoang.xlsx
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="513">
   <si>
     <t>SYSTEM TEST CASE</t>
   </si>
@@ -1883,6 +1883,9 @@
     <t xml:space="preserve">1. Display list users with following column: "ID, Username, Email, Fullname, Phone, Date created, Avatar, Status, Option" </t>
   </si>
   <si>
+    <t>Bug-27</t>
+  </si>
+  <si>
     <t>Check data in column of list users</t>
   </si>
   <si>
@@ -1952,7 +1955,7 @@
 5. Click option 'Hủy' on the popup</t>
   </si>
   <si>
-    <t>1. Popup is disappear and user status is 'Active'</t>
+    <t>1. Popup is disappeared and user status is 'Active'</t>
   </si>
   <si>
     <t>1. Login into the web server
@@ -1965,6 +1968,260 @@
     <t>1. Toast notification 'Ban nguời dùng thành công' 
 2. Status of user change to 'Inactive'
 3. Button 'Ban' change to 'Unban'</t>
+  </si>
+  <si>
+    <t>Check function button 'Unban'</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'User' tab in the menu bar
+3. Click on the 'edit' in column 'Option' of user have id = '7'
+4. Choose user is 'Ban' , click Button 'Unban'
+5. Click option 'Hủy' on the popup</t>
+  </si>
+  <si>
+    <t>1. Popup is disappeared and user status is 'Inactive'</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'User' tab in the menu bar
+3. Click on the 'edit' in column 'Option' of user have id = '7'
+4. Choose user is 'Ban' , click Button 'Unban'
+5. Click option 'Ok' on the popup</t>
+  </si>
+  <si>
+    <t>1. Toast notification 'Unban nguời dùng thành công' 
+2. Status of user change to 'Active'
+3. Button 'Ban' change to 'Ban'</t>
+  </si>
+  <si>
+    <t>Check function button 'Reset password'</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'User' tab in the menu bar
+3. Click on the 'edit' in column 'Option' of user have id = '7'
+4. Click Button 'Reset password'
+5. Click option 'Hủy' on the popup</t>
+  </si>
+  <si>
+    <t>1. Popup is disappeared</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'User' tab in the menu bar
+3. Click on the 'edit' in column 'Option' of user have id = '7'
+4. Click Button 'Reset password'
+5. Click option 'Ok' on the popup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Popup is disappered
+2. Toast notification 'Reset password thành công' 
+</t>
+  </si>
+  <si>
+    <t>Check function button 'Add balance'</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'User' tab in the menu bar
+3. Click on the 'edit' in column 'Option' of user have id = '7'
+4. Click Button 'Add balance'
+5. Click option 'Hủy' on the popup</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'User' tab in the menu bar
+3. Click on the 'edit' in column 'Option' of user have id = '7'
+4. Click Button 'Add balance'
+5. Input text 'a' into the text field
+6. Click option 'Ok' on the popup</t>
+  </si>
+  <si>
+    <t>1. Text field is not changed because cannot input string</t>
+  </si>
+  <si>
+    <t>1. User have id = '7'
+2. Text 'a'</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'User' tab in the menu bar
+3. Click on the 'edit' in column 'Option' of user have id = '7'
+4. Click Button 'Add balance'
+5. Input text '/' into the text field
+6. Click option 'Ok' on the popup</t>
+  </si>
+  <si>
+    <t>1. Text field is not changed because cannot input special character</t>
+  </si>
+  <si>
+    <t>1. User have id = '7'
+2. Character '/'</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'User' tab in the menu bar
+3. Click on the 'edit' in column 'Option' of user have id = '7'
+4. Click Button 'Add balance'
+5. Input text '121.--' into the text field
+6. Click option 'Ok' on the popup</t>
+  </si>
+  <si>
+    <t>1. Popup is disappeared and user balance is not changed</t>
+  </si>
+  <si>
+    <t>1. User have id = '7'
+2. Text '121.--'</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'User' tab in the menu bar
+3. Click on the 'edit' in column 'Option' of user have id = '7'
+4. Click Button 'Add balance'
+5. Input text '-1.0000-1110' into the text field
+6. Click option 'Ok' on the popup</t>
+  </si>
+  <si>
+    <t>1. User have id = '7'
+2. Text '-1.0000-1110'</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'User' tab in the menu bar
+3. Click on the 'edit' in column 'Option' of user have id = '7'
+4. Click Button 'Add balance'
+5. Input text '123' into the text field
+6. Click option 'Ok' on the popup</t>
+  </si>
+  <si>
+    <t>1. Popup is disappeared and user balance is increase 123 VND</t>
+  </si>
+  <si>
+    <t>1. User have id = '7'
+2. Text '123'</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'User' tab in the menu bar
+3. Click on the 'edit' in column 'Option' of user have id = '7'
+4. Click Button 'Add balance'
+5. Input text '123' into the text field
+6. Click on 'Increase' arrow
+6. Click option 'Ok' on the popup</t>
+  </si>
+  <si>
+    <t>1. Popup is disappeared and user balance is increase 124 VND</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'User' tab in the menu bar
+3. Click on the 'edit' in column 'Option' of user have id = '7'
+4. Click Button 'Add balance'
+5. Input text '123' into the text field
+6. Click on 'Decrease' arrow
+6. Click option 'Ok' on the popup</t>
+  </si>
+  <si>
+    <t>1. Popup is disappeared and user balance is increase 122 VND</t>
+  </si>
+  <si>
+    <t>Check GUI part 'Thông tin số dư'</t>
+  </si>
+  <si>
+    <t>1. Display user balance of user have id = '7' and history transaction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. User have id = '7'
+</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'User' tab in the menu bar
+3. Click on the 'edit' in column 'Option' of user have id = '7'</t>
+  </si>
+  <si>
+    <t>1. Display User's history transaction by following: ID, Amount, Type, Description, Date created</t>
+  </si>
+  <si>
+    <t>Check GUI part 'Bài đăng'</t>
+  </si>
+  <si>
+    <t>1. Display all posts of user have id = '7'</t>
+  </si>
+  <si>
+    <t>1. Display User's posts by following: ID, Content, Posted By,Date created, Status. Option</t>
+  </si>
+  <si>
+    <t>Check GUI of button 'View detail'</t>
+  </si>
+  <si>
+    <t>1. Display button 'View detail'  in column Option</t>
+  </si>
+  <si>
+    <t>Bug-30</t>
+  </si>
+  <si>
+    <t>Check function of button 'View detail'</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'User' tab in the menu bar
+3. Click on the 'edit' in column 'Option' of user have id = '7'
+4. Click on the button 'View detail' in post have id='87'</t>
+  </si>
+  <si>
+    <t>1. Navigate to page post detail of post have id = '87'</t>
+  </si>
+  <si>
+    <t>1. User have id = '7'
+2. Post have id = '87'</t>
+  </si>
+  <si>
+    <t>Check paging history transaction</t>
+  </si>
+  <si>
+    <t>1. List of transaction in page 1 is displayed
+2. Item '&lt;&lt; Previous'  is disabled
+3. Item 'Next &gt;&gt;' is enabled</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'User' tab in the menu bar
+3. Click on the 'edit' in column 'Option' of user have id = '7'
+4. Click on '2' on the paging</t>
+  </si>
+  <si>
+    <t>1. List of transaction in page 2 is displayed
+2. Item '&lt;&lt; Previous'  is enabled
+3. Item 'Next &gt;&gt;' is disabled</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'User' tab in the menu bar
+3. Click on the 'edit' in column 'Option' of user have id = '7'
+4. Click on '2' on the paging
+5. Click on '1' on the paging</t>
+  </si>
+  <si>
+    <t>1. List of transaction in page 1 is displayed
+2. "Previous" item is disabled</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'User' tab in the menu bar
+3. Click on the 'edit' in column 'Option' of user have id = '7'
+4. Click on '2' on the paging
+5. Click on '&lt;&lt; Previous' on the paging</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'User' tab in the menu bar
+3. Click on the 'edit' in column 'Option' of user have id = '7'
+4. Click on 'Next &gt;&gt;' on the paging</t>
+  </si>
+  <si>
+    <t>1. List of transaction in page 2 is displayed</t>
   </si>
   <si>
     <t>TEST REPORT</t>
@@ -3253,6 +3510,9 @@
     <xf borderId="5" fillId="0" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
+    <xf borderId="5" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="5" fillId="0" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
@@ -3264,9 +3524,6 @@
     </xf>
     <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
@@ -28110,7 +28367,7 @@
     </row>
     <row r="10" ht="52.5" customHeight="1">
       <c r="A10" s="160" t="str">
-        <f t="shared" ref="A10:A50" si="1">IF(OR(B10&lt;&gt;"",D10&lt;&gt;""),"["&amp;TEXT($B$2,"##")&amp;"-"&amp;TEXT(ROW()-9,"##")&amp;"]","")</f>
+        <f t="shared" ref="A10:A65" si="1">IF(OR(B10&lt;&gt;"",D10&lt;&gt;""),"["&amp;TEXT($B$2,"##")&amp;"-"&amp;TEXT(ROW()-9,"##")&amp;"]","")</f>
         <v>[Manager-1]</v>
       </c>
       <c r="B10" s="160" t="s">
@@ -28133,7 +28390,7 @@
       <c r="I10" s="164" t="s">
         <v>375</v>
       </c>
-      <c r="J10" s="116"/>
+      <c r="J10" s="165"/>
       <c r="K10" s="11"/>
       <c r="L10" s="119"/>
       <c r="M10" s="11"/>
@@ -28167,7 +28424,7 @@
         <v>378</v>
       </c>
       <c r="E11" s="160" t="str">
-        <f t="shared" ref="E11:E42" si="2">$A$10</f>
+        <f t="shared" ref="E11:E65" si="2">$A$10</f>
         <v>[Manager-1]</v>
       </c>
       <c r="F11" s="117"/>
@@ -28180,7 +28437,7 @@
       <c r="I11" s="164" t="s">
         <v>375</v>
       </c>
-      <c r="J11" s="116"/>
+      <c r="J11" s="165"/>
       <c r="K11" s="11"/>
       <c r="L11" s="119"/>
       <c r="M11" s="11"/>
@@ -28227,7 +28484,7 @@
       <c r="I12" s="164" t="s">
         <v>375</v>
       </c>
-      <c r="J12" s="116"/>
+      <c r="J12" s="165"/>
       <c r="K12" s="11"/>
       <c r="L12" s="119"/>
       <c r="M12" s="11"/>
@@ -28271,10 +28528,10 @@
       <c r="H13" s="163">
         <v>44302.0</v>
       </c>
-      <c r="I13" s="165" t="s">
+      <c r="I13" s="166" t="s">
         <v>375</v>
       </c>
-      <c r="J13" s="116"/>
+      <c r="J13" s="165"/>
       <c r="K13" s="11"/>
       <c r="L13" s="119"/>
       <c r="M13" s="11"/>
@@ -28318,10 +28575,10 @@
       <c r="H14" s="163">
         <v>44302.0</v>
       </c>
-      <c r="I14" s="165" t="s">
+      <c r="I14" s="166" t="s">
         <v>375</v>
       </c>
-      <c r="J14" s="116"/>
+      <c r="J14" s="165"/>
       <c r="K14" s="11"/>
       <c r="L14" s="119"/>
       <c r="M14" s="11"/>
@@ -28365,10 +28622,10 @@
       <c r="H15" s="163">
         <v>44302.0</v>
       </c>
-      <c r="I15" s="165" t="s">
+      <c r="I15" s="166" t="s">
         <v>375</v>
       </c>
-      <c r="J15" s="116"/>
+      <c r="J15" s="165"/>
       <c r="K15" s="11"/>
       <c r="L15" s="119"/>
       <c r="M15" s="11"/>
@@ -28395,10 +28652,10 @@
       <c r="B16" s="160" t="s">
         <v>386</v>
       </c>
-      <c r="C16" s="166" t="s">
+      <c r="C16" s="167" t="s">
         <v>387</v>
       </c>
-      <c r="D16" s="166" t="s">
+      <c r="D16" s="167" t="s">
         <v>388</v>
       </c>
       <c r="E16" s="160" t="str">
@@ -28412,10 +28669,10 @@
       <c r="H16" s="163">
         <v>44302.0</v>
       </c>
-      <c r="I16" s="165" t="s">
+      <c r="I16" s="166" t="s">
         <v>375</v>
       </c>
-      <c r="J16" s="116"/>
+      <c r="J16" s="165"/>
       <c r="K16" s="11"/>
       <c r="L16" s="119"/>
       <c r="M16" s="11"/>
@@ -28442,10 +28699,10 @@
       <c r="B17" s="160" t="s">
         <v>389</v>
       </c>
-      <c r="C17" s="166" t="s">
+      <c r="C17" s="167" t="s">
         <v>390</v>
       </c>
-      <c r="D17" s="166" t="s">
+      <c r="D17" s="167" t="s">
         <v>391</v>
       </c>
       <c r="E17" s="160" t="str">
@@ -28459,10 +28716,10 @@
       <c r="H17" s="163">
         <v>44302.0</v>
       </c>
-      <c r="I17" s="165" t="s">
+      <c r="I17" s="166" t="s">
         <v>375</v>
       </c>
-      <c r="J17" s="116"/>
+      <c r="J17" s="165"/>
       <c r="K17" s="11"/>
       <c r="L17" s="119"/>
       <c r="M17" s="11"/>
@@ -28489,10 +28746,10 @@
       <c r="B18" s="160" t="s">
         <v>392</v>
       </c>
-      <c r="C18" s="166" t="s">
+      <c r="C18" s="167" t="s">
         <v>393</v>
       </c>
-      <c r="D18" s="166" t="s">
+      <c r="D18" s="167" t="s">
         <v>394</v>
       </c>
       <c r="E18" s="160" t="str">
@@ -28506,10 +28763,10 @@
       <c r="H18" s="163">
         <v>44302.0</v>
       </c>
-      <c r="I18" s="165" t="s">
+      <c r="I18" s="166" t="s">
         <v>375</v>
       </c>
-      <c r="J18" s="116"/>
+      <c r="J18" s="165"/>
       <c r="K18" s="11"/>
       <c r="L18" s="119"/>
       <c r="M18" s="11"/>
@@ -28536,10 +28793,10 @@
       <c r="B19" s="160" t="s">
         <v>395</v>
       </c>
-      <c r="C19" s="166" t="s">
+      <c r="C19" s="167" t="s">
         <v>396</v>
       </c>
-      <c r="D19" s="166" t="s">
+      <c r="D19" s="167" t="s">
         <v>397</v>
       </c>
       <c r="E19" s="160" t="str">
@@ -28555,10 +28812,10 @@
       <c r="H19" s="163">
         <v>44302.0</v>
       </c>
-      <c r="I19" s="165" t="s">
+      <c r="I19" s="166" t="s">
         <v>375</v>
       </c>
-      <c r="J19" s="116"/>
+      <c r="J19" s="165"/>
       <c r="K19" s="11"/>
       <c r="L19" s="119"/>
       <c r="M19" s="11"/>
@@ -28585,10 +28842,10 @@
       <c r="B20" s="160" t="s">
         <v>395</v>
       </c>
-      <c r="C20" s="166" t="s">
+      <c r="C20" s="167" t="s">
         <v>399</v>
       </c>
-      <c r="D20" s="166" t="s">
+      <c r="D20" s="167" t="s">
         <v>400</v>
       </c>
       <c r="E20" s="160" t="str">
@@ -28604,10 +28861,10 @@
       <c r="H20" s="163">
         <v>44302.0</v>
       </c>
-      <c r="I20" s="165" t="s">
+      <c r="I20" s="166" t="s">
         <v>375</v>
       </c>
-      <c r="J20" s="116"/>
+      <c r="J20" s="165"/>
       <c r="K20" s="11"/>
       <c r="L20" s="119"/>
       <c r="M20" s="11"/>
@@ -28634,10 +28891,10 @@
       <c r="B21" s="160" t="s">
         <v>395</v>
       </c>
-      <c r="C21" s="166" t="s">
+      <c r="C21" s="167" t="s">
         <v>402</v>
       </c>
-      <c r="D21" s="166" t="s">
+      <c r="D21" s="167" t="s">
         <v>403</v>
       </c>
       <c r="E21" s="160" t="str">
@@ -28653,10 +28910,10 @@
       <c r="H21" s="163">
         <v>44302.0</v>
       </c>
-      <c r="I21" s="165" t="s">
+      <c r="I21" s="166" t="s">
         <v>375</v>
       </c>
-      <c r="J21" s="116"/>
+      <c r="J21" s="165"/>
       <c r="K21" s="11"/>
       <c r="L21" s="119"/>
       <c r="M21" s="11"/>
@@ -28683,10 +28940,10 @@
       <c r="B22" s="160" t="s">
         <v>395</v>
       </c>
-      <c r="C22" s="166" t="s">
+      <c r="C22" s="167" t="s">
         <v>404</v>
       </c>
-      <c r="D22" s="166" t="s">
+      <c r="D22" s="167" t="s">
         <v>405</v>
       </c>
       <c r="E22" s="160" t="str">
@@ -28702,10 +28959,10 @@
       <c r="H22" s="163">
         <v>44302.0</v>
       </c>
-      <c r="I22" s="165" t="s">
+      <c r="I22" s="166" t="s">
         <v>375</v>
       </c>
-      <c r="J22" s="116"/>
+      <c r="J22" s="165"/>
       <c r="K22" s="11"/>
       <c r="L22" s="119"/>
       <c r="M22" s="11"/>
@@ -28732,10 +28989,10 @@
       <c r="B23" s="160" t="s">
         <v>395</v>
       </c>
-      <c r="C23" s="166" t="s">
+      <c r="C23" s="167" t="s">
         <v>406</v>
       </c>
-      <c r="D23" s="166" t="s">
+      <c r="D23" s="167" t="s">
         <v>407</v>
       </c>
       <c r="E23" s="160" t="str">
@@ -28751,10 +29008,10 @@
       <c r="H23" s="163">
         <v>44302.0</v>
       </c>
-      <c r="I23" s="165" t="s">
+      <c r="I23" s="166" t="s">
         <v>375</v>
       </c>
-      <c r="J23" s="116"/>
+      <c r="J23" s="165"/>
       <c r="K23" s="11"/>
       <c r="L23" s="119"/>
       <c r="M23" s="11"/>
@@ -28781,10 +29038,10 @@
       <c r="B24" s="160" t="s">
         <v>395</v>
       </c>
-      <c r="C24" s="166" t="s">
+      <c r="C24" s="167" t="s">
         <v>408</v>
       </c>
-      <c r="D24" s="166" t="s">
+      <c r="D24" s="167" t="s">
         <v>409</v>
       </c>
       <c r="E24" s="160" t="str">
@@ -28800,10 +29057,10 @@
       <c r="H24" s="163">
         <v>44302.0</v>
       </c>
-      <c r="I24" s="165" t="s">
+      <c r="I24" s="166" t="s">
         <v>375</v>
       </c>
-      <c r="J24" s="116"/>
+      <c r="J24" s="165"/>
       <c r="K24" s="11"/>
       <c r="L24" s="119"/>
       <c r="M24" s="11"/>
@@ -28830,10 +29087,10 @@
       <c r="B25" s="160" t="s">
         <v>395</v>
       </c>
-      <c r="C25" s="166" t="s">
+      <c r="C25" s="167" t="s">
         <v>410</v>
       </c>
-      <c r="D25" s="166" t="s">
+      <c r="D25" s="167" t="s">
         <v>411</v>
       </c>
       <c r="E25" s="160" t="str">
@@ -28849,10 +29106,10 @@
       <c r="H25" s="163">
         <v>44302.0</v>
       </c>
-      <c r="I25" s="165" t="s">
+      <c r="I25" s="166" t="s">
         <v>375</v>
       </c>
-      <c r="J25" s="116"/>
+      <c r="J25" s="165"/>
       <c r="K25" s="70"/>
       <c r="L25" s="119"/>
       <c r="M25" s="11"/>
@@ -28879,10 +29136,10 @@
       <c r="B26" s="160" t="s">
         <v>395</v>
       </c>
-      <c r="C26" s="166" t="s">
+      <c r="C26" s="167" t="s">
         <v>412</v>
       </c>
-      <c r="D26" s="166" t="s">
+      <c r="D26" s="167" t="s">
         <v>413</v>
       </c>
       <c r="E26" s="160" t="str">
@@ -28898,10 +29155,10 @@
       <c r="H26" s="163">
         <v>44302.0</v>
       </c>
-      <c r="I26" s="165" t="s">
+      <c r="I26" s="166" t="s">
         <v>375</v>
       </c>
-      <c r="J26" s="116"/>
+      <c r="J26" s="165"/>
       <c r="K26" s="93"/>
       <c r="L26" s="115"/>
       <c r="M26" s="93"/>
@@ -28928,10 +29185,10 @@
       <c r="B27" s="160" t="s">
         <v>395</v>
       </c>
-      <c r="C27" s="166" t="s">
+      <c r="C27" s="167" t="s">
         <v>414</v>
       </c>
-      <c r="D27" s="166" t="s">
+      <c r="D27" s="167" t="s">
         <v>415</v>
       </c>
       <c r="E27" s="160" t="str">
@@ -28947,10 +29204,10 @@
       <c r="H27" s="163">
         <v>44302.0</v>
       </c>
-      <c r="I27" s="165" t="s">
+      <c r="I27" s="166" t="s">
         <v>375</v>
       </c>
-      <c r="J27" s="116"/>
+      <c r="J27" s="165"/>
       <c r="K27" s="11"/>
       <c r="L27" s="119"/>
       <c r="M27" s="11"/>
@@ -28977,10 +29234,10 @@
       <c r="B28" s="160" t="s">
         <v>395</v>
       </c>
-      <c r="C28" s="166" t="s">
+      <c r="C28" s="167" t="s">
         <v>416</v>
       </c>
-      <c r="D28" s="166" t="s">
+      <c r="D28" s="167" t="s">
         <v>417</v>
       </c>
       <c r="E28" s="160" t="str">
@@ -28996,10 +29253,10 @@
       <c r="H28" s="163">
         <v>44302.0</v>
       </c>
-      <c r="I28" s="165" t="s">
+      <c r="I28" s="166" t="s">
         <v>375</v>
       </c>
-      <c r="J28" s="116"/>
+      <c r="J28" s="165"/>
       <c r="K28" s="11"/>
       <c r="L28" s="86"/>
       <c r="M28" s="11"/>
@@ -29026,10 +29283,10 @@
       <c r="B29" s="160" t="s">
         <v>395</v>
       </c>
-      <c r="C29" s="166" t="s">
+      <c r="C29" s="167" t="s">
         <v>418</v>
       </c>
-      <c r="D29" s="166" t="s">
+      <c r="D29" s="167" t="s">
         <v>419</v>
       </c>
       <c r="E29" s="160" t="str">
@@ -29045,10 +29302,10 @@
       <c r="H29" s="163">
         <v>44302.0</v>
       </c>
-      <c r="I29" s="165" t="s">
+      <c r="I29" s="166" t="s">
         <v>375</v>
       </c>
-      <c r="J29" s="116"/>
+      <c r="J29" s="165"/>
       <c r="K29" s="93"/>
       <c r="L29" s="115"/>
       <c r="M29" s="93"/>
@@ -29075,10 +29332,10 @@
       <c r="B30" s="160" t="s">
         <v>395</v>
       </c>
-      <c r="C30" s="166" t="s">
+      <c r="C30" s="167" t="s">
         <v>420</v>
       </c>
-      <c r="D30" s="166" t="s">
+      <c r="D30" s="167" t="s">
         <v>421</v>
       </c>
       <c r="E30" s="160" t="str">
@@ -29094,10 +29351,10 @@
       <c r="H30" s="163">
         <v>44302.0</v>
       </c>
-      <c r="I30" s="165" t="s">
+      <c r="I30" s="166" t="s">
         <v>375</v>
       </c>
-      <c r="J30" s="116"/>
+      <c r="J30" s="165"/>
       <c r="K30" s="11"/>
       <c r="L30" s="119"/>
       <c r="M30" s="11"/>
@@ -29124,10 +29381,10 @@
       <c r="B31" s="160" t="s">
         <v>395</v>
       </c>
-      <c r="C31" s="166" t="s">
+      <c r="C31" s="167" t="s">
         <v>422</v>
       </c>
-      <c r="D31" s="166" t="s">
+      <c r="D31" s="167" t="s">
         <v>397</v>
       </c>
       <c r="E31" s="160" t="str">
@@ -29143,10 +29400,10 @@
       <c r="H31" s="163">
         <v>44302.0</v>
       </c>
-      <c r="I31" s="165" t="s">
+      <c r="I31" s="166" t="s">
         <v>375</v>
       </c>
-      <c r="J31" s="116"/>
+      <c r="J31" s="165"/>
       <c r="K31" s="155"/>
       <c r="L31" s="156"/>
       <c r="M31" s="155"/>
@@ -29173,10 +29430,10 @@
       <c r="B32" s="160" t="s">
         <v>395</v>
       </c>
-      <c r="C32" s="166" t="s">
+      <c r="C32" s="167" t="s">
         <v>423</v>
       </c>
-      <c r="D32" s="166" t="s">
+      <c r="D32" s="167" t="s">
         <v>405</v>
       </c>
       <c r="E32" s="160" t="str">
@@ -29192,10 +29449,10 @@
       <c r="H32" s="163">
         <v>44302.0</v>
       </c>
-      <c r="I32" s="165" t="s">
+      <c r="I32" s="166" t="s">
         <v>375</v>
       </c>
-      <c r="J32" s="116"/>
+      <c r="J32" s="165"/>
       <c r="K32" s="155"/>
       <c r="L32" s="156"/>
       <c r="M32" s="155"/>
@@ -29222,10 +29479,10 @@
       <c r="B33" s="160" t="s">
         <v>395</v>
       </c>
-      <c r="C33" s="166" t="s">
+      <c r="C33" s="167" t="s">
         <v>424</v>
       </c>
-      <c r="D33" s="166" t="s">
+      <c r="D33" s="167" t="s">
         <v>411</v>
       </c>
       <c r="E33" s="160" t="str">
@@ -29241,10 +29498,10 @@
       <c r="H33" s="163">
         <v>44302.0</v>
       </c>
-      <c r="I33" s="165" t="s">
+      <c r="I33" s="166" t="s">
         <v>375</v>
       </c>
-      <c r="J33" s="116"/>
+      <c r="J33" s="165"/>
       <c r="K33" s="155"/>
       <c r="L33" s="156"/>
       <c r="M33" s="155"/>
@@ -29271,10 +29528,10 @@
       <c r="B34" s="160" t="s">
         <v>425</v>
       </c>
-      <c r="C34" s="166" t="s">
+      <c r="C34" s="167" t="s">
         <v>426</v>
       </c>
-      <c r="D34" s="166" t="s">
+      <c r="D34" s="167" t="s">
         <v>427</v>
       </c>
       <c r="E34" s="160" t="str">
@@ -29283,15 +29540,17 @@
       </c>
       <c r="F34" s="161"/>
       <c r="G34" s="162" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H34" s="163">
         <v>44302.0</v>
       </c>
-      <c r="I34" s="165" t="s">
+      <c r="I34" s="166" t="s">
         <v>375</v>
       </c>
-      <c r="J34" s="116"/>
+      <c r="J34" s="162" t="s">
+        <v>428</v>
+      </c>
       <c r="K34" s="155"/>
       <c r="L34" s="156"/>
       <c r="M34" s="155"/>
@@ -29316,13 +29575,13 @@
         <v>[Manager-26]</v>
       </c>
       <c r="B35" s="160" t="s">
-        <v>428</v>
-      </c>
-      <c r="C35" s="166" t="s">
+        <v>429</v>
+      </c>
+      <c r="C35" s="167" t="s">
         <v>426</v>
       </c>
-      <c r="D35" s="166" t="s">
-        <v>429</v>
+      <c r="D35" s="167" t="s">
+        <v>430</v>
       </c>
       <c r="E35" s="160" t="str">
         <f t="shared" si="2"/>
@@ -29335,10 +29594,10 @@
       <c r="H35" s="163">
         <v>44302.0</v>
       </c>
-      <c r="I35" s="165" t="s">
+      <c r="I35" s="166" t="s">
         <v>375</v>
       </c>
-      <c r="J35" s="116"/>
+      <c r="J35" s="165"/>
       <c r="K35" s="155"/>
       <c r="L35" s="156"/>
       <c r="M35" s="155"/>
@@ -29363,20 +29622,20 @@
         <v>[Manager-27]</v>
       </c>
       <c r="B36" s="160" t="s">
-        <v>430</v>
-      </c>
-      <c r="C36" s="166" t="s">
         <v>431</v>
       </c>
-      <c r="D36" s="166" t="s">
+      <c r="C36" s="167" t="s">
         <v>432</v>
+      </c>
+      <c r="D36" s="167" t="s">
+        <v>433</v>
       </c>
       <c r="E36" s="160" t="str">
         <f t="shared" si="2"/>
         <v>[Manager-1]</v>
       </c>
       <c r="F36" s="161" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="G36" s="162" t="s">
         <v>83</v>
@@ -29384,10 +29643,10 @@
       <c r="H36" s="163">
         <v>44302.0</v>
       </c>
-      <c r="I36" s="165" t="s">
+      <c r="I36" s="166" t="s">
         <v>375</v>
       </c>
-      <c r="J36" s="116"/>
+      <c r="J36" s="165"/>
       <c r="K36" s="155"/>
       <c r="L36" s="156"/>
       <c r="M36" s="155"/>
@@ -29412,20 +29671,20 @@
         <v>[Manager-28]</v>
       </c>
       <c r="B37" s="160" t="s">
-        <v>434</v>
-      </c>
-      <c r="C37" s="166" t="s">
-        <v>431</v>
+        <v>435</v>
+      </c>
+      <c r="C37" s="167" t="s">
+        <v>432</v>
       </c>
       <c r="D37" s="167" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="E37" s="160" t="str">
         <f t="shared" si="2"/>
         <v>[Manager-1]</v>
       </c>
       <c r="F37" s="161" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="G37" s="162" t="s">
         <v>83</v>
@@ -29433,10 +29692,10 @@
       <c r="H37" s="163">
         <v>44302.0</v>
       </c>
-      <c r="I37" s="165" t="s">
+      <c r="I37" s="166" t="s">
         <v>375</v>
       </c>
-      <c r="J37" s="116"/>
+      <c r="J37" s="165"/>
       <c r="K37" s="155"/>
       <c r="L37" s="156"/>
       <c r="M37" s="155"/>
@@ -29461,20 +29720,20 @@
         <v>[Manager-29]</v>
       </c>
       <c r="B38" s="160" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="C38" s="167" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="D38" s="167" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="E38" s="160" t="str">
         <f t="shared" si="2"/>
         <v>[Manager-1]</v>
       </c>
       <c r="F38" s="161" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="G38" s="162" t="s">
         <v>83</v>
@@ -29482,10 +29741,10 @@
       <c r="H38" s="163">
         <v>44302.0</v>
       </c>
-      <c r="I38" s="165" t="s">
+      <c r="I38" s="166" t="s">
         <v>375</v>
       </c>
-      <c r="J38" s="116"/>
+      <c r="J38" s="165"/>
       <c r="K38" s="155"/>
       <c r="L38" s="156"/>
       <c r="M38" s="155"/>
@@ -29510,20 +29769,20 @@
         <v>[Manager-30]</v>
       </c>
       <c r="B39" s="160" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="C39" s="167" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="D39" s="167" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="E39" s="160" t="str">
         <f t="shared" si="2"/>
         <v>[Manager-1]</v>
       </c>
       <c r="F39" s="161" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="G39" s="162" t="s">
         <v>83</v>
@@ -29531,10 +29790,10 @@
       <c r="H39" s="163">
         <v>44302.0</v>
       </c>
-      <c r="I39" s="165" t="s">
+      <c r="I39" s="166" t="s">
         <v>375</v>
       </c>
-      <c r="J39" s="116"/>
+      <c r="J39" s="165"/>
       <c r="K39" s="155"/>
       <c r="L39" s="156"/>
       <c r="M39" s="155"/>
@@ -29559,20 +29818,20 @@
         <v>[Manager-31]</v>
       </c>
       <c r="B40" s="160" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="C40" s="167" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="D40" s="167" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="E40" s="160" t="str">
         <f t="shared" si="2"/>
         <v>[Manager-1]</v>
       </c>
       <c r="F40" s="161" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="G40" s="162" t="s">
         <v>83</v>
@@ -29580,10 +29839,10 @@
       <c r="H40" s="163">
         <v>44302.0</v>
       </c>
-      <c r="I40" s="168" t="s">
+      <c r="I40" s="166" t="s">
         <v>375</v>
       </c>
-      <c r="J40" s="116"/>
+      <c r="J40" s="165"/>
       <c r="K40" s="155"/>
       <c r="L40" s="156"/>
       <c r="M40" s="155"/>
@@ -29608,20 +29867,20 @@
         <v>[Manager-32]</v>
       </c>
       <c r="B41" s="160" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="C41" s="167" t="s">
-        <v>445</v>
-      </c>
-      <c r="D41" s="167" t="s">
         <v>446</v>
+      </c>
+      <c r="D41" s="168" t="s">
+        <v>447</v>
       </c>
       <c r="E41" s="160" t="str">
         <f t="shared" si="2"/>
         <v>[Manager-1]</v>
       </c>
       <c r="F41" s="161" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="G41" s="162" t="s">
         <v>83</v>
@@ -29629,10 +29888,10 @@
       <c r="H41" s="163">
         <v>44302.0</v>
       </c>
-      <c r="I41" s="168" t="s">
+      <c r="I41" s="166" t="s">
         <v>375</v>
       </c>
-      <c r="J41" s="116"/>
+      <c r="J41" s="165"/>
       <c r="K41" s="155"/>
       <c r="L41" s="156"/>
       <c r="M41" s="155"/>
@@ -29657,20 +29916,20 @@
         <v>[Manager-33]</v>
       </c>
       <c r="B42" s="160" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="C42" s="167" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="D42" s="167" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="E42" s="160" t="str">
         <f t="shared" si="2"/>
         <v>[Manager-1]</v>
       </c>
       <c r="F42" s="161" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="G42" s="162" t="s">
         <v>83</v>
@@ -29678,10 +29937,10 @@
       <c r="H42" s="163">
         <v>44302.0</v>
       </c>
-      <c r="I42" s="168" t="s">
+      <c r="I42" s="166" t="s">
         <v>375</v>
       </c>
-      <c r="J42" s="116"/>
+      <c r="J42" s="165"/>
       <c r="K42" s="155"/>
       <c r="L42" s="156"/>
       <c r="M42" s="155"/>
@@ -29700,20 +29959,37 @@
       <c r="Z42" s="155"/>
       <c r="AA42" s="155"/>
     </row>
-    <row r="43" ht="12.75" customHeight="1">
+    <row r="43" ht="94.5" customHeight="1">
       <c r="A43" s="160" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B43" s="125"/>
-      <c r="C43" s="125"/>
-      <c r="D43" s="125"/>
-      <c r="E43" s="125"/>
-      <c r="F43" s="125"/>
-      <c r="G43" s="169"/>
-      <c r="H43" s="169"/>
-      <c r="I43" s="169"/>
-      <c r="J43" s="125"/>
+        <v>[Manager-34]</v>
+      </c>
+      <c r="B43" s="160" t="s">
+        <v>450</v>
+      </c>
+      <c r="C43" s="167" t="s">
+        <v>451</v>
+      </c>
+      <c r="D43" s="168" t="s">
+        <v>452</v>
+      </c>
+      <c r="E43" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F43" s="161" t="s">
+        <v>440</v>
+      </c>
+      <c r="G43" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H43" s="163">
+        <v>44302.0</v>
+      </c>
+      <c r="I43" s="166" t="s">
+        <v>375</v>
+      </c>
+      <c r="J43" s="165"/>
       <c r="K43" s="155"/>
       <c r="L43" s="156"/>
       <c r="M43" s="155"/>
@@ -29732,20 +30008,37 @@
       <c r="Z43" s="155"/>
       <c r="AA43" s="155"/>
     </row>
-    <row r="44" ht="12.75" customHeight="1">
+    <row r="44" ht="94.5" customHeight="1">
       <c r="A44" s="160" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B44" s="125"/>
-      <c r="C44" s="125"/>
-      <c r="D44" s="125"/>
-      <c r="E44" s="125"/>
-      <c r="F44" s="125"/>
-      <c r="G44" s="169"/>
-      <c r="H44" s="169"/>
-      <c r="I44" s="169"/>
-      <c r="J44" s="125"/>
+        <v>[Manager-35]</v>
+      </c>
+      <c r="B44" s="160" t="s">
+        <v>450</v>
+      </c>
+      <c r="C44" s="167" t="s">
+        <v>453</v>
+      </c>
+      <c r="D44" s="167" t="s">
+        <v>454</v>
+      </c>
+      <c r="E44" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F44" s="161" t="s">
+        <v>440</v>
+      </c>
+      <c r="G44" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H44" s="163">
+        <v>44302.0</v>
+      </c>
+      <c r="I44" s="166" t="s">
+        <v>375</v>
+      </c>
+      <c r="J44" s="165"/>
       <c r="K44" s="155"/>
       <c r="L44" s="156"/>
       <c r="M44" s="155"/>
@@ -29764,20 +30057,37 @@
       <c r="Z44" s="155"/>
       <c r="AA44" s="155"/>
     </row>
-    <row r="45" ht="12.75" customHeight="1">
+    <row r="45" ht="89.25" customHeight="1">
       <c r="A45" s="160" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B45" s="125"/>
-      <c r="C45" s="125"/>
-      <c r="D45" s="125"/>
-      <c r="E45" s="125"/>
-      <c r="F45" s="125"/>
-      <c r="G45" s="169"/>
-      <c r="H45" s="169"/>
-      <c r="I45" s="169"/>
-      <c r="J45" s="125"/>
+        <v>[Manager-36]</v>
+      </c>
+      <c r="B45" s="160" t="s">
+        <v>455</v>
+      </c>
+      <c r="C45" s="168" t="s">
+        <v>456</v>
+      </c>
+      <c r="D45" s="168" t="s">
+        <v>457</v>
+      </c>
+      <c r="E45" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F45" s="161" t="s">
+        <v>440</v>
+      </c>
+      <c r="G45" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H45" s="163">
+        <v>44302.0</v>
+      </c>
+      <c r="I45" s="166" t="s">
+        <v>375</v>
+      </c>
+      <c r="J45" s="165"/>
       <c r="K45" s="155"/>
       <c r="L45" s="156"/>
       <c r="M45" s="155"/>
@@ -29796,20 +30106,37 @@
       <c r="Z45" s="155"/>
       <c r="AA45" s="155"/>
     </row>
-    <row r="46" ht="12.75" customHeight="1">
+    <row r="46" ht="92.25" customHeight="1">
       <c r="A46" s="160" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B46" s="125"/>
-      <c r="C46" s="125"/>
-      <c r="D46" s="125"/>
-      <c r="E46" s="125"/>
-      <c r="F46" s="125"/>
-      <c r="G46" s="169"/>
-      <c r="H46" s="169"/>
-      <c r="I46" s="169"/>
-      <c r="J46" s="125"/>
+        <v>[Manager-37]</v>
+      </c>
+      <c r="B46" s="160" t="s">
+        <v>455</v>
+      </c>
+      <c r="C46" s="168" t="s">
+        <v>458</v>
+      </c>
+      <c r="D46" s="168" t="s">
+        <v>459</v>
+      </c>
+      <c r="E46" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F46" s="161" t="s">
+        <v>440</v>
+      </c>
+      <c r="G46" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H46" s="163">
+        <v>44302.0</v>
+      </c>
+      <c r="I46" s="166" t="s">
+        <v>375</v>
+      </c>
+      <c r="J46" s="165"/>
       <c r="K46" s="155"/>
       <c r="L46" s="156"/>
       <c r="M46" s="155"/>
@@ -29828,20 +30155,37 @@
       <c r="Z46" s="155"/>
       <c r="AA46" s="155"/>
     </row>
-    <row r="47" ht="12.75" customHeight="1">
+    <row r="47" ht="99.0" customHeight="1">
       <c r="A47" s="160" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B47" s="125"/>
-      <c r="C47" s="125"/>
-      <c r="D47" s="125"/>
-      <c r="E47" s="125"/>
-      <c r="F47" s="125"/>
-      <c r="G47" s="169"/>
-      <c r="H47" s="169"/>
-      <c r="I47" s="169"/>
-      <c r="J47" s="125"/>
+        <v>[Manager-38]</v>
+      </c>
+      <c r="B47" s="160" t="s">
+        <v>460</v>
+      </c>
+      <c r="C47" s="168" t="s">
+        <v>461</v>
+      </c>
+      <c r="D47" s="168" t="s">
+        <v>457</v>
+      </c>
+      <c r="E47" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F47" s="161" t="s">
+        <v>440</v>
+      </c>
+      <c r="G47" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H47" s="163">
+        <v>44302.0</v>
+      </c>
+      <c r="I47" s="169" t="s">
+        <v>375</v>
+      </c>
+      <c r="J47" s="165"/>
       <c r="K47" s="155"/>
       <c r="L47" s="156"/>
       <c r="M47" s="155"/>
@@ -29860,20 +30204,37 @@
       <c r="Z47" s="155"/>
       <c r="AA47" s="155"/>
     </row>
-    <row r="48" ht="12.75" customHeight="1">
+    <row r="48" ht="105.0" customHeight="1">
       <c r="A48" s="160" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B48" s="125"/>
-      <c r="C48" s="125"/>
-      <c r="D48" s="125"/>
-      <c r="E48" s="125"/>
-      <c r="F48" s="125"/>
-      <c r="G48" s="169"/>
-      <c r="H48" s="169"/>
-      <c r="I48" s="169"/>
-      <c r="J48" s="125"/>
+        <v>[Manager-39]</v>
+      </c>
+      <c r="B48" s="160" t="s">
+        <v>460</v>
+      </c>
+      <c r="C48" s="168" t="s">
+        <v>462</v>
+      </c>
+      <c r="D48" s="168" t="s">
+        <v>463</v>
+      </c>
+      <c r="E48" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F48" s="161" t="s">
+        <v>464</v>
+      </c>
+      <c r="G48" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H48" s="163">
+        <v>44302.0</v>
+      </c>
+      <c r="I48" s="169" t="s">
+        <v>375</v>
+      </c>
+      <c r="J48" s="165"/>
       <c r="K48" s="155"/>
       <c r="L48" s="156"/>
       <c r="M48" s="155"/>
@@ -29892,20 +30253,37 @@
       <c r="Z48" s="155"/>
       <c r="AA48" s="155"/>
     </row>
-    <row r="49" ht="12.75" customHeight="1">
+    <row r="49" ht="106.5" customHeight="1">
       <c r="A49" s="160" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B49" s="125"/>
-      <c r="C49" s="125"/>
-      <c r="D49" s="125"/>
-      <c r="E49" s="125"/>
-      <c r="F49" s="125"/>
-      <c r="G49" s="169"/>
-      <c r="H49" s="169"/>
-      <c r="I49" s="169"/>
-      <c r="J49" s="125"/>
+        <v>[Manager-40]</v>
+      </c>
+      <c r="B49" s="160" t="s">
+        <v>460</v>
+      </c>
+      <c r="C49" s="168" t="s">
+        <v>465</v>
+      </c>
+      <c r="D49" s="168" t="s">
+        <v>466</v>
+      </c>
+      <c r="E49" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F49" s="161" t="s">
+        <v>467</v>
+      </c>
+      <c r="G49" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H49" s="163">
+        <v>44302.0</v>
+      </c>
+      <c r="I49" s="169" t="s">
+        <v>375</v>
+      </c>
+      <c r="J49" s="165"/>
       <c r="K49" s="155"/>
       <c r="L49" s="156"/>
       <c r="M49" s="155"/>
@@ -29924,20 +30302,37 @@
       <c r="Z49" s="155"/>
       <c r="AA49" s="155"/>
     </row>
-    <row r="50" ht="12.75" customHeight="1">
+    <row r="50" ht="103.5" customHeight="1">
       <c r="A50" s="160" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B50" s="125"/>
-      <c r="C50" s="125"/>
-      <c r="D50" s="125"/>
-      <c r="E50" s="125"/>
-      <c r="F50" s="125"/>
-      <c r="G50" s="169"/>
-      <c r="H50" s="169"/>
-      <c r="I50" s="169"/>
-      <c r="J50" s="125"/>
+        <v>[Manager-41]</v>
+      </c>
+      <c r="B50" s="160" t="s">
+        <v>460</v>
+      </c>
+      <c r="C50" s="168" t="s">
+        <v>468</v>
+      </c>
+      <c r="D50" s="168" t="s">
+        <v>469</v>
+      </c>
+      <c r="E50" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F50" s="161" t="s">
+        <v>470</v>
+      </c>
+      <c r="G50" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H50" s="163">
+        <v>44302.0</v>
+      </c>
+      <c r="I50" s="169" t="s">
+        <v>375</v>
+      </c>
+      <c r="J50" s="165"/>
       <c r="K50" s="155"/>
       <c r="L50" s="156"/>
       <c r="M50" s="155"/>
@@ -29956,17 +30351,37 @@
       <c r="Z50" s="155"/>
       <c r="AA50" s="155"/>
     </row>
-    <row r="51" ht="12.75" customHeight="1">
-      <c r="A51" s="50"/>
-      <c r="B51" s="50"/>
-      <c r="C51" s="170"/>
-      <c r="D51" s="170"/>
-      <c r="E51" s="50"/>
-      <c r="F51" s="50"/>
-      <c r="G51" s="171"/>
-      <c r="H51" s="171"/>
-      <c r="I51" s="171"/>
-      <c r="J51" s="50"/>
+    <row r="51" ht="103.5" customHeight="1">
+      <c r="A51" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v>[Manager-42]</v>
+      </c>
+      <c r="B51" s="160" t="s">
+        <v>460</v>
+      </c>
+      <c r="C51" s="168" t="s">
+        <v>471</v>
+      </c>
+      <c r="D51" s="168" t="s">
+        <v>469</v>
+      </c>
+      <c r="E51" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F51" s="161" t="s">
+        <v>472</v>
+      </c>
+      <c r="G51" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H51" s="163">
+        <v>44302.0</v>
+      </c>
+      <c r="I51" s="169" t="s">
+        <v>375</v>
+      </c>
+      <c r="J51" s="165"/>
       <c r="K51" s="86"/>
       <c r="L51" s="11"/>
       <c r="M51" s="11"/>
@@ -29985,17 +30400,37 @@
       <c r="Z51" s="11"/>
       <c r="AA51" s="155"/>
     </row>
-    <row r="52" ht="12.75" customHeight="1">
-      <c r="A52" s="50"/>
-      <c r="B52" s="50"/>
-      <c r="C52" s="170"/>
-      <c r="D52" s="170"/>
-      <c r="E52" s="50"/>
-      <c r="F52" s="50"/>
-      <c r="G52" s="171"/>
-      <c r="H52" s="171"/>
-      <c r="I52" s="171"/>
-      <c r="J52" s="50"/>
+    <row r="52" ht="105.75" customHeight="1">
+      <c r="A52" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v>[Manager-43]</v>
+      </c>
+      <c r="B52" s="160" t="s">
+        <v>460</v>
+      </c>
+      <c r="C52" s="168" t="s">
+        <v>473</v>
+      </c>
+      <c r="D52" s="168" t="s">
+        <v>474</v>
+      </c>
+      <c r="E52" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F52" s="161" t="s">
+        <v>475</v>
+      </c>
+      <c r="G52" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H52" s="163">
+        <v>44302.0</v>
+      </c>
+      <c r="I52" s="169" t="s">
+        <v>375</v>
+      </c>
+      <c r="J52" s="165"/>
       <c r="K52" s="86"/>
       <c r="L52" s="11"/>
       <c r="M52" s="11"/>
@@ -30014,17 +30449,37 @@
       <c r="Z52" s="11"/>
       <c r="AA52" s="155"/>
     </row>
-    <row r="53" ht="12.75" customHeight="1">
-      <c r="A53" s="50"/>
-      <c r="B53" s="50"/>
-      <c r="C53" s="170"/>
-      <c r="D53" s="170"/>
-      <c r="E53" s="50"/>
-      <c r="F53" s="50"/>
-      <c r="G53" s="171"/>
-      <c r="H53" s="171"/>
-      <c r="I53" s="171"/>
-      <c r="J53" s="50"/>
+    <row r="53" ht="124.5" customHeight="1">
+      <c r="A53" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v>[Manager-44]</v>
+      </c>
+      <c r="B53" s="160" t="s">
+        <v>460</v>
+      </c>
+      <c r="C53" s="168" t="s">
+        <v>476</v>
+      </c>
+      <c r="D53" s="168" t="s">
+        <v>477</v>
+      </c>
+      <c r="E53" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F53" s="161" t="s">
+        <v>475</v>
+      </c>
+      <c r="G53" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H53" s="163">
+        <v>44302.0</v>
+      </c>
+      <c r="I53" s="169" t="s">
+        <v>375</v>
+      </c>
+      <c r="J53" s="165"/>
       <c r="K53" s="86"/>
       <c r="L53" s="11"/>
       <c r="M53" s="11"/>
@@ -30043,17 +30498,37 @@
       <c r="Z53" s="11"/>
       <c r="AA53" s="155"/>
     </row>
-    <row r="54" ht="12.75" customHeight="1">
-      <c r="A54" s="50"/>
-      <c r="B54" s="50"/>
-      <c r="C54" s="170"/>
-      <c r="D54" s="170"/>
-      <c r="E54" s="50"/>
-      <c r="F54" s="50"/>
-      <c r="G54" s="171"/>
-      <c r="H54" s="171"/>
-      <c r="I54" s="171"/>
-      <c r="J54" s="50"/>
+    <row r="54" ht="118.5" customHeight="1">
+      <c r="A54" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v>[Manager-45]</v>
+      </c>
+      <c r="B54" s="160" t="s">
+        <v>460</v>
+      </c>
+      <c r="C54" s="168" t="s">
+        <v>478</v>
+      </c>
+      <c r="D54" s="168" t="s">
+        <v>479</v>
+      </c>
+      <c r="E54" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F54" s="161" t="s">
+        <v>475</v>
+      </c>
+      <c r="G54" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H54" s="163">
+        <v>44302.0</v>
+      </c>
+      <c r="I54" s="169" t="s">
+        <v>375</v>
+      </c>
+      <c r="J54" s="165"/>
       <c r="K54" s="86"/>
       <c r="L54" s="11"/>
       <c r="M54" s="11"/>
@@ -30072,17 +30547,37 @@
       <c r="Z54" s="11"/>
       <c r="AA54" s="155"/>
     </row>
-    <row r="55" ht="12.75" customHeight="1">
-      <c r="A55" s="50"/>
-      <c r="B55" s="50"/>
-      <c r="C55" s="50"/>
-      <c r="D55" s="170"/>
-      <c r="E55" s="50"/>
-      <c r="F55" s="50"/>
-      <c r="G55" s="171"/>
-      <c r="H55" s="171"/>
-      <c r="I55" s="171"/>
-      <c r="J55" s="50"/>
+    <row r="55" ht="56.25" customHeight="1">
+      <c r="A55" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v>[Manager-46]</v>
+      </c>
+      <c r="B55" s="160" t="s">
+        <v>480</v>
+      </c>
+      <c r="C55" s="168" t="s">
+        <v>438</v>
+      </c>
+      <c r="D55" s="168" t="s">
+        <v>481</v>
+      </c>
+      <c r="E55" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F55" s="161" t="s">
+        <v>482</v>
+      </c>
+      <c r="G55" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H55" s="163">
+        <v>44302.0</v>
+      </c>
+      <c r="I55" s="169" t="s">
+        <v>375</v>
+      </c>
+      <c r="J55" s="165"/>
       <c r="K55" s="86"/>
       <c r="L55" s="11"/>
       <c r="M55" s="11"/>
@@ -30101,17 +30596,37 @@
       <c r="Z55" s="11"/>
       <c r="AA55" s="155"/>
     </row>
-    <row r="56" ht="12.75" customHeight="1">
-      <c r="A56" s="50"/>
-      <c r="B56" s="50"/>
-      <c r="C56" s="50"/>
-      <c r="D56" s="170"/>
-      <c r="E56" s="50"/>
-      <c r="F56" s="50"/>
-      <c r="G56" s="171"/>
-      <c r="H56" s="171"/>
-      <c r="I56" s="171"/>
-      <c r="J56" s="50"/>
+    <row r="56" ht="93.75" customHeight="1">
+      <c r="A56" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v>[Manager-47]</v>
+      </c>
+      <c r="B56" s="160" t="s">
+        <v>480</v>
+      </c>
+      <c r="C56" s="168" t="s">
+        <v>483</v>
+      </c>
+      <c r="D56" s="168" t="s">
+        <v>484</v>
+      </c>
+      <c r="E56" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F56" s="161" t="s">
+        <v>482</v>
+      </c>
+      <c r="G56" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H56" s="163">
+        <v>44302.0</v>
+      </c>
+      <c r="I56" s="169" t="s">
+        <v>375</v>
+      </c>
+      <c r="J56" s="165"/>
       <c r="K56" s="86"/>
       <c r="L56" s="11"/>
       <c r="M56" s="11"/>
@@ -30130,17 +30645,37 @@
       <c r="Z56" s="11"/>
       <c r="AA56" s="155"/>
     </row>
-    <row r="57" ht="12.75" customHeight="1">
-      <c r="A57" s="50"/>
-      <c r="B57" s="50"/>
-      <c r="C57" s="50"/>
-      <c r="D57" s="170"/>
-      <c r="E57" s="50"/>
-      <c r="F57" s="50"/>
-      <c r="G57" s="171"/>
-      <c r="H57" s="171"/>
-      <c r="I57" s="171"/>
-      <c r="J57" s="50"/>
+    <row r="57" ht="67.5" customHeight="1">
+      <c r="A57" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v>[Manager-48]</v>
+      </c>
+      <c r="B57" s="160" t="s">
+        <v>485</v>
+      </c>
+      <c r="C57" s="168" t="s">
+        <v>438</v>
+      </c>
+      <c r="D57" s="168" t="s">
+        <v>486</v>
+      </c>
+      <c r="E57" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F57" s="161" t="s">
+        <v>482</v>
+      </c>
+      <c r="G57" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H57" s="163">
+        <v>44302.0</v>
+      </c>
+      <c r="I57" s="169" t="s">
+        <v>375</v>
+      </c>
+      <c r="J57" s="165"/>
       <c r="K57" s="86"/>
       <c r="L57" s="11"/>
       <c r="M57" s="11"/>
@@ -30159,17 +30694,37 @@
       <c r="Z57" s="11"/>
       <c r="AA57" s="155"/>
     </row>
-    <row r="58" ht="12.75" customHeight="1">
-      <c r="A58" s="50"/>
-      <c r="B58" s="50"/>
-      <c r="C58" s="50"/>
-      <c r="D58" s="170"/>
-      <c r="E58" s="50"/>
-      <c r="F58" s="50"/>
-      <c r="G58" s="171"/>
-      <c r="H58" s="171"/>
-      <c r="I58" s="171"/>
-      <c r="J58" s="50"/>
+    <row r="58" ht="75.0" customHeight="1">
+      <c r="A58" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v>[Manager-49]</v>
+      </c>
+      <c r="B58" s="160" t="s">
+        <v>485</v>
+      </c>
+      <c r="C58" s="168" t="s">
+        <v>483</v>
+      </c>
+      <c r="D58" s="168" t="s">
+        <v>487</v>
+      </c>
+      <c r="E58" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F58" s="161" t="s">
+        <v>482</v>
+      </c>
+      <c r="G58" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H58" s="163">
+        <v>44302.0</v>
+      </c>
+      <c r="I58" s="169" t="s">
+        <v>375</v>
+      </c>
+      <c r="J58" s="165"/>
       <c r="K58" s="86"/>
       <c r="L58" s="11"/>
       <c r="M58" s="11"/>
@@ -30188,17 +30743,39 @@
       <c r="Z58" s="11"/>
       <c r="AA58" s="155"/>
     </row>
-    <row r="59" ht="12.75" customHeight="1">
-      <c r="A59" s="50"/>
-      <c r="B59" s="50"/>
-      <c r="C59" s="50"/>
-      <c r="D59" s="170"/>
-      <c r="E59" s="50"/>
-      <c r="F59" s="50"/>
-      <c r="G59" s="171"/>
-      <c r="H59" s="171"/>
-      <c r="I59" s="171"/>
-      <c r="J59" s="50"/>
+    <row r="59" ht="64.5" customHeight="1">
+      <c r="A59" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v>[Manager-50]</v>
+      </c>
+      <c r="B59" s="160" t="s">
+        <v>488</v>
+      </c>
+      <c r="C59" s="168" t="s">
+        <v>483</v>
+      </c>
+      <c r="D59" s="168" t="s">
+        <v>489</v>
+      </c>
+      <c r="E59" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F59" s="161" t="s">
+        <v>482</v>
+      </c>
+      <c r="G59" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H59" s="163">
+        <v>44302.0</v>
+      </c>
+      <c r="I59" s="169" t="s">
+        <v>375</v>
+      </c>
+      <c r="J59" s="162" t="s">
+        <v>490</v>
+      </c>
       <c r="K59" s="86"/>
       <c r="L59" s="11"/>
       <c r="M59" s="11"/>
@@ -30217,17 +30794,37 @@
       <c r="Z59" s="11"/>
       <c r="AA59" s="155"/>
     </row>
-    <row r="60" ht="12.75" customHeight="1">
-      <c r="A60" s="50"/>
-      <c r="B60" s="50"/>
-      <c r="C60" s="50"/>
-      <c r="D60" s="170"/>
-      <c r="E60" s="50"/>
-      <c r="F60" s="50"/>
-      <c r="G60" s="171"/>
-      <c r="H60" s="171"/>
-      <c r="I60" s="171"/>
-      <c r="J60" s="50"/>
+    <row r="60" ht="93.75" customHeight="1">
+      <c r="A60" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v>[Manager-51]</v>
+      </c>
+      <c r="B60" s="160" t="s">
+        <v>491</v>
+      </c>
+      <c r="C60" s="168" t="s">
+        <v>492</v>
+      </c>
+      <c r="D60" s="168" t="s">
+        <v>493</v>
+      </c>
+      <c r="E60" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F60" s="161" t="s">
+        <v>494</v>
+      </c>
+      <c r="G60" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H60" s="163">
+        <v>44302.0</v>
+      </c>
+      <c r="I60" s="169" t="s">
+        <v>375</v>
+      </c>
+      <c r="J60" s="165"/>
       <c r="K60" s="86"/>
       <c r="L60" s="11"/>
       <c r="M60" s="11"/>
@@ -30246,17 +30843,37 @@
       <c r="Z60" s="11"/>
       <c r="AA60" s="155"/>
     </row>
-    <row r="61" ht="12.75" customHeight="1">
-      <c r="A61" s="50"/>
-      <c r="B61" s="50"/>
-      <c r="C61" s="50"/>
-      <c r="D61" s="170"/>
-      <c r="E61" s="50"/>
-      <c r="F61" s="50"/>
-      <c r="G61" s="171"/>
-      <c r="H61" s="171"/>
-      <c r="I61" s="171"/>
-      <c r="J61" s="50"/>
+    <row r="61" ht="101.25" customHeight="1">
+      <c r="A61" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v>[Manager-52]</v>
+      </c>
+      <c r="B61" s="160" t="s">
+        <v>495</v>
+      </c>
+      <c r="C61" s="168" t="s">
+        <v>483</v>
+      </c>
+      <c r="D61" s="161" t="s">
+        <v>496</v>
+      </c>
+      <c r="E61" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F61" s="161" t="s">
+        <v>482</v>
+      </c>
+      <c r="G61" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H61" s="163">
+        <v>44302.0</v>
+      </c>
+      <c r="I61" s="169" t="s">
+        <v>375</v>
+      </c>
+      <c r="J61" s="165"/>
       <c r="K61" s="86"/>
       <c r="L61" s="11"/>
       <c r="M61" s="11"/>
@@ -30275,17 +30892,37 @@
       <c r="Z61" s="11"/>
       <c r="AA61" s="155"/>
     </row>
-    <row r="62" ht="12.75" customHeight="1">
-      <c r="A62" s="50"/>
-      <c r="B62" s="50"/>
-      <c r="C62" s="50"/>
-      <c r="D62" s="170"/>
-      <c r="E62" s="50"/>
-      <c r="F62" s="50"/>
-      <c r="G62" s="171"/>
-      <c r="H62" s="171"/>
-      <c r="I62" s="171"/>
-      <c r="J62" s="50"/>
+    <row r="62" ht="79.5" customHeight="1">
+      <c r="A62" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v>[Manager-53]</v>
+      </c>
+      <c r="B62" s="160" t="s">
+        <v>495</v>
+      </c>
+      <c r="C62" s="168" t="s">
+        <v>497</v>
+      </c>
+      <c r="D62" s="161" t="s">
+        <v>498</v>
+      </c>
+      <c r="E62" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F62" s="161" t="s">
+        <v>482</v>
+      </c>
+      <c r="G62" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H62" s="163">
+        <v>44302.0</v>
+      </c>
+      <c r="I62" s="169" t="s">
+        <v>375</v>
+      </c>
+      <c r="J62" s="165"/>
       <c r="K62" s="86"/>
       <c r="L62" s="11"/>
       <c r="M62" s="11"/>
@@ -30304,17 +30941,37 @@
       <c r="Z62" s="11"/>
       <c r="AA62" s="155"/>
     </row>
-    <row r="63" ht="12.75" customHeight="1">
-      <c r="A63" s="50"/>
-      <c r="B63" s="50"/>
-      <c r="C63" s="50"/>
-      <c r="D63" s="170"/>
-      <c r="E63" s="50"/>
-      <c r="F63" s="50"/>
-      <c r="G63" s="171"/>
-      <c r="H63" s="171"/>
-      <c r="I63" s="171"/>
-      <c r="J63" s="50"/>
+    <row r="63" ht="93.75" customHeight="1">
+      <c r="A63" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v>[Manager-54]</v>
+      </c>
+      <c r="B63" s="160" t="s">
+        <v>495</v>
+      </c>
+      <c r="C63" s="168" t="s">
+        <v>499</v>
+      </c>
+      <c r="D63" s="161" t="s">
+        <v>500</v>
+      </c>
+      <c r="E63" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F63" s="161" t="s">
+        <v>494</v>
+      </c>
+      <c r="G63" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H63" s="163">
+        <v>44302.0</v>
+      </c>
+      <c r="I63" s="169" t="s">
+        <v>375</v>
+      </c>
+      <c r="J63" s="165"/>
       <c r="K63" s="86"/>
       <c r="L63" s="11"/>
       <c r="M63" s="11"/>
@@ -30333,17 +30990,37 @@
       <c r="Z63" s="11"/>
       <c r="AA63" s="155"/>
     </row>
-    <row r="64" ht="12.75" customHeight="1">
-      <c r="A64" s="50"/>
-      <c r="B64" s="50"/>
-      <c r="C64" s="50"/>
-      <c r="D64" s="170"/>
-      <c r="E64" s="50"/>
-      <c r="F64" s="50"/>
-      <c r="G64" s="171"/>
-      <c r="H64" s="171"/>
-      <c r="I64" s="171"/>
-      <c r="J64" s="50"/>
+    <row r="64" ht="91.5" customHeight="1">
+      <c r="A64" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v>[Manager-55]</v>
+      </c>
+      <c r="B64" s="160" t="s">
+        <v>495</v>
+      </c>
+      <c r="C64" s="168" t="s">
+        <v>501</v>
+      </c>
+      <c r="D64" s="161" t="s">
+        <v>500</v>
+      </c>
+      <c r="E64" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F64" s="161" t="s">
+        <v>482</v>
+      </c>
+      <c r="G64" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H64" s="163">
+        <v>44302.0</v>
+      </c>
+      <c r="I64" s="169" t="s">
+        <v>375</v>
+      </c>
+      <c r="J64" s="165"/>
       <c r="K64" s="86"/>
       <c r="L64" s="11"/>
       <c r="M64" s="11"/>
@@ -30362,17 +31039,37 @@
       <c r="Z64" s="11"/>
       <c r="AA64" s="155"/>
     </row>
-    <row r="65" ht="12.75" customHeight="1">
-      <c r="A65" s="50"/>
-      <c r="B65" s="50"/>
-      <c r="C65" s="50"/>
-      <c r="D65" s="170"/>
-      <c r="E65" s="50"/>
-      <c r="F65" s="50"/>
-      <c r="G65" s="171"/>
-      <c r="H65" s="171"/>
-      <c r="I65" s="171"/>
-      <c r="J65" s="50"/>
+    <row r="65" ht="74.25" customHeight="1">
+      <c r="A65" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v>[Manager-56]</v>
+      </c>
+      <c r="B65" s="160" t="s">
+        <v>495</v>
+      </c>
+      <c r="C65" s="168" t="s">
+        <v>502</v>
+      </c>
+      <c r="D65" s="161" t="s">
+        <v>503</v>
+      </c>
+      <c r="E65" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F65" s="161" t="s">
+        <v>482</v>
+      </c>
+      <c r="G65" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H65" s="163">
+        <v>44302.0</v>
+      </c>
+      <c r="I65" s="169" t="s">
+        <v>375</v>
+      </c>
+      <c r="J65" s="165"/>
       <c r="K65" s="86"/>
       <c r="L65" s="11"/>
       <c r="M65" s="11"/>
@@ -30401,7 +31098,7 @@
       <c r="G66" s="171"/>
       <c r="H66" s="171"/>
       <c r="I66" s="171"/>
-      <c r="J66" s="50"/>
+      <c r="J66" s="171"/>
       <c r="K66" s="86"/>
       <c r="L66" s="11"/>
       <c r="M66" s="11"/>
@@ -30430,7 +31127,7 @@
       <c r="G67" s="171"/>
       <c r="H67" s="171"/>
       <c r="I67" s="171"/>
-      <c r="J67" s="50"/>
+      <c r="J67" s="171"/>
       <c r="K67" s="86"/>
       <c r="L67" s="11"/>
       <c r="M67" s="11"/>
@@ -30459,7 +31156,7 @@
       <c r="G68" s="171"/>
       <c r="H68" s="171"/>
       <c r="I68" s="171"/>
-      <c r="J68" s="50"/>
+      <c r="J68" s="171"/>
       <c r="K68" s="86"/>
       <c r="L68" s="11"/>
       <c r="M68" s="11"/>
@@ -30488,7 +31185,7 @@
       <c r="G69" s="171"/>
       <c r="H69" s="171"/>
       <c r="I69" s="171"/>
-      <c r="J69" s="50"/>
+      <c r="J69" s="171"/>
       <c r="K69" s="86"/>
       <c r="L69" s="11"/>
       <c r="M69" s="11"/>
@@ -30517,7 +31214,7 @@
       <c r="G70" s="171"/>
       <c r="H70" s="171"/>
       <c r="I70" s="171"/>
-      <c r="J70" s="50"/>
+      <c r="J70" s="171"/>
       <c r="K70" s="86"/>
       <c r="L70" s="11"/>
       <c r="M70" s="11"/>
@@ -30546,7 +31243,7 @@
       <c r="G71" s="171"/>
       <c r="H71" s="171"/>
       <c r="I71" s="171"/>
-      <c r="J71" s="50"/>
+      <c r="J71" s="171"/>
       <c r="K71" s="86"/>
       <c r="L71" s="11"/>
       <c r="M71" s="11"/>
@@ -30575,7 +31272,7 @@
       <c r="G72" s="171"/>
       <c r="H72" s="171"/>
       <c r="I72" s="171"/>
-      <c r="J72" s="50"/>
+      <c r="J72" s="171"/>
       <c r="K72" s="86"/>
       <c r="L72" s="11"/>
       <c r="M72" s="11"/>
@@ -30598,13 +31295,13 @@
       <c r="A73" s="50"/>
       <c r="B73" s="50"/>
       <c r="C73" s="50"/>
-      <c r="D73" s="170"/>
+      <c r="D73" s="50"/>
       <c r="E73" s="50"/>
       <c r="F73" s="50"/>
       <c r="G73" s="171"/>
       <c r="H73" s="171"/>
       <c r="I73" s="171"/>
-      <c r="J73" s="50"/>
+      <c r="J73" s="171"/>
       <c r="K73" s="86"/>
       <c r="L73" s="11"/>
       <c r="M73" s="11"/>
@@ -30627,13 +31324,13 @@
       <c r="A74" s="50"/>
       <c r="B74" s="50"/>
       <c r="C74" s="50"/>
-      <c r="D74" s="170"/>
+      <c r="D74" s="50"/>
       <c r="E74" s="50"/>
       <c r="F74" s="50"/>
       <c r="G74" s="171"/>
       <c r="H74" s="171"/>
       <c r="I74" s="171"/>
-      <c r="J74" s="50"/>
+      <c r="J74" s="171"/>
       <c r="K74" s="86"/>
       <c r="L74" s="11"/>
       <c r="M74" s="11"/>
@@ -30656,13 +31353,13 @@
       <c r="A75" s="50"/>
       <c r="B75" s="50"/>
       <c r="C75" s="50"/>
-      <c r="D75" s="170"/>
+      <c r="D75" s="50"/>
       <c r="E75" s="50"/>
       <c r="F75" s="50"/>
       <c r="G75" s="171"/>
       <c r="H75" s="171"/>
       <c r="I75" s="171"/>
-      <c r="J75" s="50"/>
+      <c r="J75" s="171"/>
       <c r="K75" s="86"/>
       <c r="L75" s="11"/>
       <c r="M75" s="11"/>
@@ -30685,13 +31382,13 @@
       <c r="A76" s="50"/>
       <c r="B76" s="50"/>
       <c r="C76" s="50"/>
-      <c r="D76" s="170"/>
+      <c r="D76" s="50"/>
       <c r="E76" s="50"/>
       <c r="F76" s="50"/>
       <c r="G76" s="171"/>
       <c r="H76" s="171"/>
       <c r="I76" s="171"/>
-      <c r="J76" s="50"/>
+      <c r="J76" s="171"/>
       <c r="K76" s="86"/>
       <c r="L76" s="11"/>
       <c r="M76" s="11"/>
@@ -30720,7 +31417,7 @@
       <c r="G77" s="171"/>
       <c r="H77" s="171"/>
       <c r="I77" s="171"/>
-      <c r="J77" s="50"/>
+      <c r="J77" s="171"/>
       <c r="K77" s="86"/>
       <c r="L77" s="11"/>
       <c r="M77" s="11"/>
@@ -30749,7 +31446,7 @@
       <c r="G78" s="171"/>
       <c r="H78" s="171"/>
       <c r="I78" s="171"/>
-      <c r="J78" s="50"/>
+      <c r="J78" s="171"/>
       <c r="K78" s="86"/>
       <c r="L78" s="11"/>
       <c r="M78" s="11"/>
@@ -30778,7 +31475,7 @@
       <c r="G79" s="171"/>
       <c r="H79" s="171"/>
       <c r="I79" s="171"/>
-      <c r="J79" s="50"/>
+      <c r="J79" s="171"/>
       <c r="K79" s="86"/>
       <c r="L79" s="11"/>
       <c r="M79" s="11"/>
@@ -30807,7 +31504,7 @@
       <c r="G80" s="171"/>
       <c r="H80" s="171"/>
       <c r="I80" s="171"/>
-      <c r="J80" s="50"/>
+      <c r="J80" s="171"/>
       <c r="K80" s="86"/>
       <c r="L80" s="11"/>
       <c r="M80" s="11"/>
@@ -30836,7 +31533,7 @@
       <c r="G81" s="171"/>
       <c r="H81" s="171"/>
       <c r="I81" s="171"/>
-      <c r="J81" s="50"/>
+      <c r="J81" s="171"/>
       <c r="K81" s="86"/>
       <c r="L81" s="11"/>
       <c r="M81" s="11"/>
@@ -30865,7 +31562,7 @@
       <c r="G82" s="171"/>
       <c r="H82" s="171"/>
       <c r="I82" s="171"/>
-      <c r="J82" s="50"/>
+      <c r="J82" s="171"/>
       <c r="K82" s="86"/>
       <c r="L82" s="11"/>
       <c r="M82" s="11"/>
@@ -30892,9 +31589,9 @@
       <c r="E83" s="50"/>
       <c r="F83" s="50"/>
       <c r="G83" s="171"/>
-      <c r="H83" s="171"/>
-      <c r="I83" s="171"/>
-      <c r="J83" s="50"/>
+      <c r="H83" s="103"/>
+      <c r="I83" s="103"/>
+      <c r="J83" s="171"/>
       <c r="K83" s="86"/>
       <c r="L83" s="11"/>
       <c r="M83" s="11"/>
@@ -30921,9 +31618,9 @@
       <c r="E84" s="50"/>
       <c r="F84" s="50"/>
       <c r="G84" s="171"/>
-      <c r="H84" s="171"/>
-      <c r="I84" s="171"/>
-      <c r="J84" s="50"/>
+      <c r="H84" s="103"/>
+      <c r="I84" s="103"/>
+      <c r="J84" s="171"/>
       <c r="K84" s="86"/>
       <c r="L84" s="11"/>
       <c r="M84" s="11"/>
@@ -30950,9 +31647,9 @@
       <c r="E85" s="50"/>
       <c r="F85" s="50"/>
       <c r="G85" s="171"/>
-      <c r="H85" s="171"/>
-      <c r="I85" s="171"/>
-      <c r="J85" s="50"/>
+      <c r="H85" s="103"/>
+      <c r="I85" s="103"/>
+      <c r="J85" s="171"/>
       <c r="K85" s="86"/>
       <c r="L85" s="11"/>
       <c r="M85" s="11"/>
@@ -30979,9 +31676,9 @@
       <c r="E86" s="50"/>
       <c r="F86" s="50"/>
       <c r="G86" s="171"/>
-      <c r="H86" s="171"/>
-      <c r="I86" s="171"/>
-      <c r="J86" s="50"/>
+      <c r="H86" s="103"/>
+      <c r="I86" s="103"/>
+      <c r="J86" s="171"/>
       <c r="K86" s="86"/>
       <c r="L86" s="11"/>
       <c r="M86" s="11"/>
@@ -31268,9 +31965,9 @@
       <c r="D96" s="50"/>
       <c r="E96" s="50"/>
       <c r="F96" s="50"/>
-      <c r="G96" s="171"/>
-      <c r="H96" s="103"/>
-      <c r="I96" s="103"/>
+      <c r="G96" s="172"/>
+      <c r="H96" s="50"/>
+      <c r="I96" s="50"/>
       <c r="J96" s="50"/>
       <c r="K96" s="86"/>
       <c r="L96" s="11"/>
@@ -31297,9 +31994,9 @@
       <c r="D97" s="50"/>
       <c r="E97" s="50"/>
       <c r="F97" s="50"/>
-      <c r="G97" s="171"/>
-      <c r="H97" s="103"/>
-      <c r="I97" s="103"/>
+      <c r="G97" s="172"/>
+      <c r="H97" s="50"/>
+      <c r="I97" s="50"/>
       <c r="J97" s="50"/>
       <c r="K97" s="86"/>
       <c r="L97" s="11"/>
@@ -31326,9 +32023,9 @@
       <c r="D98" s="50"/>
       <c r="E98" s="50"/>
       <c r="F98" s="50"/>
-      <c r="G98" s="171"/>
-      <c r="H98" s="103"/>
-      <c r="I98" s="103"/>
+      <c r="G98" s="172"/>
+      <c r="H98" s="50"/>
+      <c r="I98" s="50"/>
       <c r="J98" s="50"/>
       <c r="K98" s="86"/>
       <c r="L98" s="11"/>
@@ -31355,9 +32052,9 @@
       <c r="D99" s="50"/>
       <c r="E99" s="50"/>
       <c r="F99" s="50"/>
-      <c r="G99" s="171"/>
-      <c r="H99" s="103"/>
-      <c r="I99" s="103"/>
+      <c r="G99" s="172"/>
+      <c r="H99" s="50"/>
+      <c r="I99" s="50"/>
       <c r="J99" s="50"/>
       <c r="K99" s="86"/>
       <c r="L99" s="11"/>
@@ -31523,16 +32220,16 @@
       <c r="AA104" s="155"/>
     </row>
     <row r="105" ht="12.75" customHeight="1">
-      <c r="A105" s="50"/>
-      <c r="B105" s="50"/>
-      <c r="C105" s="50"/>
-      <c r="D105" s="50"/>
-      <c r="E105" s="50"/>
-      <c r="F105" s="50"/>
-      <c r="G105" s="172"/>
-      <c r="H105" s="50"/>
-      <c r="I105" s="50"/>
-      <c r="J105" s="50"/>
+      <c r="A105" s="11"/>
+      <c r="B105" s="11"/>
+      <c r="C105" s="11"/>
+      <c r="D105" s="11"/>
+      <c r="E105" s="11"/>
+      <c r="F105" s="11"/>
+      <c r="G105" s="54"/>
+      <c r="H105" s="11"/>
+      <c r="I105" s="11"/>
+      <c r="J105" s="11"/>
       <c r="K105" s="86"/>
       <c r="L105" s="11"/>
       <c r="M105" s="11"/>
@@ -31552,16 +32249,16 @@
       <c r="AA105" s="155"/>
     </row>
     <row r="106" ht="12.75" customHeight="1">
-      <c r="A106" s="50"/>
-      <c r="B106" s="50"/>
-      <c r="C106" s="50"/>
-      <c r="D106" s="50"/>
-      <c r="E106" s="50"/>
-      <c r="F106" s="50"/>
-      <c r="G106" s="172"/>
-      <c r="H106" s="50"/>
-      <c r="I106" s="50"/>
-      <c r="J106" s="50"/>
+      <c r="A106" s="11"/>
+      <c r="B106" s="11"/>
+      <c r="C106" s="11"/>
+      <c r="D106" s="11"/>
+      <c r="E106" s="11"/>
+      <c r="F106" s="11"/>
+      <c r="G106" s="54"/>
+      <c r="H106" s="11"/>
+      <c r="I106" s="11"/>
+      <c r="J106" s="11"/>
       <c r="K106" s="86"/>
       <c r="L106" s="11"/>
       <c r="M106" s="11"/>
@@ -31581,16 +32278,16 @@
       <c r="AA106" s="155"/>
     </row>
     <row r="107" ht="12.75" customHeight="1">
-      <c r="A107" s="50"/>
-      <c r="B107" s="50"/>
-      <c r="C107" s="50"/>
-      <c r="D107" s="50"/>
-      <c r="E107" s="50"/>
-      <c r="F107" s="50"/>
-      <c r="G107" s="172"/>
-      <c r="H107" s="50"/>
-      <c r="I107" s="50"/>
-      <c r="J107" s="50"/>
+      <c r="A107" s="11"/>
+      <c r="B107" s="11"/>
+      <c r="C107" s="11"/>
+      <c r="D107" s="11"/>
+      <c r="E107" s="11"/>
+      <c r="F107" s="11"/>
+      <c r="G107" s="54"/>
+      <c r="H107" s="11"/>
+      <c r="I107" s="11"/>
+      <c r="J107" s="11"/>
       <c r="K107" s="86"/>
       <c r="L107" s="11"/>
       <c r="M107" s="11"/>
@@ -31610,16 +32307,16 @@
       <c r="AA107" s="155"/>
     </row>
     <row r="108" ht="12.75" customHeight="1">
-      <c r="A108" s="50"/>
-      <c r="B108" s="50"/>
-      <c r="C108" s="50"/>
-      <c r="D108" s="50"/>
-      <c r="E108" s="50"/>
-      <c r="F108" s="50"/>
-      <c r="G108" s="172"/>
-      <c r="H108" s="50"/>
-      <c r="I108" s="50"/>
-      <c r="J108" s="50"/>
+      <c r="A108" s="11"/>
+      <c r="B108" s="11"/>
+      <c r="C108" s="11"/>
+      <c r="D108" s="11"/>
+      <c r="E108" s="11"/>
+      <c r="F108" s="11"/>
+      <c r="G108" s="54"/>
+      <c r="H108" s="11"/>
+      <c r="I108" s="11"/>
+      <c r="J108" s="11"/>
       <c r="K108" s="86"/>
       <c r="L108" s="11"/>
       <c r="M108" s="11"/>
@@ -31790,7 +32487,7 @@
       <c r="D114" s="11"/>
       <c r="E114" s="11"/>
       <c r="F114" s="11"/>
-      <c r="G114" s="54"/>
+      <c r="G114" s="11"/>
       <c r="H114" s="11"/>
       <c r="I114" s="11"/>
       <c r="J114" s="11"/>
@@ -31819,7 +32516,7 @@
       <c r="D115" s="11"/>
       <c r="E115" s="11"/>
       <c r="F115" s="11"/>
-      <c r="G115" s="54"/>
+      <c r="G115" s="11"/>
       <c r="H115" s="11"/>
       <c r="I115" s="11"/>
       <c r="J115" s="11"/>
@@ -31848,7 +32545,7 @@
       <c r="D116" s="11"/>
       <c r="E116" s="11"/>
       <c r="F116" s="11"/>
-      <c r="G116" s="54"/>
+      <c r="G116" s="11"/>
       <c r="H116" s="11"/>
       <c r="I116" s="11"/>
       <c r="J116" s="11"/>
@@ -31877,7 +32574,7 @@
       <c r="D117" s="11"/>
       <c r="E117" s="11"/>
       <c r="F117" s="11"/>
-      <c r="G117" s="54"/>
+      <c r="G117" s="11"/>
       <c r="H117" s="11"/>
       <c r="I117" s="11"/>
       <c r="J117" s="11"/>
@@ -32885,122 +33582,10 @@
       <c r="Z151" s="11"/>
       <c r="AA151" s="155"/>
     </row>
-    <row r="152" ht="12.75" customHeight="1">
-      <c r="A152" s="11"/>
-      <c r="B152" s="11"/>
-      <c r="C152" s="11"/>
-      <c r="D152" s="11"/>
-      <c r="E152" s="11"/>
-      <c r="F152" s="11"/>
-      <c r="G152" s="11"/>
-      <c r="H152" s="11"/>
-      <c r="I152" s="11"/>
-      <c r="J152" s="11"/>
-      <c r="K152" s="86"/>
-      <c r="L152" s="11"/>
-      <c r="M152" s="11"/>
-      <c r="N152" s="11"/>
-      <c r="O152" s="11"/>
-      <c r="P152" s="11"/>
-      <c r="Q152" s="11"/>
-      <c r="R152" s="11"/>
-      <c r="S152" s="11"/>
-      <c r="T152" s="11"/>
-      <c r="U152" s="11"/>
-      <c r="V152" s="11"/>
-      <c r="W152" s="11"/>
-      <c r="X152" s="11"/>
-      <c r="Y152" s="11"/>
-      <c r="Z152" s="11"/>
-      <c r="AA152" s="155"/>
-    </row>
-    <row r="153" ht="12.75" customHeight="1">
-      <c r="A153" s="11"/>
-      <c r="B153" s="11"/>
-      <c r="C153" s="11"/>
-      <c r="D153" s="11"/>
-      <c r="E153" s="11"/>
-      <c r="F153" s="11"/>
-      <c r="G153" s="11"/>
-      <c r="H153" s="11"/>
-      <c r="I153" s="11"/>
-      <c r="J153" s="11"/>
-      <c r="K153" s="86"/>
-      <c r="L153" s="11"/>
-      <c r="M153" s="11"/>
-      <c r="N153" s="11"/>
-      <c r="O153" s="11"/>
-      <c r="P153" s="11"/>
-      <c r="Q153" s="11"/>
-      <c r="R153" s="11"/>
-      <c r="S153" s="11"/>
-      <c r="T153" s="11"/>
-      <c r="U153" s="11"/>
-      <c r="V153" s="11"/>
-      <c r="W153" s="11"/>
-      <c r="X153" s="11"/>
-      <c r="Y153" s="11"/>
-      <c r="Z153" s="11"/>
-      <c r="AA153" s="155"/>
-    </row>
-    <row r="154" ht="12.75" customHeight="1">
-      <c r="A154" s="11"/>
-      <c r="B154" s="11"/>
-      <c r="C154" s="11"/>
-      <c r="D154" s="11"/>
-      <c r="E154" s="11"/>
-      <c r="F154" s="11"/>
-      <c r="G154" s="11"/>
-      <c r="H154" s="11"/>
-      <c r="I154" s="11"/>
-      <c r="J154" s="11"/>
-      <c r="K154" s="86"/>
-      <c r="L154" s="11"/>
-      <c r="M154" s="11"/>
-      <c r="N154" s="11"/>
-      <c r="O154" s="11"/>
-      <c r="P154" s="11"/>
-      <c r="Q154" s="11"/>
-      <c r="R154" s="11"/>
-      <c r="S154" s="11"/>
-      <c r="T154" s="11"/>
-      <c r="U154" s="11"/>
-      <c r="V154" s="11"/>
-      <c r="W154" s="11"/>
-      <c r="X154" s="11"/>
-      <c r="Y154" s="11"/>
-      <c r="Z154" s="11"/>
-      <c r="AA154" s="155"/>
-    </row>
-    <row r="155" ht="12.75" customHeight="1">
-      <c r="A155" s="11"/>
-      <c r="B155" s="11"/>
-      <c r="C155" s="11"/>
-      <c r="D155" s="11"/>
-      <c r="E155" s="11"/>
-      <c r="F155" s="11"/>
-      <c r="G155" s="11"/>
-      <c r="H155" s="11"/>
-      <c r="I155" s="11"/>
-      <c r="J155" s="11"/>
-      <c r="K155" s="86"/>
-      <c r="L155" s="11"/>
-      <c r="M155" s="11"/>
-      <c r="N155" s="11"/>
-      <c r="O155" s="11"/>
-      <c r="P155" s="11"/>
-      <c r="Q155" s="11"/>
-      <c r="R155" s="11"/>
-      <c r="S155" s="11"/>
-      <c r="T155" s="11"/>
-      <c r="U155" s="11"/>
-      <c r="V155" s="11"/>
-      <c r="W155" s="11"/>
-      <c r="X155" s="11"/>
-      <c r="Y155" s="11"/>
-      <c r="Z155" s="11"/>
-      <c r="AA155" s="155"/>
-    </row>
+    <row r="152" ht="15.75" customHeight="1"/>
+    <row r="153" ht="15.75" customHeight="1"/>
+    <row r="154" ht="15.75" customHeight="1"/>
+    <row r="155" ht="15.75" customHeight="1"/>
     <row r="156" ht="15.75" customHeight="1"/>
     <row r="157" ht="15.75" customHeight="1"/>
     <row r="158" ht="15.75" customHeight="1"/>
@@ -33856,10 +34441,6 @@
     <row r="1008" ht="15.75" customHeight="1"/>
     <row r="1009" ht="15.75" customHeight="1"/>
     <row r="1010" ht="15.75" customHeight="1"/>
-    <row r="1011" ht="15.75" customHeight="1"/>
-    <row r="1012" ht="15.75" customHeight="1"/>
-    <row r="1013" ht="15.75" customHeight="1"/>
-    <row r="1014" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B2:E2"/>
@@ -33867,7 +34448,7 @@
     <mergeCell ref="B4:E4"/>
   </mergeCells>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G8:G50">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G8:G65">
       <formula1>$M$2:$M$5</formula1>
     </dataValidation>
   </dataValidations>
@@ -33904,7 +34485,7 @@
     <row r="1" ht="25.5" customHeight="1">
       <c r="A1" s="11"/>
       <c r="B1" s="173" t="s">
-        <v>449</v>
+        <v>504</v>
       </c>
       <c r="C1" s="174"/>
       <c r="D1" s="174"/>
@@ -34071,10 +34652,10 @@
     <row r="6" ht="21.75" customHeight="1">
       <c r="A6" s="175"/>
       <c r="B6" s="181" t="s">
-        <v>450</v>
+        <v>505</v>
       </c>
       <c r="C6" s="183" t="s">
-        <v>451</v>
+        <v>506</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -34190,7 +34771,7 @@
         <v>23</v>
       </c>
       <c r="C10" s="187" t="s">
-        <v>452</v>
+        <v>507</v>
       </c>
       <c r="D10" s="188" t="s">
         <v>83</v>
@@ -34205,7 +34786,7 @@
         <v>90</v>
       </c>
       <c r="H10" s="190" t="s">
-        <v>453</v>
+        <v>508</v>
       </c>
       <c r="I10" s="11"/>
       <c r="J10" s="11"/>
@@ -34374,7 +34955,7 @@
       <c r="A14" s="185"/>
       <c r="B14" s="196"/>
       <c r="C14" s="197" t="s">
-        <v>454</v>
+        <v>509</v>
       </c>
       <c r="D14" s="198">
         <f t="shared" ref="D14:H14" si="1">SUM(D9:D13)</f>
@@ -34447,7 +35028,7 @@
       <c r="A16" s="11"/>
       <c r="B16" s="11"/>
       <c r="C16" s="9" t="s">
-        <v>455</v>
+        <v>510</v>
       </c>
       <c r="D16" s="11"/>
       <c r="E16" s="203">
@@ -34455,7 +35036,7 @@
         <v>46.53465347</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>456</v>
+        <v>511</v>
       </c>
       <c r="G16" s="11"/>
       <c r="H16" s="132"/>
@@ -34482,7 +35063,7 @@
       <c r="A17" s="11"/>
       <c r="B17" s="11"/>
       <c r="C17" s="9" t="s">
-        <v>457</v>
+        <v>512</v>
       </c>
       <c r="D17" s="11"/>
       <c r="E17" s="203">
@@ -34490,7 +35071,7 @@
         <v>42.57425743</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>456</v>
+        <v>511</v>
       </c>
       <c r="G17" s="11"/>
       <c r="H17" s="132"/>

</xml_diff>

<commit_message>
HoangNH - Update test case manager
</commit_message>
<xml_diff>
--- a/3. Users/HoangNHHE130395/Testing/TestCase - Hoang.xlsx
+++ b/3. Users/HoangNHHE130395/Testing/TestCase - Hoang.xlsx
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1184" uniqueCount="550">
   <si>
     <t>SYSTEM TEST CASE</t>
   </si>
@@ -2224,6 +2224,186 @@
     <t>1. List of transaction in page 2 is displayed</t>
   </si>
   <si>
+    <t>Check paging user's list post</t>
+  </si>
+  <si>
+    <t>1. List of posts in page 1 is displayed
+2. Item '&lt;&lt; Previous'  is disabled
+3. Item 'Next &gt;&gt;' is enabled</t>
+  </si>
+  <si>
+    <t>1. List of posts in page 2 is displayed
+2. Item '&lt;&lt; Previous'  is enabled
+3. Item 'Next &gt;&gt;' is disabled</t>
+  </si>
+  <si>
+    <t>1. List of posts in page 1 is displayed
+2. "Previous" item is disabled</t>
+  </si>
+  <si>
+    <t>1. List of posts in page 2 is displayed</t>
+  </si>
+  <si>
+    <t>Function Manage Post</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+ 2. Click on 'Post' tab in the menu bar</t>
+  </si>
+  <si>
+    <t>1. Display text 'Search user' on the search box</t>
+  </si>
+  <si>
+    <t>[Manager-1]</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+ 2. Click on 'Post' tab in the menu bar
+ 3. Click on the search box 'Search user'</t>
+  </si>
+  <si>
+    <t>1. Display text 'Search user' on the search box 
+ 2. Border of the search box change to blue</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+ 2. Click on 'Post' tab in the menu bar
+ 3. Click on the search box 'Search user'
+ 4. Click out of the search box 'Search user'</t>
+  </si>
+  <si>
+    <t>1. Display text 'Search user' on the search box 
+ 2. Border of the search box change from blue to white</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+ 2. Click on 'Post' tab in the menu bar
+ 3. Click on the search box 'Search user'
+ 4. Input text 'a' on the search box</t>
+  </si>
+  <si>
+    <t>1. Display text 'a' on the search box 
+ 2. Border of the search box change to blue
+ 3. Display list of post which is posted by user contain character 'a'</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+ 2. Click on 'Post' tab in the menu bar
+ 3. Click on the search box 'Search user'
+ 4. Input text 'a' on the search box
+ 5. Input text 'a' on the search box</t>
+  </si>
+  <si>
+    <t>1. Display text 'a' on the search box 
+ 2. Border of the search box change to blue
+ 3. Display list of post which is posted by user contain character 'aa'</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+ 2. Click on 'Post' tab in the menu bar
+ 3. Click on the search box 'Search user'
+ 4. Input text 'a' on the search box
+ 5. Input text 'a' on the search box
+ 6. Press delete button on keyboard</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+ 2. Click on 'Post' tab in the menu bar
+ 3. Choose 'Content' from the drop down list
+ 4. Click on the search box 'Search user'
+ 5. Input text 'a' on the search box</t>
+  </si>
+  <si>
+    <t>1. Display text 'a' on the search box 
+ 2. Border of the search box change to blue
+ 3. Display list of post which have content contain character 'a'</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+ 2. Click on 'Post' tab in the menu bar
+ 3. Choose 'Content' from the drop down list
+ 4. Click on the search box 'Search user'
+ 5. Input text 'a' on the search box
+ 6. Input text 'a' on the search box</t>
+  </si>
+  <si>
+    <t>1. Display text 'a' on the search box 
+ 2. Border of the search box change to blue
+ 3. Display list of post which have content contain character 'aa'</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+ 2. Click on 'Post' tab in the menu bar
+ 3. Choose 'Content' from the drop down list
+ 4. Click on the search box 'Search user'
+ 5. Input text 'a' on the search box
+ 6. Input text 'a' on the search box
+ 7. Press delete button on keyboard</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+ 2. Click on 'Post' tab in the menu bar
+ 3. Choose 'Content' from the drop down list
+ 4. Click on the search box 'Search user'
+ 5. Input text 'a' on the search box
+ 6. Choose 'Posted By' from the drop down list</t>
+  </si>
+  <si>
+    <t>Check GUI list posts</t>
+  </si>
+  <si>
+    <t>1. Display User's history transaction by following: ID, Content, Image, Posted by, Date created, Status, Option
+ 2. The data of post is mapping wit the column name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Login into the web server
+ 2. Click on 'Post' tab in the menu bar
+ </t>
+  </si>
+  <si>
+    <t>1. Display button 'View detail' in column Option</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+ 2. Click on 'Post' tab in the menu bar
+ 3. Click on the 'edit' in column 'Option' of post have id = '97'</t>
+  </si>
+  <si>
+    <t>1. Navigate to page post detail of post have id = '97'</t>
+  </si>
+  <si>
+    <t>1. Post have id = '97'</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'Post' tab in the menu bar</t>
+  </si>
+  <si>
+    <t>Check paging list post</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'Post' tab in the menu bar
+3. Click on '2' on the paging</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'Post' tab in the menu bar
+3. Click on '2' on the paging
+4. Click on '1' on the paging</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'Post' tab in the menu bar
+3. Click on '2' on the paging
+4. Click on '&lt;&lt; Previous' on the paging</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'Post' tab in the menu bar
+3. Click on 'Next &gt;&gt;' on the paging</t>
+  </si>
+  <si>
     <t>TEST REPORT</t>
   </si>
   <si>
@@ -2260,7 +2440,7 @@
     <numFmt numFmtId="165" formatCode="d\-mmm\-yy"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="33">
     <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
@@ -2405,6 +2585,24 @@
       <sz val="11.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <color rgb="FF000000"/>
+      <name val="&quot;Times New Roman&quot;"/>
+    </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="&quot;Times New Roman&quot;"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="&quot;Times New Roman&quot;"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="&quot;Times New Roman&quot;"/>
     </font>
     <font>
       <sz val="10.0"/>
@@ -3084,7 +3282,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="204">
+  <cellXfs count="218">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -3519,17 +3717,59 @@
     <xf borderId="5" fillId="0" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
+    <xf borderId="11" fillId="6" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="11" fillId="6" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="12" fillId="6" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="12" fillId="6" fontId="27" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="13" fillId="6" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="13" fillId="2" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="13" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="13" fillId="2" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="13" fillId="2" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="13" fillId="2" fontId="28" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="13" fillId="0" fontId="30" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="13" fillId="2" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="13" fillId="2" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="13" fillId="2" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="13" fillId="0" fontId="30" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
     <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="13" fillId="2" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf borderId="13" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -3591,14 +3831,14 @@
     <xf borderId="57" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="58" fillId="3" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="58" fillId="3" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="21" fillId="3" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="21" fillId="3" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="21" fillId="3" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="59" fillId="3" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="59" fillId="3" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -3610,7 +3850,7 @@
     <xf borderId="1" fillId="2" fontId="1" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="28" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="2" fontId="32" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -28026,7 +28266,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="20.13"/>
-    <col customWidth="1" min="2" max="2" width="19.13"/>
+    <col customWidth="1" min="2" max="2" width="22.25"/>
     <col customWidth="1" min="3" max="3" width="39.75"/>
     <col customWidth="1" min="4" max="4" width="35.5"/>
     <col customWidth="1" min="5" max="5" width="13.5"/>
@@ -28367,7 +28607,7 @@
     </row>
     <row r="10" ht="52.5" customHeight="1">
       <c r="A10" s="160" t="str">
-        <f t="shared" ref="A10:A65" si="1">IF(OR(B10&lt;&gt;"",D10&lt;&gt;""),"["&amp;TEXT($B$2,"##")&amp;"-"&amp;TEXT(ROW()-9,"##")&amp;"]","")</f>
+        <f t="shared" ref="A10:A70" si="1">IF(OR(B10&lt;&gt;"",D10&lt;&gt;""),"["&amp;TEXT($B$2,"##")&amp;"-"&amp;TEXT(ROW()-9,"##")&amp;"]","")</f>
         <v>[Manager-1]</v>
       </c>
       <c r="B10" s="160" t="s">
@@ -28424,7 +28664,7 @@
         <v>378</v>
       </c>
       <c r="E11" s="160" t="str">
-        <f t="shared" ref="E11:E65" si="2">$A$10</f>
+        <f t="shared" ref="E11:E70" si="2">$A$10</f>
         <v>[Manager-1]</v>
       </c>
       <c r="F11" s="117"/>
@@ -29872,7 +30112,7 @@
       <c r="C41" s="167" t="s">
         <v>446</v>
       </c>
-      <c r="D41" s="168" t="s">
+      <c r="D41" s="167" t="s">
         <v>447</v>
       </c>
       <c r="E41" s="160" t="str">
@@ -29970,7 +30210,7 @@
       <c r="C43" s="167" t="s">
         <v>451</v>
       </c>
-      <c r="D43" s="168" t="s">
+      <c r="D43" s="167" t="s">
         <v>452</v>
       </c>
       <c r="E43" s="160" t="str">
@@ -30065,10 +30305,10 @@
       <c r="B45" s="160" t="s">
         <v>455</v>
       </c>
-      <c r="C45" s="168" t="s">
+      <c r="C45" s="167" t="s">
         <v>456</v>
       </c>
-      <c r="D45" s="168" t="s">
+      <c r="D45" s="167" t="s">
         <v>457</v>
       </c>
       <c r="E45" s="160" t="str">
@@ -30114,10 +30354,10 @@
       <c r="B46" s="160" t="s">
         <v>455</v>
       </c>
-      <c r="C46" s="168" t="s">
+      <c r="C46" s="167" t="s">
         <v>458</v>
       </c>
-      <c r="D46" s="168" t="s">
+      <c r="D46" s="167" t="s">
         <v>459</v>
       </c>
       <c r="E46" s="160" t="str">
@@ -30163,10 +30403,10 @@
       <c r="B47" s="160" t="s">
         <v>460</v>
       </c>
-      <c r="C47" s="168" t="s">
+      <c r="C47" s="167" t="s">
         <v>461</v>
       </c>
-      <c r="D47" s="168" t="s">
+      <c r="D47" s="167" t="s">
         <v>457</v>
       </c>
       <c r="E47" s="160" t="str">
@@ -30182,7 +30422,7 @@
       <c r="H47" s="163">
         <v>44302.0</v>
       </c>
-      <c r="I47" s="169" t="s">
+      <c r="I47" s="166" t="s">
         <v>375</v>
       </c>
       <c r="J47" s="165"/>
@@ -30212,10 +30452,10 @@
       <c r="B48" s="160" t="s">
         <v>460</v>
       </c>
-      <c r="C48" s="168" t="s">
+      <c r="C48" s="167" t="s">
         <v>462</v>
       </c>
-      <c r="D48" s="168" t="s">
+      <c r="D48" s="167" t="s">
         <v>463</v>
       </c>
       <c r="E48" s="160" t="str">
@@ -30231,7 +30471,7 @@
       <c r="H48" s="163">
         <v>44302.0</v>
       </c>
-      <c r="I48" s="169" t="s">
+      <c r="I48" s="166" t="s">
         <v>375</v>
       </c>
       <c r="J48" s="165"/>
@@ -30261,10 +30501,10 @@
       <c r="B49" s="160" t="s">
         <v>460</v>
       </c>
-      <c r="C49" s="168" t="s">
+      <c r="C49" s="167" t="s">
         <v>465</v>
       </c>
-      <c r="D49" s="168" t="s">
+      <c r="D49" s="167" t="s">
         <v>466</v>
       </c>
       <c r="E49" s="160" t="str">
@@ -30280,7 +30520,7 @@
       <c r="H49" s="163">
         <v>44302.0</v>
       </c>
-      <c r="I49" s="169" t="s">
+      <c r="I49" s="166" t="s">
         <v>375</v>
       </c>
       <c r="J49" s="165"/>
@@ -30310,10 +30550,10 @@
       <c r="B50" s="160" t="s">
         <v>460</v>
       </c>
-      <c r="C50" s="168" t="s">
+      <c r="C50" s="167" t="s">
         <v>468</v>
       </c>
-      <c r="D50" s="168" t="s">
+      <c r="D50" s="167" t="s">
         <v>469</v>
       </c>
       <c r="E50" s="160" t="str">
@@ -30329,7 +30569,7 @@
       <c r="H50" s="163">
         <v>44302.0</v>
       </c>
-      <c r="I50" s="169" t="s">
+      <c r="I50" s="166" t="s">
         <v>375</v>
       </c>
       <c r="J50" s="165"/>
@@ -30359,10 +30599,10 @@
       <c r="B51" s="160" t="s">
         <v>460</v>
       </c>
-      <c r="C51" s="168" t="s">
+      <c r="C51" s="167" t="s">
         <v>471</v>
       </c>
-      <c r="D51" s="168" t="s">
+      <c r="D51" s="167" t="s">
         <v>469</v>
       </c>
       <c r="E51" s="160" t="str">
@@ -30378,7 +30618,7 @@
       <c r="H51" s="163">
         <v>44302.0</v>
       </c>
-      <c r="I51" s="169" t="s">
+      <c r="I51" s="166" t="s">
         <v>375</v>
       </c>
       <c r="J51" s="165"/>
@@ -30408,10 +30648,10 @@
       <c r="B52" s="160" t="s">
         <v>460</v>
       </c>
-      <c r="C52" s="168" t="s">
+      <c r="C52" s="167" t="s">
         <v>473</v>
       </c>
-      <c r="D52" s="168" t="s">
+      <c r="D52" s="167" t="s">
         <v>474</v>
       </c>
       <c r="E52" s="160" t="str">
@@ -30427,7 +30667,7 @@
       <c r="H52" s="163">
         <v>44302.0</v>
       </c>
-      <c r="I52" s="169" t="s">
+      <c r="I52" s="166" t="s">
         <v>375</v>
       </c>
       <c r="J52" s="165"/>
@@ -30457,10 +30697,10 @@
       <c r="B53" s="160" t="s">
         <v>460</v>
       </c>
-      <c r="C53" s="168" t="s">
+      <c r="C53" s="167" t="s">
         <v>476</v>
       </c>
-      <c r="D53" s="168" t="s">
+      <c r="D53" s="167" t="s">
         <v>477</v>
       </c>
       <c r="E53" s="160" t="str">
@@ -30476,7 +30716,7 @@
       <c r="H53" s="163">
         <v>44302.0</v>
       </c>
-      <c r="I53" s="169" t="s">
+      <c r="I53" s="166" t="s">
         <v>375</v>
       </c>
       <c r="J53" s="165"/>
@@ -30506,10 +30746,10 @@
       <c r="B54" s="160" t="s">
         <v>460</v>
       </c>
-      <c r="C54" s="168" t="s">
+      <c r="C54" s="167" t="s">
         <v>478</v>
       </c>
-      <c r="D54" s="168" t="s">
+      <c r="D54" s="167" t="s">
         <v>479</v>
       </c>
       <c r="E54" s="160" t="str">
@@ -30525,7 +30765,7 @@
       <c r="H54" s="163">
         <v>44302.0</v>
       </c>
-      <c r="I54" s="169" t="s">
+      <c r="I54" s="166" t="s">
         <v>375</v>
       </c>
       <c r="J54" s="165"/>
@@ -30555,10 +30795,10 @@
       <c r="B55" s="160" t="s">
         <v>480</v>
       </c>
-      <c r="C55" s="168" t="s">
+      <c r="C55" s="167" t="s">
         <v>438</v>
       </c>
-      <c r="D55" s="168" t="s">
+      <c r="D55" s="167" t="s">
         <v>481</v>
       </c>
       <c r="E55" s="160" t="str">
@@ -30574,7 +30814,7 @@
       <c r="H55" s="163">
         <v>44302.0</v>
       </c>
-      <c r="I55" s="169" t="s">
+      <c r="I55" s="166" t="s">
         <v>375</v>
       </c>
       <c r="J55" s="165"/>
@@ -30604,10 +30844,10 @@
       <c r="B56" s="160" t="s">
         <v>480</v>
       </c>
-      <c r="C56" s="168" t="s">
+      <c r="C56" s="167" t="s">
         <v>483</v>
       </c>
-      <c r="D56" s="168" t="s">
+      <c r="D56" s="167" t="s">
         <v>484</v>
       </c>
       <c r="E56" s="160" t="str">
@@ -30623,7 +30863,7 @@
       <c r="H56" s="163">
         <v>44302.0</v>
       </c>
-      <c r="I56" s="169" t="s">
+      <c r="I56" s="166" t="s">
         <v>375</v>
       </c>
       <c r="J56" s="165"/>
@@ -30653,10 +30893,10 @@
       <c r="B57" s="160" t="s">
         <v>485</v>
       </c>
-      <c r="C57" s="168" t="s">
+      <c r="C57" s="167" t="s">
         <v>438</v>
       </c>
-      <c r="D57" s="168" t="s">
+      <c r="D57" s="167" t="s">
         <v>486</v>
       </c>
       <c r="E57" s="160" t="str">
@@ -30672,7 +30912,7 @@
       <c r="H57" s="163">
         <v>44302.0</v>
       </c>
-      <c r="I57" s="169" t="s">
+      <c r="I57" s="166" t="s">
         <v>375</v>
       </c>
       <c r="J57" s="165"/>
@@ -30702,10 +30942,10 @@
       <c r="B58" s="160" t="s">
         <v>485</v>
       </c>
-      <c r="C58" s="168" t="s">
+      <c r="C58" s="167" t="s">
         <v>483</v>
       </c>
-      <c r="D58" s="168" t="s">
+      <c r="D58" s="167" t="s">
         <v>487</v>
       </c>
       <c r="E58" s="160" t="str">
@@ -30721,7 +30961,7 @@
       <c r="H58" s="163">
         <v>44302.0</v>
       </c>
-      <c r="I58" s="169" t="s">
+      <c r="I58" s="166" t="s">
         <v>375</v>
       </c>
       <c r="J58" s="165"/>
@@ -30751,10 +30991,10 @@
       <c r="B59" s="160" t="s">
         <v>488</v>
       </c>
-      <c r="C59" s="168" t="s">
+      <c r="C59" s="167" t="s">
         <v>483</v>
       </c>
-      <c r="D59" s="168" t="s">
+      <c r="D59" s="167" t="s">
         <v>489</v>
       </c>
       <c r="E59" s="160" t="str">
@@ -30770,7 +31010,7 @@
       <c r="H59" s="163">
         <v>44302.0</v>
       </c>
-      <c r="I59" s="169" t="s">
+      <c r="I59" s="166" t="s">
         <v>375</v>
       </c>
       <c r="J59" s="162" t="s">
@@ -30802,10 +31042,10 @@
       <c r="B60" s="160" t="s">
         <v>491</v>
       </c>
-      <c r="C60" s="168" t="s">
+      <c r="C60" s="167" t="s">
         <v>492</v>
       </c>
-      <c r="D60" s="168" t="s">
+      <c r="D60" s="167" t="s">
         <v>493</v>
       </c>
       <c r="E60" s="160" t="str">
@@ -30821,7 +31061,7 @@
       <c r="H60" s="163">
         <v>44302.0</v>
       </c>
-      <c r="I60" s="169" t="s">
+      <c r="I60" s="166" t="s">
         <v>375</v>
       </c>
       <c r="J60" s="165"/>
@@ -30851,7 +31091,7 @@
       <c r="B61" s="160" t="s">
         <v>495</v>
       </c>
-      <c r="C61" s="168" t="s">
+      <c r="C61" s="167" t="s">
         <v>483</v>
       </c>
       <c r="D61" s="161" t="s">
@@ -30870,7 +31110,7 @@
       <c r="H61" s="163">
         <v>44302.0</v>
       </c>
-      <c r="I61" s="169" t="s">
+      <c r="I61" s="166" t="s">
         <v>375</v>
       </c>
       <c r="J61" s="165"/>
@@ -30900,7 +31140,7 @@
       <c r="B62" s="160" t="s">
         <v>495</v>
       </c>
-      <c r="C62" s="168" t="s">
+      <c r="C62" s="167" t="s">
         <v>497</v>
       </c>
       <c r="D62" s="161" t="s">
@@ -30919,7 +31159,7 @@
       <c r="H62" s="163">
         <v>44302.0</v>
       </c>
-      <c r="I62" s="169" t="s">
+      <c r="I62" s="166" t="s">
         <v>375</v>
       </c>
       <c r="J62" s="165"/>
@@ -30949,7 +31189,7 @@
       <c r="B63" s="160" t="s">
         <v>495</v>
       </c>
-      <c r="C63" s="168" t="s">
+      <c r="C63" s="167" t="s">
         <v>499</v>
       </c>
       <c r="D63" s="161" t="s">
@@ -30968,7 +31208,7 @@
       <c r="H63" s="163">
         <v>44302.0</v>
       </c>
-      <c r="I63" s="169" t="s">
+      <c r="I63" s="166" t="s">
         <v>375</v>
       </c>
       <c r="J63" s="165"/>
@@ -30998,7 +31238,7 @@
       <c r="B64" s="160" t="s">
         <v>495</v>
       </c>
-      <c r="C64" s="168" t="s">
+      <c r="C64" s="167" t="s">
         <v>501</v>
       </c>
       <c r="D64" s="161" t="s">
@@ -31017,7 +31257,7 @@
       <c r="H64" s="163">
         <v>44302.0</v>
       </c>
-      <c r="I64" s="169" t="s">
+      <c r="I64" s="166" t="s">
         <v>375</v>
       </c>
       <c r="J64" s="165"/>
@@ -31047,7 +31287,7 @@
       <c r="B65" s="160" t="s">
         <v>495</v>
       </c>
-      <c r="C65" s="168" t="s">
+      <c r="C65" s="167" t="s">
         <v>502</v>
       </c>
       <c r="D65" s="161" t="s">
@@ -31066,7 +31306,7 @@
       <c r="H65" s="163">
         <v>44302.0</v>
       </c>
-      <c r="I65" s="169" t="s">
+      <c r="I65" s="166" t="s">
         <v>375</v>
       </c>
       <c r="J65" s="165"/>
@@ -31088,17 +31328,37 @@
       <c r="Z65" s="11"/>
       <c r="AA65" s="155"/>
     </row>
-    <row r="66" ht="12.75" customHeight="1">
-      <c r="A66" s="50"/>
-      <c r="B66" s="50"/>
-      <c r="C66" s="50"/>
-      <c r="D66" s="170"/>
-      <c r="E66" s="50"/>
-      <c r="F66" s="50"/>
-      <c r="G66" s="171"/>
-      <c r="H66" s="171"/>
-      <c r="I66" s="171"/>
-      <c r="J66" s="171"/>
+    <row r="66" ht="66.75" customHeight="1">
+      <c r="A66" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v>[Manager-57]</v>
+      </c>
+      <c r="B66" s="160" t="s">
+        <v>504</v>
+      </c>
+      <c r="C66" s="167" t="s">
+        <v>483</v>
+      </c>
+      <c r="D66" s="161" t="s">
+        <v>505</v>
+      </c>
+      <c r="E66" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F66" s="161" t="s">
+        <v>482</v>
+      </c>
+      <c r="G66" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H66" s="163">
+        <v>44302.0</v>
+      </c>
+      <c r="I66" s="166" t="s">
+        <v>375</v>
+      </c>
+      <c r="J66" s="165"/>
       <c r="K66" s="86"/>
       <c r="L66" s="11"/>
       <c r="M66" s="11"/>
@@ -31117,17 +31377,37 @@
       <c r="Z66" s="11"/>
       <c r="AA66" s="155"/>
     </row>
-    <row r="67" ht="12.75" customHeight="1">
-      <c r="A67" s="50"/>
-      <c r="B67" s="50"/>
-      <c r="C67" s="50"/>
-      <c r="D67" s="170"/>
-      <c r="E67" s="50"/>
-      <c r="F67" s="50"/>
-      <c r="G67" s="171"/>
-      <c r="H67" s="171"/>
-      <c r="I67" s="171"/>
-      <c r="J67" s="171"/>
+    <row r="67" ht="78.75" customHeight="1">
+      <c r="A67" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v>[Manager-58]</v>
+      </c>
+      <c r="B67" s="160" t="s">
+        <v>504</v>
+      </c>
+      <c r="C67" s="167" t="s">
+        <v>497</v>
+      </c>
+      <c r="D67" s="161" t="s">
+        <v>506</v>
+      </c>
+      <c r="E67" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F67" s="161" t="s">
+        <v>482</v>
+      </c>
+      <c r="G67" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H67" s="163">
+        <v>44302.0</v>
+      </c>
+      <c r="I67" s="166" t="s">
+        <v>375</v>
+      </c>
+      <c r="J67" s="165"/>
       <c r="K67" s="86"/>
       <c r="L67" s="11"/>
       <c r="M67" s="11"/>
@@ -31146,17 +31426,37 @@
       <c r="Z67" s="11"/>
       <c r="AA67" s="155"/>
     </row>
-    <row r="68" ht="12.75" customHeight="1">
-      <c r="A68" s="50"/>
-      <c r="B68" s="50"/>
-      <c r="C68" s="50"/>
-      <c r="D68" s="170"/>
-      <c r="E68" s="50"/>
-      <c r="F68" s="50"/>
-      <c r="G68" s="171"/>
-      <c r="H68" s="171"/>
-      <c r="I68" s="171"/>
-      <c r="J68" s="171"/>
+    <row r="68" ht="89.25" customHeight="1">
+      <c r="A68" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v>[Manager-59]</v>
+      </c>
+      <c r="B68" s="160" t="s">
+        <v>504</v>
+      </c>
+      <c r="C68" s="167" t="s">
+        <v>499</v>
+      </c>
+      <c r="D68" s="161" t="s">
+        <v>507</v>
+      </c>
+      <c r="E68" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F68" s="161" t="s">
+        <v>494</v>
+      </c>
+      <c r="G68" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H68" s="163">
+        <v>44302.0</v>
+      </c>
+      <c r="I68" s="166" t="s">
+        <v>375</v>
+      </c>
+      <c r="J68" s="165"/>
       <c r="K68" s="86"/>
       <c r="L68" s="11"/>
       <c r="M68" s="11"/>
@@ -31175,17 +31475,37 @@
       <c r="Z68" s="11"/>
       <c r="AA68" s="155"/>
     </row>
-    <row r="69" ht="12.75" customHeight="1">
-      <c r="A69" s="50"/>
-      <c r="B69" s="50"/>
-      <c r="C69" s="50"/>
-      <c r="D69" s="170"/>
-      <c r="E69" s="50"/>
-      <c r="F69" s="50"/>
-      <c r="G69" s="171"/>
-      <c r="H69" s="171"/>
-      <c r="I69" s="171"/>
-      <c r="J69" s="171"/>
+    <row r="69" ht="84.75" customHeight="1">
+      <c r="A69" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v>[Manager-60]</v>
+      </c>
+      <c r="B69" s="160" t="s">
+        <v>504</v>
+      </c>
+      <c r="C69" s="167" t="s">
+        <v>501</v>
+      </c>
+      <c r="D69" s="161" t="s">
+        <v>507</v>
+      </c>
+      <c r="E69" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F69" s="161" t="s">
+        <v>482</v>
+      </c>
+      <c r="G69" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H69" s="163">
+        <v>44302.0</v>
+      </c>
+      <c r="I69" s="166" t="s">
+        <v>375</v>
+      </c>
+      <c r="J69" s="165"/>
       <c r="K69" s="86"/>
       <c r="L69" s="11"/>
       <c r="M69" s="11"/>
@@ -31204,17 +31524,37 @@
       <c r="Z69" s="11"/>
       <c r="AA69" s="155"/>
     </row>
-    <row r="70" ht="12.75" customHeight="1">
-      <c r="A70" s="50"/>
-      <c r="B70" s="50"/>
-      <c r="C70" s="50"/>
-      <c r="D70" s="170"/>
-      <c r="E70" s="50"/>
-      <c r="F70" s="50"/>
-      <c r="G70" s="171"/>
-      <c r="H70" s="171"/>
-      <c r="I70" s="171"/>
-      <c r="J70" s="171"/>
+    <row r="70" ht="76.5" customHeight="1">
+      <c r="A70" s="160" t="str">
+        <f t="shared" si="1"/>
+        <v>[Manager-61]</v>
+      </c>
+      <c r="B70" s="160" t="s">
+        <v>504</v>
+      </c>
+      <c r="C70" s="167" t="s">
+        <v>502</v>
+      </c>
+      <c r="D70" s="161" t="s">
+        <v>508</v>
+      </c>
+      <c r="E70" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F70" s="161" t="s">
+        <v>482</v>
+      </c>
+      <c r="G70" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H70" s="163">
+        <v>44302.0</v>
+      </c>
+      <c r="I70" s="166" t="s">
+        <v>375</v>
+      </c>
+      <c r="J70" s="165"/>
       <c r="K70" s="86"/>
       <c r="L70" s="11"/>
       <c r="M70" s="11"/>
@@ -31233,17 +31573,19 @@
       <c r="Z70" s="11"/>
       <c r="AA70" s="155"/>
     </row>
-    <row r="71" ht="12.75" customHeight="1">
-      <c r="A71" s="50"/>
-      <c r="B71" s="50"/>
-      <c r="C71" s="50"/>
+    <row r="71" ht="33.0" customHeight="1">
+      <c r="A71" s="168" t="s">
+        <v>509</v>
+      </c>
+      <c r="B71" s="169"/>
+      <c r="C71" s="170"/>
       <c r="D71" s="170"/>
-      <c r="E71" s="50"/>
-      <c r="F71" s="50"/>
-      <c r="G71" s="171"/>
+      <c r="E71" s="170"/>
+      <c r="F71" s="170"/>
+      <c r="G71" s="170"/>
       <c r="H71" s="171"/>
-      <c r="I71" s="171"/>
-      <c r="J71" s="171"/>
+      <c r="I71" s="170"/>
+      <c r="J71" s="172"/>
       <c r="K71" s="86"/>
       <c r="L71" s="11"/>
       <c r="M71" s="11"/>
@@ -31262,17 +31604,36 @@
       <c r="Z71" s="11"/>
       <c r="AA71" s="155"/>
     </row>
-    <row r="72" ht="12.75" customHeight="1">
-      <c r="A72" s="50"/>
-      <c r="B72" s="50"/>
-      <c r="C72" s="50"/>
-      <c r="D72" s="170"/>
-      <c r="E72" s="50"/>
-      <c r="F72" s="50"/>
-      <c r="G72" s="171"/>
-      <c r="H72" s="171"/>
-      <c r="I72" s="171"/>
-      <c r="J72" s="171"/>
+    <row r="72" ht="37.5" customHeight="1">
+      <c r="A72" s="160" t="str">
+        <f t="shared" ref="A72:A96" si="3">IF(OR(B72&lt;&gt;"",D72&lt;&gt;""),"["&amp;TEXT($B$2,"##")&amp;"-"&amp;TEXT(ROW()-9,"##")&amp;"]","")</f>
+        <v>[Manager-63]</v>
+      </c>
+      <c r="B72" s="173" t="s">
+        <v>386</v>
+      </c>
+      <c r="C72" s="174" t="s">
+        <v>510</v>
+      </c>
+      <c r="D72" s="174" t="s">
+        <v>511</v>
+      </c>
+      <c r="E72" s="173" t="s">
+        <v>512</v>
+      </c>
+      <c r="F72" s="175"/>
+      <c r="G72" s="176" t="s">
+        <v>83</v>
+      </c>
+      <c r="H72" s="177">
+        <v>44303.0</v>
+      </c>
+      <c r="I72" s="178" t="s">
+        <v>375</v>
+      </c>
+      <c r="J72" s="176" t="s">
+        <v>490</v>
+      </c>
       <c r="K72" s="86"/>
       <c r="L72" s="11"/>
       <c r="M72" s="11"/>
@@ -31291,17 +31652,34 @@
       <c r="Z72" s="11"/>
       <c r="AA72" s="155"/>
     </row>
-    <row r="73" ht="12.75" customHeight="1">
-      <c r="A73" s="50"/>
-      <c r="B73" s="50"/>
-      <c r="C73" s="50"/>
-      <c r="D73" s="50"/>
-      <c r="E73" s="50"/>
-      <c r="F73" s="50"/>
-      <c r="G73" s="171"/>
-      <c r="H73" s="171"/>
-      <c r="I73" s="171"/>
-      <c r="J73" s="171"/>
+    <row r="73" ht="51.75" customHeight="1">
+      <c r="A73" s="160" t="str">
+        <f t="shared" si="3"/>
+        <v>[Manager-64]</v>
+      </c>
+      <c r="B73" s="173" t="s">
+        <v>389</v>
+      </c>
+      <c r="C73" s="174" t="s">
+        <v>513</v>
+      </c>
+      <c r="D73" s="174" t="s">
+        <v>514</v>
+      </c>
+      <c r="E73" s="173" t="s">
+        <v>512</v>
+      </c>
+      <c r="F73" s="175"/>
+      <c r="G73" s="176" t="s">
+        <v>83</v>
+      </c>
+      <c r="H73" s="177">
+        <v>44303.0</v>
+      </c>
+      <c r="I73" s="178" t="s">
+        <v>375</v>
+      </c>
+      <c r="J73" s="179"/>
       <c r="K73" s="86"/>
       <c r="L73" s="11"/>
       <c r="M73" s="11"/>
@@ -31320,17 +31698,34 @@
       <c r="Z73" s="11"/>
       <c r="AA73" s="155"/>
     </row>
-    <row r="74" ht="12.75" customHeight="1">
-      <c r="A74" s="50"/>
-      <c r="B74" s="50"/>
-      <c r="C74" s="50"/>
-      <c r="D74" s="50"/>
-      <c r="E74" s="50"/>
-      <c r="F74" s="50"/>
-      <c r="G74" s="171"/>
-      <c r="H74" s="171"/>
-      <c r="I74" s="171"/>
-      <c r="J74" s="171"/>
+    <row r="74" ht="60.75" customHeight="1">
+      <c r="A74" s="160" t="str">
+        <f t="shared" si="3"/>
+        <v>[Manager-65]</v>
+      </c>
+      <c r="B74" s="173" t="s">
+        <v>392</v>
+      </c>
+      <c r="C74" s="174" t="s">
+        <v>515</v>
+      </c>
+      <c r="D74" s="174" t="s">
+        <v>516</v>
+      </c>
+      <c r="E74" s="173" t="s">
+        <v>512</v>
+      </c>
+      <c r="F74" s="180"/>
+      <c r="G74" s="176" t="s">
+        <v>83</v>
+      </c>
+      <c r="H74" s="177">
+        <v>44303.0</v>
+      </c>
+      <c r="I74" s="178" t="s">
+        <v>375</v>
+      </c>
+      <c r="J74" s="179"/>
       <c r="K74" s="86"/>
       <c r="L74" s="11"/>
       <c r="M74" s="11"/>
@@ -31349,17 +31744,36 @@
       <c r="Z74" s="11"/>
       <c r="AA74" s="155"/>
     </row>
-    <row r="75" ht="12.75" customHeight="1">
-      <c r="A75" s="50"/>
-      <c r="B75" s="50"/>
-      <c r="C75" s="50"/>
-      <c r="D75" s="50"/>
-      <c r="E75" s="50"/>
-      <c r="F75" s="50"/>
-      <c r="G75" s="171"/>
-      <c r="H75" s="171"/>
-      <c r="I75" s="171"/>
-      <c r="J75" s="171"/>
+    <row r="75" ht="68.25" customHeight="1">
+      <c r="A75" s="160" t="str">
+        <f t="shared" si="3"/>
+        <v>[Manager-66]</v>
+      </c>
+      <c r="B75" s="173" t="s">
+        <v>395</v>
+      </c>
+      <c r="C75" s="174" t="s">
+        <v>517</v>
+      </c>
+      <c r="D75" s="174" t="s">
+        <v>518</v>
+      </c>
+      <c r="E75" s="173" t="s">
+        <v>512</v>
+      </c>
+      <c r="F75" s="181" t="s">
+        <v>398</v>
+      </c>
+      <c r="G75" s="176" t="s">
+        <v>83</v>
+      </c>
+      <c r="H75" s="177">
+        <v>44303.0</v>
+      </c>
+      <c r="I75" s="178" t="s">
+        <v>375</v>
+      </c>
+      <c r="J75" s="179"/>
       <c r="K75" s="86"/>
       <c r="L75" s="11"/>
       <c r="M75" s="11"/>
@@ -31378,17 +31792,36 @@
       <c r="Z75" s="11"/>
       <c r="AA75" s="155"/>
     </row>
-    <row r="76" ht="12.75" customHeight="1">
-      <c r="A76" s="50"/>
-      <c r="B76" s="50"/>
-      <c r="C76" s="50"/>
-      <c r="D76" s="50"/>
-      <c r="E76" s="50"/>
-      <c r="F76" s="50"/>
-      <c r="G76" s="171"/>
-      <c r="H76" s="171"/>
-      <c r="I76" s="171"/>
-      <c r="J76" s="171"/>
+    <row r="76" ht="76.5" customHeight="1">
+      <c r="A76" s="160" t="str">
+        <f t="shared" si="3"/>
+        <v>[Manager-67]</v>
+      </c>
+      <c r="B76" s="173" t="s">
+        <v>395</v>
+      </c>
+      <c r="C76" s="174" t="s">
+        <v>519</v>
+      </c>
+      <c r="D76" s="174" t="s">
+        <v>520</v>
+      </c>
+      <c r="E76" s="173" t="s">
+        <v>512</v>
+      </c>
+      <c r="F76" s="181" t="s">
+        <v>401</v>
+      </c>
+      <c r="G76" s="176" t="s">
+        <v>83</v>
+      </c>
+      <c r="H76" s="177">
+        <v>44303.0</v>
+      </c>
+      <c r="I76" s="178" t="s">
+        <v>375</v>
+      </c>
+      <c r="J76" s="179"/>
       <c r="K76" s="86"/>
       <c r="L76" s="11"/>
       <c r="M76" s="11"/>
@@ -31407,17 +31840,36 @@
       <c r="Z76" s="11"/>
       <c r="AA76" s="155"/>
     </row>
-    <row r="77" ht="12.75" customHeight="1">
-      <c r="A77" s="50"/>
-      <c r="B77" s="50"/>
-      <c r="C77" s="50"/>
-      <c r="D77" s="50"/>
-      <c r="E77" s="50"/>
-      <c r="F77" s="50"/>
-      <c r="G77" s="171"/>
-      <c r="H77" s="171"/>
-      <c r="I77" s="171"/>
-      <c r="J77" s="171"/>
+    <row r="77" ht="97.5" customHeight="1">
+      <c r="A77" s="160" t="str">
+        <f t="shared" si="3"/>
+        <v>[Manager-68]</v>
+      </c>
+      <c r="B77" s="173" t="s">
+        <v>395</v>
+      </c>
+      <c r="C77" s="174" t="s">
+        <v>521</v>
+      </c>
+      <c r="D77" s="174" t="s">
+        <v>518</v>
+      </c>
+      <c r="E77" s="173" t="s">
+        <v>512</v>
+      </c>
+      <c r="F77" s="181" t="s">
+        <v>398</v>
+      </c>
+      <c r="G77" s="176" t="s">
+        <v>83</v>
+      </c>
+      <c r="H77" s="177">
+        <v>44303.0</v>
+      </c>
+      <c r="I77" s="178" t="s">
+        <v>375</v>
+      </c>
+      <c r="J77" s="179"/>
       <c r="K77" s="86"/>
       <c r="L77" s="11"/>
       <c r="M77" s="11"/>
@@ -31436,17 +31888,36 @@
       <c r="Z77" s="11"/>
       <c r="AA77" s="155"/>
     </row>
-    <row r="78" ht="12.75" customHeight="1">
-      <c r="A78" s="50"/>
-      <c r="B78" s="50"/>
-      <c r="C78" s="50"/>
-      <c r="D78" s="50"/>
-      <c r="E78" s="50"/>
-      <c r="F78" s="50"/>
-      <c r="G78" s="171"/>
-      <c r="H78" s="171"/>
-      <c r="I78" s="171"/>
-      <c r="J78" s="171"/>
+    <row r="78" ht="82.5" customHeight="1">
+      <c r="A78" s="160" t="str">
+        <f t="shared" si="3"/>
+        <v>[Manager-69]</v>
+      </c>
+      <c r="B78" s="173" t="s">
+        <v>395</v>
+      </c>
+      <c r="C78" s="174" t="s">
+        <v>522</v>
+      </c>
+      <c r="D78" s="174" t="s">
+        <v>523</v>
+      </c>
+      <c r="E78" s="173" t="s">
+        <v>512</v>
+      </c>
+      <c r="F78" s="181" t="s">
+        <v>398</v>
+      </c>
+      <c r="G78" s="176" t="s">
+        <v>83</v>
+      </c>
+      <c r="H78" s="177">
+        <v>44303.0</v>
+      </c>
+      <c r="I78" s="178" t="s">
+        <v>375</v>
+      </c>
+      <c r="J78" s="179"/>
       <c r="K78" s="86"/>
       <c r="L78" s="11"/>
       <c r="M78" s="11"/>
@@ -31465,17 +31936,36 @@
       <c r="Z78" s="11"/>
       <c r="AA78" s="155"/>
     </row>
-    <row r="79" ht="12.75" customHeight="1">
-      <c r="A79" s="50"/>
-      <c r="B79" s="50"/>
-      <c r="C79" s="50"/>
-      <c r="D79" s="50"/>
-      <c r="E79" s="50"/>
-      <c r="F79" s="50"/>
-      <c r="G79" s="171"/>
-      <c r="H79" s="171"/>
-      <c r="I79" s="171"/>
-      <c r="J79" s="171"/>
+    <row r="79" ht="93.0" customHeight="1">
+      <c r="A79" s="160" t="str">
+        <f t="shared" si="3"/>
+        <v>[Manager-70]</v>
+      </c>
+      <c r="B79" s="173" t="s">
+        <v>395</v>
+      </c>
+      <c r="C79" s="174" t="s">
+        <v>524</v>
+      </c>
+      <c r="D79" s="174" t="s">
+        <v>525</v>
+      </c>
+      <c r="E79" s="173" t="s">
+        <v>512</v>
+      </c>
+      <c r="F79" s="181" t="s">
+        <v>401</v>
+      </c>
+      <c r="G79" s="176" t="s">
+        <v>83</v>
+      </c>
+      <c r="H79" s="177">
+        <v>44303.0</v>
+      </c>
+      <c r="I79" s="178" t="s">
+        <v>375</v>
+      </c>
+      <c r="J79" s="179"/>
       <c r="K79" s="86"/>
       <c r="L79" s="11"/>
       <c r="M79" s="11"/>
@@ -31494,17 +31984,36 @@
       <c r="Z79" s="11"/>
       <c r="AA79" s="155"/>
     </row>
-    <row r="80" ht="12.75" customHeight="1">
-      <c r="A80" s="50"/>
-      <c r="B80" s="50"/>
-      <c r="C80" s="50"/>
-      <c r="D80" s="50"/>
-      <c r="E80" s="50"/>
-      <c r="F80" s="50"/>
-      <c r="G80" s="171"/>
-      <c r="H80" s="171"/>
-      <c r="I80" s="171"/>
-      <c r="J80" s="171"/>
+    <row r="80" ht="109.5" customHeight="1">
+      <c r="A80" s="160" t="str">
+        <f t="shared" si="3"/>
+        <v>[Manager-71]</v>
+      </c>
+      <c r="B80" s="173" t="s">
+        <v>395</v>
+      </c>
+      <c r="C80" s="174" t="s">
+        <v>526</v>
+      </c>
+      <c r="D80" s="174" t="s">
+        <v>523</v>
+      </c>
+      <c r="E80" s="173" t="s">
+        <v>512</v>
+      </c>
+      <c r="F80" s="181" t="s">
+        <v>398</v>
+      </c>
+      <c r="G80" s="176" t="s">
+        <v>83</v>
+      </c>
+      <c r="H80" s="177">
+        <v>44303.0</v>
+      </c>
+      <c r="I80" s="178" t="s">
+        <v>375</v>
+      </c>
+      <c r="J80" s="179"/>
       <c r="K80" s="86"/>
       <c r="L80" s="11"/>
       <c r="M80" s="11"/>
@@ -31523,17 +32032,36 @@
       <c r="Z80" s="11"/>
       <c r="AA80" s="155"/>
     </row>
-    <row r="81" ht="12.75" customHeight="1">
-      <c r="A81" s="50"/>
-      <c r="B81" s="50"/>
-      <c r="C81" s="50"/>
-      <c r="D81" s="50"/>
-      <c r="E81" s="50"/>
-      <c r="F81" s="50"/>
-      <c r="G81" s="171"/>
-      <c r="H81" s="171"/>
-      <c r="I81" s="171"/>
-      <c r="J81" s="171"/>
+    <row r="81" ht="92.25" customHeight="1">
+      <c r="A81" s="160" t="str">
+        <f t="shared" si="3"/>
+        <v>[Manager-72]</v>
+      </c>
+      <c r="B81" s="173" t="s">
+        <v>395</v>
+      </c>
+      <c r="C81" s="174" t="s">
+        <v>527</v>
+      </c>
+      <c r="D81" s="174" t="s">
+        <v>518</v>
+      </c>
+      <c r="E81" s="173" t="s">
+        <v>512</v>
+      </c>
+      <c r="F81" s="181" t="s">
+        <v>398</v>
+      </c>
+      <c r="G81" s="176" t="s">
+        <v>83</v>
+      </c>
+      <c r="H81" s="177">
+        <v>44303.0</v>
+      </c>
+      <c r="I81" s="178" t="s">
+        <v>375</v>
+      </c>
+      <c r="J81" s="179"/>
       <c r="K81" s="86"/>
       <c r="L81" s="11"/>
       <c r="M81" s="11"/>
@@ -31552,17 +32080,34 @@
       <c r="Z81" s="11"/>
       <c r="AA81" s="155"/>
     </row>
-    <row r="82" ht="12.75" customHeight="1">
-      <c r="A82" s="50"/>
-      <c r="B82" s="50"/>
-      <c r="C82" s="50"/>
-      <c r="D82" s="50"/>
-      <c r="E82" s="50"/>
-      <c r="F82" s="50"/>
-      <c r="G82" s="171"/>
-      <c r="H82" s="171"/>
-      <c r="I82" s="171"/>
-      <c r="J82" s="171"/>
+    <row r="82" ht="40.5" customHeight="1">
+      <c r="A82" s="160" t="str">
+        <f t="shared" si="3"/>
+        <v>[Manager-73]</v>
+      </c>
+      <c r="B82" s="173" t="s">
+        <v>528</v>
+      </c>
+      <c r="C82" s="182" t="s">
+        <v>510</v>
+      </c>
+      <c r="D82" s="182" t="s">
+        <v>529</v>
+      </c>
+      <c r="E82" s="173" t="s">
+        <v>512</v>
+      </c>
+      <c r="F82" s="180"/>
+      <c r="G82" s="176" t="s">
+        <v>83</v>
+      </c>
+      <c r="H82" s="177">
+        <v>44303.0</v>
+      </c>
+      <c r="I82" s="178" t="s">
+        <v>375</v>
+      </c>
+      <c r="J82" s="179"/>
       <c r="K82" s="86"/>
       <c r="L82" s="11"/>
       <c r="M82" s="11"/>
@@ -31581,17 +32126,34 @@
       <c r="Z82" s="11"/>
       <c r="AA82" s="155"/>
     </row>
-    <row r="83" ht="12.75" customHeight="1">
-      <c r="A83" s="50"/>
-      <c r="B83" s="50"/>
-      <c r="C83" s="50"/>
-      <c r="D83" s="50"/>
-      <c r="E83" s="50"/>
-      <c r="F83" s="50"/>
-      <c r="G83" s="171"/>
-      <c r="H83" s="103"/>
-      <c r="I83" s="103"/>
-      <c r="J83" s="171"/>
+    <row r="83" ht="60.75" customHeight="1">
+      <c r="A83" s="160" t="str">
+        <f t="shared" si="3"/>
+        <v>[Manager-74]</v>
+      </c>
+      <c r="B83" s="173" t="s">
+        <v>488</v>
+      </c>
+      <c r="C83" s="182" t="s">
+        <v>530</v>
+      </c>
+      <c r="D83" s="182" t="s">
+        <v>531</v>
+      </c>
+      <c r="E83" s="173" t="s">
+        <v>512</v>
+      </c>
+      <c r="F83" s="181"/>
+      <c r="G83" s="176" t="s">
+        <v>83</v>
+      </c>
+      <c r="H83" s="177">
+        <v>44303.0</v>
+      </c>
+      <c r="I83" s="178" t="s">
+        <v>375</v>
+      </c>
+      <c r="J83" s="179"/>
       <c r="K83" s="86"/>
       <c r="L83" s="11"/>
       <c r="M83" s="11"/>
@@ -31610,17 +32172,36 @@
       <c r="Z83" s="11"/>
       <c r="AA83" s="155"/>
     </row>
-    <row r="84" ht="12.75" customHeight="1">
-      <c r="A84" s="50"/>
-      <c r="B84" s="50"/>
-      <c r="C84" s="50"/>
-      <c r="D84" s="50"/>
-      <c r="E84" s="50"/>
-      <c r="F84" s="50"/>
-      <c r="G84" s="171"/>
-      <c r="H84" s="103"/>
-      <c r="I84" s="103"/>
-      <c r="J84" s="171"/>
+    <row r="84" ht="62.25" customHeight="1">
+      <c r="A84" s="160" t="str">
+        <f t="shared" si="3"/>
+        <v>[Manager-75]</v>
+      </c>
+      <c r="B84" s="173" t="s">
+        <v>491</v>
+      </c>
+      <c r="C84" s="182" t="s">
+        <v>532</v>
+      </c>
+      <c r="D84" s="182" t="s">
+        <v>533</v>
+      </c>
+      <c r="E84" s="173" t="s">
+        <v>512</v>
+      </c>
+      <c r="F84" s="181" t="s">
+        <v>534</v>
+      </c>
+      <c r="G84" s="176" t="s">
+        <v>83</v>
+      </c>
+      <c r="H84" s="177">
+        <v>44303.0</v>
+      </c>
+      <c r="I84" s="178" t="s">
+        <v>375</v>
+      </c>
+      <c r="J84" s="179"/>
       <c r="K84" s="86"/>
       <c r="L84" s="11"/>
       <c r="M84" s="11"/>
@@ -31639,17 +32220,35 @@
       <c r="Z84" s="11"/>
       <c r="AA84" s="155"/>
     </row>
-    <row r="85" ht="12.75" customHeight="1">
-      <c r="A85" s="50"/>
-      <c r="B85" s="50"/>
-      <c r="C85" s="50"/>
-      <c r="D85" s="50"/>
-      <c r="E85" s="50"/>
-      <c r="F85" s="50"/>
-      <c r="G85" s="171"/>
-      <c r="H85" s="103"/>
-      <c r="I85" s="103"/>
-      <c r="J85" s="171"/>
+    <row r="85" ht="51.75" customHeight="1">
+      <c r="A85" s="160" t="str">
+        <f t="shared" si="3"/>
+        <v>[Manager-76]</v>
+      </c>
+      <c r="B85" s="160" t="s">
+        <v>504</v>
+      </c>
+      <c r="C85" s="183" t="s">
+        <v>535</v>
+      </c>
+      <c r="D85" s="161" t="s">
+        <v>505</v>
+      </c>
+      <c r="E85" s="160" t="str">
+        <f t="shared" ref="E85:E89" si="4">$A$10</f>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F85" s="161"/>
+      <c r="G85" s="176" t="s">
+        <v>83</v>
+      </c>
+      <c r="H85" s="177">
+        <v>44303.0</v>
+      </c>
+      <c r="I85" s="178" t="s">
+        <v>375</v>
+      </c>
+      <c r="J85" s="179"/>
       <c r="K85" s="86"/>
       <c r="L85" s="11"/>
       <c r="M85" s="11"/>
@@ -31668,17 +32267,35 @@
       <c r="Z85" s="11"/>
       <c r="AA85" s="155"/>
     </row>
-    <row r="86" ht="12.75" customHeight="1">
-      <c r="A86" s="50"/>
-      <c r="B86" s="50"/>
-      <c r="C86" s="50"/>
-      <c r="D86" s="50"/>
-      <c r="E86" s="50"/>
-      <c r="F86" s="50"/>
-      <c r="G86" s="171"/>
-      <c r="H86" s="103"/>
-      <c r="I86" s="103"/>
-      <c r="J86" s="171"/>
+    <row r="86" ht="89.25" customHeight="1">
+      <c r="A86" s="160" t="str">
+        <f t="shared" si="3"/>
+        <v>[Manager-77]</v>
+      </c>
+      <c r="B86" s="160" t="s">
+        <v>536</v>
+      </c>
+      <c r="C86" s="183" t="s">
+        <v>537</v>
+      </c>
+      <c r="D86" s="161" t="s">
+        <v>506</v>
+      </c>
+      <c r="E86" s="160" t="str">
+        <f t="shared" si="4"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F86" s="161"/>
+      <c r="G86" s="176" t="s">
+        <v>83</v>
+      </c>
+      <c r="H86" s="177">
+        <v>44303.0</v>
+      </c>
+      <c r="I86" s="178" t="s">
+        <v>375</v>
+      </c>
+      <c r="J86" s="179"/>
       <c r="K86" s="86"/>
       <c r="L86" s="11"/>
       <c r="M86" s="11"/>
@@ -31697,17 +32314,35 @@
       <c r="Z86" s="11"/>
       <c r="AA86" s="155"/>
     </row>
-    <row r="87" ht="12.75" customHeight="1">
-      <c r="A87" s="50"/>
-      <c r="B87" s="50"/>
-      <c r="C87" s="50"/>
-      <c r="D87" s="50"/>
-      <c r="E87" s="50"/>
-      <c r="F87" s="50"/>
-      <c r="G87" s="171"/>
-      <c r="H87" s="103"/>
-      <c r="I87" s="103"/>
-      <c r="J87" s="50"/>
+    <row r="87" ht="63.0" customHeight="1">
+      <c r="A87" s="160" t="str">
+        <f t="shared" si="3"/>
+        <v>[Manager-78]</v>
+      </c>
+      <c r="B87" s="160" t="s">
+        <v>536</v>
+      </c>
+      <c r="C87" s="183" t="s">
+        <v>538</v>
+      </c>
+      <c r="D87" s="161" t="s">
+        <v>507</v>
+      </c>
+      <c r="E87" s="160" t="str">
+        <f t="shared" si="4"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F87" s="161"/>
+      <c r="G87" s="176" t="s">
+        <v>83</v>
+      </c>
+      <c r="H87" s="177">
+        <v>44303.0</v>
+      </c>
+      <c r="I87" s="178" t="s">
+        <v>375</v>
+      </c>
+      <c r="J87" s="179"/>
       <c r="K87" s="86"/>
       <c r="L87" s="11"/>
       <c r="M87" s="11"/>
@@ -31726,17 +32361,35 @@
       <c r="Z87" s="11"/>
       <c r="AA87" s="155"/>
     </row>
-    <row r="88" ht="12.75" customHeight="1">
-      <c r="A88" s="50"/>
-      <c r="B88" s="50"/>
-      <c r="C88" s="50"/>
-      <c r="D88" s="50"/>
-      <c r="E88" s="50"/>
-      <c r="F88" s="50"/>
-      <c r="G88" s="171"/>
-      <c r="H88" s="103"/>
-      <c r="I88" s="103"/>
-      <c r="J88" s="50"/>
+    <row r="88" ht="67.5" customHeight="1">
+      <c r="A88" s="160" t="str">
+        <f t="shared" si="3"/>
+        <v>[Manager-79]</v>
+      </c>
+      <c r="B88" s="160" t="s">
+        <v>536</v>
+      </c>
+      <c r="C88" s="183" t="s">
+        <v>539</v>
+      </c>
+      <c r="D88" s="161" t="s">
+        <v>507</v>
+      </c>
+      <c r="E88" s="160" t="str">
+        <f t="shared" si="4"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F88" s="161"/>
+      <c r="G88" s="176" t="s">
+        <v>83</v>
+      </c>
+      <c r="H88" s="177">
+        <v>44303.0</v>
+      </c>
+      <c r="I88" s="178" t="s">
+        <v>375</v>
+      </c>
+      <c r="J88" s="179"/>
       <c r="K88" s="86"/>
       <c r="L88" s="11"/>
       <c r="M88" s="11"/>
@@ -31755,17 +32408,35 @@
       <c r="Z88" s="11"/>
       <c r="AA88" s="155"/>
     </row>
-    <row r="89" ht="12.75" customHeight="1">
-      <c r="A89" s="50"/>
-      <c r="B89" s="50"/>
-      <c r="C89" s="50"/>
-      <c r="D89" s="50"/>
-      <c r="E89" s="50"/>
-      <c r="F89" s="50"/>
-      <c r="G89" s="171"/>
-      <c r="H89" s="103"/>
-      <c r="I89" s="103"/>
-      <c r="J89" s="50"/>
+    <row r="89" ht="47.25" customHeight="1">
+      <c r="A89" s="160" t="str">
+        <f t="shared" si="3"/>
+        <v>[Manager-80]</v>
+      </c>
+      <c r="B89" s="160" t="s">
+        <v>536</v>
+      </c>
+      <c r="C89" s="183" t="s">
+        <v>540</v>
+      </c>
+      <c r="D89" s="161" t="s">
+        <v>508</v>
+      </c>
+      <c r="E89" s="160" t="str">
+        <f t="shared" si="4"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F89" s="161"/>
+      <c r="G89" s="176" t="s">
+        <v>83</v>
+      </c>
+      <c r="H89" s="177">
+        <v>44303.0</v>
+      </c>
+      <c r="I89" s="178" t="s">
+        <v>375</v>
+      </c>
+      <c r="J89" s="179"/>
       <c r="K89" s="86"/>
       <c r="L89" s="11"/>
       <c r="M89" s="11"/>
@@ -31785,16 +32456,27 @@
       <c r="AA89" s="155"/>
     </row>
     <row r="90" ht="12.75" customHeight="1">
-      <c r="A90" s="50"/>
-      <c r="B90" s="50"/>
-      <c r="C90" s="50"/>
-      <c r="D90" s="50"/>
-      <c r="E90" s="50"/>
-      <c r="F90" s="50"/>
-      <c r="G90" s="171"/>
-      <c r="H90" s="103"/>
-      <c r="I90" s="103"/>
-      <c r="J90" s="50"/>
+      <c r="A90" s="160" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="B90" s="184"/>
+      <c r="C90" s="185"/>
+      <c r="D90" s="185"/>
+      <c r="E90" s="173" t="s">
+        <v>512</v>
+      </c>
+      <c r="F90" s="180"/>
+      <c r="G90" s="176" t="s">
+        <v>83</v>
+      </c>
+      <c r="H90" s="177">
+        <v>44303.0</v>
+      </c>
+      <c r="I90" s="178" t="s">
+        <v>375</v>
+      </c>
+      <c r="J90" s="179"/>
       <c r="K90" s="86"/>
       <c r="L90" s="11"/>
       <c r="M90" s="11"/>
@@ -31814,16 +32496,27 @@
       <c r="AA90" s="155"/>
     </row>
     <row r="91" ht="12.75" customHeight="1">
-      <c r="A91" s="50"/>
-      <c r="B91" s="50"/>
-      <c r="C91" s="50"/>
-      <c r="D91" s="50"/>
-      <c r="E91" s="50"/>
-      <c r="F91" s="50"/>
-      <c r="G91" s="171"/>
-      <c r="H91" s="103"/>
-      <c r="I91" s="103"/>
-      <c r="J91" s="50"/>
+      <c r="A91" s="160" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="B91" s="184"/>
+      <c r="C91" s="185"/>
+      <c r="D91" s="185"/>
+      <c r="E91" s="173" t="s">
+        <v>512</v>
+      </c>
+      <c r="F91" s="180"/>
+      <c r="G91" s="176" t="s">
+        <v>83</v>
+      </c>
+      <c r="H91" s="177">
+        <v>44303.0</v>
+      </c>
+      <c r="I91" s="178" t="s">
+        <v>375</v>
+      </c>
+      <c r="J91" s="179"/>
       <c r="K91" s="86"/>
       <c r="L91" s="11"/>
       <c r="M91" s="11"/>
@@ -31843,16 +32536,27 @@
       <c r="AA91" s="155"/>
     </row>
     <row r="92" ht="12.75" customHeight="1">
-      <c r="A92" s="50"/>
-      <c r="B92" s="50"/>
-      <c r="C92" s="50"/>
-      <c r="D92" s="50"/>
-      <c r="E92" s="50"/>
-      <c r="F92" s="50"/>
-      <c r="G92" s="171"/>
-      <c r="H92" s="103"/>
-      <c r="I92" s="103"/>
-      <c r="J92" s="50"/>
+      <c r="A92" s="160" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="B92" s="184"/>
+      <c r="C92" s="185"/>
+      <c r="D92" s="185"/>
+      <c r="E92" s="173" t="s">
+        <v>512</v>
+      </c>
+      <c r="F92" s="180"/>
+      <c r="G92" s="176" t="s">
+        <v>83</v>
+      </c>
+      <c r="H92" s="177">
+        <v>44303.0</v>
+      </c>
+      <c r="I92" s="178" t="s">
+        <v>375</v>
+      </c>
+      <c r="J92" s="179"/>
       <c r="K92" s="86"/>
       <c r="L92" s="11"/>
       <c r="M92" s="11"/>
@@ -31872,16 +32576,27 @@
       <c r="AA92" s="155"/>
     </row>
     <row r="93" ht="12.75" customHeight="1">
-      <c r="A93" s="50"/>
-      <c r="B93" s="50"/>
-      <c r="C93" s="50"/>
-      <c r="D93" s="50"/>
-      <c r="E93" s="50"/>
-      <c r="F93" s="50"/>
-      <c r="G93" s="171"/>
-      <c r="H93" s="103"/>
-      <c r="I93" s="103"/>
-      <c r="J93" s="50"/>
+      <c r="A93" s="160" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="B93" s="184"/>
+      <c r="C93" s="185"/>
+      <c r="D93" s="185"/>
+      <c r="E93" s="173" t="s">
+        <v>512</v>
+      </c>
+      <c r="F93" s="180"/>
+      <c r="G93" s="176" t="s">
+        <v>83</v>
+      </c>
+      <c r="H93" s="177">
+        <v>44303.0</v>
+      </c>
+      <c r="I93" s="178" t="s">
+        <v>375</v>
+      </c>
+      <c r="J93" s="179"/>
       <c r="K93" s="86"/>
       <c r="L93" s="11"/>
       <c r="M93" s="11"/>
@@ -31901,16 +32616,27 @@
       <c r="AA93" s="155"/>
     </row>
     <row r="94" ht="12.75" customHeight="1">
-      <c r="A94" s="50"/>
-      <c r="B94" s="50"/>
-      <c r="C94" s="50"/>
-      <c r="D94" s="50"/>
-      <c r="E94" s="50"/>
-      <c r="F94" s="50"/>
-      <c r="G94" s="171"/>
-      <c r="H94" s="103"/>
-      <c r="I94" s="103"/>
-      <c r="J94" s="50"/>
+      <c r="A94" s="160" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="B94" s="184"/>
+      <c r="C94" s="185"/>
+      <c r="D94" s="185"/>
+      <c r="E94" s="173" t="s">
+        <v>512</v>
+      </c>
+      <c r="F94" s="180"/>
+      <c r="G94" s="176" t="s">
+        <v>83</v>
+      </c>
+      <c r="H94" s="177">
+        <v>44303.0</v>
+      </c>
+      <c r="I94" s="178" t="s">
+        <v>375</v>
+      </c>
+      <c r="J94" s="179"/>
       <c r="K94" s="86"/>
       <c r="L94" s="11"/>
       <c r="M94" s="11"/>
@@ -31930,16 +32656,27 @@
       <c r="AA94" s="155"/>
     </row>
     <row r="95" ht="12.75" customHeight="1">
-      <c r="A95" s="50"/>
-      <c r="B95" s="50"/>
-      <c r="C95" s="50"/>
-      <c r="D95" s="50"/>
-      <c r="E95" s="50"/>
-      <c r="F95" s="50"/>
-      <c r="G95" s="171"/>
-      <c r="H95" s="103"/>
-      <c r="I95" s="103"/>
-      <c r="J95" s="50"/>
+      <c r="A95" s="160" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="B95" s="184"/>
+      <c r="C95" s="185"/>
+      <c r="D95" s="185"/>
+      <c r="E95" s="173" t="s">
+        <v>512</v>
+      </c>
+      <c r="F95" s="180"/>
+      <c r="G95" s="176" t="s">
+        <v>83</v>
+      </c>
+      <c r="H95" s="177">
+        <v>44303.0</v>
+      </c>
+      <c r="I95" s="178" t="s">
+        <v>375</v>
+      </c>
+      <c r="J95" s="179"/>
       <c r="K95" s="86"/>
       <c r="L95" s="11"/>
       <c r="M95" s="11"/>
@@ -31959,16 +32696,27 @@
       <c r="AA95" s="155"/>
     </row>
     <row r="96" ht="12.75" customHeight="1">
-      <c r="A96" s="50"/>
-      <c r="B96" s="50"/>
-      <c r="C96" s="50"/>
-      <c r="D96" s="50"/>
-      <c r="E96" s="50"/>
-      <c r="F96" s="50"/>
-      <c r="G96" s="172"/>
-      <c r="H96" s="50"/>
-      <c r="I96" s="50"/>
-      <c r="J96" s="50"/>
+      <c r="A96" s="160" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="B96" s="184"/>
+      <c r="C96" s="185"/>
+      <c r="D96" s="185"/>
+      <c r="E96" s="173" t="s">
+        <v>512</v>
+      </c>
+      <c r="F96" s="180"/>
+      <c r="G96" s="176" t="s">
+        <v>83</v>
+      </c>
+      <c r="H96" s="177">
+        <v>44303.0</v>
+      </c>
+      <c r="I96" s="178" t="s">
+        <v>375</v>
+      </c>
+      <c r="J96" s="179"/>
       <c r="K96" s="86"/>
       <c r="L96" s="11"/>
       <c r="M96" s="11"/>
@@ -31994,7 +32742,7 @@
       <c r="D97" s="50"/>
       <c r="E97" s="50"/>
       <c r="F97" s="50"/>
-      <c r="G97" s="172"/>
+      <c r="G97" s="186"/>
       <c r="H97" s="50"/>
       <c r="I97" s="50"/>
       <c r="J97" s="50"/>
@@ -32023,7 +32771,7 @@
       <c r="D98" s="50"/>
       <c r="E98" s="50"/>
       <c r="F98" s="50"/>
-      <c r="G98" s="172"/>
+      <c r="G98" s="186"/>
       <c r="H98" s="50"/>
       <c r="I98" s="50"/>
       <c r="J98" s="50"/>
@@ -32052,7 +32800,7 @@
       <c r="D99" s="50"/>
       <c r="E99" s="50"/>
       <c r="F99" s="50"/>
-      <c r="G99" s="172"/>
+      <c r="G99" s="186"/>
       <c r="H99" s="50"/>
       <c r="I99" s="50"/>
       <c r="J99" s="50"/>
@@ -32081,7 +32829,7 @@
       <c r="D100" s="50"/>
       <c r="E100" s="50"/>
       <c r="F100" s="50"/>
-      <c r="G100" s="172"/>
+      <c r="G100" s="186"/>
       <c r="H100" s="50"/>
       <c r="I100" s="50"/>
       <c r="J100" s="50"/>
@@ -32110,7 +32858,7 @@
       <c r="D101" s="50"/>
       <c r="E101" s="50"/>
       <c r="F101" s="50"/>
-      <c r="G101" s="172"/>
+      <c r="G101" s="186"/>
       <c r="H101" s="50"/>
       <c r="I101" s="50"/>
       <c r="J101" s="50"/>
@@ -32139,7 +32887,7 @@
       <c r="D102" s="50"/>
       <c r="E102" s="50"/>
       <c r="F102" s="50"/>
-      <c r="G102" s="172"/>
+      <c r="G102" s="186"/>
       <c r="H102" s="50"/>
       <c r="I102" s="50"/>
       <c r="J102" s="50"/>
@@ -32168,7 +32916,7 @@
       <c r="D103" s="50"/>
       <c r="E103" s="50"/>
       <c r="F103" s="50"/>
-      <c r="G103" s="172"/>
+      <c r="G103" s="186"/>
       <c r="H103" s="50"/>
       <c r="I103" s="50"/>
       <c r="J103" s="50"/>
@@ -32197,7 +32945,7 @@
       <c r="D104" s="50"/>
       <c r="E104" s="50"/>
       <c r="F104" s="50"/>
-      <c r="G104" s="172"/>
+      <c r="G104" s="186"/>
       <c r="H104" s="50"/>
       <c r="I104" s="50"/>
       <c r="J104" s="50"/>
@@ -32220,16 +32968,16 @@
       <c r="AA104" s="155"/>
     </row>
     <row r="105" ht="12.75" customHeight="1">
-      <c r="A105" s="11"/>
-      <c r="B105" s="11"/>
-      <c r="C105" s="11"/>
-      <c r="D105" s="11"/>
-      <c r="E105" s="11"/>
-      <c r="F105" s="11"/>
-      <c r="G105" s="54"/>
-      <c r="H105" s="11"/>
-      <c r="I105" s="11"/>
-      <c r="J105" s="11"/>
+      <c r="A105" s="50"/>
+      <c r="B105" s="50"/>
+      <c r="C105" s="50"/>
+      <c r="D105" s="50"/>
+      <c r="E105" s="50"/>
+      <c r="F105" s="50"/>
+      <c r="G105" s="186"/>
+      <c r="H105" s="50"/>
+      <c r="I105" s="50"/>
+      <c r="J105" s="50"/>
       <c r="K105" s="86"/>
       <c r="L105" s="11"/>
       <c r="M105" s="11"/>
@@ -32249,16 +32997,16 @@
       <c r="AA105" s="155"/>
     </row>
     <row r="106" ht="12.75" customHeight="1">
-      <c r="A106" s="11"/>
-      <c r="B106" s="11"/>
-      <c r="C106" s="11"/>
-      <c r="D106" s="11"/>
-      <c r="E106" s="11"/>
-      <c r="F106" s="11"/>
-      <c r="G106" s="54"/>
-      <c r="H106" s="11"/>
-      <c r="I106" s="11"/>
-      <c r="J106" s="11"/>
+      <c r="A106" s="50"/>
+      <c r="B106" s="50"/>
+      <c r="C106" s="50"/>
+      <c r="D106" s="50"/>
+      <c r="E106" s="50"/>
+      <c r="F106" s="50"/>
+      <c r="G106" s="186"/>
+      <c r="H106" s="50"/>
+      <c r="I106" s="50"/>
+      <c r="J106" s="50"/>
       <c r="K106" s="86"/>
       <c r="L106" s="11"/>
       <c r="M106" s="11"/>
@@ -32278,16 +33026,16 @@
       <c r="AA106" s="155"/>
     </row>
     <row r="107" ht="12.75" customHeight="1">
-      <c r="A107" s="11"/>
-      <c r="B107" s="11"/>
-      <c r="C107" s="11"/>
-      <c r="D107" s="11"/>
-      <c r="E107" s="11"/>
-      <c r="F107" s="11"/>
-      <c r="G107" s="54"/>
-      <c r="H107" s="11"/>
-      <c r="I107" s="11"/>
-      <c r="J107" s="11"/>
+      <c r="A107" s="50"/>
+      <c r="B107" s="50"/>
+      <c r="C107" s="50"/>
+      <c r="D107" s="50"/>
+      <c r="E107" s="50"/>
+      <c r="F107" s="50"/>
+      <c r="G107" s="186"/>
+      <c r="H107" s="50"/>
+      <c r="I107" s="50"/>
+      <c r="J107" s="50"/>
       <c r="K107" s="86"/>
       <c r="L107" s="11"/>
       <c r="M107" s="11"/>
@@ -32307,16 +33055,16 @@
       <c r="AA107" s="155"/>
     </row>
     <row r="108" ht="12.75" customHeight="1">
-      <c r="A108" s="11"/>
-      <c r="B108" s="11"/>
-      <c r="C108" s="11"/>
-      <c r="D108" s="11"/>
-      <c r="E108" s="11"/>
-      <c r="F108" s="11"/>
-      <c r="G108" s="54"/>
-      <c r="H108" s="11"/>
-      <c r="I108" s="11"/>
-      <c r="J108" s="11"/>
+      <c r="A108" s="50"/>
+      <c r="B108" s="50"/>
+      <c r="C108" s="50"/>
+      <c r="D108" s="50"/>
+      <c r="E108" s="50"/>
+      <c r="F108" s="50"/>
+      <c r="G108" s="186"/>
+      <c r="H108" s="50"/>
+      <c r="I108" s="50"/>
+      <c r="J108" s="50"/>
       <c r="K108" s="86"/>
       <c r="L108" s="11"/>
       <c r="M108" s="11"/>
@@ -32336,16 +33084,16 @@
       <c r="AA108" s="155"/>
     </row>
     <row r="109" ht="12.75" customHeight="1">
-      <c r="A109" s="11"/>
-      <c r="B109" s="11"/>
-      <c r="C109" s="11"/>
-      <c r="D109" s="11"/>
-      <c r="E109" s="11"/>
-      <c r="F109" s="11"/>
-      <c r="G109" s="54"/>
-      <c r="H109" s="11"/>
-      <c r="I109" s="11"/>
-      <c r="J109" s="11"/>
+      <c r="A109" s="50"/>
+      <c r="B109" s="50"/>
+      <c r="C109" s="50"/>
+      <c r="D109" s="50"/>
+      <c r="E109" s="50"/>
+      <c r="F109" s="50"/>
+      <c r="G109" s="186"/>
+      <c r="H109" s="50"/>
+      <c r="I109" s="50"/>
+      <c r="J109" s="50"/>
       <c r="K109" s="86"/>
       <c r="L109" s="11"/>
       <c r="M109" s="11"/>
@@ -32365,16 +33113,16 @@
       <c r="AA109" s="155"/>
     </row>
     <row r="110" ht="12.75" customHeight="1">
-      <c r="A110" s="11"/>
-      <c r="B110" s="11"/>
-      <c r="C110" s="11"/>
-      <c r="D110" s="11"/>
-      <c r="E110" s="11"/>
-      <c r="F110" s="11"/>
-      <c r="G110" s="54"/>
-      <c r="H110" s="11"/>
-      <c r="I110" s="11"/>
-      <c r="J110" s="11"/>
+      <c r="A110" s="50"/>
+      <c r="B110" s="50"/>
+      <c r="C110" s="50"/>
+      <c r="D110" s="50"/>
+      <c r="E110" s="50"/>
+      <c r="F110" s="50"/>
+      <c r="G110" s="186"/>
+      <c r="H110" s="50"/>
+      <c r="I110" s="50"/>
+      <c r="J110" s="50"/>
       <c r="K110" s="86"/>
       <c r="L110" s="11"/>
       <c r="M110" s="11"/>
@@ -32394,16 +33142,16 @@
       <c r="AA110" s="155"/>
     </row>
     <row r="111" ht="12.75" customHeight="1">
-      <c r="A111" s="11"/>
-      <c r="B111" s="11"/>
-      <c r="C111" s="11"/>
-      <c r="D111" s="11"/>
-      <c r="E111" s="11"/>
-      <c r="F111" s="11"/>
-      <c r="G111" s="54"/>
-      <c r="H111" s="11"/>
-      <c r="I111" s="11"/>
-      <c r="J111" s="11"/>
+      <c r="A111" s="50"/>
+      <c r="B111" s="50"/>
+      <c r="C111" s="50"/>
+      <c r="D111" s="50"/>
+      <c r="E111" s="50"/>
+      <c r="F111" s="50"/>
+      <c r="G111" s="186"/>
+      <c r="H111" s="50"/>
+      <c r="I111" s="50"/>
+      <c r="J111" s="50"/>
       <c r="K111" s="86"/>
       <c r="L111" s="11"/>
       <c r="M111" s="11"/>
@@ -32423,16 +33171,16 @@
       <c r="AA111" s="155"/>
     </row>
     <row r="112" ht="12.75" customHeight="1">
-      <c r="A112" s="11"/>
-      <c r="B112" s="11"/>
-      <c r="C112" s="11"/>
-      <c r="D112" s="11"/>
-      <c r="E112" s="11"/>
-      <c r="F112" s="11"/>
-      <c r="G112" s="54"/>
-      <c r="H112" s="11"/>
-      <c r="I112" s="11"/>
-      <c r="J112" s="11"/>
+      <c r="A112" s="50"/>
+      <c r="B112" s="50"/>
+      <c r="C112" s="50"/>
+      <c r="D112" s="50"/>
+      <c r="E112" s="50"/>
+      <c r="F112" s="50"/>
+      <c r="G112" s="186"/>
+      <c r="H112" s="50"/>
+      <c r="I112" s="50"/>
+      <c r="J112" s="50"/>
       <c r="K112" s="86"/>
       <c r="L112" s="11"/>
       <c r="M112" s="11"/>
@@ -32452,16 +33200,16 @@
       <c r="AA112" s="155"/>
     </row>
     <row r="113" ht="12.75" customHeight="1">
-      <c r="A113" s="11"/>
-      <c r="B113" s="11"/>
-      <c r="C113" s="11"/>
-      <c r="D113" s="11"/>
-      <c r="E113" s="11"/>
-      <c r="F113" s="11"/>
-      <c r="G113" s="54"/>
-      <c r="H113" s="11"/>
-      <c r="I113" s="11"/>
-      <c r="J113" s="11"/>
+      <c r="A113" s="50"/>
+      <c r="B113" s="50"/>
+      <c r="C113" s="50"/>
+      <c r="D113" s="50"/>
+      <c r="E113" s="50"/>
+      <c r="F113" s="50"/>
+      <c r="G113" s="186"/>
+      <c r="H113" s="50"/>
+      <c r="I113" s="50"/>
+      <c r="J113" s="50"/>
       <c r="K113" s="86"/>
       <c r="L113" s="11"/>
       <c r="M113" s="11"/>
@@ -32481,16 +33229,16 @@
       <c r="AA113" s="155"/>
     </row>
     <row r="114" ht="12.75" customHeight="1">
-      <c r="A114" s="11"/>
-      <c r="B114" s="11"/>
-      <c r="C114" s="11"/>
-      <c r="D114" s="11"/>
-      <c r="E114" s="11"/>
-      <c r="F114" s="11"/>
-      <c r="G114" s="11"/>
-      <c r="H114" s="11"/>
-      <c r="I114" s="11"/>
-      <c r="J114" s="11"/>
+      <c r="A114" s="50"/>
+      <c r="B114" s="50"/>
+      <c r="C114" s="50"/>
+      <c r="D114" s="50"/>
+      <c r="E114" s="50"/>
+      <c r="F114" s="50"/>
+      <c r="G114" s="50"/>
+      <c r="H114" s="50"/>
+      <c r="I114" s="50"/>
+      <c r="J114" s="50"/>
       <c r="K114" s="86"/>
       <c r="L114" s="11"/>
       <c r="M114" s="11"/>
@@ -32510,16 +33258,16 @@
       <c r="AA114" s="155"/>
     </row>
     <row r="115" ht="12.75" customHeight="1">
-      <c r="A115" s="11"/>
-      <c r="B115" s="11"/>
-      <c r="C115" s="11"/>
-      <c r="D115" s="11"/>
-      <c r="E115" s="11"/>
-      <c r="F115" s="11"/>
-      <c r="G115" s="11"/>
-      <c r="H115" s="11"/>
-      <c r="I115" s="11"/>
-      <c r="J115" s="11"/>
+      <c r="A115" s="50"/>
+      <c r="B115" s="50"/>
+      <c r="C115" s="50"/>
+      <c r="D115" s="50"/>
+      <c r="E115" s="50"/>
+      <c r="F115" s="50"/>
+      <c r="G115" s="50"/>
+      <c r="H115" s="50"/>
+      <c r="I115" s="50"/>
+      <c r="J115" s="50"/>
       <c r="K115" s="86"/>
       <c r="L115" s="11"/>
       <c r="M115" s="11"/>
@@ -32539,16 +33287,16 @@
       <c r="AA115" s="155"/>
     </row>
     <row r="116" ht="12.75" customHeight="1">
-      <c r="A116" s="11"/>
-      <c r="B116" s="11"/>
-      <c r="C116" s="11"/>
-      <c r="D116" s="11"/>
-      <c r="E116" s="11"/>
-      <c r="F116" s="11"/>
-      <c r="G116" s="11"/>
-      <c r="H116" s="11"/>
-      <c r="I116" s="11"/>
-      <c r="J116" s="11"/>
+      <c r="A116" s="50"/>
+      <c r="B116" s="50"/>
+      <c r="C116" s="50"/>
+      <c r="D116" s="50"/>
+      <c r="E116" s="50"/>
+      <c r="F116" s="50"/>
+      <c r="G116" s="50"/>
+      <c r="H116" s="50"/>
+      <c r="I116" s="50"/>
+      <c r="J116" s="50"/>
       <c r="K116" s="86"/>
       <c r="L116" s="11"/>
       <c r="M116" s="11"/>
@@ -32568,16 +33316,16 @@
       <c r="AA116" s="155"/>
     </row>
     <row r="117" ht="12.75" customHeight="1">
-      <c r="A117" s="11"/>
-      <c r="B117" s="11"/>
-      <c r="C117" s="11"/>
-      <c r="D117" s="11"/>
-      <c r="E117" s="11"/>
-      <c r="F117" s="11"/>
-      <c r="G117" s="11"/>
-      <c r="H117" s="11"/>
-      <c r="I117" s="11"/>
-      <c r="J117" s="11"/>
+      <c r="A117" s="50"/>
+      <c r="B117" s="50"/>
+      <c r="C117" s="50"/>
+      <c r="D117" s="50"/>
+      <c r="E117" s="50"/>
+      <c r="F117" s="50"/>
+      <c r="G117" s="50"/>
+      <c r="H117" s="50"/>
+      <c r="I117" s="50"/>
+      <c r="J117" s="50"/>
       <c r="K117" s="86"/>
       <c r="L117" s="11"/>
       <c r="M117" s="11"/>
@@ -32597,16 +33345,16 @@
       <c r="AA117" s="155"/>
     </row>
     <row r="118" ht="12.75" customHeight="1">
-      <c r="A118" s="11"/>
-      <c r="B118" s="11"/>
-      <c r="C118" s="11"/>
-      <c r="D118" s="11"/>
-      <c r="E118" s="11"/>
-      <c r="F118" s="11"/>
-      <c r="G118" s="11"/>
-      <c r="H118" s="11"/>
-      <c r="I118" s="11"/>
-      <c r="J118" s="11"/>
+      <c r="A118" s="50"/>
+      <c r="B118" s="50"/>
+      <c r="C118" s="50"/>
+      <c r="D118" s="50"/>
+      <c r="E118" s="50"/>
+      <c r="F118" s="50"/>
+      <c r="G118" s="50"/>
+      <c r="H118" s="50"/>
+      <c r="I118" s="50"/>
+      <c r="J118" s="50"/>
       <c r="K118" s="86"/>
       <c r="L118" s="11"/>
       <c r="M118" s="11"/>
@@ -32626,16 +33374,16 @@
       <c r="AA118" s="155"/>
     </row>
     <row r="119" ht="12.75" customHeight="1">
-      <c r="A119" s="11"/>
-      <c r="B119" s="11"/>
-      <c r="C119" s="11"/>
-      <c r="D119" s="11"/>
-      <c r="E119" s="11"/>
-      <c r="F119" s="11"/>
-      <c r="G119" s="11"/>
-      <c r="H119" s="11"/>
-      <c r="I119" s="11"/>
-      <c r="J119" s="11"/>
+      <c r="A119" s="50"/>
+      <c r="B119" s="50"/>
+      <c r="C119" s="50"/>
+      <c r="D119" s="50"/>
+      <c r="E119" s="50"/>
+      <c r="F119" s="50"/>
+      <c r="G119" s="50"/>
+      <c r="H119" s="50"/>
+      <c r="I119" s="50"/>
+      <c r="J119" s="50"/>
       <c r="K119" s="86"/>
       <c r="L119" s="11"/>
       <c r="M119" s="11"/>
@@ -32655,16 +33403,16 @@
       <c r="AA119" s="155"/>
     </row>
     <row r="120" ht="12.75" customHeight="1">
-      <c r="A120" s="11"/>
-      <c r="B120" s="11"/>
-      <c r="C120" s="11"/>
-      <c r="D120" s="11"/>
-      <c r="E120" s="11"/>
-      <c r="F120" s="11"/>
-      <c r="G120" s="11"/>
-      <c r="H120" s="11"/>
-      <c r="I120" s="11"/>
-      <c r="J120" s="11"/>
+      <c r="A120" s="50"/>
+      <c r="B120" s="50"/>
+      <c r="C120" s="50"/>
+      <c r="D120" s="50"/>
+      <c r="E120" s="50"/>
+      <c r="F120" s="50"/>
+      <c r="G120" s="50"/>
+      <c r="H120" s="50"/>
+      <c r="I120" s="50"/>
+      <c r="J120" s="50"/>
       <c r="K120" s="86"/>
       <c r="L120" s="11"/>
       <c r="M120" s="11"/>
@@ -32684,16 +33432,16 @@
       <c r="AA120" s="155"/>
     </row>
     <row r="121" ht="12.75" customHeight="1">
-      <c r="A121" s="11"/>
-      <c r="B121" s="11"/>
-      <c r="C121" s="11"/>
-      <c r="D121" s="11"/>
-      <c r="E121" s="11"/>
-      <c r="F121" s="11"/>
-      <c r="G121" s="11"/>
-      <c r="H121" s="11"/>
-      <c r="I121" s="11"/>
-      <c r="J121" s="11"/>
+      <c r="A121" s="50"/>
+      <c r="B121" s="50"/>
+      <c r="C121" s="50"/>
+      <c r="D121" s="50"/>
+      <c r="E121" s="50"/>
+      <c r="F121" s="50"/>
+      <c r="G121" s="50"/>
+      <c r="H121" s="50"/>
+      <c r="I121" s="50"/>
+      <c r="J121" s="50"/>
       <c r="K121" s="86"/>
       <c r="L121" s="11"/>
       <c r="M121" s="11"/>
@@ -32713,16 +33461,16 @@
       <c r="AA121" s="155"/>
     </row>
     <row r="122" ht="12.75" customHeight="1">
-      <c r="A122" s="11"/>
-      <c r="B122" s="11"/>
-      <c r="C122" s="11"/>
-      <c r="D122" s="11"/>
-      <c r="E122" s="11"/>
-      <c r="F122" s="11"/>
-      <c r="G122" s="11"/>
-      <c r="H122" s="11"/>
-      <c r="I122" s="11"/>
-      <c r="J122" s="11"/>
+      <c r="A122" s="50"/>
+      <c r="B122" s="50"/>
+      <c r="C122" s="50"/>
+      <c r="D122" s="50"/>
+      <c r="E122" s="50"/>
+      <c r="F122" s="50"/>
+      <c r="G122" s="50"/>
+      <c r="H122" s="50"/>
+      <c r="I122" s="50"/>
+      <c r="J122" s="50"/>
       <c r="K122" s="86"/>
       <c r="L122" s="11"/>
       <c r="M122" s="11"/>
@@ -34448,7 +35196,7 @@
     <mergeCell ref="B4:E4"/>
   </mergeCells>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G8:G65">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G8:G73">
       <formula1>$M$2:$M$5</formula1>
     </dataValidation>
   </dataValidations>
@@ -34484,15 +35232,15 @@
   <sheetData>
     <row r="1" ht="25.5" customHeight="1">
       <c r="A1" s="11"/>
-      <c r="B1" s="173" t="s">
-        <v>504</v>
-      </c>
-      <c r="C1" s="174"/>
-      <c r="D1" s="174"/>
-      <c r="E1" s="174"/>
-      <c r="F1" s="174"/>
-      <c r="G1" s="174"/>
-      <c r="H1" s="174"/>
+      <c r="B1" s="187" t="s">
+        <v>541</v>
+      </c>
+      <c r="C1" s="188"/>
+      <c r="D1" s="188"/>
+      <c r="E1" s="188"/>
+      <c r="F1" s="188"/>
+      <c r="G1" s="188"/>
+      <c r="H1" s="188"/>
       <c r="I1" s="11"/>
       <c r="J1" s="11"/>
       <c r="K1" s="11"/>
@@ -34513,14 +35261,14 @@
       <c r="Z1" s="11"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="175"/>
-      <c r="B2" s="175"/>
+      <c r="A2" s="189"/>
+      <c r="B2" s="189"/>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
       <c r="F2" s="11"/>
       <c r="G2" s="11"/>
-      <c r="H2" s="176"/>
+      <c r="H2" s="190"/>
       <c r="I2" s="11"/>
       <c r="J2" s="11"/>
       <c r="K2" s="11"/>
@@ -34542,19 +35290,19 @@
     </row>
     <row r="3" ht="12.0" customHeight="1">
       <c r="A3" s="11"/>
-      <c r="B3" s="177" t="s">
+      <c r="B3" s="191" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="49" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="6"/>
-      <c r="E3" s="178" t="s">
+      <c r="E3" s="192" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="6"/>
-      <c r="G3" s="179"/>
-      <c r="H3" s="180" t="s">
+      <c r="G3" s="193"/>
+      <c r="H3" s="194" t="s">
         <v>4</v>
       </c>
       <c r="I3" s="11"/>
@@ -34578,19 +35326,19 @@
     </row>
     <row r="4" ht="12.0" customHeight="1">
       <c r="A4" s="11"/>
-      <c r="B4" s="177" t="s">
+      <c r="B4" s="191" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="49" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="6"/>
-      <c r="E4" s="178" t="s">
+      <c r="E4" s="192" t="s">
         <v>6</v>
       </c>
       <c r="F4" s="6"/>
-      <c r="G4" s="179"/>
-      <c r="H4" s="180" t="s">
+      <c r="G4" s="193"/>
+      <c r="H4" s="194" t="s">
         <v>7</v>
       </c>
       <c r="I4" s="11"/>
@@ -34614,7 +35362,7 @@
     </row>
     <row r="5" ht="12.0" customHeight="1">
       <c r="A5" s="11"/>
-      <c r="B5" s="181" t="s">
+      <c r="B5" s="195" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="49" t="str">
@@ -34622,12 +35370,12 @@
         <v>SoFa_Test Report_vx.x</v>
       </c>
       <c r="D5" s="6"/>
-      <c r="E5" s="178" t="s">
+      <c r="E5" s="192" t="s">
         <v>9</v>
       </c>
       <c r="F5" s="6"/>
-      <c r="G5" s="179"/>
-      <c r="H5" s="182">
+      <c r="G5" s="193"/>
+      <c r="H5" s="196">
         <v>44534.0</v>
       </c>
       <c r="I5" s="11"/>
@@ -34650,12 +35398,12 @@
       <c r="Z5" s="11"/>
     </row>
     <row r="6" ht="21.75" customHeight="1">
-      <c r="A6" s="175"/>
-      <c r="B6" s="181" t="s">
-        <v>505</v>
-      </c>
-      <c r="C6" s="183" t="s">
-        <v>506</v>
+      <c r="A6" s="189"/>
+      <c r="B6" s="195" t="s">
+        <v>542</v>
+      </c>
+      <c r="C6" s="197" t="s">
+        <v>543</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -34682,14 +35430,14 @@
       <c r="Z6" s="11"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="175"/>
+      <c r="A7" s="189"/>
       <c r="B7" s="25"/>
-      <c r="C7" s="184"/>
+      <c r="C7" s="198"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
-      <c r="H7" s="176"/>
+      <c r="H7" s="190"/>
       <c r="I7" s="11"/>
       <c r="J7" s="11"/>
       <c r="K7" s="11"/>
@@ -34712,12 +35460,12 @@
     <row r="8" ht="12.75" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="25"/>
-      <c r="C8" s="184"/>
+      <c r="C8" s="198"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
-      <c r="H8" s="176"/>
+      <c r="H8" s="190"/>
       <c r="I8" s="11"/>
       <c r="J8" s="11"/>
       <c r="K8" s="11"/>
@@ -34766,27 +35514,27 @@
       <c r="Z9" s="11"/>
     </row>
     <row r="10" ht="12.75" customHeight="1">
-      <c r="A10" s="185"/>
-      <c r="B10" s="186" t="s">
+      <c r="A10" s="199"/>
+      <c r="B10" s="200" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="187" t="s">
-        <v>507</v>
-      </c>
-      <c r="D10" s="188" t="s">
+      <c r="C10" s="201" t="s">
+        <v>544</v>
+      </c>
+      <c r="D10" s="202" t="s">
         <v>83</v>
       </c>
-      <c r="E10" s="187" t="s">
+      <c r="E10" s="201" t="s">
         <v>86</v>
       </c>
-      <c r="F10" s="187" t="s">
+      <c r="F10" s="201" t="s">
         <v>89</v>
       </c>
-      <c r="G10" s="189" t="s">
+      <c r="G10" s="203" t="s">
         <v>90</v>
       </c>
-      <c r="H10" s="190" t="s">
-        <v>508</v>
+      <c r="H10" s="204" t="s">
+        <v>545</v>
       </c>
       <c r="I10" s="11"/>
       <c r="J10" s="11"/>
@@ -34808,31 +35556,31 @@
       <c r="Z10" s="11"/>
     </row>
     <row r="11" ht="12.75" customHeight="1">
-      <c r="A11" s="185"/>
-      <c r="B11" s="191">
+      <c r="A11" s="199"/>
+      <c r="B11" s="205">
         <v>1.0</v>
       </c>
-      <c r="C11" s="192" t="str">
+      <c r="C11" s="206" t="str">
         <f>Guest!B2</f>
         <v>Guest</v>
       </c>
-      <c r="D11" s="193">
+      <c r="D11" s="207">
         <f>Guest!A6</f>
         <v>43</v>
       </c>
-      <c r="E11" s="193">
+      <c r="E11" s="207">
         <f>Guest!B6</f>
         <v>4</v>
       </c>
-      <c r="F11" s="193">
+      <c r="F11" s="207">
         <f>Guest!C6</f>
         <v>3</v>
       </c>
-      <c r="G11" s="194">
+      <c r="G11" s="208">
         <f>Guest!D6</f>
         <v>0</v>
       </c>
-      <c r="H11" s="195">
+      <c r="H11" s="209">
         <f>Guest!E6</f>
         <v>50</v>
       </c>
@@ -34856,31 +35604,31 @@
       <c r="Z11" s="11"/>
     </row>
     <row r="12" ht="12.75" customHeight="1">
-      <c r="A12" s="185"/>
-      <c r="B12" s="191">
+      <c r="A12" s="199"/>
+      <c r="B12" s="205">
         <v>2.0</v>
       </c>
-      <c r="C12" s="192" t="str">
+      <c r="C12" s="206" t="str">
         <f>User!B2</f>
         <v>User</v>
       </c>
-      <c r="D12" s="193">
+      <c r="D12" s="207">
         <f>User!A6</f>
         <v>0</v>
       </c>
-      <c r="E12" s="193">
+      <c r="E12" s="207">
         <f>User!B6</f>
         <v>0</v>
       </c>
-      <c r="F12" s="193">
+      <c r="F12" s="207">
         <f>User!C6</f>
         <v>51</v>
       </c>
-      <c r="G12" s="193">
+      <c r="G12" s="207">
         <f>User!D6</f>
         <v>0</v>
       </c>
-      <c r="H12" s="193">
+      <c r="H12" s="207">
         <f>User!E6</f>
         <v>51</v>
       </c>
@@ -34904,31 +35652,31 @@
       <c r="Z12" s="11"/>
     </row>
     <row r="13" ht="12.75" customHeight="1">
-      <c r="A13" s="185"/>
-      <c r="B13" s="191">
+      <c r="A13" s="199"/>
+      <c r="B13" s="205">
         <v>1.0</v>
       </c>
-      <c r="C13" s="192" t="str">
+      <c r="C13" s="206" t="str">
         <f>Manager!B2</f>
         <v>Manager</v>
       </c>
-      <c r="D13" s="193">
+      <c r="D13" s="207">
         <f>Manager!A6</f>
         <v>0</v>
       </c>
-      <c r="E13" s="193">
+      <c r="E13" s="207">
         <f>Manager!B6</f>
         <v>0</v>
       </c>
-      <c r="F13" s="193">
+      <c r="F13" s="207">
         <f>Manager!C6</f>
         <v>0</v>
       </c>
-      <c r="G13" s="194">
+      <c r="G13" s="208">
         <f>Manager!D6</f>
         <v>0</v>
       </c>
-      <c r="H13" s="195">
+      <c r="H13" s="209">
         <f>Manager!E6</f>
         <v>0</v>
       </c>
@@ -34952,28 +35700,28 @@
       <c r="Z13" s="11"/>
     </row>
     <row r="14" ht="12.75" customHeight="1">
-      <c r="A14" s="185"/>
-      <c r="B14" s="196"/>
-      <c r="C14" s="197" t="s">
-        <v>509</v>
-      </c>
-      <c r="D14" s="198">
+      <c r="A14" s="199"/>
+      <c r="B14" s="210"/>
+      <c r="C14" s="211" t="s">
+        <v>546</v>
+      </c>
+      <c r="D14" s="212">
         <f t="shared" ref="D14:H14" si="1">SUM(D9:D13)</f>
         <v>43</v>
       </c>
-      <c r="E14" s="198">
+      <c r="E14" s="212">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="F14" s="198">
+      <c r="F14" s="212">
         <f t="shared" si="1"/>
         <v>54</v>
       </c>
-      <c r="G14" s="198">
+      <c r="G14" s="212">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H14" s="199">
+      <c r="H14" s="213">
         <f t="shared" si="1"/>
         <v>101</v>
       </c>
@@ -34998,13 +35746,13 @@
     </row>
     <row r="15" ht="12.75" customHeight="1">
       <c r="A15" s="11"/>
-      <c r="B15" s="200"/>
+      <c r="B15" s="214"/>
       <c r="C15" s="11"/>
-      <c r="D15" s="201"/>
-      <c r="E15" s="202"/>
-      <c r="F15" s="202"/>
-      <c r="G15" s="202"/>
-      <c r="H15" s="202"/>
+      <c r="D15" s="215"/>
+      <c r="E15" s="216"/>
+      <c r="F15" s="216"/>
+      <c r="G15" s="216"/>
+      <c r="H15" s="216"/>
       <c r="I15" s="11"/>
       <c r="J15" s="11"/>
       <c r="K15" s="11"/>
@@ -35028,15 +35776,15 @@
       <c r="A16" s="11"/>
       <c r="B16" s="11"/>
       <c r="C16" s="9" t="s">
-        <v>510</v>
+        <v>547</v>
       </c>
       <c r="D16" s="11"/>
-      <c r="E16" s="203">
+      <c r="E16" s="217">
         <f>(D14+E14)*100/(H14-G14)</f>
         <v>46.53465347</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>511</v>
+        <v>548</v>
       </c>
       <c r="G16" s="11"/>
       <c r="H16" s="132"/>
@@ -35063,15 +35811,15 @@
       <c r="A17" s="11"/>
       <c r="B17" s="11"/>
       <c r="C17" s="9" t="s">
-        <v>512</v>
+        <v>549</v>
       </c>
       <c r="D17" s="11"/>
-      <c r="E17" s="203">
+      <c r="E17" s="217">
         <f>D14*100/(H14-G14)</f>
         <v>42.57425743</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>511</v>
+        <v>548</v>
       </c>
       <c r="G17" s="11"/>
       <c r="H17" s="132"/>

</xml_diff>

<commit_message>
HoangNH - Update test case manager manage post
</commit_message>
<xml_diff>
--- a/3. Users/HoangNHHE130395/Testing/TestCase - Hoang.xlsx
+++ b/3. Users/HoangNHHE130395/Testing/TestCase - Hoang.xlsx
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1184" uniqueCount="550">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1258" uniqueCount="570">
   <si>
     <t>SYSTEM TEST CASE</t>
   </si>
@@ -2375,11 +2375,11 @@
     <t>1. Post have id = '97'</t>
   </si>
   <si>
+    <t>Check paging list post</t>
+  </si>
+  <si>
     <t>1. Login into the web server
 2. Click on 'Post' tab in the menu bar</t>
-  </si>
-  <si>
-    <t>Check paging list post</t>
   </si>
   <si>
     <t>1. Login into the web server
@@ -2402,6 +2402,98 @@
     <t>1. Login into the web server
 2. Click on 'Post' tab in the menu bar
 3. Click on 'Next &gt;&gt;' on the paging</t>
+  </si>
+  <si>
+    <t>Check GUI of post detail</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'Post' tab in the menu bar
+3. Click on the 'edit' in column 'Option' of post have id = '97'</t>
+  </si>
+  <si>
+    <t>1. Display the information of the post by following: "Posted By, Date Created, Name, Total Like, Rate, List Comments"</t>
+  </si>
+  <si>
+    <t>Check GUI list comment</t>
+  </si>
+  <si>
+    <t>1. Display comment by following: User, Comment, Date
+ 2. The data of comment is mapping wit the column name</t>
+  </si>
+  <si>
+    <t>Check function click on username</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Display detail information of user have id = '7' </t>
+  </si>
+  <si>
+    <t>1. Post have id = '97'
+2. Comment of user have id = '7'</t>
+  </si>
+  <si>
+    <t>Check paging list comment</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'Post' tab in the menu bar
+3. Click on the 'edit' in column 'Option' of post have id = '85'
+4. Click on '2' on the paging</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'Post' tab in the menu bar
+3. Click on the 'edit' in column 'Option' of post have id = '85'
+4. Click on '2' on the paging
+5. Click on '1' on the paging</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'Post' tab in the menu bar
+3. Click on the 'edit' in column 'Option' of post have id = '85'
+4. Click on '2' on the paging
+5. Click on '&lt;&lt; Previous' on the paging</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'Post' tab in the menu bar
+3. Click on the 'edit' in column 'Option' of post have id = '85'
+4. Click on 'Next &gt;&gt;' on the paging</t>
+  </si>
+  <si>
+    <t>Check function button 'Xoá'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Login into the web server
+2. Click on 'Post' tab in the menu bar
+3. Click on the 'edit' in column 'Option' of post have id = '84'
+4. Click on button 'Xóa'
+</t>
+  </si>
+  <si>
+    <t>1. Display popup confirm 'Bạn có muốn xoá bài viết này'</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'Post' tab in the menu bar
+3. Click on the 'edit' in column 'Option' of post have id = '84'
+4. Click on button 'Xóa'
+5. Click on 'Hủy'</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'Post' tab in the menu bar
+3. Click on the 'edit' in column 'Option' of post have id = '84'
+4. Click on button 'Xóa'
+5. Click on 'Ok'</t>
+  </si>
+  <si>
+    <t>1. Popup is disappeared
+2. Toast message 'Xóa bài đăng thành công'
+3. The post is deleted and back to list post</t>
+  </si>
+  <si>
+    <t>Function Manage Voucher</t>
   </si>
   <si>
     <t>TEST REPORT</t>
@@ -3282,7 +3374,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="218">
+  <cellXfs count="215">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -3718,7 +3810,7 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="11" fillId="6" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="11" fillId="6" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" wrapText="0"/>
@@ -3764,15 +3856,6 @@
     </xf>
     <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="13" fillId="2" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="13" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="24" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
@@ -31606,7 +31689,7 @@
     </row>
     <row r="72" ht="37.5" customHeight="1">
       <c r="A72" s="160" t="str">
-        <f t="shared" ref="A72:A96" si="3">IF(OR(B72&lt;&gt;"",D72&lt;&gt;""),"["&amp;TEXT($B$2,"##")&amp;"-"&amp;TEXT(ROW()-9,"##")&amp;"]","")</f>
+        <f t="shared" ref="A72:A100" si="3">IF(OR(B72&lt;&gt;"",D72&lt;&gt;""),"["&amp;TEXT($B$2,"##")&amp;"-"&amp;TEXT(ROW()-9,"##")&amp;"]","")</f>
         <v>[Manager-63]</v>
       </c>
       <c r="B72" s="173" t="s">
@@ -32080,7 +32163,7 @@
       <c r="Z81" s="11"/>
       <c r="AA81" s="155"/>
     </row>
-    <row r="82" ht="40.5" customHeight="1">
+    <row r="82" ht="72.75" customHeight="1">
       <c r="A82" s="160" t="str">
         <f t="shared" si="3"/>
         <v>[Manager-73]</v>
@@ -32226,10 +32309,10 @@
         <v>[Manager-76]</v>
       </c>
       <c r="B85" s="160" t="s">
-        <v>504</v>
+        <v>535</v>
       </c>
       <c r="C85" s="183" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="D85" s="161" t="s">
         <v>505</v>
@@ -32273,7 +32356,7 @@
         <v>[Manager-77]</v>
       </c>
       <c r="B86" s="160" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C86" s="183" t="s">
         <v>537</v>
@@ -32320,7 +32403,7 @@
         <v>[Manager-78]</v>
       </c>
       <c r="B87" s="160" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C87" s="183" t="s">
         <v>538</v>
@@ -32367,7 +32450,7 @@
         <v>[Manager-79]</v>
       </c>
       <c r="B88" s="160" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C88" s="183" t="s">
         <v>539</v>
@@ -32414,7 +32497,7 @@
         <v>[Manager-80]</v>
       </c>
       <c r="B89" s="160" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C89" s="183" t="s">
         <v>540</v>
@@ -32455,18 +32538,26 @@
       <c r="Z89" s="11"/>
       <c r="AA89" s="155"/>
     </row>
-    <row r="90" ht="12.75" customHeight="1">
+    <row r="90" ht="68.25" customHeight="1">
       <c r="A90" s="160" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B90" s="184"/>
-      <c r="C90" s="185"/>
-      <c r="D90" s="185"/>
+        <v>[Manager-81]</v>
+      </c>
+      <c r="B90" s="173" t="s">
+        <v>541</v>
+      </c>
+      <c r="C90" s="182" t="s">
+        <v>542</v>
+      </c>
+      <c r="D90" s="174" t="s">
+        <v>543</v>
+      </c>
       <c r="E90" s="173" t="s">
         <v>512</v>
       </c>
-      <c r="F90" s="180"/>
+      <c r="F90" s="181" t="s">
+        <v>534</v>
+      </c>
       <c r="G90" s="176" t="s">
         <v>83</v>
       </c>
@@ -32495,14 +32586,20 @@
       <c r="Z90" s="11"/>
       <c r="AA90" s="155"/>
     </row>
-    <row r="91" ht="12.75" customHeight="1">
+    <row r="91" ht="87.0" customHeight="1">
       <c r="A91" s="160" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B91" s="184"/>
-      <c r="C91" s="185"/>
-      <c r="D91" s="185"/>
+        <v>[Manager-82]</v>
+      </c>
+      <c r="B91" s="173" t="s">
+        <v>544</v>
+      </c>
+      <c r="C91" s="182" t="s">
+        <v>542</v>
+      </c>
+      <c r="D91" s="182" t="s">
+        <v>545</v>
+      </c>
       <c r="E91" s="173" t="s">
         <v>512</v>
       </c>
@@ -32535,18 +32632,26 @@
       <c r="Z91" s="11"/>
       <c r="AA91" s="155"/>
     </row>
-    <row r="92" ht="12.75" customHeight="1">
+    <row r="92" ht="61.5" customHeight="1">
       <c r="A92" s="160" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B92" s="184"/>
-      <c r="C92" s="185"/>
-      <c r="D92" s="185"/>
+        <v>[Manager-83]</v>
+      </c>
+      <c r="B92" s="173" t="s">
+        <v>546</v>
+      </c>
+      <c r="C92" s="182" t="s">
+        <v>542</v>
+      </c>
+      <c r="D92" s="183" t="s">
+        <v>547</v>
+      </c>
       <c r="E92" s="173" t="s">
         <v>512</v>
       </c>
-      <c r="F92" s="180"/>
+      <c r="F92" s="181" t="s">
+        <v>548</v>
+      </c>
       <c r="G92" s="176" t="s">
         <v>83</v>
       </c>
@@ -32575,18 +32680,25 @@
       <c r="Z92" s="11"/>
       <c r="AA92" s="155"/>
     </row>
-    <row r="93" ht="12.75" customHeight="1">
+    <row r="93" ht="44.25" customHeight="1">
       <c r="A93" s="160" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B93" s="184"/>
-      <c r="C93" s="185"/>
-      <c r="D93" s="185"/>
-      <c r="E93" s="173" t="s">
-        <v>512</v>
-      </c>
-      <c r="F93" s="180"/>
+        <v>[Manager-84]</v>
+      </c>
+      <c r="B93" s="160" t="s">
+        <v>549</v>
+      </c>
+      <c r="C93" s="183" t="s">
+        <v>536</v>
+      </c>
+      <c r="D93" s="161" t="s">
+        <v>505</v>
+      </c>
+      <c r="E93" s="160" t="str">
+        <f t="shared" ref="E93:E100" si="5">$A$10</f>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F93" s="161"/>
       <c r="G93" s="176" t="s">
         <v>83</v>
       </c>
@@ -32615,18 +32727,25 @@
       <c r="Z93" s="11"/>
       <c r="AA93" s="155"/>
     </row>
-    <row r="94" ht="12.75" customHeight="1">
+    <row r="94" ht="75.75" customHeight="1">
       <c r="A94" s="160" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B94" s="184"/>
-      <c r="C94" s="185"/>
-      <c r="D94" s="185"/>
-      <c r="E94" s="173" t="s">
-        <v>512</v>
-      </c>
-      <c r="F94" s="180"/>
+        <v>[Manager-85]</v>
+      </c>
+      <c r="B94" s="160" t="s">
+        <v>549</v>
+      </c>
+      <c r="C94" s="183" t="s">
+        <v>550</v>
+      </c>
+      <c r="D94" s="161" t="s">
+        <v>506</v>
+      </c>
+      <c r="E94" s="160" t="str">
+        <f t="shared" si="5"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F94" s="161"/>
       <c r="G94" s="176" t="s">
         <v>83</v>
       </c>
@@ -32655,18 +32774,25 @@
       <c r="Z94" s="11"/>
       <c r="AA94" s="155"/>
     </row>
-    <row r="95" ht="12.75" customHeight="1">
+    <row r="95" ht="85.5" customHeight="1">
       <c r="A95" s="160" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B95" s="184"/>
-      <c r="C95" s="185"/>
-      <c r="D95" s="185"/>
-      <c r="E95" s="173" t="s">
-        <v>512</v>
-      </c>
-      <c r="F95" s="180"/>
+        <v>[Manager-86]</v>
+      </c>
+      <c r="B95" s="160" t="s">
+        <v>549</v>
+      </c>
+      <c r="C95" s="183" t="s">
+        <v>551</v>
+      </c>
+      <c r="D95" s="161" t="s">
+        <v>507</v>
+      </c>
+      <c r="E95" s="160" t="str">
+        <f t="shared" si="5"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F95" s="161"/>
       <c r="G95" s="176" t="s">
         <v>83</v>
       </c>
@@ -32695,18 +32821,25 @@
       <c r="Z95" s="11"/>
       <c r="AA95" s="155"/>
     </row>
-    <row r="96" ht="12.75" customHeight="1">
+    <row r="96" ht="88.5" customHeight="1">
       <c r="A96" s="160" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B96" s="184"/>
-      <c r="C96" s="185"/>
-      <c r="D96" s="185"/>
-      <c r="E96" s="173" t="s">
-        <v>512</v>
-      </c>
-      <c r="F96" s="180"/>
+        <v>[Manager-87]</v>
+      </c>
+      <c r="B96" s="160" t="s">
+        <v>549</v>
+      </c>
+      <c r="C96" s="183" t="s">
+        <v>552</v>
+      </c>
+      <c r="D96" s="161" t="s">
+        <v>507</v>
+      </c>
+      <c r="E96" s="160" t="str">
+        <f t="shared" si="5"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F96" s="161"/>
       <c r="G96" s="176" t="s">
         <v>83</v>
       </c>
@@ -32735,17 +32868,35 @@
       <c r="Z96" s="11"/>
       <c r="AA96" s="155"/>
     </row>
-    <row r="97" ht="12.75" customHeight="1">
-      <c r="A97" s="50"/>
-      <c r="B97" s="50"/>
-      <c r="C97" s="50"/>
-      <c r="D97" s="50"/>
-      <c r="E97" s="50"/>
-      <c r="F97" s="50"/>
-      <c r="G97" s="186"/>
-      <c r="H97" s="50"/>
-      <c r="I97" s="50"/>
-      <c r="J97" s="50"/>
+    <row r="97" ht="77.25" customHeight="1">
+      <c r="A97" s="160" t="str">
+        <f t="shared" si="3"/>
+        <v>[Manager-88]</v>
+      </c>
+      <c r="B97" s="160" t="s">
+        <v>549</v>
+      </c>
+      <c r="C97" s="183" t="s">
+        <v>553</v>
+      </c>
+      <c r="D97" s="161" t="s">
+        <v>508</v>
+      </c>
+      <c r="E97" s="160" t="str">
+        <f t="shared" si="5"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F97" s="161"/>
+      <c r="G97" s="176" t="s">
+        <v>83</v>
+      </c>
+      <c r="H97" s="177">
+        <v>44303.0</v>
+      </c>
+      <c r="I97" s="178" t="s">
+        <v>375</v>
+      </c>
+      <c r="J97" s="179"/>
       <c r="K97" s="86"/>
       <c r="L97" s="11"/>
       <c r="M97" s="11"/>
@@ -32764,17 +32915,35 @@
       <c r="Z97" s="11"/>
       <c r="AA97" s="155"/>
     </row>
-    <row r="98" ht="12.75" customHeight="1">
-      <c r="A98" s="50"/>
-      <c r="B98" s="50"/>
-      <c r="C98" s="50"/>
-      <c r="D98" s="50"/>
-      <c r="E98" s="50"/>
-      <c r="F98" s="50"/>
-      <c r="G98" s="186"/>
-      <c r="H98" s="50"/>
-      <c r="I98" s="50"/>
-      <c r="J98" s="50"/>
+    <row r="98" ht="79.5" customHeight="1">
+      <c r="A98" s="160" t="str">
+        <f t="shared" si="3"/>
+        <v>[Manager-89]</v>
+      </c>
+      <c r="B98" s="160" t="s">
+        <v>554</v>
+      </c>
+      <c r="C98" s="183" t="s">
+        <v>555</v>
+      </c>
+      <c r="D98" s="161" t="s">
+        <v>556</v>
+      </c>
+      <c r="E98" s="160" t="str">
+        <f t="shared" si="5"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F98" s="161"/>
+      <c r="G98" s="176" t="s">
+        <v>83</v>
+      </c>
+      <c r="H98" s="177">
+        <v>44303.0</v>
+      </c>
+      <c r="I98" s="178" t="s">
+        <v>375</v>
+      </c>
+      <c r="J98" s="179"/>
       <c r="K98" s="86"/>
       <c r="L98" s="11"/>
       <c r="M98" s="11"/>
@@ -32793,17 +32962,35 @@
       <c r="Z98" s="11"/>
       <c r="AA98" s="155"/>
     </row>
-    <row r="99" ht="12.75" customHeight="1">
-      <c r="A99" s="50"/>
-      <c r="B99" s="50"/>
-      <c r="C99" s="50"/>
-      <c r="D99" s="50"/>
-      <c r="E99" s="50"/>
-      <c r="F99" s="50"/>
-      <c r="G99" s="186"/>
-      <c r="H99" s="50"/>
-      <c r="I99" s="50"/>
-      <c r="J99" s="50"/>
+    <row r="99" ht="85.5" customHeight="1">
+      <c r="A99" s="160" t="str">
+        <f t="shared" si="3"/>
+        <v>[Manager-90]</v>
+      </c>
+      <c r="B99" s="160" t="s">
+        <v>554</v>
+      </c>
+      <c r="C99" s="183" t="s">
+        <v>557</v>
+      </c>
+      <c r="D99" s="161" t="s">
+        <v>457</v>
+      </c>
+      <c r="E99" s="160" t="str">
+        <f t="shared" si="5"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F99" s="161"/>
+      <c r="G99" s="176" t="s">
+        <v>83</v>
+      </c>
+      <c r="H99" s="177">
+        <v>44303.0</v>
+      </c>
+      <c r="I99" s="178" t="s">
+        <v>375</v>
+      </c>
+      <c r="J99" s="179"/>
       <c r="K99" s="86"/>
       <c r="L99" s="11"/>
       <c r="M99" s="11"/>
@@ -32822,17 +33009,35 @@
       <c r="Z99" s="11"/>
       <c r="AA99" s="155"/>
     </row>
-    <row r="100" ht="12.75" customHeight="1">
-      <c r="A100" s="50"/>
-      <c r="B100" s="50"/>
-      <c r="C100" s="50"/>
-      <c r="D100" s="50"/>
-      <c r="E100" s="50"/>
-      <c r="F100" s="50"/>
-      <c r="G100" s="186"/>
-      <c r="H100" s="50"/>
-      <c r="I100" s="50"/>
-      <c r="J100" s="50"/>
+    <row r="100" ht="87.75" customHeight="1">
+      <c r="A100" s="160" t="str">
+        <f t="shared" si="3"/>
+        <v>[Manager-91]</v>
+      </c>
+      <c r="B100" s="160" t="s">
+        <v>554</v>
+      </c>
+      <c r="C100" s="183" t="s">
+        <v>558</v>
+      </c>
+      <c r="D100" s="161" t="s">
+        <v>559</v>
+      </c>
+      <c r="E100" s="160" t="str">
+        <f t="shared" si="5"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F100" s="161"/>
+      <c r="G100" s="176" t="s">
+        <v>83</v>
+      </c>
+      <c r="H100" s="177">
+        <v>44303.0</v>
+      </c>
+      <c r="I100" s="178" t="s">
+        <v>375</v>
+      </c>
+      <c r="J100" s="179"/>
       <c r="K100" s="86"/>
       <c r="L100" s="11"/>
       <c r="M100" s="11"/>
@@ -32851,17 +33056,19 @@
       <c r="Z100" s="11"/>
       <c r="AA100" s="155"/>
     </row>
-    <row r="101" ht="12.75" customHeight="1">
-      <c r="A101" s="50"/>
-      <c r="B101" s="50"/>
-      <c r="C101" s="50"/>
-      <c r="D101" s="50"/>
-      <c r="E101" s="50"/>
-      <c r="F101" s="50"/>
-      <c r="G101" s="186"/>
-      <c r="H101" s="50"/>
-      <c r="I101" s="50"/>
-      <c r="J101" s="50"/>
+    <row r="101" ht="30.75" customHeight="1">
+      <c r="A101" s="168" t="s">
+        <v>560</v>
+      </c>
+      <c r="B101" s="169"/>
+      <c r="C101" s="170"/>
+      <c r="D101" s="170"/>
+      <c r="E101" s="170"/>
+      <c r="F101" s="170"/>
+      <c r="G101" s="170"/>
+      <c r="H101" s="171"/>
+      <c r="I101" s="170"/>
+      <c r="J101" s="172"/>
       <c r="K101" s="86"/>
       <c r="L101" s="11"/>
       <c r="M101" s="11"/>
@@ -32881,16 +33088,28 @@
       <c r="AA101" s="155"/>
     </row>
     <row r="102" ht="12.75" customHeight="1">
-      <c r="A102" s="50"/>
-      <c r="B102" s="50"/>
-      <c r="C102" s="50"/>
-      <c r="D102" s="50"/>
-      <c r="E102" s="50"/>
-      <c r="F102" s="50"/>
-      <c r="G102" s="186"/>
-      <c r="H102" s="50"/>
-      <c r="I102" s="50"/>
-      <c r="J102" s="50"/>
+      <c r="A102" s="160" t="str">
+        <f t="shared" ref="A102:A118" si="6">IF(OR(B102&lt;&gt;"",D102&lt;&gt;""),"["&amp;TEXT($B$2,"##")&amp;"-"&amp;TEXT(ROW()-9,"##")&amp;"]","")</f>
+        <v/>
+      </c>
+      <c r="B102" s="160"/>
+      <c r="C102" s="183"/>
+      <c r="D102" s="161"/>
+      <c r="E102" s="160" t="str">
+        <f t="shared" ref="E102:E118" si="7">$A$10</f>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F102" s="161"/>
+      <c r="G102" s="176" t="s">
+        <v>83</v>
+      </c>
+      <c r="H102" s="177">
+        <v>44304.0</v>
+      </c>
+      <c r="I102" s="178" t="s">
+        <v>375</v>
+      </c>
+      <c r="J102" s="179"/>
       <c r="K102" s="86"/>
       <c r="L102" s="11"/>
       <c r="M102" s="11"/>
@@ -32910,16 +33129,28 @@
       <c r="AA102" s="155"/>
     </row>
     <row r="103" ht="12.75" customHeight="1">
-      <c r="A103" s="50"/>
-      <c r="B103" s="50"/>
-      <c r="C103" s="50"/>
-      <c r="D103" s="50"/>
-      <c r="E103" s="50"/>
-      <c r="F103" s="50"/>
-      <c r="G103" s="186"/>
-      <c r="H103" s="50"/>
-      <c r="I103" s="50"/>
-      <c r="J103" s="50"/>
+      <c r="A103" s="160" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="B103" s="160"/>
+      <c r="C103" s="183"/>
+      <c r="D103" s="161"/>
+      <c r="E103" s="160" t="str">
+        <f t="shared" si="7"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F103" s="161"/>
+      <c r="G103" s="176" t="s">
+        <v>83</v>
+      </c>
+      <c r="H103" s="177">
+        <v>44304.0</v>
+      </c>
+      <c r="I103" s="178" t="s">
+        <v>375</v>
+      </c>
+      <c r="J103" s="179"/>
       <c r="K103" s="86"/>
       <c r="L103" s="11"/>
       <c r="M103" s="11"/>
@@ -32939,16 +33170,28 @@
       <c r="AA103" s="155"/>
     </row>
     <row r="104" ht="12.75" customHeight="1">
-      <c r="A104" s="50"/>
-      <c r="B104" s="50"/>
-      <c r="C104" s="50"/>
-      <c r="D104" s="50"/>
-      <c r="E104" s="50"/>
-      <c r="F104" s="50"/>
-      <c r="G104" s="186"/>
-      <c r="H104" s="50"/>
-      <c r="I104" s="50"/>
-      <c r="J104" s="50"/>
+      <c r="A104" s="160" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="B104" s="160"/>
+      <c r="C104" s="183"/>
+      <c r="D104" s="161"/>
+      <c r="E104" s="160" t="str">
+        <f t="shared" si="7"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F104" s="161"/>
+      <c r="G104" s="176" t="s">
+        <v>83</v>
+      </c>
+      <c r="H104" s="177">
+        <v>44304.0</v>
+      </c>
+      <c r="I104" s="178" t="s">
+        <v>375</v>
+      </c>
+      <c r="J104" s="179"/>
       <c r="K104" s="86"/>
       <c r="L104" s="11"/>
       <c r="M104" s="11"/>
@@ -32968,16 +33211,28 @@
       <c r="AA104" s="155"/>
     </row>
     <row r="105" ht="12.75" customHeight="1">
-      <c r="A105" s="50"/>
-      <c r="B105" s="50"/>
-      <c r="C105" s="50"/>
-      <c r="D105" s="50"/>
-      <c r="E105" s="50"/>
-      <c r="F105" s="50"/>
-      <c r="G105" s="186"/>
-      <c r="H105" s="50"/>
-      <c r="I105" s="50"/>
-      <c r="J105" s="50"/>
+      <c r="A105" s="160" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="B105" s="160"/>
+      <c r="C105" s="183"/>
+      <c r="D105" s="161"/>
+      <c r="E105" s="160" t="str">
+        <f t="shared" si="7"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F105" s="161"/>
+      <c r="G105" s="176" t="s">
+        <v>83</v>
+      </c>
+      <c r="H105" s="177">
+        <v>44304.0</v>
+      </c>
+      <c r="I105" s="178" t="s">
+        <v>375</v>
+      </c>
+      <c r="J105" s="179"/>
       <c r="K105" s="86"/>
       <c r="L105" s="11"/>
       <c r="M105" s="11"/>
@@ -32997,16 +33252,28 @@
       <c r="AA105" s="155"/>
     </row>
     <row r="106" ht="12.75" customHeight="1">
-      <c r="A106" s="50"/>
-      <c r="B106" s="50"/>
-      <c r="C106" s="50"/>
-      <c r="D106" s="50"/>
-      <c r="E106" s="50"/>
-      <c r="F106" s="50"/>
-      <c r="G106" s="186"/>
-      <c r="H106" s="50"/>
-      <c r="I106" s="50"/>
-      <c r="J106" s="50"/>
+      <c r="A106" s="160" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="B106" s="160"/>
+      <c r="C106" s="183"/>
+      <c r="D106" s="161"/>
+      <c r="E106" s="160" t="str">
+        <f t="shared" si="7"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F106" s="161"/>
+      <c r="G106" s="176" t="s">
+        <v>83</v>
+      </c>
+      <c r="H106" s="177">
+        <v>44304.0</v>
+      </c>
+      <c r="I106" s="178" t="s">
+        <v>375</v>
+      </c>
+      <c r="J106" s="179"/>
       <c r="K106" s="86"/>
       <c r="L106" s="11"/>
       <c r="M106" s="11"/>
@@ -33026,16 +33293,28 @@
       <c r="AA106" s="155"/>
     </row>
     <row r="107" ht="12.75" customHeight="1">
-      <c r="A107" s="50"/>
-      <c r="B107" s="50"/>
-      <c r="C107" s="50"/>
-      <c r="D107" s="50"/>
-      <c r="E107" s="50"/>
-      <c r="F107" s="50"/>
-      <c r="G107" s="186"/>
-      <c r="H107" s="50"/>
-      <c r="I107" s="50"/>
-      <c r="J107" s="50"/>
+      <c r="A107" s="160" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="B107" s="160"/>
+      <c r="C107" s="183"/>
+      <c r="D107" s="161"/>
+      <c r="E107" s="160" t="str">
+        <f t="shared" si="7"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F107" s="161"/>
+      <c r="G107" s="176" t="s">
+        <v>83</v>
+      </c>
+      <c r="H107" s="177">
+        <v>44304.0</v>
+      </c>
+      <c r="I107" s="178" t="s">
+        <v>375</v>
+      </c>
+      <c r="J107" s="179"/>
       <c r="K107" s="86"/>
       <c r="L107" s="11"/>
       <c r="M107" s="11"/>
@@ -33055,16 +33334,28 @@
       <c r="AA107" s="155"/>
     </row>
     <row r="108" ht="12.75" customHeight="1">
-      <c r="A108" s="50"/>
-      <c r="B108" s="50"/>
-      <c r="C108" s="50"/>
-      <c r="D108" s="50"/>
-      <c r="E108" s="50"/>
-      <c r="F108" s="50"/>
-      <c r="G108" s="186"/>
-      <c r="H108" s="50"/>
-      <c r="I108" s="50"/>
-      <c r="J108" s="50"/>
+      <c r="A108" s="160" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="B108" s="160"/>
+      <c r="C108" s="183"/>
+      <c r="D108" s="161"/>
+      <c r="E108" s="160" t="str">
+        <f t="shared" si="7"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F108" s="161"/>
+      <c r="G108" s="176" t="s">
+        <v>83</v>
+      </c>
+      <c r="H108" s="177">
+        <v>44304.0</v>
+      </c>
+      <c r="I108" s="178" t="s">
+        <v>375</v>
+      </c>
+      <c r="J108" s="179"/>
       <c r="K108" s="86"/>
       <c r="L108" s="11"/>
       <c r="M108" s="11"/>
@@ -33084,16 +33375,28 @@
       <c r="AA108" s="155"/>
     </row>
     <row r="109" ht="12.75" customHeight="1">
-      <c r="A109" s="50"/>
-      <c r="B109" s="50"/>
-      <c r="C109" s="50"/>
-      <c r="D109" s="50"/>
-      <c r="E109" s="50"/>
-      <c r="F109" s="50"/>
-      <c r="G109" s="186"/>
-      <c r="H109" s="50"/>
-      <c r="I109" s="50"/>
-      <c r="J109" s="50"/>
+      <c r="A109" s="160" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="B109" s="160"/>
+      <c r="C109" s="183"/>
+      <c r="D109" s="161"/>
+      <c r="E109" s="160" t="str">
+        <f t="shared" si="7"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F109" s="161"/>
+      <c r="G109" s="176" t="s">
+        <v>83</v>
+      </c>
+      <c r="H109" s="177">
+        <v>44304.0</v>
+      </c>
+      <c r="I109" s="178" t="s">
+        <v>375</v>
+      </c>
+      <c r="J109" s="179"/>
       <c r="K109" s="86"/>
       <c r="L109" s="11"/>
       <c r="M109" s="11"/>
@@ -33113,16 +33416,28 @@
       <c r="AA109" s="155"/>
     </row>
     <row r="110" ht="12.75" customHeight="1">
-      <c r="A110" s="50"/>
-      <c r="B110" s="50"/>
-      <c r="C110" s="50"/>
-      <c r="D110" s="50"/>
-      <c r="E110" s="50"/>
-      <c r="F110" s="50"/>
-      <c r="G110" s="186"/>
-      <c r="H110" s="50"/>
-      <c r="I110" s="50"/>
-      <c r="J110" s="50"/>
+      <c r="A110" s="160" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="B110" s="160"/>
+      <c r="C110" s="183"/>
+      <c r="D110" s="161"/>
+      <c r="E110" s="160" t="str">
+        <f t="shared" si="7"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F110" s="161"/>
+      <c r="G110" s="176" t="s">
+        <v>83</v>
+      </c>
+      <c r="H110" s="177">
+        <v>44304.0</v>
+      </c>
+      <c r="I110" s="178" t="s">
+        <v>375</v>
+      </c>
+      <c r="J110" s="179"/>
       <c r="K110" s="86"/>
       <c r="L110" s="11"/>
       <c r="M110" s="11"/>
@@ -33142,16 +33457,28 @@
       <c r="AA110" s="155"/>
     </row>
     <row r="111" ht="12.75" customHeight="1">
-      <c r="A111" s="50"/>
-      <c r="B111" s="50"/>
-      <c r="C111" s="50"/>
-      <c r="D111" s="50"/>
-      <c r="E111" s="50"/>
-      <c r="F111" s="50"/>
-      <c r="G111" s="186"/>
-      <c r="H111" s="50"/>
-      <c r="I111" s="50"/>
-      <c r="J111" s="50"/>
+      <c r="A111" s="160" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="B111" s="160"/>
+      <c r="C111" s="183"/>
+      <c r="D111" s="161"/>
+      <c r="E111" s="160" t="str">
+        <f t="shared" si="7"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F111" s="161"/>
+      <c r="G111" s="176" t="s">
+        <v>83</v>
+      </c>
+      <c r="H111" s="177">
+        <v>44304.0</v>
+      </c>
+      <c r="I111" s="178" t="s">
+        <v>375</v>
+      </c>
+      <c r="J111" s="179"/>
       <c r="K111" s="86"/>
       <c r="L111" s="11"/>
       <c r="M111" s="11"/>
@@ -33171,16 +33498,28 @@
       <c r="AA111" s="155"/>
     </row>
     <row r="112" ht="12.75" customHeight="1">
-      <c r="A112" s="50"/>
-      <c r="B112" s="50"/>
-      <c r="C112" s="50"/>
-      <c r="D112" s="50"/>
-      <c r="E112" s="50"/>
-      <c r="F112" s="50"/>
-      <c r="G112" s="186"/>
-      <c r="H112" s="50"/>
-      <c r="I112" s="50"/>
-      <c r="J112" s="50"/>
+      <c r="A112" s="160" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="B112" s="160"/>
+      <c r="C112" s="183"/>
+      <c r="D112" s="161"/>
+      <c r="E112" s="160" t="str">
+        <f t="shared" si="7"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F112" s="161"/>
+      <c r="G112" s="176" t="s">
+        <v>83</v>
+      </c>
+      <c r="H112" s="177">
+        <v>44304.0</v>
+      </c>
+      <c r="I112" s="178" t="s">
+        <v>375</v>
+      </c>
+      <c r="J112" s="179"/>
       <c r="K112" s="86"/>
       <c r="L112" s="11"/>
       <c r="M112" s="11"/>
@@ -33200,16 +33539,28 @@
       <c r="AA112" s="155"/>
     </row>
     <row r="113" ht="12.75" customHeight="1">
-      <c r="A113" s="50"/>
-      <c r="B113" s="50"/>
-      <c r="C113" s="50"/>
-      <c r="D113" s="50"/>
-      <c r="E113" s="50"/>
-      <c r="F113" s="50"/>
-      <c r="G113" s="186"/>
-      <c r="H113" s="50"/>
-      <c r="I113" s="50"/>
-      <c r="J113" s="50"/>
+      <c r="A113" s="160" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="B113" s="160"/>
+      <c r="C113" s="183"/>
+      <c r="D113" s="161"/>
+      <c r="E113" s="160" t="str">
+        <f t="shared" si="7"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F113" s="161"/>
+      <c r="G113" s="176" t="s">
+        <v>83</v>
+      </c>
+      <c r="H113" s="177">
+        <v>44304.0</v>
+      </c>
+      <c r="I113" s="178" t="s">
+        <v>375</v>
+      </c>
+      <c r="J113" s="179"/>
       <c r="K113" s="86"/>
       <c r="L113" s="11"/>
       <c r="M113" s="11"/>
@@ -33229,16 +33580,28 @@
       <c r="AA113" s="155"/>
     </row>
     <row r="114" ht="12.75" customHeight="1">
-      <c r="A114" s="50"/>
-      <c r="B114" s="50"/>
-      <c r="C114" s="50"/>
-      <c r="D114" s="50"/>
-      <c r="E114" s="50"/>
-      <c r="F114" s="50"/>
-      <c r="G114" s="50"/>
-      <c r="H114" s="50"/>
-      <c r="I114" s="50"/>
-      <c r="J114" s="50"/>
+      <c r="A114" s="160" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="B114" s="160"/>
+      <c r="C114" s="183"/>
+      <c r="D114" s="161"/>
+      <c r="E114" s="160" t="str">
+        <f t="shared" si="7"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F114" s="161"/>
+      <c r="G114" s="176" t="s">
+        <v>83</v>
+      </c>
+      <c r="H114" s="177">
+        <v>44304.0</v>
+      </c>
+      <c r="I114" s="178" t="s">
+        <v>375</v>
+      </c>
+      <c r="J114" s="179"/>
       <c r="K114" s="86"/>
       <c r="L114" s="11"/>
       <c r="M114" s="11"/>
@@ -33258,16 +33621,28 @@
       <c r="AA114" s="155"/>
     </row>
     <row r="115" ht="12.75" customHeight="1">
-      <c r="A115" s="50"/>
-      <c r="B115" s="50"/>
-      <c r="C115" s="50"/>
-      <c r="D115" s="50"/>
-      <c r="E115" s="50"/>
-      <c r="F115" s="50"/>
-      <c r="G115" s="50"/>
-      <c r="H115" s="50"/>
-      <c r="I115" s="50"/>
-      <c r="J115" s="50"/>
+      <c r="A115" s="160" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="B115" s="160"/>
+      <c r="C115" s="183"/>
+      <c r="D115" s="161"/>
+      <c r="E115" s="160" t="str">
+        <f t="shared" si="7"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F115" s="161"/>
+      <c r="G115" s="176" t="s">
+        <v>83</v>
+      </c>
+      <c r="H115" s="177">
+        <v>44304.0</v>
+      </c>
+      <c r="I115" s="178" t="s">
+        <v>375</v>
+      </c>
+      <c r="J115" s="179"/>
       <c r="K115" s="86"/>
       <c r="L115" s="11"/>
       <c r="M115" s="11"/>
@@ -33287,16 +33662,28 @@
       <c r="AA115" s="155"/>
     </row>
     <row r="116" ht="12.75" customHeight="1">
-      <c r="A116" s="50"/>
-      <c r="B116" s="50"/>
-      <c r="C116" s="50"/>
-      <c r="D116" s="50"/>
-      <c r="E116" s="50"/>
-      <c r="F116" s="50"/>
-      <c r="G116" s="50"/>
-      <c r="H116" s="50"/>
-      <c r="I116" s="50"/>
-      <c r="J116" s="50"/>
+      <c r="A116" s="160" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="B116" s="160"/>
+      <c r="C116" s="183"/>
+      <c r="D116" s="161"/>
+      <c r="E116" s="160" t="str">
+        <f t="shared" si="7"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F116" s="161"/>
+      <c r="G116" s="176" t="s">
+        <v>83</v>
+      </c>
+      <c r="H116" s="177">
+        <v>44304.0</v>
+      </c>
+      <c r="I116" s="178" t="s">
+        <v>375</v>
+      </c>
+      <c r="J116" s="179"/>
       <c r="K116" s="86"/>
       <c r="L116" s="11"/>
       <c r="M116" s="11"/>
@@ -33316,16 +33703,28 @@
       <c r="AA116" s="155"/>
     </row>
     <row r="117" ht="12.75" customHeight="1">
-      <c r="A117" s="50"/>
-      <c r="B117" s="50"/>
-      <c r="C117" s="50"/>
-      <c r="D117" s="50"/>
-      <c r="E117" s="50"/>
-      <c r="F117" s="50"/>
-      <c r="G117" s="50"/>
-      <c r="H117" s="50"/>
-      <c r="I117" s="50"/>
-      <c r="J117" s="50"/>
+      <c r="A117" s="160" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="B117" s="160"/>
+      <c r="C117" s="183"/>
+      <c r="D117" s="161"/>
+      <c r="E117" s="160" t="str">
+        <f t="shared" si="7"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F117" s="161"/>
+      <c r="G117" s="176" t="s">
+        <v>83</v>
+      </c>
+      <c r="H117" s="177">
+        <v>44304.0</v>
+      </c>
+      <c r="I117" s="178" t="s">
+        <v>375</v>
+      </c>
+      <c r="J117" s="179"/>
       <c r="K117" s="86"/>
       <c r="L117" s="11"/>
       <c r="M117" s="11"/>
@@ -33345,16 +33744,28 @@
       <c r="AA117" s="155"/>
     </row>
     <row r="118" ht="12.75" customHeight="1">
-      <c r="A118" s="50"/>
-      <c r="B118" s="50"/>
-      <c r="C118" s="50"/>
-      <c r="D118" s="50"/>
-      <c r="E118" s="50"/>
-      <c r="F118" s="50"/>
-      <c r="G118" s="50"/>
-      <c r="H118" s="50"/>
-      <c r="I118" s="50"/>
-      <c r="J118" s="50"/>
+      <c r="A118" s="160" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="B118" s="160"/>
+      <c r="C118" s="183"/>
+      <c r="D118" s="161"/>
+      <c r="E118" s="160" t="str">
+        <f t="shared" si="7"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F118" s="161"/>
+      <c r="G118" s="176" t="s">
+        <v>83</v>
+      </c>
+      <c r="H118" s="177">
+        <v>44304.0</v>
+      </c>
+      <c r="I118" s="178" t="s">
+        <v>375</v>
+      </c>
+      <c r="J118" s="179"/>
       <c r="K118" s="86"/>
       <c r="L118" s="11"/>
       <c r="M118" s="11"/>
@@ -35196,7 +35607,7 @@
     <mergeCell ref="B4:E4"/>
   </mergeCells>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G8:G73">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G8:G73 G101">
       <formula1>$M$2:$M$5</formula1>
     </dataValidation>
   </dataValidations>
@@ -35232,15 +35643,15 @@
   <sheetData>
     <row r="1" ht="25.5" customHeight="1">
       <c r="A1" s="11"/>
-      <c r="B1" s="187" t="s">
-        <v>541</v>
-      </c>
-      <c r="C1" s="188"/>
-      <c r="D1" s="188"/>
-      <c r="E1" s="188"/>
-      <c r="F1" s="188"/>
-      <c r="G1" s="188"/>
-      <c r="H1" s="188"/>
+      <c r="B1" s="184" t="s">
+        <v>561</v>
+      </c>
+      <c r="C1" s="185"/>
+      <c r="D1" s="185"/>
+      <c r="E1" s="185"/>
+      <c r="F1" s="185"/>
+      <c r="G1" s="185"/>
+      <c r="H1" s="185"/>
       <c r="I1" s="11"/>
       <c r="J1" s="11"/>
       <c r="K1" s="11"/>
@@ -35261,14 +35672,14 @@
       <c r="Z1" s="11"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="189"/>
-      <c r="B2" s="189"/>
+      <c r="A2" s="186"/>
+      <c r="B2" s="186"/>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
       <c r="F2" s="11"/>
       <c r="G2" s="11"/>
-      <c r="H2" s="190"/>
+      <c r="H2" s="187"/>
       <c r="I2" s="11"/>
       <c r="J2" s="11"/>
       <c r="K2" s="11"/>
@@ -35290,19 +35701,19 @@
     </row>
     <row r="3" ht="12.0" customHeight="1">
       <c r="A3" s="11"/>
-      <c r="B3" s="191" t="s">
+      <c r="B3" s="188" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="49" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="6"/>
-      <c r="E3" s="192" t="s">
+      <c r="E3" s="189" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="6"/>
-      <c r="G3" s="193"/>
-      <c r="H3" s="194" t="s">
+      <c r="G3" s="190"/>
+      <c r="H3" s="191" t="s">
         <v>4</v>
       </c>
       <c r="I3" s="11"/>
@@ -35326,19 +35737,19 @@
     </row>
     <row r="4" ht="12.0" customHeight="1">
       <c r="A4" s="11"/>
-      <c r="B4" s="191" t="s">
+      <c r="B4" s="188" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="49" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="6"/>
-      <c r="E4" s="192" t="s">
+      <c r="E4" s="189" t="s">
         <v>6</v>
       </c>
       <c r="F4" s="6"/>
-      <c r="G4" s="193"/>
-      <c r="H4" s="194" t="s">
+      <c r="G4" s="190"/>
+      <c r="H4" s="191" t="s">
         <v>7</v>
       </c>
       <c r="I4" s="11"/>
@@ -35362,7 +35773,7 @@
     </row>
     <row r="5" ht="12.0" customHeight="1">
       <c r="A5" s="11"/>
-      <c r="B5" s="195" t="s">
+      <c r="B5" s="192" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="49" t="str">
@@ -35370,12 +35781,12 @@
         <v>SoFa_Test Report_vx.x</v>
       </c>
       <c r="D5" s="6"/>
-      <c r="E5" s="192" t="s">
+      <c r="E5" s="189" t="s">
         <v>9</v>
       </c>
       <c r="F5" s="6"/>
-      <c r="G5" s="193"/>
-      <c r="H5" s="196">
+      <c r="G5" s="190"/>
+      <c r="H5" s="193">
         <v>44534.0</v>
       </c>
       <c r="I5" s="11"/>
@@ -35398,12 +35809,12 @@
       <c r="Z5" s="11"/>
     </row>
     <row r="6" ht="21.75" customHeight="1">
-      <c r="A6" s="189"/>
-      <c r="B6" s="195" t="s">
-        <v>542</v>
-      </c>
-      <c r="C6" s="197" t="s">
-        <v>543</v>
+      <c r="A6" s="186"/>
+      <c r="B6" s="192" t="s">
+        <v>562</v>
+      </c>
+      <c r="C6" s="194" t="s">
+        <v>563</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -35430,14 +35841,14 @@
       <c r="Z6" s="11"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="189"/>
+      <c r="A7" s="186"/>
       <c r="B7" s="25"/>
-      <c r="C7" s="198"/>
+      <c r="C7" s="195"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
-      <c r="H7" s="190"/>
+      <c r="H7" s="187"/>
       <c r="I7" s="11"/>
       <c r="J7" s="11"/>
       <c r="K7" s="11"/>
@@ -35460,12 +35871,12 @@
     <row r="8" ht="12.75" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="25"/>
-      <c r="C8" s="198"/>
+      <c r="C8" s="195"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
-      <c r="H8" s="190"/>
+      <c r="H8" s="187"/>
       <c r="I8" s="11"/>
       <c r="J8" s="11"/>
       <c r="K8" s="11"/>
@@ -35514,27 +35925,27 @@
       <c r="Z9" s="11"/>
     </row>
     <row r="10" ht="12.75" customHeight="1">
-      <c r="A10" s="199"/>
-      <c r="B10" s="200" t="s">
+      <c r="A10" s="196"/>
+      <c r="B10" s="197" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="201" t="s">
-        <v>544</v>
-      </c>
-      <c r="D10" s="202" t="s">
+      <c r="C10" s="198" t="s">
+        <v>564</v>
+      </c>
+      <c r="D10" s="199" t="s">
         <v>83</v>
       </c>
-      <c r="E10" s="201" t="s">
+      <c r="E10" s="198" t="s">
         <v>86</v>
       </c>
-      <c r="F10" s="201" t="s">
+      <c r="F10" s="198" t="s">
         <v>89</v>
       </c>
-      <c r="G10" s="203" t="s">
+      <c r="G10" s="200" t="s">
         <v>90</v>
       </c>
-      <c r="H10" s="204" t="s">
-        <v>545</v>
+      <c r="H10" s="201" t="s">
+        <v>565</v>
       </c>
       <c r="I10" s="11"/>
       <c r="J10" s="11"/>
@@ -35556,31 +35967,31 @@
       <c r="Z10" s="11"/>
     </row>
     <row r="11" ht="12.75" customHeight="1">
-      <c r="A11" s="199"/>
-      <c r="B11" s="205">
+      <c r="A11" s="196"/>
+      <c r="B11" s="202">
         <v>1.0</v>
       </c>
-      <c r="C11" s="206" t="str">
+      <c r="C11" s="203" t="str">
         <f>Guest!B2</f>
         <v>Guest</v>
       </c>
-      <c r="D11" s="207">
+      <c r="D11" s="204">
         <f>Guest!A6</f>
         <v>43</v>
       </c>
-      <c r="E11" s="207">
+      <c r="E11" s="204">
         <f>Guest!B6</f>
         <v>4</v>
       </c>
-      <c r="F11" s="207">
+      <c r="F11" s="204">
         <f>Guest!C6</f>
         <v>3</v>
       </c>
-      <c r="G11" s="208">
+      <c r="G11" s="205">
         <f>Guest!D6</f>
         <v>0</v>
       </c>
-      <c r="H11" s="209">
+      <c r="H11" s="206">
         <f>Guest!E6</f>
         <v>50</v>
       </c>
@@ -35604,31 +36015,31 @@
       <c r="Z11" s="11"/>
     </row>
     <row r="12" ht="12.75" customHeight="1">
-      <c r="A12" s="199"/>
-      <c r="B12" s="205">
+      <c r="A12" s="196"/>
+      <c r="B12" s="202">
         <v>2.0</v>
       </c>
-      <c r="C12" s="206" t="str">
+      <c r="C12" s="203" t="str">
         <f>User!B2</f>
         <v>User</v>
       </c>
-      <c r="D12" s="207">
+      <c r="D12" s="204">
         <f>User!A6</f>
         <v>0</v>
       </c>
-      <c r="E12" s="207">
+      <c r="E12" s="204">
         <f>User!B6</f>
         <v>0</v>
       </c>
-      <c r="F12" s="207">
+      <c r="F12" s="204">
         <f>User!C6</f>
         <v>51</v>
       </c>
-      <c r="G12" s="207">
+      <c r="G12" s="204">
         <f>User!D6</f>
         <v>0</v>
       </c>
-      <c r="H12" s="207">
+      <c r="H12" s="204">
         <f>User!E6</f>
         <v>51</v>
       </c>
@@ -35652,31 +36063,31 @@
       <c r="Z12" s="11"/>
     </row>
     <row r="13" ht="12.75" customHeight="1">
-      <c r="A13" s="199"/>
-      <c r="B13" s="205">
+      <c r="A13" s="196"/>
+      <c r="B13" s="202">
         <v>1.0</v>
       </c>
-      <c r="C13" s="206" t="str">
+      <c r="C13" s="203" t="str">
         <f>Manager!B2</f>
         <v>Manager</v>
       </c>
-      <c r="D13" s="207">
+      <c r="D13" s="204">
         <f>Manager!A6</f>
         <v>0</v>
       </c>
-      <c r="E13" s="207">
+      <c r="E13" s="204">
         <f>Manager!B6</f>
         <v>0</v>
       </c>
-      <c r="F13" s="207">
+      <c r="F13" s="204">
         <f>Manager!C6</f>
         <v>0</v>
       </c>
-      <c r="G13" s="208">
+      <c r="G13" s="205">
         <f>Manager!D6</f>
         <v>0</v>
       </c>
-      <c r="H13" s="209">
+      <c r="H13" s="206">
         <f>Manager!E6</f>
         <v>0</v>
       </c>
@@ -35700,28 +36111,28 @@
       <c r="Z13" s="11"/>
     </row>
     <row r="14" ht="12.75" customHeight="1">
-      <c r="A14" s="199"/>
-      <c r="B14" s="210"/>
-      <c r="C14" s="211" t="s">
-        <v>546</v>
-      </c>
-      <c r="D14" s="212">
+      <c r="A14" s="196"/>
+      <c r="B14" s="207"/>
+      <c r="C14" s="208" t="s">
+        <v>566</v>
+      </c>
+      <c r="D14" s="209">
         <f t="shared" ref="D14:H14" si="1">SUM(D9:D13)</f>
         <v>43</v>
       </c>
-      <c r="E14" s="212">
+      <c r="E14" s="209">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="F14" s="212">
+      <c r="F14" s="209">
         <f t="shared" si="1"/>
         <v>54</v>
       </c>
-      <c r="G14" s="212">
+      <c r="G14" s="209">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H14" s="213">
+      <c r="H14" s="210">
         <f t="shared" si="1"/>
         <v>101</v>
       </c>
@@ -35746,13 +36157,13 @@
     </row>
     <row r="15" ht="12.75" customHeight="1">
       <c r="A15" s="11"/>
-      <c r="B15" s="214"/>
+      <c r="B15" s="211"/>
       <c r="C15" s="11"/>
-      <c r="D15" s="215"/>
-      <c r="E15" s="216"/>
-      <c r="F15" s="216"/>
-      <c r="G15" s="216"/>
-      <c r="H15" s="216"/>
+      <c r="D15" s="212"/>
+      <c r="E15" s="213"/>
+      <c r="F15" s="213"/>
+      <c r="G15" s="213"/>
+      <c r="H15" s="213"/>
       <c r="I15" s="11"/>
       <c r="J15" s="11"/>
       <c r="K15" s="11"/>
@@ -35776,15 +36187,15 @@
       <c r="A16" s="11"/>
       <c r="B16" s="11"/>
       <c r="C16" s="9" t="s">
-        <v>547</v>
+        <v>567</v>
       </c>
       <c r="D16" s="11"/>
-      <c r="E16" s="217">
+      <c r="E16" s="214">
         <f>(D14+E14)*100/(H14-G14)</f>
         <v>46.53465347</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>548</v>
+        <v>568</v>
       </c>
       <c r="G16" s="11"/>
       <c r="H16" s="132"/>
@@ -35811,15 +36222,15 @@
       <c r="A17" s="11"/>
       <c r="B17" s="11"/>
       <c r="C17" s="9" t="s">
-        <v>549</v>
+        <v>569</v>
       </c>
       <c r="D17" s="11"/>
-      <c r="E17" s="217">
+      <c r="E17" s="214">
         <f>D14*100/(H14-G14)</f>
         <v>42.57425743</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>548</v>
+        <v>568</v>
       </c>
       <c r="G17" s="11"/>
       <c r="H17" s="132"/>

</xml_diff>

<commit_message>
HoangNH - Update test case manage report
</commit_message>
<xml_diff>
--- a/3. Users/HoangNHHE130395/Testing/TestCase - Hoang.xlsx
+++ b/3. Users/HoangNHHE130395/Testing/TestCase - Hoang.xlsx
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1258" uniqueCount="570">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1318" uniqueCount="605">
   <si>
     <t>SYSTEM TEST CASE</t>
   </si>
@@ -2493,7 +2493,148 @@
 3. The post is deleted and back to list post</t>
   </si>
   <si>
-    <t>Function Manage Voucher</t>
+    <t>Function Manage Report</t>
+  </si>
+  <si>
+    <t>Check GUI list reports post</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+ 2. Click on 'Report' tab in the menu bar</t>
+  </si>
+  <si>
+    <t>1. Display the list ò reports by following: ID, From Account, To post, Posted by, Reason, Status, Detail, Option
+ 2. The data of post is mapping wit the column name</t>
+  </si>
+  <si>
+    <t>Check GUI of button 'View detail' of list report post</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Login into the web server
+ 2. Click on 'Report' tab in the menu bar
+ </t>
+  </si>
+  <si>
+    <t>1. Display button 'View' in column Detail</t>
+  </si>
+  <si>
+    <t>Check function click on 'From Account' of list reports post</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'Report' tab in the menu bar
+3. Click on the 'From Account' 'Viên1 Mai'</t>
+  </si>
+  <si>
+    <t>1. Navigate to user 'Viên1 Mai' detail information</t>
+  </si>
+  <si>
+    <t>1. User 'Viên1 Mai'</t>
+  </si>
+  <si>
+    <t>Check function click on 'Posted By' of list reports post</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'Report' tab in the menu bar
+3. Click on the 'Posted By' 'Mai Văn Viên'</t>
+  </si>
+  <si>
+    <t>1. Navigate to user 'Mai Văn Viên' detail information</t>
+  </si>
+  <si>
+    <t>1. User 'Mai Văn Viên'</t>
+  </si>
+  <si>
+    <t>Check function of button 'View' of list reports post</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'Report' tab in the menu bar
+3. From report have id= '11' click 'View'</t>
+  </si>
+  <si>
+    <t>1. Report have id = '11'
+2. Post have id = '87'</t>
+  </si>
+  <si>
+    <t>Check function button 'Delete'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Login into the web server
+2. Click on 'Report' tab in the menu bar
+3. From report have id= '12' click 'Delete'
+</t>
+  </si>
+  <si>
+    <t>1. Display popup confirm 'Bạn có muốn xoá post này'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Report have id = '12'
+</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'Report' tab in the menu bar
+3. From report have id= '12' click 'Delete'
+5. Click on 'Hủy'</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'Report' tab in the menu bar
+3. From report have id= '12' click 'Delete'
+5. Click on 'Ok'</t>
+  </si>
+  <si>
+    <t>1. Popup is disappeared
+2. Toast message 'Xóa bài đăng thành công'
+3. The post's status is deleted</t>
+  </si>
+  <si>
+    <t>Check GUI list reports user</t>
+  </si>
+  <si>
+    <t>1. Display the list ò reports by following: ID, From Account, To Account, Reason, Status, Detail, Option
+ 2. The data of post is mapping wit the column name</t>
+  </si>
+  <si>
+    <t>Check GUI of button 'View detail' of list report user</t>
+  </si>
+  <si>
+    <t>Check function click on 'From Account' of list reports user</t>
+  </si>
+  <si>
+    <t>Check function click on 'To Account' of list reports user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Login into the web server
+2. Click on 'Report' tab in the menu bar
+3. From report have id= '18' click 'Ban'
+</t>
+  </si>
+  <si>
+    <t>1. Display popup confirm 'Bạn có muốn ban user này'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Report have id = '18'
+</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'Report' tab in the menu bar
+3. From report have id= '18' click 'Ban'
+5. Click on 'Hủy'</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'Report' tab in the menu bar
+3. From report have id= '18' click 'Delete'
+5. Click on 'Ok'</t>
+  </si>
+  <si>
+    <t>1. Popup is disappeared
+2. Toast message 'Ban user thành công'
+3. The user's status is banned</t>
   </si>
   <si>
     <t>TEST REPORT</t>
@@ -2532,7 +2673,7 @@
     <numFmt numFmtId="165" formatCode="d\-mmm\-yy"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="33">
+  <fonts count="34">
     <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
@@ -2690,6 +2831,11 @@
     <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
+      <name val="&quot;Times New Roman&quot;"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color theme="1"/>
       <name val="&quot;Times New Roman&quot;"/>
     </font>
     <font>
@@ -3374,7 +3520,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="215">
+  <cellXfs count="217">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -3857,6 +4003,12 @@
     <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
+    <xf borderId="13" fillId="0" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="13" fillId="0" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
     <xf borderId="24" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3914,14 +4066,14 @@
     <xf borderId="57" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="58" fillId="3" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="58" fillId="3" fontId="32" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="21" fillId="3" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="21" fillId="3" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="21" fillId="3" fontId="32" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="59" fillId="3" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="59" fillId="3" fontId="32" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -3933,7 +4085,7 @@
     <xf borderId="1" fillId="2" fontId="1" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="32" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="2" fontId="33" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -28348,7 +28500,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.13"/>
+    <col customWidth="1" min="1" max="1" width="22.0"/>
     <col customWidth="1" min="2" max="2" width="22.25"/>
     <col customWidth="1" min="3" max="3" width="39.75"/>
     <col customWidth="1" min="4" max="4" width="35.5"/>
@@ -32311,7 +32463,7 @@
       <c r="B85" s="160" t="s">
         <v>535</v>
       </c>
-      <c r="C85" s="183" t="s">
+      <c r="C85" s="167" t="s">
         <v>536</v>
       </c>
       <c r="D85" s="161" t="s">
@@ -32358,7 +32510,7 @@
       <c r="B86" s="160" t="s">
         <v>535</v>
       </c>
-      <c r="C86" s="183" t="s">
+      <c r="C86" s="167" t="s">
         <v>537</v>
       </c>
       <c r="D86" s="161" t="s">
@@ -32405,7 +32557,7 @@
       <c r="B87" s="160" t="s">
         <v>535</v>
       </c>
-      <c r="C87" s="183" t="s">
+      <c r="C87" s="167" t="s">
         <v>538</v>
       </c>
       <c r="D87" s="161" t="s">
@@ -32452,7 +32604,7 @@
       <c r="B88" s="160" t="s">
         <v>535</v>
       </c>
-      <c r="C88" s="183" t="s">
+      <c r="C88" s="167" t="s">
         <v>539</v>
       </c>
       <c r="D88" s="161" t="s">
@@ -32499,7 +32651,7 @@
       <c r="B89" s="160" t="s">
         <v>535</v>
       </c>
-      <c r="C89" s="183" t="s">
+      <c r="C89" s="167" t="s">
         <v>540</v>
       </c>
       <c r="D89" s="161" t="s">
@@ -32643,7 +32795,7 @@
       <c r="C92" s="182" t="s">
         <v>542</v>
       </c>
-      <c r="D92" s="183" t="s">
+      <c r="D92" s="167" t="s">
         <v>547</v>
       </c>
       <c r="E92" s="173" t="s">
@@ -32688,7 +32840,7 @@
       <c r="B93" s="160" t="s">
         <v>549</v>
       </c>
-      <c r="C93" s="183" t="s">
+      <c r="C93" s="167" t="s">
         <v>536</v>
       </c>
       <c r="D93" s="161" t="s">
@@ -32735,7 +32887,7 @@
       <c r="B94" s="160" t="s">
         <v>549</v>
       </c>
-      <c r="C94" s="183" t="s">
+      <c r="C94" s="167" t="s">
         <v>550</v>
       </c>
       <c r="D94" s="161" t="s">
@@ -32782,7 +32934,7 @@
       <c r="B95" s="160" t="s">
         <v>549</v>
       </c>
-      <c r="C95" s="183" t="s">
+      <c r="C95" s="167" t="s">
         <v>551</v>
       </c>
       <c r="D95" s="161" t="s">
@@ -32829,7 +32981,7 @@
       <c r="B96" s="160" t="s">
         <v>549</v>
       </c>
-      <c r="C96" s="183" t="s">
+      <c r="C96" s="167" t="s">
         <v>552</v>
       </c>
       <c r="D96" s="161" t="s">
@@ -32876,7 +33028,7 @@
       <c r="B97" s="160" t="s">
         <v>549</v>
       </c>
-      <c r="C97" s="183" t="s">
+      <c r="C97" s="167" t="s">
         <v>553</v>
       </c>
       <c r="D97" s="161" t="s">
@@ -32923,7 +33075,7 @@
       <c r="B98" s="160" t="s">
         <v>554</v>
       </c>
-      <c r="C98" s="183" t="s">
+      <c r="C98" s="167" t="s">
         <v>555</v>
       </c>
       <c r="D98" s="161" t="s">
@@ -32970,7 +33122,7 @@
       <c r="B99" s="160" t="s">
         <v>554</v>
       </c>
-      <c r="C99" s="183" t="s">
+      <c r="C99" s="167" t="s">
         <v>557</v>
       </c>
       <c r="D99" s="161" t="s">
@@ -33017,7 +33169,7 @@
       <c r="B100" s="160" t="s">
         <v>554</v>
       </c>
-      <c r="C100" s="183" t="s">
+      <c r="C100" s="167" t="s">
         <v>558</v>
       </c>
       <c r="D100" s="161" t="s">
@@ -33087,14 +33239,20 @@
       <c r="Z101" s="11"/>
       <c r="AA101" s="155"/>
     </row>
-    <row r="102" ht="12.75" customHeight="1">
+    <row r="102" ht="78.75" customHeight="1">
       <c r="A102" s="160" t="str">
         <f t="shared" ref="A102:A118" si="6">IF(OR(B102&lt;&gt;"",D102&lt;&gt;""),"["&amp;TEXT($B$2,"##")&amp;"-"&amp;TEXT(ROW()-9,"##")&amp;"]","")</f>
-        <v/>
-      </c>
-      <c r="B102" s="160"/>
-      <c r="C102" s="183"/>
-      <c r="D102" s="161"/>
+        <v>[Manager-93]</v>
+      </c>
+      <c r="B102" s="173" t="s">
+        <v>561</v>
+      </c>
+      <c r="C102" s="182" t="s">
+        <v>562</v>
+      </c>
+      <c r="D102" s="182" t="s">
+        <v>563</v>
+      </c>
       <c r="E102" s="160" t="str">
         <f t="shared" ref="E102:E118" si="7">$A$10</f>
         <v>[Manager-1]</v>
@@ -33128,14 +33286,20 @@
       <c r="Z102" s="11"/>
       <c r="AA102" s="155"/>
     </row>
-    <row r="103" ht="12.75" customHeight="1">
+    <row r="103" ht="42.0" customHeight="1">
       <c r="A103" s="160" t="str">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="B103" s="160"/>
-      <c r="C103" s="183"/>
-      <c r="D103" s="161"/>
+        <v>[Manager-94]</v>
+      </c>
+      <c r="B103" s="173" t="s">
+        <v>564</v>
+      </c>
+      <c r="C103" s="182" t="s">
+        <v>565</v>
+      </c>
+      <c r="D103" s="182" t="s">
+        <v>566</v>
+      </c>
       <c r="E103" s="160" t="str">
         <f t="shared" si="7"/>
         <v>[Manager-1]</v>
@@ -33169,19 +33333,27 @@
       <c r="Z103" s="11"/>
       <c r="AA103" s="155"/>
     </row>
-    <row r="104" ht="12.75" customHeight="1">
+    <row r="104" ht="57.75" customHeight="1">
       <c r="A104" s="160" t="str">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="B104" s="160"/>
-      <c r="C104" s="183"/>
-      <c r="D104" s="161"/>
+        <v>[Manager-95]</v>
+      </c>
+      <c r="B104" s="160" t="s">
+        <v>567</v>
+      </c>
+      <c r="C104" s="183" t="s">
+        <v>568</v>
+      </c>
+      <c r="D104" s="183" t="s">
+        <v>569</v>
+      </c>
       <c r="E104" s="160" t="str">
         <f t="shared" si="7"/>
         <v>[Manager-1]</v>
       </c>
-      <c r="F104" s="161"/>
+      <c r="F104" s="161" t="s">
+        <v>570</v>
+      </c>
       <c r="G104" s="176" t="s">
         <v>83</v>
       </c>
@@ -33210,19 +33382,27 @@
       <c r="Z104" s="11"/>
       <c r="AA104" s="155"/>
     </row>
-    <row r="105" ht="12.75" customHeight="1">
+    <row r="105" ht="51.75" customHeight="1">
       <c r="A105" s="160" t="str">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="B105" s="160"/>
-      <c r="C105" s="183"/>
-      <c r="D105" s="161"/>
+        <v>[Manager-96]</v>
+      </c>
+      <c r="B105" s="160" t="s">
+        <v>571</v>
+      </c>
+      <c r="C105" s="183" t="s">
+        <v>572</v>
+      </c>
+      <c r="D105" s="183" t="s">
+        <v>573</v>
+      </c>
       <c r="E105" s="160" t="str">
         <f t="shared" si="7"/>
         <v>[Manager-1]</v>
       </c>
-      <c r="F105" s="161"/>
+      <c r="F105" s="161" t="s">
+        <v>574</v>
+      </c>
       <c r="G105" s="176" t="s">
         <v>83</v>
       </c>
@@ -33251,19 +33431,27 @@
       <c r="Z105" s="11"/>
       <c r="AA105" s="155"/>
     </row>
-    <row r="106" ht="12.75" customHeight="1">
+    <row r="106" ht="59.25" customHeight="1">
       <c r="A106" s="160" t="str">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="B106" s="160"/>
-      <c r="C106" s="183"/>
-      <c r="D106" s="161"/>
+        <v>[Manager-97]</v>
+      </c>
+      <c r="B106" s="160" t="s">
+        <v>575</v>
+      </c>
+      <c r="C106" s="183" t="s">
+        <v>576</v>
+      </c>
+      <c r="D106" s="183" t="s">
+        <v>493</v>
+      </c>
       <c r="E106" s="160" t="str">
         <f t="shared" si="7"/>
         <v>[Manager-1]</v>
       </c>
-      <c r="F106" s="161"/>
+      <c r="F106" s="161" t="s">
+        <v>577</v>
+      </c>
       <c r="G106" s="176" t="s">
         <v>83</v>
       </c>
@@ -33292,19 +33480,27 @@
       <c r="Z106" s="11"/>
       <c r="AA106" s="155"/>
     </row>
-    <row r="107" ht="12.75" customHeight="1">
+    <row r="107" ht="56.25" customHeight="1">
       <c r="A107" s="160" t="str">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="B107" s="160"/>
-      <c r="C107" s="183"/>
-      <c r="D107" s="161"/>
+        <v>[Manager-98]</v>
+      </c>
+      <c r="B107" s="160" t="s">
+        <v>575</v>
+      </c>
+      <c r="C107" s="183" t="s">
+        <v>576</v>
+      </c>
+      <c r="D107" s="183" t="s">
+        <v>493</v>
+      </c>
       <c r="E107" s="160" t="str">
         <f t="shared" si="7"/>
         <v>[Manager-1]</v>
       </c>
-      <c r="F107" s="161"/>
+      <c r="F107" s="161" t="s">
+        <v>577</v>
+      </c>
       <c r="G107" s="176" t="s">
         <v>83</v>
       </c>
@@ -33333,19 +33529,27 @@
       <c r="Z107" s="11"/>
       <c r="AA107" s="155"/>
     </row>
-    <row r="108" ht="12.75" customHeight="1">
+    <row r="108" ht="75.75" customHeight="1">
       <c r="A108" s="160" t="str">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="B108" s="160"/>
-      <c r="C108" s="183"/>
-      <c r="D108" s="161"/>
+        <v>[Manager-99]</v>
+      </c>
+      <c r="B108" s="160" t="s">
+        <v>578</v>
+      </c>
+      <c r="C108" s="183" t="s">
+        <v>579</v>
+      </c>
+      <c r="D108" s="161" t="s">
+        <v>580</v>
+      </c>
       <c r="E108" s="160" t="str">
         <f t="shared" si="7"/>
         <v>[Manager-1]</v>
       </c>
-      <c r="F108" s="161"/>
+      <c r="F108" s="161" t="s">
+        <v>581</v>
+      </c>
       <c r="G108" s="176" t="s">
         <v>83</v>
       </c>
@@ -33374,19 +33578,27 @@
       <c r="Z108" s="11"/>
       <c r="AA108" s="155"/>
     </row>
-    <row r="109" ht="12.75" customHeight="1">
+    <row r="109" ht="88.5" customHeight="1">
       <c r="A109" s="160" t="str">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="B109" s="160"/>
-      <c r="C109" s="183"/>
-      <c r="D109" s="161"/>
+        <v>[Manager-100]</v>
+      </c>
+      <c r="B109" s="160" t="s">
+        <v>578</v>
+      </c>
+      <c r="C109" s="183" t="s">
+        <v>582</v>
+      </c>
+      <c r="D109" s="161" t="s">
+        <v>457</v>
+      </c>
       <c r="E109" s="160" t="str">
         <f t="shared" si="7"/>
         <v>[Manager-1]</v>
       </c>
-      <c r="F109" s="161"/>
+      <c r="F109" s="161" t="s">
+        <v>581</v>
+      </c>
       <c r="G109" s="176" t="s">
         <v>83</v>
       </c>
@@ -33415,26 +33627,34 @@
       <c r="Z109" s="11"/>
       <c r="AA109" s="155"/>
     </row>
-    <row r="110" ht="12.75" customHeight="1">
+    <row r="110" ht="92.25" customHeight="1">
       <c r="A110" s="160" t="str">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="B110" s="160"/>
-      <c r="C110" s="183"/>
-      <c r="D110" s="161"/>
+        <v>[Manager-101]</v>
+      </c>
+      <c r="B110" s="160" t="s">
+        <v>578</v>
+      </c>
+      <c r="C110" s="183" t="s">
+        <v>583</v>
+      </c>
+      <c r="D110" s="161" t="s">
+        <v>584</v>
+      </c>
       <c r="E110" s="160" t="str">
         <f t="shared" si="7"/>
         <v>[Manager-1]</v>
       </c>
-      <c r="F110" s="161"/>
+      <c r="F110" s="161" t="s">
+        <v>581</v>
+      </c>
       <c r="G110" s="176" t="s">
         <v>83</v>
       </c>
       <c r="H110" s="177">
         <v>44304.0</v>
       </c>
-      <c r="I110" s="178" t="s">
+      <c r="I110" s="184" t="s">
         <v>375</v>
       </c>
       <c r="J110" s="179"/>
@@ -33456,14 +33676,20 @@
       <c r="Z110" s="11"/>
       <c r="AA110" s="155"/>
     </row>
-    <row r="111" ht="12.75" customHeight="1">
+    <row r="111" ht="71.25" customHeight="1">
       <c r="A111" s="160" t="str">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="B111" s="160"/>
-      <c r="C111" s="183"/>
-      <c r="D111" s="161"/>
+        <v>[Manager-102]</v>
+      </c>
+      <c r="B111" s="173" t="s">
+        <v>585</v>
+      </c>
+      <c r="C111" s="185" t="s">
+        <v>562</v>
+      </c>
+      <c r="D111" s="185" t="s">
+        <v>586</v>
+      </c>
       <c r="E111" s="160" t="str">
         <f t="shared" si="7"/>
         <v>[Manager-1]</v>
@@ -33475,7 +33701,7 @@
       <c r="H111" s="177">
         <v>44304.0</v>
       </c>
-      <c r="I111" s="178" t="s">
+      <c r="I111" s="184" t="s">
         <v>375</v>
       </c>
       <c r="J111" s="179"/>
@@ -33497,14 +33723,20 @@
       <c r="Z111" s="11"/>
       <c r="AA111" s="155"/>
     </row>
-    <row r="112" ht="12.75" customHeight="1">
+    <row r="112" ht="50.25" customHeight="1">
       <c r="A112" s="160" t="str">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="B112" s="160"/>
-      <c r="C112" s="183"/>
-      <c r="D112" s="161"/>
+        <v>[Manager-103]</v>
+      </c>
+      <c r="B112" s="173" t="s">
+        <v>587</v>
+      </c>
+      <c r="C112" s="185" t="s">
+        <v>565</v>
+      </c>
+      <c r="D112" s="185" t="s">
+        <v>566</v>
+      </c>
       <c r="E112" s="160" t="str">
         <f t="shared" si="7"/>
         <v>[Manager-1]</v>
@@ -33516,7 +33748,7 @@
       <c r="H112" s="177">
         <v>44304.0</v>
       </c>
-      <c r="I112" s="178" t="s">
+      <c r="I112" s="184" t="s">
         <v>375</v>
       </c>
       <c r="J112" s="179"/>
@@ -33538,19 +33770,27 @@
       <c r="Z112" s="11"/>
       <c r="AA112" s="155"/>
     </row>
-    <row r="113" ht="12.75" customHeight="1">
+    <row r="113" ht="63.0" customHeight="1">
       <c r="A113" s="160" t="str">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="B113" s="160"/>
-      <c r="C113" s="183"/>
-      <c r="D113" s="161"/>
+        <v>[Manager-104]</v>
+      </c>
+      <c r="B113" s="160" t="s">
+        <v>588</v>
+      </c>
+      <c r="C113" s="183" t="s">
+        <v>568</v>
+      </c>
+      <c r="D113" s="183" t="s">
+        <v>569</v>
+      </c>
       <c r="E113" s="160" t="str">
         <f t="shared" si="7"/>
         <v>[Manager-1]</v>
       </c>
-      <c r="F113" s="161"/>
+      <c r="F113" s="161" t="s">
+        <v>570</v>
+      </c>
       <c r="G113" s="176" t="s">
         <v>83</v>
       </c>
@@ -33579,19 +33819,27 @@
       <c r="Z113" s="11"/>
       <c r="AA113" s="155"/>
     </row>
-    <row r="114" ht="12.75" customHeight="1">
+    <row r="114" ht="52.5" customHeight="1">
       <c r="A114" s="160" t="str">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="B114" s="160"/>
-      <c r="C114" s="183"/>
-      <c r="D114" s="161"/>
+        <v>[Manager-105]</v>
+      </c>
+      <c r="B114" s="160" t="s">
+        <v>589</v>
+      </c>
+      <c r="C114" s="183" t="s">
+        <v>572</v>
+      </c>
+      <c r="D114" s="183" t="s">
+        <v>573</v>
+      </c>
       <c r="E114" s="160" t="str">
         <f t="shared" si="7"/>
         <v>[Manager-1]</v>
       </c>
-      <c r="F114" s="161"/>
+      <c r="F114" s="161" t="s">
+        <v>574</v>
+      </c>
       <c r="G114" s="176" t="s">
         <v>83</v>
       </c>
@@ -33620,19 +33868,27 @@
       <c r="Z114" s="11"/>
       <c r="AA114" s="155"/>
     </row>
-    <row r="115" ht="12.75" customHeight="1">
+    <row r="115" ht="51.75" customHeight="1">
       <c r="A115" s="160" t="str">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="B115" s="160"/>
-      <c r="C115" s="183"/>
-      <c r="D115" s="161"/>
+        <v>[Manager-106]</v>
+      </c>
+      <c r="B115" s="160" t="s">
+        <v>443</v>
+      </c>
+      <c r="C115" s="183" t="s">
+        <v>590</v>
+      </c>
+      <c r="D115" s="161" t="s">
+        <v>591</v>
+      </c>
       <c r="E115" s="160" t="str">
         <f t="shared" si="7"/>
         <v>[Manager-1]</v>
       </c>
-      <c r="F115" s="161"/>
+      <c r="F115" s="161" t="s">
+        <v>592</v>
+      </c>
       <c r="G115" s="176" t="s">
         <v>83</v>
       </c>
@@ -33661,19 +33917,27 @@
       <c r="Z115" s="11"/>
       <c r="AA115" s="155"/>
     </row>
-    <row r="116" ht="12.75" customHeight="1">
+    <row r="116" ht="67.5" customHeight="1">
       <c r="A116" s="160" t="str">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="B116" s="160"/>
-      <c r="C116" s="183"/>
-      <c r="D116" s="161"/>
+        <v>[Manager-107]</v>
+      </c>
+      <c r="B116" s="160" t="s">
+        <v>443</v>
+      </c>
+      <c r="C116" s="183" t="s">
+        <v>593</v>
+      </c>
+      <c r="D116" s="161" t="s">
+        <v>457</v>
+      </c>
       <c r="E116" s="160" t="str">
         <f t="shared" si="7"/>
         <v>[Manager-1]</v>
       </c>
-      <c r="F116" s="161"/>
+      <c r="F116" s="161" t="s">
+        <v>592</v>
+      </c>
       <c r="G116" s="176" t="s">
         <v>83</v>
       </c>
@@ -33702,19 +33966,27 @@
       <c r="Z116" s="11"/>
       <c r="AA116" s="155"/>
     </row>
-    <row r="117" ht="12.75" customHeight="1">
+    <row r="117" ht="67.5" customHeight="1">
       <c r="A117" s="160" t="str">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="B117" s="160"/>
-      <c r="C117" s="183"/>
-      <c r="D117" s="161"/>
+        <v>[Manager-108]</v>
+      </c>
+      <c r="B117" s="160" t="s">
+        <v>443</v>
+      </c>
+      <c r="C117" s="183" t="s">
+        <v>594</v>
+      </c>
+      <c r="D117" s="161" t="s">
+        <v>595</v>
+      </c>
       <c r="E117" s="160" t="str">
         <f t="shared" si="7"/>
         <v>[Manager-1]</v>
       </c>
-      <c r="F117" s="161"/>
+      <c r="F117" s="161" t="s">
+        <v>592</v>
+      </c>
       <c r="G117" s="176" t="s">
         <v>83</v>
       </c>
@@ -33749,7 +34021,7 @@
         <v/>
       </c>
       <c r="B118" s="160"/>
-      <c r="C118" s="183"/>
+      <c r="C118" s="167"/>
       <c r="D118" s="161"/>
       <c r="E118" s="160" t="str">
         <f t="shared" si="7"/>
@@ -35643,15 +35915,15 @@
   <sheetData>
     <row r="1" ht="25.5" customHeight="1">
       <c r="A1" s="11"/>
-      <c r="B1" s="184" t="s">
-        <v>561</v>
-      </c>
-      <c r="C1" s="185"/>
-      <c r="D1" s="185"/>
-      <c r="E1" s="185"/>
-      <c r="F1" s="185"/>
-      <c r="G1" s="185"/>
-      <c r="H1" s="185"/>
+      <c r="B1" s="186" t="s">
+        <v>596</v>
+      </c>
+      <c r="C1" s="187"/>
+      <c r="D1" s="187"/>
+      <c r="E1" s="187"/>
+      <c r="F1" s="187"/>
+      <c r="G1" s="187"/>
+      <c r="H1" s="187"/>
       <c r="I1" s="11"/>
       <c r="J1" s="11"/>
       <c r="K1" s="11"/>
@@ -35672,14 +35944,14 @@
       <c r="Z1" s="11"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="186"/>
-      <c r="B2" s="186"/>
+      <c r="A2" s="188"/>
+      <c r="B2" s="188"/>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
       <c r="F2" s="11"/>
       <c r="G2" s="11"/>
-      <c r="H2" s="187"/>
+      <c r="H2" s="189"/>
       <c r="I2" s="11"/>
       <c r="J2" s="11"/>
       <c r="K2" s="11"/>
@@ -35701,19 +35973,19 @@
     </row>
     <row r="3" ht="12.0" customHeight="1">
       <c r="A3" s="11"/>
-      <c r="B3" s="188" t="s">
+      <c r="B3" s="190" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="49" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="6"/>
-      <c r="E3" s="189" t="s">
+      <c r="E3" s="191" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="6"/>
-      <c r="G3" s="190"/>
-      <c r="H3" s="191" t="s">
+      <c r="G3" s="192"/>
+      <c r="H3" s="193" t="s">
         <v>4</v>
       </c>
       <c r="I3" s="11"/>
@@ -35737,19 +36009,19 @@
     </row>
     <row r="4" ht="12.0" customHeight="1">
       <c r="A4" s="11"/>
-      <c r="B4" s="188" t="s">
+      <c r="B4" s="190" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="49" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="6"/>
-      <c r="E4" s="189" t="s">
+      <c r="E4" s="191" t="s">
         <v>6</v>
       </c>
       <c r="F4" s="6"/>
-      <c r="G4" s="190"/>
-      <c r="H4" s="191" t="s">
+      <c r="G4" s="192"/>
+      <c r="H4" s="193" t="s">
         <v>7</v>
       </c>
       <c r="I4" s="11"/>
@@ -35773,7 +36045,7 @@
     </row>
     <row r="5" ht="12.0" customHeight="1">
       <c r="A5" s="11"/>
-      <c r="B5" s="192" t="s">
+      <c r="B5" s="194" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="49" t="str">
@@ -35781,12 +36053,12 @@
         <v>SoFa_Test Report_vx.x</v>
       </c>
       <c r="D5" s="6"/>
-      <c r="E5" s="189" t="s">
+      <c r="E5" s="191" t="s">
         <v>9</v>
       </c>
       <c r="F5" s="6"/>
-      <c r="G5" s="190"/>
-      <c r="H5" s="193">
+      <c r="G5" s="192"/>
+      <c r="H5" s="195">
         <v>44534.0</v>
       </c>
       <c r="I5" s="11"/>
@@ -35809,12 +36081,12 @@
       <c r="Z5" s="11"/>
     </row>
     <row r="6" ht="21.75" customHeight="1">
-      <c r="A6" s="186"/>
-      <c r="B6" s="192" t="s">
-        <v>562</v>
-      </c>
-      <c r="C6" s="194" t="s">
-        <v>563</v>
+      <c r="A6" s="188"/>
+      <c r="B6" s="194" t="s">
+        <v>597</v>
+      </c>
+      <c r="C6" s="196" t="s">
+        <v>598</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -35841,14 +36113,14 @@
       <c r="Z6" s="11"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="186"/>
+      <c r="A7" s="188"/>
       <c r="B7" s="25"/>
-      <c r="C7" s="195"/>
+      <c r="C7" s="197"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
-      <c r="H7" s="187"/>
+      <c r="H7" s="189"/>
       <c r="I7" s="11"/>
       <c r="J7" s="11"/>
       <c r="K7" s="11"/>
@@ -35871,12 +36143,12 @@
     <row r="8" ht="12.75" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="25"/>
-      <c r="C8" s="195"/>
+      <c r="C8" s="197"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
-      <c r="H8" s="187"/>
+      <c r="H8" s="189"/>
       <c r="I8" s="11"/>
       <c r="J8" s="11"/>
       <c r="K8" s="11"/>
@@ -35925,27 +36197,27 @@
       <c r="Z9" s="11"/>
     </row>
     <row r="10" ht="12.75" customHeight="1">
-      <c r="A10" s="196"/>
-      <c r="B10" s="197" t="s">
+      <c r="A10" s="198"/>
+      <c r="B10" s="199" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="198" t="s">
-        <v>564</v>
-      </c>
-      <c r="D10" s="199" t="s">
+      <c r="C10" s="200" t="s">
+        <v>599</v>
+      </c>
+      <c r="D10" s="201" t="s">
         <v>83</v>
       </c>
-      <c r="E10" s="198" t="s">
+      <c r="E10" s="200" t="s">
         <v>86</v>
       </c>
-      <c r="F10" s="198" t="s">
+      <c r="F10" s="200" t="s">
         <v>89</v>
       </c>
-      <c r="G10" s="200" t="s">
+      <c r="G10" s="202" t="s">
         <v>90</v>
       </c>
-      <c r="H10" s="201" t="s">
-        <v>565</v>
+      <c r="H10" s="203" t="s">
+        <v>600</v>
       </c>
       <c r="I10" s="11"/>
       <c r="J10" s="11"/>
@@ -35967,31 +36239,31 @@
       <c r="Z10" s="11"/>
     </row>
     <row r="11" ht="12.75" customHeight="1">
-      <c r="A11" s="196"/>
-      <c r="B11" s="202">
+      <c r="A11" s="198"/>
+      <c r="B11" s="204">
         <v>1.0</v>
       </c>
-      <c r="C11" s="203" t="str">
+      <c r="C11" s="205" t="str">
         <f>Guest!B2</f>
         <v>Guest</v>
       </c>
-      <c r="D11" s="204">
+      <c r="D11" s="206">
         <f>Guest!A6</f>
         <v>43</v>
       </c>
-      <c r="E11" s="204">
+      <c r="E11" s="206">
         <f>Guest!B6</f>
         <v>4</v>
       </c>
-      <c r="F11" s="204">
+      <c r="F11" s="206">
         <f>Guest!C6</f>
         <v>3</v>
       </c>
-      <c r="G11" s="205">
+      <c r="G11" s="207">
         <f>Guest!D6</f>
         <v>0</v>
       </c>
-      <c r="H11" s="206">
+      <c r="H11" s="208">
         <f>Guest!E6</f>
         <v>50</v>
       </c>
@@ -36015,31 +36287,31 @@
       <c r="Z11" s="11"/>
     </row>
     <row r="12" ht="12.75" customHeight="1">
-      <c r="A12" s="196"/>
-      <c r="B12" s="202">
+      <c r="A12" s="198"/>
+      <c r="B12" s="204">
         <v>2.0</v>
       </c>
-      <c r="C12" s="203" t="str">
+      <c r="C12" s="205" t="str">
         <f>User!B2</f>
         <v>User</v>
       </c>
-      <c r="D12" s="204">
+      <c r="D12" s="206">
         <f>User!A6</f>
         <v>0</v>
       </c>
-      <c r="E12" s="204">
+      <c r="E12" s="206">
         <f>User!B6</f>
         <v>0</v>
       </c>
-      <c r="F12" s="204">
+      <c r="F12" s="206">
         <f>User!C6</f>
         <v>51</v>
       </c>
-      <c r="G12" s="204">
+      <c r="G12" s="206">
         <f>User!D6</f>
         <v>0</v>
       </c>
-      <c r="H12" s="204">
+      <c r="H12" s="206">
         <f>User!E6</f>
         <v>51</v>
       </c>
@@ -36063,31 +36335,31 @@
       <c r="Z12" s="11"/>
     </row>
     <row r="13" ht="12.75" customHeight="1">
-      <c r="A13" s="196"/>
-      <c r="B13" s="202">
+      <c r="A13" s="198"/>
+      <c r="B13" s="204">
         <v>1.0</v>
       </c>
-      <c r="C13" s="203" t="str">
+      <c r="C13" s="205" t="str">
         <f>Manager!B2</f>
         <v>Manager</v>
       </c>
-      <c r="D13" s="204">
+      <c r="D13" s="206">
         <f>Manager!A6</f>
         <v>0</v>
       </c>
-      <c r="E13" s="204">
+      <c r="E13" s="206">
         <f>Manager!B6</f>
         <v>0</v>
       </c>
-      <c r="F13" s="204">
+      <c r="F13" s="206">
         <f>Manager!C6</f>
         <v>0</v>
       </c>
-      <c r="G13" s="205">
+      <c r="G13" s="207">
         <f>Manager!D6</f>
         <v>0</v>
       </c>
-      <c r="H13" s="206">
+      <c r="H13" s="208">
         <f>Manager!E6</f>
         <v>0</v>
       </c>
@@ -36111,28 +36383,28 @@
       <c r="Z13" s="11"/>
     </row>
     <row r="14" ht="12.75" customHeight="1">
-      <c r="A14" s="196"/>
-      <c r="B14" s="207"/>
-      <c r="C14" s="208" t="s">
-        <v>566</v>
-      </c>
-      <c r="D14" s="209">
+      <c r="A14" s="198"/>
+      <c r="B14" s="209"/>
+      <c r="C14" s="210" t="s">
+        <v>601</v>
+      </c>
+      <c r="D14" s="211">
         <f t="shared" ref="D14:H14" si="1">SUM(D9:D13)</f>
         <v>43</v>
       </c>
-      <c r="E14" s="209">
+      <c r="E14" s="211">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="F14" s="209">
+      <c r="F14" s="211">
         <f t="shared" si="1"/>
         <v>54</v>
       </c>
-      <c r="G14" s="209">
+      <c r="G14" s="211">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H14" s="210">
+      <c r="H14" s="212">
         <f t="shared" si="1"/>
         <v>101</v>
       </c>
@@ -36157,13 +36429,13 @@
     </row>
     <row r="15" ht="12.75" customHeight="1">
       <c r="A15" s="11"/>
-      <c r="B15" s="211"/>
+      <c r="B15" s="213"/>
       <c r="C15" s="11"/>
-      <c r="D15" s="212"/>
-      <c r="E15" s="213"/>
-      <c r="F15" s="213"/>
-      <c r="G15" s="213"/>
-      <c r="H15" s="213"/>
+      <c r="D15" s="214"/>
+      <c r="E15" s="215"/>
+      <c r="F15" s="215"/>
+      <c r="G15" s="215"/>
+      <c r="H15" s="215"/>
       <c r="I15" s="11"/>
       <c r="J15" s="11"/>
       <c r="K15" s="11"/>
@@ -36187,15 +36459,15 @@
       <c r="A16" s="11"/>
       <c r="B16" s="11"/>
       <c r="C16" s="9" t="s">
-        <v>567</v>
+        <v>602</v>
       </c>
       <c r="D16" s="11"/>
-      <c r="E16" s="214">
+      <c r="E16" s="216">
         <f>(D14+E14)*100/(H14-G14)</f>
         <v>46.53465347</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>568</v>
+        <v>603</v>
       </c>
       <c r="G16" s="11"/>
       <c r="H16" s="132"/>
@@ -36222,15 +36494,15 @@
       <c r="A17" s="11"/>
       <c r="B17" s="11"/>
       <c r="C17" s="9" t="s">
-        <v>569</v>
+        <v>604</v>
       </c>
       <c r="D17" s="11"/>
-      <c r="E17" s="214">
+      <c r="E17" s="216">
         <f>D14*100/(H14-G14)</f>
         <v>42.57425743</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>568</v>
+        <v>603</v>
       </c>
       <c r="G17" s="11"/>
       <c r="H17" s="132"/>

</xml_diff>

<commit_message>
HoangNH - Update Test Case Manage Voucher Manager
</commit_message>
<xml_diff>
--- a/3. Users/HoangNHHE130395/Testing/TestCase - Hoang.xlsx
+++ b/3. Users/HoangNHHE130395/Testing/TestCase - Hoang.xlsx
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1318" uniqueCount="605">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1549" uniqueCount="650">
   <si>
     <t>SYSTEM TEST CASE</t>
   </si>
@@ -2635,6 +2635,252 @@
     <t>1. Popup is disappeared
 2. Toast message 'Ban user thành công'
 3. The user's status is banned</t>
+  </si>
+  <si>
+    <t>Function Manage Voucher</t>
+  </si>
+  <si>
+    <t>Check GUI search box 'Search Voucher'</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'Voucher' tab in the menu bar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Display text 'Voucher' on the search box </t>
+  </si>
+  <si>
+    <t>Check focus on search box 'Search Voucher'</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'Voucher' tab in the menu bar
+3. Click on the search box 'Search Voucher'</t>
+  </si>
+  <si>
+    <t>1. Display text 'Search Voucher' on the search box 
+2. Border of the search box change to blue</t>
+  </si>
+  <si>
+    <t>Check focus out search box 'Search Voucher'</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'Voucher' tab in the menu bar
+3. Click on the search box 'Search Voucher'
+4. Click out of the search box 'Search Voucher'</t>
+  </si>
+  <si>
+    <t>1. Display text 'Search Voucher' on the search box 
+2. Border of the search box change from blue to white</t>
+  </si>
+  <si>
+    <t>Check function seach box 'Search Voucher'</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'Voucher' tab in the menu bar
+3. Click on the search box 'Search Voucher'
+4. Input text 'a' on the search box</t>
+  </si>
+  <si>
+    <t>1. Display text 'a' on the search box 
+2. Border of the search box change to blue
+3. Display list of voucher have title contain character 'a'</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'Voucher' tab in the menu bar
+3. Click on the search box 'Search Voucher'
+4. Input text 'a' on the search box
+5. Input text 'a' on the search box</t>
+  </si>
+  <si>
+    <t>1. Display text 'aa' on the search box 
+2. Border of the search box change to blue
+3. Display list of voucher have title contain character 'aa'</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'Voucher' tab in the menu bar
+3. Click on the search box 'Search Voucher'
+4. Input text 'a' on the search box
+5. Input text 'a' on the search box
+6. Press delete button on keyboard</t>
+  </si>
+  <si>
+    <t>1. Display text 'aa' on the search box 
+2. Border of the search box change to blue
+3. Display list of voucher have title contain character 'a'</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'Voucher' tab in the menu bar
+3. Choose 'Content' from the drop down list
+4. Click on the search box 'Search Voucher'
+5. Input text 'a' on the search box</t>
+  </si>
+  <si>
+    <t>1. Display text 'aa' on the search box 
+2. Border of the search box change to blue
+3. Display list of voucher have content contain character 'a'</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'Voucher' tab in the menu bar
+3. Choose 'Content' from the drop down list
+4. Click on the search box 'Search Voucher'
+5. Input text 'a' on the search box
+6. Input text 'a' on the search box</t>
+  </si>
+  <si>
+    <t>1. Display text 'aa' on the search box 
+2. Border of the search box change to blue
+3. Display list of voucher have content contain character 'aa'</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'Voucher' tab in the menu bar
+3. Choose 'Content' from the drop down list
+4. Click on the search box 'Search Voucher'
+5. Input text 'a' on the search box
+6. Input text 'a' on the search box
+7. Press delete button on keyboard</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'Voucher' tab in the menu bar
+3. Choose 'Code' from the drop down list
+4. Click on the search box 'Search Voucher'
+5. Input text 'a' on the search box</t>
+  </si>
+  <si>
+    <t>1. Display text 'a' on the search box 
+2. Border of the search box change to blue
+3. Display list of voucher have code contain character 'a'</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'Voucher' tab in the menu bar
+3. Choose 'Code' from the drop down list
+4. Click on the search box 'Search Voucher'
+5. Input text 'a' on the search box
+6. Input text 'a' on the search box</t>
+  </si>
+  <si>
+    <t>1. Display text 'a' on the search box 
+2. Border of the search box change to blue
+3. Display list of voucher have code contain character 'aa'</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'Voucher' tab in the menu bar
+3. Choose 'Code' from the drop down list
+4. Click on the search box 'Search Voucher'
+5. Input text 'a' on the search box
+6. Input text 'a' on the search box
+7. Press delete button on keyboard</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'Voucher' tab in the menu bar
+3. Choose 'Created By' from the drop down list
+4. Click on the search box 'Search Voucher'
+5. Input text 'a' on the search box</t>
+  </si>
+  <si>
+    <t>1. Display text 'a' on the search box 
+2. Border of the search box change to blue
+3. Display list of voucher have created by contain character 'a'</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'Voucher' tab in the menu bar
+3. Choose 'Created By' from the drop down list
+4. Click on the search box 'Search Voucher'
+5. Input text 'a' on the search box
+6. Input text 'a' on the search box</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'User' tab in the menu bar
+3. Choose 'Created By' from the drop down list
+4. Click on the search box 'Search Voucher'
+5. Input text 'a' on the search box
+6. Input text 'a' on the search box
+7. Press delete button on keyboard</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'Voucher' tab in the menu bar
+3. Choose 'Created By' from the drop down list
+4. Click on the search box 'Search Voucher'
+5. Input text 'a' on the search box
+6. Choose 'Title' from the drop down list</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'Voucher' tab in the menu bar
+3. Choose 'Created By' from the drop down list
+4. Click on the search box 'Search Voucher'
+5. Input text 'a' on the search box
+6. Choose 'Content' from the drop down list</t>
+  </si>
+  <si>
+    <t>1. Display text 'a' on the search box 
+2. Border of the search box change to blue
+3. Display list of voucher have content contain character 'a'</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'Voucher' tab in the menu bar
+3. Choose 'Created By' from the drop down list
+4. Click on the search box 'Search Voucher'
+5. Input text 'a' on the search box
+6. Choose 'Code' from the drop down list</t>
+  </si>
+  <si>
+    <t>Check GUI list Voucher</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+ 2. Click on 'Voucher' tab in the menu bar</t>
+  </si>
+  <si>
+    <t>1. Display the list of reports by following: ID, Content, Code, Created By, Expired created, option
+ 2. The data of post is mapping wit the column name</t>
+  </si>
+  <si>
+    <t>Check GUI of button 'Delete' of list voucher</t>
+  </si>
+  <si>
+    <t>1. Display button 'Delete' in column 'Option'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Login into the web server
+2. Click on 'Voucher' tab in the menu bar
+3. From list choose voucher have id= '3' click 'Delete'
+</t>
+  </si>
+  <si>
+    <t>1. Display popup confirm 'Bạn có muốn xoá voucher này'</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'Voucher' tab in the menu bar
+3. From list choose voucher have id= '3' click 'Delete'
+4. Click on 'Hủy'</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'Voucher' tab in the menu bar
+3. From list choose voucher have id= '3' click 'Delete'
+4. Click on 'Ok'</t>
+  </si>
+  <si>
+    <t>1. Popup is disappeared
+2. Toast message 'Xóa Voucher thành công'
+3. The list is updated</t>
   </si>
   <si>
     <t>TEST REPORT</t>
@@ -4003,8 +4249,8 @@
     <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="13" fillId="0" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="13" fillId="0" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
@@ -33241,7 +33487,7 @@
     </row>
     <row r="102" ht="78.75" customHeight="1">
       <c r="A102" s="160" t="str">
-        <f t="shared" ref="A102:A118" si="6">IF(OR(B102&lt;&gt;"",D102&lt;&gt;""),"["&amp;TEXT($B$2,"##")&amp;"-"&amp;TEXT(ROW()-9,"##")&amp;"]","")</f>
+        <f t="shared" ref="A102:A117" si="6">IF(OR(B102&lt;&gt;"",D102&lt;&gt;""),"["&amp;TEXT($B$2,"##")&amp;"-"&amp;TEXT(ROW()-9,"##")&amp;"]","")</f>
         <v>[Manager-93]</v>
       </c>
       <c r="B102" s="173" t="s">
@@ -33254,7 +33500,7 @@
         <v>563</v>
       </c>
       <c r="E102" s="160" t="str">
-        <f t="shared" ref="E102:E118" si="7">$A$10</f>
+        <f t="shared" ref="E102:E117" si="7">$A$10</f>
         <v>[Manager-1]</v>
       </c>
       <c r="F102" s="161"/>
@@ -33341,10 +33587,10 @@
       <c r="B104" s="160" t="s">
         <v>567</v>
       </c>
-      <c r="C104" s="183" t="s">
+      <c r="C104" s="167" t="s">
         <v>568</v>
       </c>
-      <c r="D104" s="183" t="s">
+      <c r="D104" s="167" t="s">
         <v>569</v>
       </c>
       <c r="E104" s="160" t="str">
@@ -33390,10 +33636,10 @@
       <c r="B105" s="160" t="s">
         <v>571</v>
       </c>
-      <c r="C105" s="183" t="s">
+      <c r="C105" s="167" t="s">
         <v>572</v>
       </c>
-      <c r="D105" s="183" t="s">
+      <c r="D105" s="167" t="s">
         <v>573</v>
       </c>
       <c r="E105" s="160" t="str">
@@ -33439,10 +33685,10 @@
       <c r="B106" s="160" t="s">
         <v>575</v>
       </c>
-      <c r="C106" s="183" t="s">
+      <c r="C106" s="167" t="s">
         <v>576</v>
       </c>
-      <c r="D106" s="183" t="s">
+      <c r="D106" s="167" t="s">
         <v>493</v>
       </c>
       <c r="E106" s="160" t="str">
@@ -33488,10 +33734,10 @@
       <c r="B107" s="160" t="s">
         <v>575</v>
       </c>
-      <c r="C107" s="183" t="s">
+      <c r="C107" s="167" t="s">
         <v>576</v>
       </c>
-      <c r="D107" s="183" t="s">
+      <c r="D107" s="167" t="s">
         <v>493</v>
       </c>
       <c r="E107" s="160" t="str">
@@ -33537,7 +33783,7 @@
       <c r="B108" s="160" t="s">
         <v>578</v>
       </c>
-      <c r="C108" s="183" t="s">
+      <c r="C108" s="167" t="s">
         <v>579</v>
       </c>
       <c r="D108" s="161" t="s">
@@ -33586,7 +33832,7 @@
       <c r="B109" s="160" t="s">
         <v>578</v>
       </c>
-      <c r="C109" s="183" t="s">
+      <c r="C109" s="167" t="s">
         <v>582</v>
       </c>
       <c r="D109" s="161" t="s">
@@ -33635,7 +33881,7 @@
       <c r="B110" s="160" t="s">
         <v>578</v>
       </c>
-      <c r="C110" s="183" t="s">
+      <c r="C110" s="167" t="s">
         <v>583</v>
       </c>
       <c r="D110" s="161" t="s">
@@ -33654,7 +33900,7 @@
       <c r="H110" s="177">
         <v>44304.0</v>
       </c>
-      <c r="I110" s="184" t="s">
+      <c r="I110" s="178" t="s">
         <v>375</v>
       </c>
       <c r="J110" s="179"/>
@@ -33684,10 +33930,10 @@
       <c r="B111" s="173" t="s">
         <v>585</v>
       </c>
-      <c r="C111" s="185" t="s">
+      <c r="C111" s="182" t="s">
         <v>562</v>
       </c>
-      <c r="D111" s="185" t="s">
+      <c r="D111" s="182" t="s">
         <v>586</v>
       </c>
       <c r="E111" s="160" t="str">
@@ -33701,7 +33947,7 @@
       <c r="H111" s="177">
         <v>44304.0</v>
       </c>
-      <c r="I111" s="184" t="s">
+      <c r="I111" s="178" t="s">
         <v>375</v>
       </c>
       <c r="J111" s="179"/>
@@ -33731,10 +33977,10 @@
       <c r="B112" s="173" t="s">
         <v>587</v>
       </c>
-      <c r="C112" s="185" t="s">
+      <c r="C112" s="182" t="s">
         <v>565</v>
       </c>
-      <c r="D112" s="185" t="s">
+      <c r="D112" s="182" t="s">
         <v>566</v>
       </c>
       <c r="E112" s="160" t="str">
@@ -33748,7 +33994,7 @@
       <c r="H112" s="177">
         <v>44304.0</v>
       </c>
-      <c r="I112" s="184" t="s">
+      <c r="I112" s="178" t="s">
         <v>375</v>
       </c>
       <c r="J112" s="179"/>
@@ -33778,10 +34024,10 @@
       <c r="B113" s="160" t="s">
         <v>588</v>
       </c>
-      <c r="C113" s="183" t="s">
+      <c r="C113" s="167" t="s">
         <v>568</v>
       </c>
-      <c r="D113" s="183" t="s">
+      <c r="D113" s="167" t="s">
         <v>569</v>
       </c>
       <c r="E113" s="160" t="str">
@@ -33827,10 +34073,10 @@
       <c r="B114" s="160" t="s">
         <v>589</v>
       </c>
-      <c r="C114" s="183" t="s">
+      <c r="C114" s="167" t="s">
         <v>572</v>
       </c>
-      <c r="D114" s="183" t="s">
+      <c r="D114" s="167" t="s">
         <v>573</v>
       </c>
       <c r="E114" s="160" t="str">
@@ -33876,7 +34122,7 @@
       <c r="B115" s="160" t="s">
         <v>443</v>
       </c>
-      <c r="C115" s="183" t="s">
+      <c r="C115" s="167" t="s">
         <v>590</v>
       </c>
       <c r="D115" s="161" t="s">
@@ -33925,7 +34171,7 @@
       <c r="B116" s="160" t="s">
         <v>443</v>
       </c>
-      <c r="C116" s="183" t="s">
+      <c r="C116" s="167" t="s">
         <v>593</v>
       </c>
       <c r="D116" s="161" t="s">
@@ -33974,7 +34220,7 @@
       <c r="B117" s="160" t="s">
         <v>443</v>
       </c>
-      <c r="C117" s="183" t="s">
+      <c r="C117" s="167" t="s">
         <v>594</v>
       </c>
       <c r="D117" s="161" t="s">
@@ -34015,29 +34261,19 @@
       <c r="Z117" s="11"/>
       <c r="AA117" s="155"/>
     </row>
-    <row r="118" ht="12.75" customHeight="1">
-      <c r="A118" s="160" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="B118" s="160"/>
-      <c r="C118" s="167"/>
-      <c r="D118" s="161"/>
-      <c r="E118" s="160" t="str">
-        <f t="shared" si="7"/>
-        <v>[Manager-1]</v>
-      </c>
-      <c r="F118" s="161"/>
-      <c r="G118" s="176" t="s">
-        <v>83</v>
-      </c>
-      <c r="H118" s="177">
-        <v>44304.0</v>
-      </c>
-      <c r="I118" s="178" t="s">
-        <v>375</v>
-      </c>
-      <c r="J118" s="179"/>
+    <row r="118" ht="36.75" customHeight="1">
+      <c r="A118" s="168" t="s">
+        <v>596</v>
+      </c>
+      <c r="B118" s="169"/>
+      <c r="C118" s="170"/>
+      <c r="D118" s="170"/>
+      <c r="E118" s="170"/>
+      <c r="F118" s="170"/>
+      <c r="G118" s="170"/>
+      <c r="H118" s="171"/>
+      <c r="I118" s="170"/>
+      <c r="J118" s="172"/>
       <c r="K118" s="86"/>
       <c r="L118" s="11"/>
       <c r="M118" s="11"/>
@@ -34056,17 +34292,35 @@
       <c r="Z118" s="11"/>
       <c r="AA118" s="155"/>
     </row>
-    <row r="119" ht="12.75" customHeight="1">
-      <c r="A119" s="50"/>
-      <c r="B119" s="50"/>
-      <c r="C119" s="50"/>
-      <c r="D119" s="50"/>
-      <c r="E119" s="50"/>
-      <c r="F119" s="50"/>
-      <c r="G119" s="50"/>
-      <c r="H119" s="50"/>
-      <c r="I119" s="50"/>
-      <c r="J119" s="50"/>
+    <row r="119" ht="34.5" customHeight="1">
+      <c r="A119" s="160" t="str">
+        <f t="shared" ref="A119:A141" si="8">IF(OR(B119&lt;&gt;"",D119&lt;&gt;""),"["&amp;TEXT($B$2,"##")&amp;"-"&amp;TEXT(ROW()-9,"##")&amp;"]","")</f>
+        <v>[Manager-110]</v>
+      </c>
+      <c r="B119" s="160" t="s">
+        <v>597</v>
+      </c>
+      <c r="C119" s="183" t="s">
+        <v>598</v>
+      </c>
+      <c r="D119" s="183" t="s">
+        <v>599</v>
+      </c>
+      <c r="E119" s="160" t="str">
+        <f t="shared" ref="E119:E141" si="9">$A$10</f>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F119" s="117"/>
+      <c r="G119" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H119" s="163">
+        <v>44305.0</v>
+      </c>
+      <c r="I119" s="184" t="s">
+        <v>375</v>
+      </c>
+      <c r="J119" s="179"/>
       <c r="K119" s="86"/>
       <c r="L119" s="11"/>
       <c r="M119" s="11"/>
@@ -34085,17 +34339,35 @@
       <c r="Z119" s="11"/>
       <c r="AA119" s="155"/>
     </row>
-    <row r="120" ht="12.75" customHeight="1">
-      <c r="A120" s="50"/>
-      <c r="B120" s="50"/>
-      <c r="C120" s="50"/>
-      <c r="D120" s="50"/>
-      <c r="E120" s="50"/>
-      <c r="F120" s="50"/>
-      <c r="G120" s="50"/>
-      <c r="H120" s="50"/>
-      <c r="I120" s="50"/>
-      <c r="J120" s="50"/>
+    <row r="120" ht="48.75" customHeight="1">
+      <c r="A120" s="160" t="str">
+        <f t="shared" si="8"/>
+        <v>[Manager-111]</v>
+      </c>
+      <c r="B120" s="160" t="s">
+        <v>600</v>
+      </c>
+      <c r="C120" s="183" t="s">
+        <v>601</v>
+      </c>
+      <c r="D120" s="183" t="s">
+        <v>602</v>
+      </c>
+      <c r="E120" s="160" t="str">
+        <f t="shared" si="9"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F120" s="117"/>
+      <c r="G120" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H120" s="163">
+        <v>44305.0</v>
+      </c>
+      <c r="I120" s="184" t="s">
+        <v>375</v>
+      </c>
+      <c r="J120" s="179"/>
       <c r="K120" s="86"/>
       <c r="L120" s="11"/>
       <c r="M120" s="11"/>
@@ -34114,17 +34386,35 @@
       <c r="Z120" s="11"/>
       <c r="AA120" s="155"/>
     </row>
-    <row r="121" ht="12.75" customHeight="1">
-      <c r="A121" s="50"/>
-      <c r="B121" s="50"/>
-      <c r="C121" s="50"/>
-      <c r="D121" s="50"/>
-      <c r="E121" s="50"/>
-      <c r="F121" s="50"/>
-      <c r="G121" s="50"/>
-      <c r="H121" s="50"/>
-      <c r="I121" s="50"/>
-      <c r="J121" s="50"/>
+    <row r="121" ht="63.0" customHeight="1">
+      <c r="A121" s="160" t="str">
+        <f t="shared" si="8"/>
+        <v>[Manager-112]</v>
+      </c>
+      <c r="B121" s="160" t="s">
+        <v>603</v>
+      </c>
+      <c r="C121" s="183" t="s">
+        <v>604</v>
+      </c>
+      <c r="D121" s="183" t="s">
+        <v>605</v>
+      </c>
+      <c r="E121" s="160" t="str">
+        <f t="shared" si="9"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F121" s="117"/>
+      <c r="G121" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H121" s="163">
+        <v>44305.0</v>
+      </c>
+      <c r="I121" s="184" t="s">
+        <v>375</v>
+      </c>
+      <c r="J121" s="179"/>
       <c r="K121" s="86"/>
       <c r="L121" s="11"/>
       <c r="M121" s="11"/>
@@ -34143,17 +34433,37 @@
       <c r="Z121" s="11"/>
       <c r="AA121" s="155"/>
     </row>
-    <row r="122" ht="12.75" customHeight="1">
-      <c r="A122" s="50"/>
-      <c r="B122" s="50"/>
-      <c r="C122" s="50"/>
-      <c r="D122" s="50"/>
-      <c r="E122" s="50"/>
-      <c r="F122" s="50"/>
-      <c r="G122" s="50"/>
-      <c r="H122" s="50"/>
-      <c r="I122" s="50"/>
-      <c r="J122" s="50"/>
+    <row r="122" ht="64.5" customHeight="1">
+      <c r="A122" s="160" t="str">
+        <f t="shared" si="8"/>
+        <v>[Manager-113]</v>
+      </c>
+      <c r="B122" s="160" t="s">
+        <v>606</v>
+      </c>
+      <c r="C122" s="183" t="s">
+        <v>607</v>
+      </c>
+      <c r="D122" s="183" t="s">
+        <v>608</v>
+      </c>
+      <c r="E122" s="160" t="str">
+        <f t="shared" si="9"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F122" s="161" t="s">
+        <v>398</v>
+      </c>
+      <c r="G122" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H122" s="163">
+        <v>44305.0</v>
+      </c>
+      <c r="I122" s="184" t="s">
+        <v>375</v>
+      </c>
+      <c r="J122" s="179"/>
       <c r="K122" s="86"/>
       <c r="L122" s="11"/>
       <c r="M122" s="11"/>
@@ -34172,17 +34482,37 @@
       <c r="Z122" s="11"/>
       <c r="AA122" s="155"/>
     </row>
-    <row r="123" ht="12.75" customHeight="1">
-      <c r="A123" s="11"/>
-      <c r="B123" s="11"/>
-      <c r="C123" s="11"/>
-      <c r="D123" s="11"/>
-      <c r="E123" s="11"/>
-      <c r="F123" s="11"/>
-      <c r="G123" s="11"/>
-      <c r="H123" s="11"/>
-      <c r="I123" s="11"/>
-      <c r="J123" s="11"/>
+    <row r="123" ht="80.25" customHeight="1">
+      <c r="A123" s="160" t="str">
+        <f t="shared" si="8"/>
+        <v>[Manager-114]</v>
+      </c>
+      <c r="B123" s="160" t="s">
+        <v>606</v>
+      </c>
+      <c r="C123" s="183" t="s">
+        <v>609</v>
+      </c>
+      <c r="D123" s="183" t="s">
+        <v>610</v>
+      </c>
+      <c r="E123" s="160" t="str">
+        <f t="shared" si="9"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F123" s="161" t="s">
+        <v>401</v>
+      </c>
+      <c r="G123" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H123" s="163">
+        <v>44305.0</v>
+      </c>
+      <c r="I123" s="184" t="s">
+        <v>375</v>
+      </c>
+      <c r="J123" s="179"/>
       <c r="K123" s="86"/>
       <c r="L123" s="11"/>
       <c r="M123" s="11"/>
@@ -34201,17 +34531,37 @@
       <c r="Z123" s="11"/>
       <c r="AA123" s="155"/>
     </row>
-    <row r="124" ht="12.75" customHeight="1">
-      <c r="A124" s="11"/>
-      <c r="B124" s="11"/>
-      <c r="C124" s="11"/>
-      <c r="D124" s="11"/>
-      <c r="E124" s="11"/>
-      <c r="F124" s="11"/>
-      <c r="G124" s="11"/>
-      <c r="H124" s="11"/>
-      <c r="I124" s="11"/>
-      <c r="J124" s="11"/>
+    <row r="124" ht="85.5" customHeight="1">
+      <c r="A124" s="160" t="str">
+        <f t="shared" si="8"/>
+        <v>[Manager-115]</v>
+      </c>
+      <c r="B124" s="160" t="s">
+        <v>606</v>
+      </c>
+      <c r="C124" s="183" t="s">
+        <v>611</v>
+      </c>
+      <c r="D124" s="183" t="s">
+        <v>612</v>
+      </c>
+      <c r="E124" s="160" t="str">
+        <f t="shared" si="9"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F124" s="161" t="s">
+        <v>401</v>
+      </c>
+      <c r="G124" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H124" s="163">
+        <v>44305.0</v>
+      </c>
+      <c r="I124" s="184" t="s">
+        <v>375</v>
+      </c>
+      <c r="J124" s="179"/>
       <c r="K124" s="86"/>
       <c r="L124" s="11"/>
       <c r="M124" s="11"/>
@@ -34230,17 +34580,37 @@
       <c r="Z124" s="11"/>
       <c r="AA124" s="155"/>
     </row>
-    <row r="125" ht="12.75" customHeight="1">
-      <c r="A125" s="11"/>
-      <c r="B125" s="11"/>
-      <c r="C125" s="11"/>
-      <c r="D125" s="11"/>
-      <c r="E125" s="11"/>
-      <c r="F125" s="11"/>
-      <c r="G125" s="11"/>
-      <c r="H125" s="11"/>
-      <c r="I125" s="11"/>
-      <c r="J125" s="11"/>
+    <row r="125" ht="72.75" customHeight="1">
+      <c r="A125" s="160" t="str">
+        <f t="shared" si="8"/>
+        <v>[Manager-116]</v>
+      </c>
+      <c r="B125" s="160" t="s">
+        <v>606</v>
+      </c>
+      <c r="C125" s="183" t="s">
+        <v>613</v>
+      </c>
+      <c r="D125" s="183" t="s">
+        <v>614</v>
+      </c>
+      <c r="E125" s="160" t="str">
+        <f t="shared" si="9"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F125" s="161" t="s">
+        <v>398</v>
+      </c>
+      <c r="G125" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H125" s="163">
+        <v>44305.0</v>
+      </c>
+      <c r="I125" s="184" t="s">
+        <v>375</v>
+      </c>
+      <c r="J125" s="179"/>
       <c r="K125" s="86"/>
       <c r="L125" s="11"/>
       <c r="M125" s="11"/>
@@ -34259,17 +34629,37 @@
       <c r="Z125" s="11"/>
       <c r="AA125" s="155"/>
     </row>
-    <row r="126" ht="12.75" customHeight="1">
-      <c r="A126" s="11"/>
-      <c r="B126" s="11"/>
-      <c r="C126" s="11"/>
-      <c r="D126" s="11"/>
-      <c r="E126" s="11"/>
-      <c r="F126" s="11"/>
-      <c r="G126" s="11"/>
-      <c r="H126" s="11"/>
-      <c r="I126" s="11"/>
-      <c r="J126" s="11"/>
+    <row r="126" ht="88.5" customHeight="1">
+      <c r="A126" s="160" t="str">
+        <f t="shared" si="8"/>
+        <v>[Manager-117]</v>
+      </c>
+      <c r="B126" s="160" t="s">
+        <v>606</v>
+      </c>
+      <c r="C126" s="183" t="s">
+        <v>615</v>
+      </c>
+      <c r="D126" s="183" t="s">
+        <v>616</v>
+      </c>
+      <c r="E126" s="160" t="str">
+        <f t="shared" si="9"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F126" s="161" t="s">
+        <v>401</v>
+      </c>
+      <c r="G126" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H126" s="163">
+        <v>44305.0</v>
+      </c>
+      <c r="I126" s="184" t="s">
+        <v>375</v>
+      </c>
+      <c r="J126" s="179"/>
       <c r="K126" s="86"/>
       <c r="L126" s="11"/>
       <c r="M126" s="11"/>
@@ -34288,17 +34678,37 @@
       <c r="Z126" s="11"/>
       <c r="AA126" s="155"/>
     </row>
-    <row r="127" ht="12.75" customHeight="1">
-      <c r="A127" s="11"/>
-      <c r="B127" s="11"/>
-      <c r="C127" s="11"/>
-      <c r="D127" s="11"/>
-      <c r="E127" s="11"/>
-      <c r="F127" s="11"/>
-      <c r="G127" s="11"/>
-      <c r="H127" s="11"/>
-      <c r="I127" s="11"/>
-      <c r="J127" s="11"/>
+    <row r="127" ht="102.0" customHeight="1">
+      <c r="A127" s="160" t="str">
+        <f t="shared" si="8"/>
+        <v>[Manager-118]</v>
+      </c>
+      <c r="B127" s="160" t="s">
+        <v>606</v>
+      </c>
+      <c r="C127" s="183" t="s">
+        <v>617</v>
+      </c>
+      <c r="D127" s="183" t="s">
+        <v>614</v>
+      </c>
+      <c r="E127" s="160" t="str">
+        <f t="shared" si="9"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F127" s="161" t="s">
+        <v>401</v>
+      </c>
+      <c r="G127" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H127" s="163">
+        <v>44305.0</v>
+      </c>
+      <c r="I127" s="184" t="s">
+        <v>375</v>
+      </c>
+      <c r="J127" s="179"/>
       <c r="K127" s="86"/>
       <c r="L127" s="11"/>
       <c r="M127" s="11"/>
@@ -34317,17 +34727,37 @@
       <c r="Z127" s="11"/>
       <c r="AA127" s="155"/>
     </row>
-    <row r="128" ht="12.75" customHeight="1">
-      <c r="A128" s="11"/>
-      <c r="B128" s="11"/>
-      <c r="C128" s="11"/>
-      <c r="D128" s="11"/>
-      <c r="E128" s="11"/>
-      <c r="F128" s="11"/>
-      <c r="G128" s="11"/>
-      <c r="H128" s="11"/>
-      <c r="I128" s="11"/>
-      <c r="J128" s="11"/>
+    <row r="128" ht="79.5" customHeight="1">
+      <c r="A128" s="160" t="str">
+        <f t="shared" si="8"/>
+        <v>[Manager-119]</v>
+      </c>
+      <c r="B128" s="160" t="s">
+        <v>606</v>
+      </c>
+      <c r="C128" s="183" t="s">
+        <v>618</v>
+      </c>
+      <c r="D128" s="183" t="s">
+        <v>619</v>
+      </c>
+      <c r="E128" s="160" t="str">
+        <f t="shared" si="9"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F128" s="161" t="s">
+        <v>398</v>
+      </c>
+      <c r="G128" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H128" s="163">
+        <v>44305.0</v>
+      </c>
+      <c r="I128" s="184" t="s">
+        <v>375</v>
+      </c>
+      <c r="J128" s="179"/>
       <c r="K128" s="86"/>
       <c r="L128" s="11"/>
       <c r="M128" s="11"/>
@@ -34346,17 +34776,37 @@
       <c r="Z128" s="11"/>
       <c r="AA128" s="155"/>
     </row>
-    <row r="129" ht="12.75" customHeight="1">
-      <c r="A129" s="11"/>
-      <c r="B129" s="11"/>
-      <c r="C129" s="11"/>
-      <c r="D129" s="11"/>
-      <c r="E129" s="11"/>
-      <c r="F129" s="11"/>
-      <c r="G129" s="11"/>
-      <c r="H129" s="11"/>
-      <c r="I129" s="11"/>
-      <c r="J129" s="11"/>
+    <row r="129" ht="91.5" customHeight="1">
+      <c r="A129" s="160" t="str">
+        <f t="shared" si="8"/>
+        <v>[Manager-120]</v>
+      </c>
+      <c r="B129" s="160" t="s">
+        <v>606</v>
+      </c>
+      <c r="C129" s="183" t="s">
+        <v>620</v>
+      </c>
+      <c r="D129" s="183" t="s">
+        <v>621</v>
+      </c>
+      <c r="E129" s="160" t="str">
+        <f t="shared" si="9"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F129" s="161" t="s">
+        <v>401</v>
+      </c>
+      <c r="G129" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H129" s="163">
+        <v>44305.0</v>
+      </c>
+      <c r="I129" s="184" t="s">
+        <v>375</v>
+      </c>
+      <c r="J129" s="179"/>
       <c r="K129" s="86"/>
       <c r="L129" s="11"/>
       <c r="M129" s="11"/>
@@ -34375,17 +34825,37 @@
       <c r="Z129" s="11"/>
       <c r="AA129" s="155"/>
     </row>
-    <row r="130" ht="12.75" customHeight="1">
-      <c r="A130" s="11"/>
-      <c r="B130" s="11"/>
-      <c r="C130" s="11"/>
-      <c r="D130" s="11"/>
-      <c r="E130" s="11"/>
-      <c r="F130" s="11"/>
-      <c r="G130" s="11"/>
-      <c r="H130" s="11"/>
-      <c r="I130" s="11"/>
-      <c r="J130" s="11"/>
+    <row r="130" ht="102.0" customHeight="1">
+      <c r="A130" s="160" t="str">
+        <f t="shared" si="8"/>
+        <v>[Manager-121]</v>
+      </c>
+      <c r="B130" s="160" t="s">
+        <v>606</v>
+      </c>
+      <c r="C130" s="183" t="s">
+        <v>622</v>
+      </c>
+      <c r="D130" s="183" t="s">
+        <v>619</v>
+      </c>
+      <c r="E130" s="160" t="str">
+        <f t="shared" si="9"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F130" s="161" t="s">
+        <v>401</v>
+      </c>
+      <c r="G130" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H130" s="163">
+        <v>44305.0</v>
+      </c>
+      <c r="I130" s="184" t="s">
+        <v>375</v>
+      </c>
+      <c r="J130" s="179"/>
       <c r="K130" s="86"/>
       <c r="L130" s="11"/>
       <c r="M130" s="11"/>
@@ -34404,17 +34874,37 @@
       <c r="Z130" s="11"/>
       <c r="AA130" s="155"/>
     </row>
-    <row r="131" ht="12.75" customHeight="1">
-      <c r="A131" s="11"/>
-      <c r="B131" s="11"/>
-      <c r="C131" s="11"/>
-      <c r="D131" s="11"/>
-      <c r="E131" s="11"/>
-      <c r="F131" s="11"/>
-      <c r="G131" s="11"/>
-      <c r="H131" s="11"/>
-      <c r="I131" s="11"/>
-      <c r="J131" s="11"/>
+    <row r="131" ht="78.0" customHeight="1">
+      <c r="A131" s="160" t="str">
+        <f t="shared" si="8"/>
+        <v>[Manager-122]</v>
+      </c>
+      <c r="B131" s="160" t="s">
+        <v>606</v>
+      </c>
+      <c r="C131" s="183" t="s">
+        <v>623</v>
+      </c>
+      <c r="D131" s="183" t="s">
+        <v>624</v>
+      </c>
+      <c r="E131" s="160" t="str">
+        <f t="shared" si="9"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F131" s="161" t="s">
+        <v>398</v>
+      </c>
+      <c r="G131" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H131" s="163">
+        <v>44305.0</v>
+      </c>
+      <c r="I131" s="184" t="s">
+        <v>375</v>
+      </c>
+      <c r="J131" s="179"/>
       <c r="K131" s="86"/>
       <c r="L131" s="11"/>
       <c r="M131" s="11"/>
@@ -34433,17 +34923,37 @@
       <c r="Z131" s="11"/>
       <c r="AA131" s="155"/>
     </row>
-    <row r="132" ht="12.75" customHeight="1">
-      <c r="A132" s="11"/>
-      <c r="B132" s="11"/>
-      <c r="C132" s="11"/>
-      <c r="D132" s="11"/>
-      <c r="E132" s="11"/>
-      <c r="F132" s="11"/>
-      <c r="G132" s="11"/>
-      <c r="H132" s="11"/>
-      <c r="I132" s="11"/>
-      <c r="J132" s="11"/>
+    <row r="132" ht="94.5" customHeight="1">
+      <c r="A132" s="160" t="str">
+        <f t="shared" si="8"/>
+        <v>[Manager-123]</v>
+      </c>
+      <c r="B132" s="160" t="s">
+        <v>606</v>
+      </c>
+      <c r="C132" s="183" t="s">
+        <v>625</v>
+      </c>
+      <c r="D132" s="183" t="s">
+        <v>624</v>
+      </c>
+      <c r="E132" s="160" t="str">
+        <f t="shared" si="9"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F132" s="161" t="s">
+        <v>401</v>
+      </c>
+      <c r="G132" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H132" s="163">
+        <v>44305.0</v>
+      </c>
+      <c r="I132" s="184" t="s">
+        <v>375</v>
+      </c>
+      <c r="J132" s="179"/>
       <c r="K132" s="86"/>
       <c r="L132" s="11"/>
       <c r="M132" s="11"/>
@@ -34462,17 +34972,37 @@
       <c r="Z132" s="11"/>
       <c r="AA132" s="155"/>
     </row>
-    <row r="133" ht="12.75" customHeight="1">
-      <c r="A133" s="11"/>
-      <c r="B133" s="11"/>
-      <c r="C133" s="11"/>
-      <c r="D133" s="11"/>
-      <c r="E133" s="11"/>
-      <c r="F133" s="11"/>
-      <c r="G133" s="11"/>
-      <c r="H133" s="11"/>
-      <c r="I133" s="11"/>
-      <c r="J133" s="11"/>
+    <row r="133" ht="102.0" customHeight="1">
+      <c r="A133" s="160" t="str">
+        <f t="shared" si="8"/>
+        <v>[Manager-124]</v>
+      </c>
+      <c r="B133" s="160" t="s">
+        <v>606</v>
+      </c>
+      <c r="C133" s="183" t="s">
+        <v>626</v>
+      </c>
+      <c r="D133" s="183" t="s">
+        <v>624</v>
+      </c>
+      <c r="E133" s="160" t="str">
+        <f t="shared" si="9"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F133" s="161" t="s">
+        <v>401</v>
+      </c>
+      <c r="G133" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H133" s="163">
+        <v>44305.0</v>
+      </c>
+      <c r="I133" s="184" t="s">
+        <v>375</v>
+      </c>
+      <c r="J133" s="179"/>
       <c r="K133" s="86"/>
       <c r="L133" s="11"/>
       <c r="M133" s="11"/>
@@ -34491,17 +35021,37 @@
       <c r="Z133" s="11"/>
       <c r="AA133" s="155"/>
     </row>
-    <row r="134" ht="12.75" customHeight="1">
-      <c r="A134" s="11"/>
-      <c r="B134" s="11"/>
-      <c r="C134" s="11"/>
-      <c r="D134" s="11"/>
-      <c r="E134" s="11"/>
-      <c r="F134" s="11"/>
-      <c r="G134" s="11"/>
-      <c r="H134" s="11"/>
-      <c r="I134" s="11"/>
-      <c r="J134" s="11"/>
+    <row r="134" ht="88.5" customHeight="1">
+      <c r="A134" s="160" t="str">
+        <f t="shared" si="8"/>
+        <v>[Manager-125]</v>
+      </c>
+      <c r="B134" s="160" t="s">
+        <v>606</v>
+      </c>
+      <c r="C134" s="183" t="s">
+        <v>627</v>
+      </c>
+      <c r="D134" s="183" t="s">
+        <v>608</v>
+      </c>
+      <c r="E134" s="160" t="str">
+        <f t="shared" si="9"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F134" s="161" t="s">
+        <v>398</v>
+      </c>
+      <c r="G134" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H134" s="163">
+        <v>44305.0</v>
+      </c>
+      <c r="I134" s="184" t="s">
+        <v>375</v>
+      </c>
+      <c r="J134" s="179"/>
       <c r="K134" s="86"/>
       <c r="L134" s="11"/>
       <c r="M134" s="11"/>
@@ -34520,17 +35070,37 @@
       <c r="Z134" s="11"/>
       <c r="AA134" s="155"/>
     </row>
-    <row r="135" ht="12.75" customHeight="1">
-      <c r="A135" s="11"/>
-      <c r="B135" s="11"/>
-      <c r="C135" s="11"/>
-      <c r="D135" s="11"/>
-      <c r="E135" s="11"/>
-      <c r="F135" s="11"/>
-      <c r="G135" s="11"/>
-      <c r="H135" s="11"/>
-      <c r="I135" s="11"/>
-      <c r="J135" s="11"/>
+    <row r="135" ht="87.0" customHeight="1">
+      <c r="A135" s="160" t="str">
+        <f t="shared" si="8"/>
+        <v>[Manager-126]</v>
+      </c>
+      <c r="B135" s="160" t="s">
+        <v>606</v>
+      </c>
+      <c r="C135" s="183" t="s">
+        <v>628</v>
+      </c>
+      <c r="D135" s="183" t="s">
+        <v>629</v>
+      </c>
+      <c r="E135" s="160" t="str">
+        <f t="shared" si="9"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F135" s="161" t="s">
+        <v>398</v>
+      </c>
+      <c r="G135" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H135" s="163">
+        <v>44305.0</v>
+      </c>
+      <c r="I135" s="184" t="s">
+        <v>375</v>
+      </c>
+      <c r="J135" s="179"/>
       <c r="K135" s="86"/>
       <c r="L135" s="11"/>
       <c r="M135" s="11"/>
@@ -34549,17 +35119,37 @@
       <c r="Z135" s="11"/>
       <c r="AA135" s="155"/>
     </row>
-    <row r="136" ht="12.75" customHeight="1">
-      <c r="A136" s="11"/>
-      <c r="B136" s="11"/>
-      <c r="C136" s="11"/>
-      <c r="D136" s="11"/>
-      <c r="E136" s="11"/>
-      <c r="F136" s="11"/>
-      <c r="G136" s="11"/>
-      <c r="H136" s="11"/>
-      <c r="I136" s="11"/>
-      <c r="J136" s="11"/>
+    <row r="136" ht="86.25" customHeight="1">
+      <c r="A136" s="160" t="str">
+        <f t="shared" si="8"/>
+        <v>[Manager-127]</v>
+      </c>
+      <c r="B136" s="160" t="s">
+        <v>606</v>
+      </c>
+      <c r="C136" s="183" t="s">
+        <v>630</v>
+      </c>
+      <c r="D136" s="183" t="s">
+        <v>619</v>
+      </c>
+      <c r="E136" s="160" t="str">
+        <f t="shared" si="9"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F136" s="161" t="s">
+        <v>398</v>
+      </c>
+      <c r="G136" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H136" s="163">
+        <v>44305.0</v>
+      </c>
+      <c r="I136" s="184" t="s">
+        <v>375</v>
+      </c>
+      <c r="J136" s="179"/>
       <c r="K136" s="86"/>
       <c r="L136" s="11"/>
       <c r="M136" s="11"/>
@@ -34578,17 +35168,35 @@
       <c r="Z136" s="11"/>
       <c r="AA136" s="155"/>
     </row>
-    <row r="137" ht="12.75" customHeight="1">
-      <c r="A137" s="11"/>
-      <c r="B137" s="11"/>
-      <c r="C137" s="11"/>
-      <c r="D137" s="11"/>
-      <c r="E137" s="11"/>
-      <c r="F137" s="11"/>
-      <c r="G137" s="11"/>
-      <c r="H137" s="11"/>
-      <c r="I137" s="11"/>
-      <c r="J137" s="11"/>
+    <row r="137" ht="75.75" customHeight="1">
+      <c r="A137" s="160" t="str">
+        <f t="shared" si="8"/>
+        <v>[Manager-128]</v>
+      </c>
+      <c r="B137" s="173" t="s">
+        <v>631</v>
+      </c>
+      <c r="C137" s="185" t="s">
+        <v>632</v>
+      </c>
+      <c r="D137" s="185" t="s">
+        <v>633</v>
+      </c>
+      <c r="E137" s="160" t="str">
+        <f t="shared" si="9"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F137" s="161"/>
+      <c r="G137" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H137" s="163">
+        <v>44305.0</v>
+      </c>
+      <c r="I137" s="184" t="s">
+        <v>375</v>
+      </c>
+      <c r="J137" s="179"/>
       <c r="K137" s="86"/>
       <c r="L137" s="11"/>
       <c r="M137" s="11"/>
@@ -34607,17 +35215,35 @@
       <c r="Z137" s="11"/>
       <c r="AA137" s="155"/>
     </row>
-    <row r="138" ht="12.75" customHeight="1">
-      <c r="A138" s="11"/>
-      <c r="B138" s="11"/>
-      <c r="C138" s="11"/>
-      <c r="D138" s="11"/>
-      <c r="E138" s="11"/>
-      <c r="F138" s="11"/>
-      <c r="G138" s="11"/>
-      <c r="H138" s="11"/>
-      <c r="I138" s="11"/>
-      <c r="J138" s="11"/>
+    <row r="138" ht="54.0" customHeight="1">
+      <c r="A138" s="160" t="str">
+        <f t="shared" si="8"/>
+        <v>[Manager-129]</v>
+      </c>
+      <c r="B138" s="173" t="s">
+        <v>634</v>
+      </c>
+      <c r="C138" s="185" t="s">
+        <v>632</v>
+      </c>
+      <c r="D138" s="185" t="s">
+        <v>635</v>
+      </c>
+      <c r="E138" s="160" t="str">
+        <f t="shared" si="9"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F138" s="161"/>
+      <c r="G138" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H138" s="163">
+        <v>44305.0</v>
+      </c>
+      <c r="I138" s="184" t="s">
+        <v>375</v>
+      </c>
+      <c r="J138" s="179"/>
       <c r="K138" s="86"/>
       <c r="L138" s="11"/>
       <c r="M138" s="11"/>
@@ -34636,17 +35262,35 @@
       <c r="Z138" s="11"/>
       <c r="AA138" s="155"/>
     </row>
-    <row r="139" ht="12.75" customHeight="1">
-      <c r="A139" s="11"/>
-      <c r="B139" s="11"/>
-      <c r="C139" s="11"/>
-      <c r="D139" s="11"/>
-      <c r="E139" s="11"/>
-      <c r="F139" s="11"/>
-      <c r="G139" s="11"/>
-      <c r="H139" s="11"/>
-      <c r="I139" s="11"/>
-      <c r="J139" s="11"/>
+    <row r="139" ht="57.75" customHeight="1">
+      <c r="A139" s="160" t="str">
+        <f t="shared" si="8"/>
+        <v>[Manager-130]</v>
+      </c>
+      <c r="B139" s="160" t="s">
+        <v>578</v>
+      </c>
+      <c r="C139" s="183" t="s">
+        <v>636</v>
+      </c>
+      <c r="D139" s="161" t="s">
+        <v>637</v>
+      </c>
+      <c r="E139" s="160" t="str">
+        <f t="shared" si="9"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F139" s="161"/>
+      <c r="G139" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H139" s="163">
+        <v>44305.0</v>
+      </c>
+      <c r="I139" s="184" t="s">
+        <v>375</v>
+      </c>
+      <c r="J139" s="179"/>
       <c r="K139" s="86"/>
       <c r="L139" s="11"/>
       <c r="M139" s="11"/>
@@ -34665,17 +35309,35 @@
       <c r="Z139" s="11"/>
       <c r="AA139" s="155"/>
     </row>
-    <row r="140" ht="12.75" customHeight="1">
-      <c r="A140" s="11"/>
-      <c r="B140" s="11"/>
-      <c r="C140" s="11"/>
-      <c r="D140" s="11"/>
-      <c r="E140" s="11"/>
-      <c r="F140" s="11"/>
-      <c r="G140" s="11"/>
-      <c r="H140" s="11"/>
-      <c r="I140" s="11"/>
-      <c r="J140" s="11"/>
+    <row r="140" ht="76.5" customHeight="1">
+      <c r="A140" s="160" t="str">
+        <f t="shared" si="8"/>
+        <v>[Manager-131]</v>
+      </c>
+      <c r="B140" s="160" t="s">
+        <v>578</v>
+      </c>
+      <c r="C140" s="183" t="s">
+        <v>638</v>
+      </c>
+      <c r="D140" s="161" t="s">
+        <v>457</v>
+      </c>
+      <c r="E140" s="160" t="str">
+        <f t="shared" si="9"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F140" s="161"/>
+      <c r="G140" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H140" s="163">
+        <v>44305.0</v>
+      </c>
+      <c r="I140" s="184" t="s">
+        <v>375</v>
+      </c>
+      <c r="J140" s="179"/>
       <c r="K140" s="86"/>
       <c r="L140" s="11"/>
       <c r="M140" s="11"/>
@@ -34694,17 +35356,35 @@
       <c r="Z140" s="11"/>
       <c r="AA140" s="155"/>
     </row>
-    <row r="141" ht="12.75" customHeight="1">
-      <c r="A141" s="11"/>
-      <c r="B141" s="11"/>
-      <c r="C141" s="11"/>
-      <c r="D141" s="11"/>
-      <c r="E141" s="11"/>
-      <c r="F141" s="11"/>
-      <c r="G141" s="11"/>
-      <c r="H141" s="11"/>
-      <c r="I141" s="11"/>
-      <c r="J141" s="11"/>
+    <row r="141" ht="69.0" customHeight="1">
+      <c r="A141" s="160" t="str">
+        <f t="shared" si="8"/>
+        <v>[Manager-132]</v>
+      </c>
+      <c r="B141" s="160" t="s">
+        <v>578</v>
+      </c>
+      <c r="C141" s="183" t="s">
+        <v>639</v>
+      </c>
+      <c r="D141" s="161" t="s">
+        <v>640</v>
+      </c>
+      <c r="E141" s="160" t="str">
+        <f t="shared" si="9"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F141" s="161"/>
+      <c r="G141" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H141" s="163">
+        <v>44305.0</v>
+      </c>
+      <c r="I141" s="184" t="s">
+        <v>375</v>
+      </c>
+      <c r="J141" s="179"/>
       <c r="K141" s="86"/>
       <c r="L141" s="11"/>
       <c r="M141" s="11"/>
@@ -34723,17 +35403,19 @@
       <c r="Z141" s="11"/>
       <c r="AA141" s="155"/>
     </row>
-    <row r="142" ht="12.75" customHeight="1">
-      <c r="A142" s="11"/>
-      <c r="B142" s="11"/>
-      <c r="C142" s="11"/>
-      <c r="D142" s="11"/>
-      <c r="E142" s="11"/>
-      <c r="F142" s="11"/>
-      <c r="G142" s="11"/>
-      <c r="H142" s="11"/>
-      <c r="I142" s="11"/>
-      <c r="J142" s="11"/>
+    <row r="142" ht="27.75" customHeight="1">
+      <c r="A142" s="168" t="s">
+        <v>596</v>
+      </c>
+      <c r="B142" s="169"/>
+      <c r="C142" s="170"/>
+      <c r="D142" s="170"/>
+      <c r="E142" s="170"/>
+      <c r="F142" s="170"/>
+      <c r="G142" s="170"/>
+      <c r="H142" s="171"/>
+      <c r="I142" s="170"/>
+      <c r="J142" s="172"/>
       <c r="K142" s="86"/>
       <c r="L142" s="11"/>
       <c r="M142" s="11"/>
@@ -34752,17 +35434,35 @@
       <c r="Z142" s="11"/>
       <c r="AA142" s="155"/>
     </row>
-    <row r="143" ht="12.75" customHeight="1">
-      <c r="A143" s="11"/>
-      <c r="B143" s="11"/>
-      <c r="C143" s="11"/>
-      <c r="D143" s="11"/>
-      <c r="E143" s="11"/>
-      <c r="F143" s="11"/>
-      <c r="G143" s="11"/>
-      <c r="H143" s="11"/>
-      <c r="I143" s="11"/>
-      <c r="J143" s="11"/>
+    <row r="143" ht="49.5" customHeight="1">
+      <c r="A143" s="160" t="str">
+        <f t="shared" ref="A143:A170" si="10">IF(OR(B143&lt;&gt;"",D143&lt;&gt;""),"["&amp;TEXT($B$2,"##")&amp;"-"&amp;TEXT(ROW()-9,"##")&amp;"]","")</f>
+        <v>[Manager-134]</v>
+      </c>
+      <c r="B143" s="160" t="s">
+        <v>597</v>
+      </c>
+      <c r="C143" s="183" t="s">
+        <v>598</v>
+      </c>
+      <c r="D143" s="183" t="s">
+        <v>599</v>
+      </c>
+      <c r="E143" s="160" t="str">
+        <f t="shared" ref="E143:E170" si="11">$A$10</f>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F143" s="161"/>
+      <c r="G143" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H143" s="163">
+        <v>44306.0</v>
+      </c>
+      <c r="I143" s="184" t="s">
+        <v>375</v>
+      </c>
+      <c r="J143" s="179"/>
       <c r="K143" s="86"/>
       <c r="L143" s="11"/>
       <c r="M143" s="11"/>
@@ -34781,17 +35481,35 @@
       <c r="Z143" s="11"/>
       <c r="AA143" s="155"/>
     </row>
-    <row r="144" ht="12.75" customHeight="1">
-      <c r="A144" s="11"/>
-      <c r="B144" s="11"/>
-      <c r="C144" s="11"/>
-      <c r="D144" s="11"/>
-      <c r="E144" s="11"/>
-      <c r="F144" s="11"/>
-      <c r="G144" s="11"/>
-      <c r="H144" s="11"/>
-      <c r="I144" s="11"/>
-      <c r="J144" s="11"/>
+    <row r="144" ht="51.0" customHeight="1">
+      <c r="A144" s="160" t="str">
+        <f t="shared" si="10"/>
+        <v>[Manager-135]</v>
+      </c>
+      <c r="B144" s="160" t="s">
+        <v>600</v>
+      </c>
+      <c r="C144" s="183" t="s">
+        <v>601</v>
+      </c>
+      <c r="D144" s="183" t="s">
+        <v>602</v>
+      </c>
+      <c r="E144" s="160" t="str">
+        <f t="shared" si="11"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F144" s="161"/>
+      <c r="G144" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H144" s="163">
+        <v>44306.0</v>
+      </c>
+      <c r="I144" s="184" t="s">
+        <v>375</v>
+      </c>
+      <c r="J144" s="179"/>
       <c r="K144" s="86"/>
       <c r="L144" s="11"/>
       <c r="M144" s="11"/>
@@ -34810,17 +35528,35 @@
       <c r="Z144" s="11"/>
       <c r="AA144" s="155"/>
     </row>
-    <row r="145" ht="12.75" customHeight="1">
-      <c r="A145" s="11"/>
-      <c r="B145" s="11"/>
-      <c r="C145" s="11"/>
-      <c r="D145" s="11"/>
-      <c r="E145" s="11"/>
-      <c r="F145" s="11"/>
-      <c r="G145" s="11"/>
-      <c r="H145" s="11"/>
-      <c r="I145" s="11"/>
-      <c r="J145" s="11"/>
+    <row r="145" ht="59.25" customHeight="1">
+      <c r="A145" s="160" t="str">
+        <f t="shared" si="10"/>
+        <v>[Manager-136]</v>
+      </c>
+      <c r="B145" s="160" t="s">
+        <v>603</v>
+      </c>
+      <c r="C145" s="183" t="s">
+        <v>604</v>
+      </c>
+      <c r="D145" s="183" t="s">
+        <v>605</v>
+      </c>
+      <c r="E145" s="160" t="str">
+        <f t="shared" si="11"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F145" s="161"/>
+      <c r="G145" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H145" s="163">
+        <v>44306.0</v>
+      </c>
+      <c r="I145" s="184" t="s">
+        <v>375</v>
+      </c>
+      <c r="J145" s="179"/>
       <c r="K145" s="86"/>
       <c r="L145" s="11"/>
       <c r="M145" s="11"/>
@@ -34839,17 +35575,35 @@
       <c r="Z145" s="11"/>
       <c r="AA145" s="155"/>
     </row>
-    <row r="146" ht="12.75" customHeight="1">
-      <c r="A146" s="11"/>
-      <c r="B146" s="11"/>
-      <c r="C146" s="11"/>
-      <c r="D146" s="11"/>
-      <c r="E146" s="11"/>
-      <c r="F146" s="11"/>
-      <c r="G146" s="11"/>
-      <c r="H146" s="11"/>
-      <c r="I146" s="11"/>
-      <c r="J146" s="11"/>
+    <row r="146" ht="70.5" customHeight="1">
+      <c r="A146" s="160" t="str">
+        <f t="shared" si="10"/>
+        <v>[Manager-137]</v>
+      </c>
+      <c r="B146" s="160" t="s">
+        <v>606</v>
+      </c>
+      <c r="C146" s="183" t="s">
+        <v>607</v>
+      </c>
+      <c r="D146" s="183" t="s">
+        <v>608</v>
+      </c>
+      <c r="E146" s="160" t="str">
+        <f t="shared" si="11"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F146" s="161"/>
+      <c r="G146" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H146" s="163">
+        <v>44306.0</v>
+      </c>
+      <c r="I146" s="184" t="s">
+        <v>375</v>
+      </c>
+      <c r="J146" s="179"/>
       <c r="K146" s="86"/>
       <c r="L146" s="11"/>
       <c r="M146" s="11"/>
@@ -34868,17 +35622,35 @@
       <c r="Z146" s="11"/>
       <c r="AA146" s="155"/>
     </row>
-    <row r="147" ht="12.75" customHeight="1">
-      <c r="A147" s="11"/>
-      <c r="B147" s="11"/>
-      <c r="C147" s="11"/>
-      <c r="D147" s="11"/>
-      <c r="E147" s="11"/>
-      <c r="F147" s="11"/>
-      <c r="G147" s="11"/>
-      <c r="H147" s="11"/>
-      <c r="I147" s="11"/>
-      <c r="J147" s="11"/>
+    <row r="147" ht="81.75" customHeight="1">
+      <c r="A147" s="160" t="str">
+        <f t="shared" si="10"/>
+        <v>[Manager-138]</v>
+      </c>
+      <c r="B147" s="160" t="s">
+        <v>606</v>
+      </c>
+      <c r="C147" s="183" t="s">
+        <v>609</v>
+      </c>
+      <c r="D147" s="183" t="s">
+        <v>610</v>
+      </c>
+      <c r="E147" s="160" t="str">
+        <f t="shared" si="11"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F147" s="161"/>
+      <c r="G147" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H147" s="163">
+        <v>44306.0</v>
+      </c>
+      <c r="I147" s="184" t="s">
+        <v>375</v>
+      </c>
+      <c r="J147" s="179"/>
       <c r="K147" s="86"/>
       <c r="L147" s="11"/>
       <c r="M147" s="11"/>
@@ -34897,17 +35669,35 @@
       <c r="Z147" s="11"/>
       <c r="AA147" s="155"/>
     </row>
-    <row r="148" ht="12.75" customHeight="1">
-      <c r="A148" s="11"/>
-      <c r="B148" s="11"/>
-      <c r="C148" s="11"/>
-      <c r="D148" s="11"/>
-      <c r="E148" s="11"/>
-      <c r="F148" s="11"/>
-      <c r="G148" s="11"/>
-      <c r="H148" s="11"/>
-      <c r="I148" s="11"/>
-      <c r="J148" s="11"/>
+    <row r="148" ht="93.0" customHeight="1">
+      <c r="A148" s="160" t="str">
+        <f t="shared" si="10"/>
+        <v>[Manager-139]</v>
+      </c>
+      <c r="B148" s="160" t="s">
+        <v>606</v>
+      </c>
+      <c r="C148" s="183" t="s">
+        <v>611</v>
+      </c>
+      <c r="D148" s="183" t="s">
+        <v>612</v>
+      </c>
+      <c r="E148" s="160" t="str">
+        <f t="shared" si="11"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F148" s="161"/>
+      <c r="G148" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H148" s="163">
+        <v>44306.0</v>
+      </c>
+      <c r="I148" s="184" t="s">
+        <v>375</v>
+      </c>
+      <c r="J148" s="179"/>
       <c r="K148" s="86"/>
       <c r="L148" s="11"/>
       <c r="M148" s="11"/>
@@ -34926,17 +35716,35 @@
       <c r="Z148" s="11"/>
       <c r="AA148" s="155"/>
     </row>
-    <row r="149" ht="12.75" customHeight="1">
-      <c r="A149" s="11"/>
-      <c r="B149" s="11"/>
-      <c r="C149" s="11"/>
-      <c r="D149" s="11"/>
-      <c r="E149" s="11"/>
-      <c r="F149" s="11"/>
-      <c r="G149" s="11"/>
-      <c r="H149" s="11"/>
-      <c r="I149" s="11"/>
-      <c r="J149" s="11"/>
+    <row r="149" ht="80.25" customHeight="1">
+      <c r="A149" s="160" t="str">
+        <f t="shared" si="10"/>
+        <v>[Manager-140]</v>
+      </c>
+      <c r="B149" s="160" t="s">
+        <v>606</v>
+      </c>
+      <c r="C149" s="183" t="s">
+        <v>613</v>
+      </c>
+      <c r="D149" s="183" t="s">
+        <v>614</v>
+      </c>
+      <c r="E149" s="160" t="str">
+        <f t="shared" si="11"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F149" s="161"/>
+      <c r="G149" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H149" s="163">
+        <v>44306.0</v>
+      </c>
+      <c r="I149" s="184" t="s">
+        <v>375</v>
+      </c>
+      <c r="J149" s="179"/>
       <c r="K149" s="86"/>
       <c r="L149" s="11"/>
       <c r="M149" s="11"/>
@@ -34955,17 +35763,35 @@
       <c r="Z149" s="11"/>
       <c r="AA149" s="155"/>
     </row>
-    <row r="150" ht="12.75" customHeight="1">
-      <c r="A150" s="11"/>
-      <c r="B150" s="11"/>
-      <c r="C150" s="11"/>
-      <c r="D150" s="11"/>
-      <c r="E150" s="11"/>
-      <c r="F150" s="11"/>
-      <c r="G150" s="11"/>
-      <c r="H150" s="11"/>
-      <c r="I150" s="11"/>
-      <c r="J150" s="11"/>
+    <row r="150" ht="87.75" customHeight="1">
+      <c r="A150" s="160" t="str">
+        <f t="shared" si="10"/>
+        <v>[Manager-141]</v>
+      </c>
+      <c r="B150" s="160" t="s">
+        <v>606</v>
+      </c>
+      <c r="C150" s="183" t="s">
+        <v>615</v>
+      </c>
+      <c r="D150" s="183" t="s">
+        <v>616</v>
+      </c>
+      <c r="E150" s="160" t="str">
+        <f t="shared" si="11"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F150" s="161"/>
+      <c r="G150" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H150" s="163">
+        <v>44306.0</v>
+      </c>
+      <c r="I150" s="184" t="s">
+        <v>375</v>
+      </c>
+      <c r="J150" s="179"/>
       <c r="K150" s="86"/>
       <c r="L150" s="11"/>
       <c r="M150" s="11"/>
@@ -34984,17 +35810,35 @@
       <c r="Z150" s="11"/>
       <c r="AA150" s="155"/>
     </row>
-    <row r="151" ht="12.75" customHeight="1">
-      <c r="A151" s="11"/>
-      <c r="B151" s="11"/>
-      <c r="C151" s="11"/>
-      <c r="D151" s="11"/>
-      <c r="E151" s="11"/>
-      <c r="F151" s="11"/>
-      <c r="G151" s="11"/>
-      <c r="H151" s="11"/>
-      <c r="I151" s="11"/>
-      <c r="J151" s="11"/>
+    <row r="151" ht="109.5" customHeight="1">
+      <c r="A151" s="160" t="str">
+        <f t="shared" si="10"/>
+        <v>[Manager-142]</v>
+      </c>
+      <c r="B151" s="160" t="s">
+        <v>606</v>
+      </c>
+      <c r="C151" s="183" t="s">
+        <v>617</v>
+      </c>
+      <c r="D151" s="183" t="s">
+        <v>614</v>
+      </c>
+      <c r="E151" s="160" t="str">
+        <f t="shared" si="11"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F151" s="161"/>
+      <c r="G151" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H151" s="163">
+        <v>44306.0</v>
+      </c>
+      <c r="I151" s="184" t="s">
+        <v>375</v>
+      </c>
+      <c r="J151" s="179"/>
       <c r="K151" s="86"/>
       <c r="L151" s="11"/>
       <c r="M151" s="11"/>
@@ -35013,25 +35857,459 @@
       <c r="Z151" s="11"/>
       <c r="AA151" s="155"/>
     </row>
-    <row r="152" ht="15.75" customHeight="1"/>
-    <row r="153" ht="15.75" customHeight="1"/>
-    <row r="154" ht="15.75" customHeight="1"/>
-    <row r="155" ht="15.75" customHeight="1"/>
-    <row r="156" ht="15.75" customHeight="1"/>
-    <row r="157" ht="15.75" customHeight="1"/>
-    <row r="158" ht="15.75" customHeight="1"/>
-    <row r="159" ht="15.75" customHeight="1"/>
-    <row r="160" ht="15.75" customHeight="1"/>
-    <row r="161" ht="15.75" customHeight="1"/>
-    <row r="162" ht="15.75" customHeight="1"/>
-    <row r="163" ht="15.75" customHeight="1"/>
-    <row r="164" ht="15.75" customHeight="1"/>
-    <row r="165" ht="15.75" customHeight="1"/>
-    <row r="166" ht="15.75" customHeight="1"/>
-    <row r="167" ht="15.75" customHeight="1"/>
-    <row r="168" ht="15.75" customHeight="1"/>
-    <row r="169" ht="15.75" customHeight="1"/>
-    <row r="170" ht="15.75" customHeight="1"/>
+    <row r="152" ht="109.5" customHeight="1">
+      <c r="A152" s="160" t="str">
+        <f t="shared" si="10"/>
+        <v>[Manager-143]</v>
+      </c>
+      <c r="B152" s="160" t="s">
+        <v>606</v>
+      </c>
+      <c r="C152" s="167" t="s">
+        <v>618</v>
+      </c>
+      <c r="D152" s="167" t="s">
+        <v>619</v>
+      </c>
+      <c r="E152" s="160" t="str">
+        <f t="shared" si="11"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F152" s="161"/>
+      <c r="G152" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H152" s="163">
+        <v>44306.0</v>
+      </c>
+      <c r="I152" s="166" t="s">
+        <v>375</v>
+      </c>
+      <c r="J152" s="179"/>
+    </row>
+    <row r="153" ht="15.75" customHeight="1">
+      <c r="A153" s="160" t="str">
+        <f t="shared" si="10"/>
+        <v>[Manager-144]</v>
+      </c>
+      <c r="B153" s="160" t="s">
+        <v>606</v>
+      </c>
+      <c r="C153" s="167" t="s">
+        <v>620</v>
+      </c>
+      <c r="D153" s="167" t="s">
+        <v>621</v>
+      </c>
+      <c r="E153" s="160" t="str">
+        <f t="shared" si="11"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F153" s="161"/>
+      <c r="G153" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H153" s="163">
+        <v>44306.0</v>
+      </c>
+      <c r="I153" s="166" t="s">
+        <v>375</v>
+      </c>
+      <c r="J153" s="179"/>
+    </row>
+    <row r="154" ht="15.75" customHeight="1">
+      <c r="A154" s="160" t="str">
+        <f t="shared" si="10"/>
+        <v>[Manager-145]</v>
+      </c>
+      <c r="B154" s="160" t="s">
+        <v>606</v>
+      </c>
+      <c r="C154" s="167" t="s">
+        <v>622</v>
+      </c>
+      <c r="D154" s="167" t="s">
+        <v>619</v>
+      </c>
+      <c r="E154" s="160" t="str">
+        <f t="shared" si="11"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F154" s="161"/>
+      <c r="G154" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H154" s="163">
+        <v>44306.0</v>
+      </c>
+      <c r="I154" s="166" t="s">
+        <v>375</v>
+      </c>
+      <c r="J154" s="179"/>
+    </row>
+    <row r="155" ht="15.75" customHeight="1">
+      <c r="A155" s="160" t="str">
+        <f t="shared" si="10"/>
+        <v>[Manager-146]</v>
+      </c>
+      <c r="B155" s="160" t="s">
+        <v>606</v>
+      </c>
+      <c r="C155" s="167" t="s">
+        <v>623</v>
+      </c>
+      <c r="D155" s="167" t="s">
+        <v>624</v>
+      </c>
+      <c r="E155" s="160" t="str">
+        <f t="shared" si="11"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F155" s="161"/>
+      <c r="G155" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H155" s="163">
+        <v>44306.0</v>
+      </c>
+      <c r="I155" s="166" t="s">
+        <v>375</v>
+      </c>
+      <c r="J155" s="179"/>
+    </row>
+    <row r="156" ht="15.75" customHeight="1">
+      <c r="A156" s="160" t="str">
+        <f t="shared" si="10"/>
+        <v>[Manager-147]</v>
+      </c>
+      <c r="B156" s="160" t="s">
+        <v>606</v>
+      </c>
+      <c r="C156" s="167" t="s">
+        <v>625</v>
+      </c>
+      <c r="D156" s="167" t="s">
+        <v>624</v>
+      </c>
+      <c r="E156" s="160" t="str">
+        <f t="shared" si="11"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F156" s="161"/>
+      <c r="G156" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H156" s="163">
+        <v>44306.0</v>
+      </c>
+      <c r="I156" s="166" t="s">
+        <v>375</v>
+      </c>
+      <c r="J156" s="179"/>
+    </row>
+    <row r="157" ht="15.75" customHeight="1">
+      <c r="A157" s="160" t="str">
+        <f t="shared" si="10"/>
+        <v>[Manager-148]</v>
+      </c>
+      <c r="B157" s="160" t="s">
+        <v>606</v>
+      </c>
+      <c r="C157" s="167" t="s">
+        <v>626</v>
+      </c>
+      <c r="D157" s="167" t="s">
+        <v>624</v>
+      </c>
+      <c r="E157" s="160" t="str">
+        <f t="shared" si="11"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F157" s="161"/>
+      <c r="G157" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H157" s="163">
+        <v>44306.0</v>
+      </c>
+      <c r="I157" s="166" t="s">
+        <v>375</v>
+      </c>
+      <c r="J157" s="179"/>
+    </row>
+    <row r="158" ht="15.75" customHeight="1">
+      <c r="A158" s="160" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="E158" s="160" t="str">
+        <f t="shared" si="11"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F158" s="161"/>
+      <c r="G158" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H158" s="163">
+        <v>44306.0</v>
+      </c>
+      <c r="I158" s="166" t="s">
+        <v>375</v>
+      </c>
+      <c r="J158" s="179"/>
+    </row>
+    <row r="159" ht="15.75" customHeight="1">
+      <c r="A159" s="160" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="E159" s="160" t="str">
+        <f t="shared" si="11"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F159" s="161"/>
+      <c r="G159" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H159" s="163">
+        <v>44306.0</v>
+      </c>
+      <c r="I159" s="166" t="s">
+        <v>375</v>
+      </c>
+      <c r="J159" s="179"/>
+    </row>
+    <row r="160" ht="15.75" customHeight="1">
+      <c r="A160" s="160" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="E160" s="160" t="str">
+        <f t="shared" si="11"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F160" s="161"/>
+      <c r="G160" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H160" s="163">
+        <v>44306.0</v>
+      </c>
+      <c r="I160" s="166" t="s">
+        <v>375</v>
+      </c>
+      <c r="J160" s="179"/>
+    </row>
+    <row r="161" ht="15.75" customHeight="1">
+      <c r="A161" s="160" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="E161" s="160" t="str">
+        <f t="shared" si="11"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F161" s="161"/>
+      <c r="G161" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H161" s="163">
+        <v>44306.0</v>
+      </c>
+      <c r="I161" s="166" t="s">
+        <v>375</v>
+      </c>
+      <c r="J161" s="179"/>
+    </row>
+    <row r="162" ht="15.75" customHeight="1">
+      <c r="A162" s="160" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="E162" s="160" t="str">
+        <f t="shared" si="11"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F162" s="161"/>
+      <c r="G162" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H162" s="163">
+        <v>44306.0</v>
+      </c>
+      <c r="I162" s="166" t="s">
+        <v>375</v>
+      </c>
+      <c r="J162" s="179"/>
+    </row>
+    <row r="163" ht="15.75" customHeight="1">
+      <c r="A163" s="160" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="E163" s="160" t="str">
+        <f t="shared" si="11"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F163" s="161"/>
+      <c r="G163" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H163" s="163">
+        <v>44306.0</v>
+      </c>
+      <c r="I163" s="166" t="s">
+        <v>375</v>
+      </c>
+      <c r="J163" s="179"/>
+    </row>
+    <row r="164" ht="15.75" customHeight="1">
+      <c r="A164" s="160" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="E164" s="160" t="str">
+        <f t="shared" si="11"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F164" s="161"/>
+      <c r="G164" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H164" s="163">
+        <v>44306.0</v>
+      </c>
+      <c r="I164" s="166" t="s">
+        <v>375</v>
+      </c>
+      <c r="J164" s="179"/>
+    </row>
+    <row r="165" ht="15.75" customHeight="1">
+      <c r="A165" s="160" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="E165" s="160" t="str">
+        <f t="shared" si="11"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F165" s="161"/>
+      <c r="G165" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H165" s="163">
+        <v>44306.0</v>
+      </c>
+      <c r="I165" s="166" t="s">
+        <v>375</v>
+      </c>
+      <c r="J165" s="179"/>
+    </row>
+    <row r="166" ht="15.75" customHeight="1">
+      <c r="A166" s="160" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="E166" s="160" t="str">
+        <f t="shared" si="11"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F166" s="161"/>
+      <c r="G166" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H166" s="163">
+        <v>44306.0</v>
+      </c>
+      <c r="I166" s="166" t="s">
+        <v>375</v>
+      </c>
+      <c r="J166" s="179"/>
+    </row>
+    <row r="167" ht="15.75" customHeight="1">
+      <c r="A167" s="160" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="E167" s="160" t="str">
+        <f t="shared" si="11"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F167" s="161"/>
+      <c r="G167" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H167" s="163">
+        <v>44306.0</v>
+      </c>
+      <c r="I167" s="166" t="s">
+        <v>375</v>
+      </c>
+      <c r="J167" s="179"/>
+    </row>
+    <row r="168" ht="15.75" customHeight="1">
+      <c r="A168" s="160" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="E168" s="160" t="str">
+        <f t="shared" si="11"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F168" s="161"/>
+      <c r="G168" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H168" s="163">
+        <v>44306.0</v>
+      </c>
+      <c r="I168" s="166" t="s">
+        <v>375</v>
+      </c>
+      <c r="J168" s="179"/>
+    </row>
+    <row r="169" ht="15.75" customHeight="1">
+      <c r="A169" s="160" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="E169" s="160" t="str">
+        <f t="shared" si="11"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F169" s="161"/>
+      <c r="G169" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H169" s="163">
+        <v>44306.0</v>
+      </c>
+      <c r="I169" s="166" t="s">
+        <v>375</v>
+      </c>
+      <c r="J169" s="179"/>
+    </row>
+    <row r="170" ht="15.75" customHeight="1">
+      <c r="A170" s="160" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="E170" s="160" t="str">
+        <f t="shared" si="11"/>
+        <v>[Manager-1]</v>
+      </c>
+      <c r="F170" s="161"/>
+      <c r="G170" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="H170" s="163">
+        <v>44306.0</v>
+      </c>
+      <c r="I170" s="166" t="s">
+        <v>375</v>
+      </c>
+      <c r="J170" s="179"/>
+    </row>
     <row r="171" ht="15.75" customHeight="1"/>
     <row r="172" ht="15.75" customHeight="1"/>
     <row r="173" ht="15.75" customHeight="1"/>
@@ -35879,7 +37157,7 @@
     <mergeCell ref="B4:E4"/>
   </mergeCells>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G8:G73 G101">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G8:G73 G101 G118:G170">
       <formula1>$M$2:$M$5</formula1>
     </dataValidation>
   </dataValidations>
@@ -35916,7 +37194,7 @@
     <row r="1" ht="25.5" customHeight="1">
       <c r="A1" s="11"/>
       <c r="B1" s="186" t="s">
-        <v>596</v>
+        <v>641</v>
       </c>
       <c r="C1" s="187"/>
       <c r="D1" s="187"/>
@@ -36083,10 +37361,10 @@
     <row r="6" ht="21.75" customHeight="1">
       <c r="A6" s="188"/>
       <c r="B6" s="194" t="s">
-        <v>597</v>
+        <v>642</v>
       </c>
       <c r="C6" s="196" t="s">
-        <v>598</v>
+        <v>643</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -36202,7 +37480,7 @@
         <v>23</v>
       </c>
       <c r="C10" s="200" t="s">
-        <v>599</v>
+        <v>644</v>
       </c>
       <c r="D10" s="201" t="s">
         <v>83</v>
@@ -36217,7 +37495,7 @@
         <v>90</v>
       </c>
       <c r="H10" s="203" t="s">
-        <v>600</v>
+        <v>645</v>
       </c>
       <c r="I10" s="11"/>
       <c r="J10" s="11"/>
@@ -36386,7 +37664,7 @@
       <c r="A14" s="198"/>
       <c r="B14" s="209"/>
       <c r="C14" s="210" t="s">
-        <v>601</v>
+        <v>646</v>
       </c>
       <c r="D14" s="211">
         <f t="shared" ref="D14:H14" si="1">SUM(D9:D13)</f>
@@ -36459,7 +37737,7 @@
       <c r="A16" s="11"/>
       <c r="B16" s="11"/>
       <c r="C16" s="9" t="s">
-        <v>602</v>
+        <v>647</v>
       </c>
       <c r="D16" s="11"/>
       <c r="E16" s="216">
@@ -36467,7 +37745,7 @@
         <v>46.53465347</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>603</v>
+        <v>648</v>
       </c>
       <c r="G16" s="11"/>
       <c r="H16" s="132"/>
@@ -36494,7 +37772,7 @@
       <c r="A17" s="11"/>
       <c r="B17" s="11"/>
       <c r="C17" s="9" t="s">
-        <v>604</v>
+        <v>649</v>
       </c>
       <c r="D17" s="11"/>
       <c r="E17" s="216">
@@ -36502,7 +37780,7 @@
         <v>42.57425743</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>603</v>
+        <v>648</v>
       </c>
       <c r="G17" s="11"/>
       <c r="H17" s="132"/>

</xml_diff>

<commit_message>
HoangNH - Update test case manager Manage Feedback
</commit_message>
<xml_diff>
--- a/3. Users/HoangNHHE130395/Testing/TestCase - Hoang.xlsx
+++ b/3. Users/HoangNHHE130395/Testing/TestCase - Hoang.xlsx
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1549" uniqueCount="650">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1543" uniqueCount="686">
   <si>
     <t>SYSTEM TEST CASE</t>
   </si>
@@ -2881,6 +2881,199 @@
     <t>1. Popup is disappeared
 2. Toast message 'Xóa Voucher thành công'
 3. The list is updated</t>
+  </si>
+  <si>
+    <t>Function Manage Feedback</t>
+  </si>
+  <si>
+    <t>Check GUI search box 'Search Feecback'</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'Feedback' tab in the menu bar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Display text 'Search feedback' on the search box </t>
+  </si>
+  <si>
+    <t>Check focus on search box 'Search Feedback'</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'Feedback' tab in the menu bar
+3. Click on the search box 'Search Feedback'</t>
+  </si>
+  <si>
+    <t>1. Display text 'Search Feedback' on the search box 
+2. Border of the search box change to blue</t>
+  </si>
+  <si>
+    <t>Check focus out search box 'Search Feedback'</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'Feedback' tab in the menu bar
+3. Click on the search box 'Search Feedback'
+4. Click out of the search box 'Search Feedback'</t>
+  </si>
+  <si>
+    <t>1. Display text 'Search Feedback' on the search box 
+2. Border of the search box change from blue to white</t>
+  </si>
+  <si>
+    <t>Check function seach box 'Search Feedback'</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'Feedback' tab in the menu bar
+3. Click on the search box 'Search Feedback'
+4. Input text 'a' on the search box</t>
+  </si>
+  <si>
+    <t>1. Display text 'a' on the search box 
+2. Border of the search box change to blue
+3. Display list of Feedback have send by contain character 'a'</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'Feedback' tab in the menu bar
+3. Click on the search box 'Search Feedback'
+4. Input text 'a' on the search box
+5. Input text 'a' on the search box</t>
+  </si>
+  <si>
+    <t>1. Display text 'aa' on the search box 
+2. Border of the search box change to blue
+3. Display list of Feedback have title Send By character 'aa'</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'Feedback' tab in the menu bar
+3. Click on the search box 'Search Feedback'
+4. Input text 'a' on the search box
+5. Input text 'a' on the search box
+6. Press delete button on keyboard</t>
+  </si>
+  <si>
+    <t>1. Display text 'a' on the search box 
+2. Border of the search box change to blue
+3. Display list of Feedback have Send By contain character 'a'</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'Feedback' tab in the menu bar
+3. Choose 'Title' from the drop down list
+4. Click on the search box 'Search Feedback'
+5. Input text 'a' on the search box</t>
+  </si>
+  <si>
+    <t>1. Display text 'a' on the search box 
+2. Border of the search box change to blue
+3. Display list of Feedback have title contain character 'a'</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'Feedback' tab in the menu bar
+3. Choose 'Title' from the drop down list
+4. Click on the search box 'Search Voucher'
+5. Input text 'a' on the search box
+6. Input text 'a' on the search box</t>
+  </si>
+  <si>
+    <t>1. Display text 'aa' on the search box 
+2. Border of the search box change to blue
+3. Display list of Feedback have title contain character 'aa'</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'Feedback' tab in the menu bar
+3. Choose 'Title' from the drop down list
+4. Click on the search box 'Search Voucher'
+5. Input text 'a' on the search box
+6. Input text 'a' on the search box
+7. Press delete button on keyboard</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'Feedback' tab in the menu bar
+3. Choose 'Content' from the drop down list
+4. Click on the search box 'Search Feedback'
+5. Input text 'a' on the search box</t>
+  </si>
+  <si>
+    <t>1. Display text 'a' on the search box 
+2. Border of the search box change to blue
+3. Display list of Feedback have Content contain character 'a'</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'Feedback' tab in the menu bar
+3. Choose 'Content' from the drop down list
+4. Click on the search box 'Search Voucher'
+5. Input text 'a' on the search box
+6. Input text 'a' on the search box</t>
+  </si>
+  <si>
+    <t>1. Display text 'aa' on the search box 
+2. Border of the search box change to blue
+3. Display list of Feedback have Content contain character 'aa'</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'Feedback' tab in the menu bar
+3. Choose 'Content' from the drop down list
+4. Click on the search box 'Search Voucher'
+5. Input text 'a' on the search box
+6. Input text 'a' on the search box
+7. Press delete button on keyboard</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'Feedback' tab in the menu bar
+3. Choose 'Title' from the drop down list
+4. Click on the search box 'Search Feedback'
+5. Input text 'a' on the search box
+6. Choose 'Send By' from the drop down list</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'Feedback' tab in the menu bar
+3. Choose 'Title' from the drop down list
+4. Click on the search box 'Search Feedback'
+5. Input text 'a' on the search box
+6. Choose 'Content' from the drop down list</t>
+  </si>
+  <si>
+    <t>Check function button 'Accept'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Login into the web server
+2. Click on 'Feedback' tab in the menu bar
+3. From list choose feedback have id= '7' click 'Accept'
+</t>
+  </si>
+  <si>
+    <t>1. Display popup confirm 'Đọc feed back này và gửi thông báo cho người dùng?'</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'Feedback' tab in the menu bar
+3. From list choose feedback have id= '7' click 'Accept'
+4. Click on 'Hủy'</t>
+  </si>
+  <si>
+    <t>1. Login into the web server
+2. Click on 'Feedback' tab in the menu bar
+3. From list choose feedback have id= '7' click 'Accept'
+4. Click on 'Ok'</t>
+  </si>
+  <si>
+    <t>1. Popup is disappeared
+2. Toast message 'Đã xác nhận feedback'
+3. The list is updated</t>
+  </si>
+  <si>
+    <t>Bug-59</t>
   </si>
   <si>
     <t>TEST REPORT</t>
@@ -3766,7 +3959,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="217">
+  <cellXfs count="218">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -4254,6 +4447,9 @@
     </xf>
     <xf borderId="13" fillId="0" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="24" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
@@ -35405,7 +35601,7 @@
     </row>
     <row r="142" ht="27.75" customHeight="1">
       <c r="A142" s="168" t="s">
-        <v>596</v>
+        <v>641</v>
       </c>
       <c r="B142" s="169"/>
       <c r="C142" s="170"/>
@@ -35436,20 +35632,20 @@
     </row>
     <row r="143" ht="49.5" customHeight="1">
       <c r="A143" s="160" t="str">
-        <f t="shared" ref="A143:A170" si="10">IF(OR(B143&lt;&gt;"",D143&lt;&gt;""),"["&amp;TEXT($B$2,"##")&amp;"-"&amp;TEXT(ROW()-9,"##")&amp;"]","")</f>
+        <f t="shared" ref="A143:A159" si="10">IF(OR(B143&lt;&gt;"",D143&lt;&gt;""),"["&amp;TEXT($B$2,"##")&amp;"-"&amp;TEXT(ROW()-9,"##")&amp;"]","")</f>
         <v>[Manager-134]</v>
       </c>
       <c r="B143" s="160" t="s">
-        <v>597</v>
+        <v>642</v>
       </c>
       <c r="C143" s="183" t="s">
-        <v>598</v>
+        <v>643</v>
       </c>
       <c r="D143" s="183" t="s">
-        <v>599</v>
+        <v>644</v>
       </c>
       <c r="E143" s="160" t="str">
-        <f t="shared" ref="E143:E170" si="11">$A$10</f>
+        <f t="shared" ref="E143:E159" si="11">$A$10</f>
         <v>[Manager-1]</v>
       </c>
       <c r="F143" s="161"/>
@@ -35487,13 +35683,13 @@
         <v>[Manager-135]</v>
       </c>
       <c r="B144" s="160" t="s">
-        <v>600</v>
+        <v>645</v>
       </c>
       <c r="C144" s="183" t="s">
-        <v>601</v>
+        <v>646</v>
       </c>
       <c r="D144" s="183" t="s">
-        <v>602</v>
+        <v>647</v>
       </c>
       <c r="E144" s="160" t="str">
         <f t="shared" si="11"/>
@@ -35510,7 +35706,7 @@
         <v>375</v>
       </c>
       <c r="J144" s="179"/>
-      <c r="K144" s="86"/>
+      <c r="K144" s="186"/>
       <c r="L144" s="11"/>
       <c r="M144" s="11"/>
       <c r="N144" s="11"/>
@@ -35534,13 +35730,13 @@
         <v>[Manager-136]</v>
       </c>
       <c r="B145" s="160" t="s">
-        <v>603</v>
+        <v>648</v>
       </c>
       <c r="C145" s="183" t="s">
-        <v>604</v>
+        <v>649</v>
       </c>
       <c r="D145" s="183" t="s">
-        <v>605</v>
+        <v>650</v>
       </c>
       <c r="E145" s="160" t="str">
         <f t="shared" si="11"/>
@@ -35581,19 +35777,21 @@
         <v>[Manager-137]</v>
       </c>
       <c r="B146" s="160" t="s">
-        <v>606</v>
+        <v>651</v>
       </c>
       <c r="C146" s="183" t="s">
-        <v>607</v>
+        <v>652</v>
       </c>
       <c r="D146" s="183" t="s">
-        <v>608</v>
+        <v>653</v>
       </c>
       <c r="E146" s="160" t="str">
         <f t="shared" si="11"/>
         <v>[Manager-1]</v>
       </c>
-      <c r="F146" s="161"/>
+      <c r="F146" s="161" t="s">
+        <v>398</v>
+      </c>
       <c r="G146" s="162" t="s">
         <v>83</v>
       </c>
@@ -35628,19 +35826,21 @@
         <v>[Manager-138]</v>
       </c>
       <c r="B147" s="160" t="s">
-        <v>606</v>
+        <v>651</v>
       </c>
       <c r="C147" s="183" t="s">
-        <v>609</v>
+        <v>654</v>
       </c>
       <c r="D147" s="183" t="s">
-        <v>610</v>
+        <v>655</v>
       </c>
       <c r="E147" s="160" t="str">
         <f t="shared" si="11"/>
         <v>[Manager-1]</v>
       </c>
-      <c r="F147" s="161"/>
+      <c r="F147" s="161" t="s">
+        <v>401</v>
+      </c>
       <c r="G147" s="162" t="s">
         <v>83</v>
       </c>
@@ -35675,19 +35875,21 @@
         <v>[Manager-139]</v>
       </c>
       <c r="B148" s="160" t="s">
-        <v>606</v>
+        <v>651</v>
       </c>
       <c r="C148" s="183" t="s">
-        <v>611</v>
+        <v>656</v>
       </c>
       <c r="D148" s="183" t="s">
-        <v>612</v>
+        <v>657</v>
       </c>
       <c r="E148" s="160" t="str">
         <f t="shared" si="11"/>
         <v>[Manager-1]</v>
       </c>
-      <c r="F148" s="161"/>
+      <c r="F148" s="161" t="s">
+        <v>401</v>
+      </c>
       <c r="G148" s="162" t="s">
         <v>83</v>
       </c>
@@ -35722,19 +35924,21 @@
         <v>[Manager-140]</v>
       </c>
       <c r="B149" s="160" t="s">
-        <v>606</v>
+        <v>651</v>
       </c>
       <c r="C149" s="183" t="s">
-        <v>613</v>
+        <v>658</v>
       </c>
       <c r="D149" s="183" t="s">
-        <v>614</v>
+        <v>659</v>
       </c>
       <c r="E149" s="160" t="str">
         <f t="shared" si="11"/>
         <v>[Manager-1]</v>
       </c>
-      <c r="F149" s="161"/>
+      <c r="F149" s="161" t="s">
+        <v>398</v>
+      </c>
       <c r="G149" s="162" t="s">
         <v>83</v>
       </c>
@@ -35769,19 +35973,21 @@
         <v>[Manager-141]</v>
       </c>
       <c r="B150" s="160" t="s">
-        <v>606</v>
+        <v>651</v>
       </c>
       <c r="C150" s="183" t="s">
-        <v>615</v>
+        <v>660</v>
       </c>
       <c r="D150" s="183" t="s">
-        <v>616</v>
+        <v>661</v>
       </c>
       <c r="E150" s="160" t="str">
         <f t="shared" si="11"/>
         <v>[Manager-1]</v>
       </c>
-      <c r="F150" s="161"/>
+      <c r="F150" s="161" t="s">
+        <v>401</v>
+      </c>
       <c r="G150" s="162" t="s">
         <v>83</v>
       </c>
@@ -35816,19 +36022,21 @@
         <v>[Manager-142]</v>
       </c>
       <c r="B151" s="160" t="s">
-        <v>606</v>
+        <v>651</v>
       </c>
       <c r="C151" s="183" t="s">
-        <v>617</v>
+        <v>662</v>
       </c>
       <c r="D151" s="183" t="s">
-        <v>614</v>
+        <v>659</v>
       </c>
       <c r="E151" s="160" t="str">
         <f t="shared" si="11"/>
         <v>[Manager-1]</v>
       </c>
-      <c r="F151" s="161"/>
+      <c r="F151" s="161" t="s">
+        <v>401</v>
+      </c>
       <c r="G151" s="162" t="s">
         <v>83</v>
       </c>
@@ -35863,19 +36071,21 @@
         <v>[Manager-143]</v>
       </c>
       <c r="B152" s="160" t="s">
-        <v>606</v>
-      </c>
-      <c r="C152" s="167" t="s">
-        <v>618</v>
-      </c>
-      <c r="D152" s="167" t="s">
-        <v>619</v>
+        <v>651</v>
+      </c>
+      <c r="C152" s="183" t="s">
+        <v>663</v>
+      </c>
+      <c r="D152" s="183" t="s">
+        <v>664</v>
       </c>
       <c r="E152" s="160" t="str">
         <f t="shared" si="11"/>
         <v>[Manager-1]</v>
       </c>
-      <c r="F152" s="161"/>
+      <c r="F152" s="161" t="s">
+        <v>398</v>
+      </c>
       <c r="G152" s="162" t="s">
         <v>83</v>
       </c>
@@ -35887,25 +36097,27 @@
       </c>
       <c r="J152" s="179"/>
     </row>
-    <row r="153" ht="15.75" customHeight="1">
+    <row r="153" ht="97.5" customHeight="1">
       <c r="A153" s="160" t="str">
         <f t="shared" si="10"/>
         <v>[Manager-144]</v>
       </c>
       <c r="B153" s="160" t="s">
-        <v>606</v>
-      </c>
-      <c r="C153" s="167" t="s">
-        <v>620</v>
-      </c>
-      <c r="D153" s="167" t="s">
-        <v>621</v>
+        <v>651</v>
+      </c>
+      <c r="C153" s="183" t="s">
+        <v>665</v>
+      </c>
+      <c r="D153" s="183" t="s">
+        <v>666</v>
       </c>
       <c r="E153" s="160" t="str">
         <f t="shared" si="11"/>
         <v>[Manager-1]</v>
       </c>
-      <c r="F153" s="161"/>
+      <c r="F153" s="161" t="s">
+        <v>401</v>
+      </c>
       <c r="G153" s="162" t="s">
         <v>83</v>
       </c>
@@ -35923,19 +36135,21 @@
         <v>[Manager-145]</v>
       </c>
       <c r="B154" s="160" t="s">
-        <v>606</v>
-      </c>
-      <c r="C154" s="167" t="s">
-        <v>622</v>
-      </c>
-      <c r="D154" s="167" t="s">
-        <v>619</v>
+        <v>651</v>
+      </c>
+      <c r="C154" s="183" t="s">
+        <v>667</v>
+      </c>
+      <c r="D154" s="183" t="s">
+        <v>664</v>
       </c>
       <c r="E154" s="160" t="str">
         <f t="shared" si="11"/>
         <v>[Manager-1]</v>
       </c>
-      <c r="F154" s="161"/>
+      <c r="F154" s="161" t="s">
+        <v>401</v>
+      </c>
       <c r="G154" s="162" t="s">
         <v>83</v>
       </c>
@@ -35947,19 +36161,19 @@
       </c>
       <c r="J154" s="179"/>
     </row>
-    <row r="155" ht="15.75" customHeight="1">
+    <row r="155" ht="98.25" customHeight="1">
       <c r="A155" s="160" t="str">
         <f t="shared" si="10"/>
         <v>[Manager-146]</v>
       </c>
       <c r="B155" s="160" t="s">
-        <v>606</v>
-      </c>
-      <c r="C155" s="167" t="s">
-        <v>623</v>
-      </c>
-      <c r="D155" s="167" t="s">
-        <v>624</v>
+        <v>651</v>
+      </c>
+      <c r="C155" s="183" t="s">
+        <v>668</v>
+      </c>
+      <c r="D155" s="183" t="s">
+        <v>657</v>
       </c>
       <c r="E155" s="160" t="str">
         <f t="shared" si="11"/>
@@ -35977,19 +36191,19 @@
       </c>
       <c r="J155" s="179"/>
     </row>
-    <row r="156" ht="15.75" customHeight="1">
+    <row r="156" ht="93.0" customHeight="1">
       <c r="A156" s="160" t="str">
         <f t="shared" si="10"/>
         <v>[Manager-147]</v>
       </c>
       <c r="B156" s="160" t="s">
-        <v>606</v>
-      </c>
-      <c r="C156" s="167" t="s">
-        <v>625</v>
-      </c>
-      <c r="D156" s="167" t="s">
-        <v>624</v>
+        <v>651</v>
+      </c>
+      <c r="C156" s="183" t="s">
+        <v>669</v>
+      </c>
+      <c r="D156" s="183" t="s">
+        <v>664</v>
       </c>
       <c r="E156" s="160" t="str">
         <f t="shared" si="11"/>
@@ -36007,19 +36221,19 @@
       </c>
       <c r="J156" s="179"/>
     </row>
-    <row r="157" ht="15.75" customHeight="1">
+    <row r="157" ht="67.5" customHeight="1">
       <c r="A157" s="160" t="str">
         <f t="shared" si="10"/>
         <v>[Manager-148]</v>
       </c>
       <c r="B157" s="160" t="s">
-        <v>606</v>
-      </c>
-      <c r="C157" s="167" t="s">
-        <v>626</v>
-      </c>
-      <c r="D157" s="167" t="s">
-        <v>624</v>
+        <v>670</v>
+      </c>
+      <c r="C157" s="183" t="s">
+        <v>671</v>
+      </c>
+      <c r="D157" s="161" t="s">
+        <v>672</v>
       </c>
       <c r="E157" s="160" t="str">
         <f t="shared" si="11"/>
@@ -36040,7 +36254,16 @@
     <row r="158" ht="15.75" customHeight="1">
       <c r="A158" s="160" t="str">
         <f t="shared" si="10"/>
-        <v/>
+        <v>[Manager-149]</v>
+      </c>
+      <c r="B158" s="160" t="s">
+        <v>670</v>
+      </c>
+      <c r="C158" s="183" t="s">
+        <v>673</v>
+      </c>
+      <c r="D158" s="161" t="s">
+        <v>457</v>
       </c>
       <c r="E158" s="160" t="str">
         <f t="shared" si="11"/>
@@ -36061,7 +36284,16 @@
     <row r="159" ht="15.75" customHeight="1">
       <c r="A159" s="160" t="str">
         <f t="shared" si="10"/>
-        <v/>
+        <v>[Manager-150]</v>
+      </c>
+      <c r="B159" s="160" t="s">
+        <v>670</v>
+      </c>
+      <c r="C159" s="183" t="s">
+        <v>674</v>
+      </c>
+      <c r="D159" s="161" t="s">
+        <v>675</v>
       </c>
       <c r="E159" s="160" t="str">
         <f t="shared" si="11"/>
@@ -36069,7 +36301,7 @@
       </c>
       <c r="F159" s="161"/>
       <c r="G159" s="162" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H159" s="163">
         <v>44306.0</v>
@@ -36077,239 +36309,21 @@
       <c r="I159" s="166" t="s">
         <v>375</v>
       </c>
-      <c r="J159" s="179"/>
-    </row>
-    <row r="160" ht="15.75" customHeight="1">
-      <c r="A160" s="160" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="E160" s="160" t="str">
-        <f t="shared" si="11"/>
-        <v>[Manager-1]</v>
-      </c>
-      <c r="F160" s="161"/>
-      <c r="G160" s="162" t="s">
-        <v>83</v>
-      </c>
-      <c r="H160" s="163">
-        <v>44306.0</v>
-      </c>
-      <c r="I160" s="166" t="s">
-        <v>375</v>
-      </c>
-      <c r="J160" s="179"/>
-    </row>
-    <row r="161" ht="15.75" customHeight="1">
-      <c r="A161" s="160" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="E161" s="160" t="str">
-        <f t="shared" si="11"/>
-        <v>[Manager-1]</v>
-      </c>
-      <c r="F161" s="161"/>
-      <c r="G161" s="162" t="s">
-        <v>83</v>
-      </c>
-      <c r="H161" s="163">
-        <v>44306.0</v>
-      </c>
-      <c r="I161" s="166" t="s">
-        <v>375</v>
-      </c>
-      <c r="J161" s="179"/>
-    </row>
-    <row r="162" ht="15.75" customHeight="1">
-      <c r="A162" s="160" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="E162" s="160" t="str">
-        <f t="shared" si="11"/>
-        <v>[Manager-1]</v>
-      </c>
-      <c r="F162" s="161"/>
-      <c r="G162" s="162" t="s">
-        <v>83</v>
-      </c>
-      <c r="H162" s="163">
-        <v>44306.0</v>
-      </c>
-      <c r="I162" s="166" t="s">
-        <v>375</v>
-      </c>
-      <c r="J162" s="179"/>
-    </row>
-    <row r="163" ht="15.75" customHeight="1">
-      <c r="A163" s="160" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="E163" s="160" t="str">
-        <f t="shared" si="11"/>
-        <v>[Manager-1]</v>
-      </c>
-      <c r="F163" s="161"/>
-      <c r="G163" s="162" t="s">
-        <v>83</v>
-      </c>
-      <c r="H163" s="163">
-        <v>44306.0</v>
-      </c>
-      <c r="I163" s="166" t="s">
-        <v>375</v>
-      </c>
-      <c r="J163" s="179"/>
-    </row>
-    <row r="164" ht="15.75" customHeight="1">
-      <c r="A164" s="160" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="E164" s="160" t="str">
-        <f t="shared" si="11"/>
-        <v>[Manager-1]</v>
-      </c>
-      <c r="F164" s="161"/>
-      <c r="G164" s="162" t="s">
-        <v>83</v>
-      </c>
-      <c r="H164" s="163">
-        <v>44306.0</v>
-      </c>
-      <c r="I164" s="166" t="s">
-        <v>375</v>
-      </c>
-      <c r="J164" s="179"/>
-    </row>
-    <row r="165" ht="15.75" customHeight="1">
-      <c r="A165" s="160" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="E165" s="160" t="str">
-        <f t="shared" si="11"/>
-        <v>[Manager-1]</v>
-      </c>
-      <c r="F165" s="161"/>
-      <c r="G165" s="162" t="s">
-        <v>83</v>
-      </c>
-      <c r="H165" s="163">
-        <v>44306.0</v>
-      </c>
-      <c r="I165" s="166" t="s">
-        <v>375</v>
-      </c>
-      <c r="J165" s="179"/>
-    </row>
-    <row r="166" ht="15.75" customHeight="1">
-      <c r="A166" s="160" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="E166" s="160" t="str">
-        <f t="shared" si="11"/>
-        <v>[Manager-1]</v>
-      </c>
-      <c r="F166" s="161"/>
-      <c r="G166" s="162" t="s">
-        <v>83</v>
-      </c>
-      <c r="H166" s="163">
-        <v>44306.0</v>
-      </c>
-      <c r="I166" s="166" t="s">
-        <v>375</v>
-      </c>
-      <c r="J166" s="179"/>
-    </row>
-    <row r="167" ht="15.75" customHeight="1">
-      <c r="A167" s="160" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="E167" s="160" t="str">
-        <f t="shared" si="11"/>
-        <v>[Manager-1]</v>
-      </c>
-      <c r="F167" s="161"/>
-      <c r="G167" s="162" t="s">
-        <v>83</v>
-      </c>
-      <c r="H167" s="163">
-        <v>44306.0</v>
-      </c>
-      <c r="I167" s="166" t="s">
-        <v>375</v>
-      </c>
-      <c r="J167" s="179"/>
-    </row>
-    <row r="168" ht="15.75" customHeight="1">
-      <c r="A168" s="160" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="E168" s="160" t="str">
-        <f t="shared" si="11"/>
-        <v>[Manager-1]</v>
-      </c>
-      <c r="F168" s="161"/>
-      <c r="G168" s="162" t="s">
-        <v>83</v>
-      </c>
-      <c r="H168" s="163">
-        <v>44306.0</v>
-      </c>
-      <c r="I168" s="166" t="s">
-        <v>375</v>
-      </c>
-      <c r="J168" s="179"/>
-    </row>
-    <row r="169" ht="15.75" customHeight="1">
-      <c r="A169" s="160" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="E169" s="160" t="str">
-        <f t="shared" si="11"/>
-        <v>[Manager-1]</v>
-      </c>
-      <c r="F169" s="161"/>
-      <c r="G169" s="162" t="s">
-        <v>83</v>
-      </c>
-      <c r="H169" s="163">
-        <v>44306.0</v>
-      </c>
-      <c r="I169" s="166" t="s">
-        <v>375</v>
-      </c>
-      <c r="J169" s="179"/>
-    </row>
-    <row r="170" ht="15.75" customHeight="1">
-      <c r="A170" s="160" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="E170" s="160" t="str">
-        <f t="shared" si="11"/>
-        <v>[Manager-1]</v>
-      </c>
-      <c r="F170" s="161"/>
-      <c r="G170" s="162" t="s">
-        <v>83</v>
-      </c>
-      <c r="H170" s="163">
-        <v>44306.0</v>
-      </c>
-      <c r="I170" s="166" t="s">
-        <v>375</v>
-      </c>
-      <c r="J170" s="179"/>
-    </row>
+      <c r="J159" s="162" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="160" ht="15.75" customHeight="1"/>
+    <row r="161" ht="15.75" customHeight="1"/>
+    <row r="162" ht="15.75" customHeight="1"/>
+    <row r="163" ht="15.75" customHeight="1"/>
+    <row r="164" ht="15.75" customHeight="1"/>
+    <row r="165" ht="15.75" customHeight="1"/>
+    <row r="166" ht="15.75" customHeight="1"/>
+    <row r="167" ht="15.75" customHeight="1"/>
+    <row r="168" ht="15.75" customHeight="1"/>
+    <row r="169" ht="15.75" customHeight="1"/>
+    <row r="170" ht="15.75" customHeight="1"/>
     <row r="171" ht="15.75" customHeight="1"/>
     <row r="172" ht="15.75" customHeight="1"/>
     <row r="173" ht="15.75" customHeight="1"/>
@@ -37139,17 +37153,6 @@
     <row r="997" ht="15.75" customHeight="1"/>
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
-    <row r="1000" ht="15.75" customHeight="1"/>
-    <row r="1001" ht="15.75" customHeight="1"/>
-    <row r="1002" ht="15.75" customHeight="1"/>
-    <row r="1003" ht="15.75" customHeight="1"/>
-    <row r="1004" ht="15.75" customHeight="1"/>
-    <row r="1005" ht="15.75" customHeight="1"/>
-    <row r="1006" ht="15.75" customHeight="1"/>
-    <row r="1007" ht="15.75" customHeight="1"/>
-    <row r="1008" ht="15.75" customHeight="1"/>
-    <row r="1009" ht="15.75" customHeight="1"/>
-    <row r="1010" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B2:E2"/>
@@ -37157,7 +37160,7 @@
     <mergeCell ref="B4:E4"/>
   </mergeCells>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G8:G73 G101 G118:G170">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G8:G73 G101 G118:G159">
       <formula1>$M$2:$M$5</formula1>
     </dataValidation>
   </dataValidations>
@@ -37193,15 +37196,15 @@
   <sheetData>
     <row r="1" ht="25.5" customHeight="1">
       <c r="A1" s="11"/>
-      <c r="B1" s="186" t="s">
-        <v>641</v>
-      </c>
-      <c r="C1" s="187"/>
-      <c r="D1" s="187"/>
-      <c r="E1" s="187"/>
-      <c r="F1" s="187"/>
-      <c r="G1" s="187"/>
-      <c r="H1" s="187"/>
+      <c r="B1" s="187" t="s">
+        <v>677</v>
+      </c>
+      <c r="C1" s="188"/>
+      <c r="D1" s="188"/>
+      <c r="E1" s="188"/>
+      <c r="F1" s="188"/>
+      <c r="G1" s="188"/>
+      <c r="H1" s="188"/>
       <c r="I1" s="11"/>
       <c r="J1" s="11"/>
       <c r="K1" s="11"/>
@@ -37222,14 +37225,14 @@
       <c r="Z1" s="11"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="188"/>
-      <c r="B2" s="188"/>
+      <c r="A2" s="189"/>
+      <c r="B2" s="189"/>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
       <c r="F2" s="11"/>
       <c r="G2" s="11"/>
-      <c r="H2" s="189"/>
+      <c r="H2" s="190"/>
       <c r="I2" s="11"/>
       <c r="J2" s="11"/>
       <c r="K2" s="11"/>
@@ -37251,19 +37254,19 @@
     </row>
     <row r="3" ht="12.0" customHeight="1">
       <c r="A3" s="11"/>
-      <c r="B3" s="190" t="s">
+      <c r="B3" s="191" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="49" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="6"/>
-      <c r="E3" s="191" t="s">
+      <c r="E3" s="192" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="6"/>
-      <c r="G3" s="192"/>
-      <c r="H3" s="193" t="s">
+      <c r="G3" s="193"/>
+      <c r="H3" s="194" t="s">
         <v>4</v>
       </c>
       <c r="I3" s="11"/>
@@ -37287,19 +37290,19 @@
     </row>
     <row r="4" ht="12.0" customHeight="1">
       <c r="A4" s="11"/>
-      <c r="B4" s="190" t="s">
+      <c r="B4" s="191" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="49" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="6"/>
-      <c r="E4" s="191" t="s">
+      <c r="E4" s="192" t="s">
         <v>6</v>
       </c>
       <c r="F4" s="6"/>
-      <c r="G4" s="192"/>
-      <c r="H4" s="193" t="s">
+      <c r="G4" s="193"/>
+      <c r="H4" s="194" t="s">
         <v>7</v>
       </c>
       <c r="I4" s="11"/>
@@ -37323,7 +37326,7 @@
     </row>
     <row r="5" ht="12.0" customHeight="1">
       <c r="A5" s="11"/>
-      <c r="B5" s="194" t="s">
+      <c r="B5" s="195" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="49" t="str">
@@ -37331,12 +37334,12 @@
         <v>SoFa_Test Report_vx.x</v>
       </c>
       <c r="D5" s="6"/>
-      <c r="E5" s="191" t="s">
+      <c r="E5" s="192" t="s">
         <v>9</v>
       </c>
       <c r="F5" s="6"/>
-      <c r="G5" s="192"/>
-      <c r="H5" s="195">
+      <c r="G5" s="193"/>
+      <c r="H5" s="196">
         <v>44534.0</v>
       </c>
       <c r="I5" s="11"/>
@@ -37359,12 +37362,12 @@
       <c r="Z5" s="11"/>
     </row>
     <row r="6" ht="21.75" customHeight="1">
-      <c r="A6" s="188"/>
-      <c r="B6" s="194" t="s">
-        <v>642</v>
-      </c>
-      <c r="C6" s="196" t="s">
-        <v>643</v>
+      <c r="A6" s="189"/>
+      <c r="B6" s="195" t="s">
+        <v>678</v>
+      </c>
+      <c r="C6" s="197" t="s">
+        <v>679</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -37391,14 +37394,14 @@
       <c r="Z6" s="11"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="188"/>
+      <c r="A7" s="189"/>
       <c r="B7" s="25"/>
-      <c r="C7" s="197"/>
+      <c r="C7" s="198"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
-      <c r="H7" s="189"/>
+      <c r="H7" s="190"/>
       <c r="I7" s="11"/>
       <c r="J7" s="11"/>
       <c r="K7" s="11"/>
@@ -37421,12 +37424,12 @@
     <row r="8" ht="12.75" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="25"/>
-      <c r="C8" s="197"/>
+      <c r="C8" s="198"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
-      <c r="H8" s="189"/>
+      <c r="H8" s="190"/>
       <c r="I8" s="11"/>
       <c r="J8" s="11"/>
       <c r="K8" s="11"/>
@@ -37475,27 +37478,27 @@
       <c r="Z9" s="11"/>
     </row>
     <row r="10" ht="12.75" customHeight="1">
-      <c r="A10" s="198"/>
-      <c r="B10" s="199" t="s">
+      <c r="A10" s="199"/>
+      <c r="B10" s="200" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="200" t="s">
-        <v>644</v>
-      </c>
-      <c r="D10" s="201" t="s">
+      <c r="C10" s="201" t="s">
+        <v>680</v>
+      </c>
+      <c r="D10" s="202" t="s">
         <v>83</v>
       </c>
-      <c r="E10" s="200" t="s">
+      <c r="E10" s="201" t="s">
         <v>86</v>
       </c>
-      <c r="F10" s="200" t="s">
+      <c r="F10" s="201" t="s">
         <v>89</v>
       </c>
-      <c r="G10" s="202" t="s">
+      <c r="G10" s="203" t="s">
         <v>90</v>
       </c>
-      <c r="H10" s="203" t="s">
-        <v>645</v>
+      <c r="H10" s="204" t="s">
+        <v>681</v>
       </c>
       <c r="I10" s="11"/>
       <c r="J10" s="11"/>
@@ -37517,31 +37520,31 @@
       <c r="Z10" s="11"/>
     </row>
     <row r="11" ht="12.75" customHeight="1">
-      <c r="A11" s="198"/>
-      <c r="B11" s="204">
+      <c r="A11" s="199"/>
+      <c r="B11" s="205">
         <v>1.0</v>
       </c>
-      <c r="C11" s="205" t="str">
+      <c r="C11" s="206" t="str">
         <f>Guest!B2</f>
         <v>Guest</v>
       </c>
-      <c r="D11" s="206">
+      <c r="D11" s="207">
         <f>Guest!A6</f>
         <v>43</v>
       </c>
-      <c r="E11" s="206">
+      <c r="E11" s="207">
         <f>Guest!B6</f>
         <v>4</v>
       </c>
-      <c r="F11" s="206">
+      <c r="F11" s="207">
         <f>Guest!C6</f>
         <v>3</v>
       </c>
-      <c r="G11" s="207">
+      <c r="G11" s="208">
         <f>Guest!D6</f>
         <v>0</v>
       </c>
-      <c r="H11" s="208">
+      <c r="H11" s="209">
         <f>Guest!E6</f>
         <v>50</v>
       </c>
@@ -37565,31 +37568,31 @@
       <c r="Z11" s="11"/>
     </row>
     <row r="12" ht="12.75" customHeight="1">
-      <c r="A12" s="198"/>
-      <c r="B12" s="204">
+      <c r="A12" s="199"/>
+      <c r="B12" s="205">
         <v>2.0</v>
       </c>
-      <c r="C12" s="205" t="str">
+      <c r="C12" s="206" t="str">
         <f>User!B2</f>
         <v>User</v>
       </c>
-      <c r="D12" s="206">
+      <c r="D12" s="207">
         <f>User!A6</f>
         <v>0</v>
       </c>
-      <c r="E12" s="206">
+      <c r="E12" s="207">
         <f>User!B6</f>
         <v>0</v>
       </c>
-      <c r="F12" s="206">
+      <c r="F12" s="207">
         <f>User!C6</f>
         <v>51</v>
       </c>
-      <c r="G12" s="206">
+      <c r="G12" s="207">
         <f>User!D6</f>
         <v>0</v>
       </c>
-      <c r="H12" s="206">
+      <c r="H12" s="207">
         <f>User!E6</f>
         <v>51</v>
       </c>
@@ -37613,31 +37616,31 @@
       <c r="Z12" s="11"/>
     </row>
     <row r="13" ht="12.75" customHeight="1">
-      <c r="A13" s="198"/>
-      <c r="B13" s="204">
+      <c r="A13" s="199"/>
+      <c r="B13" s="205">
         <v>1.0</v>
       </c>
-      <c r="C13" s="205" t="str">
+      <c r="C13" s="206" t="str">
         <f>Manager!B2</f>
         <v>Manager</v>
       </c>
-      <c r="D13" s="206">
+      <c r="D13" s="207">
         <f>Manager!A6</f>
         <v>0</v>
       </c>
-      <c r="E13" s="206">
+      <c r="E13" s="207">
         <f>Manager!B6</f>
         <v>0</v>
       </c>
-      <c r="F13" s="206">
+      <c r="F13" s="207">
         <f>Manager!C6</f>
         <v>0</v>
       </c>
-      <c r="G13" s="207">
+      <c r="G13" s="208">
         <f>Manager!D6</f>
         <v>0</v>
       </c>
-      <c r="H13" s="208">
+      <c r="H13" s="209">
         <f>Manager!E6</f>
         <v>0</v>
       </c>
@@ -37661,28 +37664,28 @@
       <c r="Z13" s="11"/>
     </row>
     <row r="14" ht="12.75" customHeight="1">
-      <c r="A14" s="198"/>
-      <c r="B14" s="209"/>
-      <c r="C14" s="210" t="s">
-        <v>646</v>
-      </c>
-      <c r="D14" s="211">
+      <c r="A14" s="199"/>
+      <c r="B14" s="210"/>
+      <c r="C14" s="211" t="s">
+        <v>682</v>
+      </c>
+      <c r="D14" s="212">
         <f t="shared" ref="D14:H14" si="1">SUM(D9:D13)</f>
         <v>43</v>
       </c>
-      <c r="E14" s="211">
+      <c r="E14" s="212">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="F14" s="211">
+      <c r="F14" s="212">
         <f t="shared" si="1"/>
         <v>54</v>
       </c>
-      <c r="G14" s="211">
+      <c r="G14" s="212">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H14" s="212">
+      <c r="H14" s="213">
         <f t="shared" si="1"/>
         <v>101</v>
       </c>
@@ -37707,13 +37710,13 @@
     </row>
     <row r="15" ht="12.75" customHeight="1">
       <c r="A15" s="11"/>
-      <c r="B15" s="213"/>
+      <c r="B15" s="214"/>
       <c r="C15" s="11"/>
-      <c r="D15" s="214"/>
-      <c r="E15" s="215"/>
-      <c r="F15" s="215"/>
-      <c r="G15" s="215"/>
-      <c r="H15" s="215"/>
+      <c r="D15" s="215"/>
+      <c r="E15" s="216"/>
+      <c r="F15" s="216"/>
+      <c r="G15" s="216"/>
+      <c r="H15" s="216"/>
       <c r="I15" s="11"/>
       <c r="J15" s="11"/>
       <c r="K15" s="11"/>
@@ -37737,15 +37740,15 @@
       <c r="A16" s="11"/>
       <c r="B16" s="11"/>
       <c r="C16" s="9" t="s">
-        <v>647</v>
+        <v>683</v>
       </c>
       <c r="D16" s="11"/>
-      <c r="E16" s="216">
+      <c r="E16" s="217">
         <f>(D14+E14)*100/(H14-G14)</f>
         <v>46.53465347</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>648</v>
+        <v>684</v>
       </c>
       <c r="G16" s="11"/>
       <c r="H16" s="132"/>
@@ -37772,15 +37775,15 @@
       <c r="A17" s="11"/>
       <c r="B17" s="11"/>
       <c r="C17" s="9" t="s">
-        <v>649</v>
+        <v>685</v>
       </c>
       <c r="D17" s="11"/>
-      <c r="E17" s="216">
+      <c r="E17" s="217">
         <f>D14*100/(H14-G14)</f>
         <v>42.57425743</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>648</v>
+        <v>684</v>
       </c>
       <c r="G17" s="11"/>
       <c r="H17" s="132"/>

</xml_diff>